<commit_message>
New models + cov sim functions
New models added to load_G_models() and coverage sim functions moved to functions.py
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ADEC929-2C7C-BB46-95F9-B7EEF413DF92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F4A8D6-C114-1D4D-B891-5F005F6D3458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20820" yWindow="6080" windowWidth="23460" windowHeight="18480" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19200" windowHeight="14840" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Keeping up with the thesis</t>
   </si>
@@ -44,16 +44,10 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Number of words written</t>
-  </si>
-  <si>
     <t>Percentage finished</t>
   </si>
   <si>
     <t>Numbers</t>
-  </si>
-  <si>
-    <t>Pages written</t>
   </si>
   <si>
     <t>Words per page:</t>
@@ -66,6 +60,15 @@
   </si>
   <si>
     <t>Maybe a lil' plot here?</t>
+  </si>
+  <si>
+    <t>Words written today</t>
+  </si>
+  <si>
+    <t>Words written total</t>
+  </si>
+  <si>
+    <t>Pages written total</t>
   </si>
 </sst>
 </file>
@@ -158,15 +161,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -195,6 +189,17 @@
     <border>
       <left/>
       <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -316,30 +321,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
@@ -356,17 +348,61 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="170" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="171" fontId="0" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -686,422 +722,439 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="21.83203125" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="0.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="6" width="12.1640625" customWidth="1"/>
+    <col min="7" max="7" width="1.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="20"/>
     </row>
     <row r="2" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="19" t="s">
+      <c r="A2" s="21"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="22"/>
+    </row>
+    <row r="3" spans="1:11" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="23"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="25"/>
+    </row>
+    <row r="4" spans="1:11" ht="5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:11" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="H5" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="I5" s="30"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="15"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B6" s="12">
+        <v>45138</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="16">
+        <f>D6/$J$6</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="17">
+        <f>D6/$J$8</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="4"/>
+      <c r="J6" s="6">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B7" s="12">
+        <v>45139</v>
+      </c>
+      <c r="C7" s="2">
+        <v>156</v>
+      </c>
+      <c r="D7" s="2">
+        <v>156</v>
+      </c>
+      <c r="E7" s="16">
+        <f t="shared" ref="E7:E27" si="0">D7/$J$6</f>
+        <v>0.45614035087719296</v>
+      </c>
+      <c r="F7" s="17">
+        <f t="shared" ref="F7:F27" si="1">D7/$J$8</f>
+        <v>7.6023391812865496E-3</v>
+      </c>
+      <c r="H7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="7"/>
-      <c r="I5" s="8"/>
-      <c r="K5" s="23"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B6" s="20">
-        <v>45138</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0</v>
-      </c>
-      <c r="D6" s="24">
-        <f>C6/$I$6</f>
-        <v>0</v>
-      </c>
-      <c r="E6" s="25">
-        <f>C6/$I$8</f>
-        <v>0</v>
-      </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="10" t="s">
+      <c r="I7" s="8"/>
+      <c r="J7" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="12">
+        <v>45140</v>
+      </c>
+      <c r="C8" s="2">
+        <f>D8-D7</f>
+        <v>38</v>
+      </c>
+      <c r="D8" s="2">
+        <v>194</v>
+      </c>
+      <c r="E8" s="16">
+        <f t="shared" si="0"/>
+        <v>0.56725146198830412</v>
+      </c>
+      <c r="F8" s="17">
+        <f t="shared" si="1"/>
+        <v>9.4541910331384024E-3</v>
+      </c>
+      <c r="H8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="9"/>
-      <c r="I6" s="11">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B7" s="20">
-        <v>45139</v>
-      </c>
-      <c r="C7" s="3">
-        <v>156</v>
-      </c>
-      <c r="D7" s="24">
-        <f t="shared" ref="D7:D27" si="0">C7/$I$6</f>
-        <v>0.45614035087719296</v>
-      </c>
-      <c r="E7" s="25">
-        <f t="shared" ref="E7:E27" si="1">C7/$I$8</f>
-        <v>7.6023391812865496E-3</v>
-      </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="12" t="s">
+      <c r="I8" s="10"/>
+      <c r="J8" s="11">
+        <v>20520</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B9" s="13"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F9" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B10" s="13"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="11">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="21"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E8" s="25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F8" s="5"/>
-      <c r="G8" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="15"/>
-      <c r="I8" s="16">
-        <v>20520</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B9" s="21"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E9" s="25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="21"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E10" s="25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B11" s="21"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E11" s="25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F11" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B12" s="21"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E12" s="25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F12" s="5"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="33"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B13" s="21"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E13" s="25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F13" s="5"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F13" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B14" s="21"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E14" s="25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F14" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="33"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B15" s="21"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E15" s="25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F15" s="5"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="33"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B16" s="21"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E16" s="25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F16" s="5"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F16" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B17" s="21"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E17" s="25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F17" s="5"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B18" s="21"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E18" s="25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F18" s="5"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F18" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B19" s="21"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E19" s="25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F19" s="5"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B20" s="21"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E20" s="25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F20" s="5"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B21" s="21"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E21" s="25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F21" s="5"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B22" s="21"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E22" s="25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F22" s="5"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B23" s="21"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E23" s="25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F23" s="5"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F23" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B24" s="21"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E24" s="25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F24" s="5"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F24" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B25" s="21"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E25" s="25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F25" s="5"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B26" s="21"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E26" s="25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F26" s="5"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F26" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="22"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E27" s="25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F27" s="5"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F27" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G10:I16"/>
-    <mergeCell ref="A1:J3"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
+  <mergeCells count="5">
+    <mergeCell ref="A1:K3"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Coverage simulation running + First actual writing
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F4A8D6-C114-1D4D-B891-5F005F6D3458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{723D694D-7632-F44A-B585-CF5D1162F1C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19200" windowHeight="14840" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="14420" windowHeight="14840" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -722,7 +722,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -879,16 +879,23 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B9" s="13"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="B9" s="12">
+        <v>45141</v>
+      </c>
+      <c r="C9" s="2">
+        <f>D9-D8</f>
+        <v>486</v>
+      </c>
+      <c r="D9" s="2">
+        <v>680</v>
+      </c>
       <c r="E9" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.9883040935672514</v>
       </c>
       <c r="F9" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.3138401559454189E-2</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Writing introduction about climate change
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{723D694D-7632-F44A-B585-CF5D1162F1C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8698AF99-4C47-2D49-B953-8D4418BA6ACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14420" windowHeight="14840" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
@@ -722,7 +722,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -899,16 +899,23 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="13"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="B10" s="12">
+        <v>45142</v>
+      </c>
+      <c r="C10" s="2">
+        <f>D10-D9</f>
+        <v>346</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1026</v>
+      </c>
       <c r="E10" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F10" s="17">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="H10" s="33" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Wrote 2.5 page in one day!
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,13 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976712EA-0CA9-A943-A839-6AD377A1F8C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112606ED-906F-F84A-AC23-BD69AE95816E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14420" windowHeight="14840" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$B$6:$B$27</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$D$6:$D$27</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$6:$B$27</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$D$6:$D$27</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$B$6:$B$27</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$D$6:$D$27</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Keeping up with the thesis</t>
   </si>
@@ -59,9 +67,6 @@
     <t>Words per thesis:</t>
   </si>
   <si>
-    <t>Maybe a lil' plot here?</t>
-  </si>
-  <si>
     <t>Words written today</t>
   </si>
   <si>
@@ -71,7 +76,16 @@
     <t>Pages written total</t>
   </si>
   <si>
-    <t>try to get 1000</t>
+    <t>Statistics</t>
+  </si>
+  <si>
+    <t>Remaining words:</t>
+  </si>
+  <si>
+    <t>Average pace:</t>
+  </si>
+  <si>
+    <t>Remaining days:</t>
   </si>
 </sst>
 </file>
@@ -82,7 +96,7 @@
     <numFmt numFmtId="170" formatCode="0.0"/>
     <numFmt numFmtId="171" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -98,6 +112,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -105,7 +128,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -150,7 +173,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -324,11 +353,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -337,7 +363,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -350,62 +375,112 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="170" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="171" fontId="0" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="170" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="171" fontId="0" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -423,6 +498,919 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Total words written</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-DK"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$6:$B$27</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yy</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>45138</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45139</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45140</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45141</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45142</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45145</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45146</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$6:$D$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>680</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1026</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1755</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2614</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E621-8F4D-8065-FED201971DA0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="294074880"/>
+        <c:axId val="656428208"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="294074880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-3120000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="656428208"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="656428208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="294074880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-DK"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>8466</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>8465</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>8467</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>220132</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D800AF5-326E-7E52-C2A1-7BBCADECF694}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -724,8 +1712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4213BD91-B5D1-3B47-8D3F-04331482504C}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -734,285 +1722,302 @@
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" customWidth="1"/>
     <col min="5" max="6" width="12.1640625" customWidth="1"/>
-    <col min="7" max="7" width="1.1640625" customWidth="1"/>
+    <col min="7" max="7" width="1" customWidth="1"/>
+    <col min="11" max="11" width="0.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="20"/>
+      <c r="A1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="26"/>
     </row>
     <row r="2" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="21"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="22"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="29"/>
     </row>
     <row r="3" spans="1:11" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="25"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="32"/>
     </row>
     <row r="4" spans="1:11" ht="5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:11" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="E5" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="35" t="s">
+      <c r="F5" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="29" t="s">
+      <c r="H5" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="30"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="15"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="12"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B6" s="12">
+      <c r="B6" s="9">
         <v>45138</v>
       </c>
-      <c r="C6" s="2">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0</v>
-      </c>
-      <c r="E6" s="16">
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="13">
         <f>D6/$J$6</f>
         <v>0</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="14">
         <f>D6/$J$8</f>
         <v>0</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="6">
+      <c r="I6" s="3"/>
+      <c r="J6" s="46">
         <v>342</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B7" s="12">
+      <c r="B7" s="9">
         <v>45139</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>156</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>156</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="13">
         <f t="shared" ref="E7:E27" si="0">D7/$J$6</f>
         <v>0.45614035087719296</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="14">
         <f t="shared" ref="F7:F27" si="1">D7/$J$8</f>
         <v>7.6023391812865496E-3</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="8"/>
-      <c r="J7" s="6">
+      <c r="I7" s="6"/>
+      <c r="J7" s="46">
         <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="12">
+      <c r="B8" s="9">
         <v>45140</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <f>D8-D7</f>
         <v>38</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>194</v>
       </c>
-      <c r="E8" s="16">
+      <c r="E8" s="13">
         <f t="shared" si="0"/>
         <v>0.56725146198830412</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="14">
         <f t="shared" si="1"/>
         <v>9.4541910331384024E-3</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="10"/>
-      <c r="J8" s="11">
+      <c r="I8" s="8"/>
+      <c r="J8" s="47">
+        <f>J6*J7</f>
         <v>20520</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B9" s="12">
+    <row r="9" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="9">
         <v>45141</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <f>D9-D8</f>
         <v>486</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>680</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="13">
         <f t="shared" si="0"/>
         <v>1.9883040935672514</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="14">
         <f t="shared" si="1"/>
         <v>3.3138401559454189E-2</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="12">
+      <c r="B10" s="9">
         <v>45142</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <f>D10-D9</f>
         <v>346</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <v>1026</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="13">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F10" s="17">
+      <c r="F10" s="14">
         <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
-      <c r="H10" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B11" s="12">
+      <c r="H10" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="35"/>
+      <c r="J10" s="36"/>
+    </row>
+    <row r="11" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="9">
         <v>45145</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <f>D11-D10</f>
         <v>729</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <v>1755</v>
       </c>
-      <c r="E11" s="16">
+      <c r="E11" s="13">
         <f t="shared" si="0"/>
         <v>5.1315789473684212</v>
       </c>
-      <c r="F11" s="17">
+      <c r="F11" s="14">
         <f t="shared" si="1"/>
         <v>8.5526315789473686E-2</v>
       </c>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="39"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B12" s="12">
+      <c r="B12" s="9">
         <v>45146</v>
       </c>
-      <c r="C12" s="2" t="e">
+      <c r="C12" s="1">
         <f>D12-D11</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D12" s="2" t="s">
+        <v>859</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2614</v>
+      </c>
+      <c r="E12" s="13">
+        <f t="shared" si="0"/>
+        <v>7.6432748538011692</v>
+      </c>
+      <c r="F12" s="14">
+        <f t="shared" si="1"/>
+        <v>0.12738791423001949</v>
+      </c>
+      <c r="H12" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="16" t="e">
+      <c r="I12" s="42"/>
+      <c r="J12" s="48">
+        <f>J8-MAX(D6:D27)</f>
+        <v>17906</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B13" s="9"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="13">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F12" s="17" t="e">
+        <v>0</v>
+      </c>
+      <c r="F13" s="14">
         <f t="shared" si="1"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B13" s="13"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="16">
+        <v>0</v>
+      </c>
+      <c r="H13" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="I13" s="43"/>
+      <c r="J13" s="48">
+        <f>AVERAGE(C9:C27)</f>
+        <v>605</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="10"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F13" s="17">
+      <c r="F14" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B14" s="13"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="16">
+      <c r="H14" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" s="45"/>
+      <c r="J14" s="49">
+        <f>J12/J13</f>
+        <v>29.596694214876035</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B15" s="10"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F14" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B15" s="13"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F15" s="17">
+      <c r="F15" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1021,172 +2026,174 @@
       <c r="J15" s="33"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B16" s="13"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="16">
+      <c r="B16" s="10"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F16" s="17">
+      <c r="F16" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B17" s="13"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="16">
+      <c r="B17" s="10"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F17" s="17">
+      <c r="F17" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B18" s="13"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="16">
+      <c r="B18" s="10"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F18" s="17">
+      <c r="F18" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B19" s="13"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="16">
+      <c r="B19" s="10"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F19" s="17">
+      <c r="F19" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B20" s="13"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="16">
+      <c r="B20" s="10"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F20" s="17">
+      <c r="F20" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B21" s="13"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="16">
+      <c r="B21" s="10"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F21" s="17">
+      <c r="F21" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B22" s="13"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="16">
+      <c r="B22" s="10"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F22" s="17">
+      <c r="F22" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B23" s="13"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="16">
+      <c r="B23" s="10"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F23" s="17">
+      <c r="F23" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B24" s="13"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="16">
+      <c r="B24" s="10"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F24" s="17">
+      <c r="F24" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B25" s="13"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="16">
+      <c r="B25" s="10"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F25" s="17">
+      <c r="F25" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B26" s="13"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="16">
+      <c r="B26" s="10"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F26" s="17">
+      <c r="F26" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="14"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="26">
+      <c r="B27" s="11"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F27" s="27">
+      <c r="F27" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="9">
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
     <mergeCell ref="A1:K3"/>
     <mergeCell ref="H5:J5"/>
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H10:J11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Man kan ikke vinde hver gang
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112606ED-906F-F84A-AC23-BD69AE95816E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B378A207-6CEB-6048-A926-524E4A27CBD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14420" windowHeight="14840" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
@@ -611,6 +611,9 @@
                 <c:pt idx="6">
                   <c:v>45146</c:v>
                 </c:pt>
+                <c:pt idx="7">
+                  <c:v>45147</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -640,6 +643,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>2614</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2721</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1712,8 +1718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4213BD91-B5D1-3B47-8D3F-04331482504C}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1964,27 +1970,34 @@
       <c r="I12" s="42"/>
       <c r="J12" s="48">
         <f>J8-MAX(D6:D27)</f>
-        <v>17906</v>
+        <v>17799</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B13" s="9"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="B13" s="9">
+        <v>45147</v>
+      </c>
+      <c r="C13" s="1">
+        <f>D13-D12</f>
+        <v>107</v>
+      </c>
+      <c r="D13" s="1">
+        <v>2721</v>
+      </c>
       <c r="E13" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7.9561403508771926</v>
       </c>
       <c r="F13" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.13260233918128655</v>
       </c>
       <c r="H13" s="40" t="s">
         <v>12</v>
       </c>
       <c r="I13" s="43"/>
       <c r="J13" s="48">
-        <f>AVERAGE(C9:C27)</f>
+        <f>AVERAGE(C9:C12)</f>
         <v>605</v>
       </c>
     </row>
@@ -2006,7 +2019,7 @@
       <c r="I14" s="45"/>
       <c r="J14" s="49">
         <f>J12/J13</f>
-        <v>29.596694214876035</v>
+        <v>29.419834710743803</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Great writing day! 4000 words milestone!
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,21 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B378A207-6CEB-6048-A926-524E4A27CBD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC66F44-71F4-C240-B1BF-AF65E031D799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="14420" windowHeight="14840" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="14420" windowHeight="17900" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$B$6:$B$27</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$D$6:$D$27</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$6:$B$27</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$D$6:$D$27</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$B$6:$B$27</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$D$6:$D$27</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -43,8 +35,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Keeping up with the thesis</t>
   </si>
@@ -87,12 +101,46 @@
   <si>
     <t>Remaining days:</t>
   </si>
+  <si>
+    <t>Sorted wordcount</t>
+  </si>
+  <si>
+    <t>Sorted dates</t>
+  </si>
+  <si>
+    <t>Best day</t>
+  </si>
+  <si>
+    <t>Second best</t>
+  </si>
+  <si>
+    <t>Third best</t>
+  </si>
+  <si>
+    <t>Fourth best</t>
+  </si>
+  <si>
+    <t>Fifth best</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Sorted words not current</t>
+  </si>
+  <si>
+    <t>Sorted words current</t>
+  </si>
+  <si>
+    <t>100w change</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="170" formatCode="0.0"/>
     <numFmt numFmtId="171" formatCode="0.0%"/>
   </numFmts>
@@ -190,21 +238,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -348,52 +381,66 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="170" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="4" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="0" fillId="4" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="4" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -401,7 +448,7 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -413,12 +460,12 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -428,19 +475,19 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -449,43 +496,50 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
+    <cellStyle name="Per cent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -614,6 +668,9 @@
                 <c:pt idx="7">
                   <c:v>45147</c:v>
                 </c:pt>
+                <c:pt idx="8">
+                  <c:v>45148</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -646,6 +703,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>2721</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -790,7 +850,10 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:schemeClr val="accent1">
+        <a:lumMod val="40000"/>
+        <a:lumOff val="60000"/>
+      </a:schemeClr>
     </a:solidFill>
     <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
@@ -810,6 +873,383 @@
             <a:schemeClr val="tx1"/>
           </a:solidFill>
         </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-DK"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1050"/>
+              <a:t>Most productive days</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-DK"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Not today</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$L$29:$L$33</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Best day</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Second best</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Third best</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Fourth best</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Fifth best</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$P$29:$P$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>859</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>729</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>486</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>346</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000018-9653-1C40-B598-CD7F7B9C621B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Today</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$L$29:$L$33</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Best day</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Second best</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Third best</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Fourth best</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Fifth best</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Q$29:$Q$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1279</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000019-9653-1C40-B598-CD7F7B9C621B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="52"/>
+        <c:overlap val="96"/>
+        <c:axId val="813497808"/>
+        <c:axId val="813359696"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="813497808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="813359696"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="813359696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700">
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="813497808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="accent6">
+        <a:lumMod val="40000"/>
+        <a:lumOff val="60000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
       </a:pPr>
       <a:endParaRPr lang="en-DK"/>
     </a:p>
@@ -862,6 +1302,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -1025,6 +1505,509 @@
       <a:solidFill>
         <a:schemeClr val="phClr"/>
       </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1414,6 +2397,102 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>825499</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>206374</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4FB04AB-DBDF-7691-65FA-9151E3CFD3E2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>7936</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>531812</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>7936</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rectangle 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8279344-2A5F-EAFE-463C-CECAD37EC517}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7310438" y="5667374"/>
+          <a:ext cx="5453062" cy="4627562"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1716,10 +2795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4213BD91-B5D1-3B47-8D3F-04331482504C}">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:Q50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1733,72 +2812,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="26"/>
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="25"/>
     </row>
     <row r="2" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="27"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="29"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="28"/>
     </row>
     <row r="3" spans="1:11" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="30"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="32"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="31"/>
     </row>
     <row r="4" spans="1:11" ht="5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:11" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="21" t="s">
+      <c r="H5" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="22"/>
-      <c r="J5" s="23"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="22"/>
       <c r="K5" s="12"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B6" s="9">
+      <c r="B6" s="51">
         <v>45138</v>
       </c>
       <c r="C6" s="1">
@@ -1819,7 +2898,7 @@
         <v>4</v>
       </c>
       <c r="I6" s="3"/>
-      <c r="J6" s="46">
+      <c r="J6" s="45">
         <v>342</v>
       </c>
     </row>
@@ -1834,19 +2913,19 @@
         <v>156</v>
       </c>
       <c r="E7" s="13">
-        <f t="shared" ref="E7:E27" si="0">D7/$J$6</f>
+        <f t="shared" ref="E7:E37" si="0">D7/$J$6</f>
         <v>0.45614035087719296</v>
       </c>
       <c r="F7" s="14">
-        <f t="shared" ref="F7:F27" si="1">D7/$J$8</f>
-        <v>7.6023391812865496E-3</v>
+        <f t="shared" ref="F7:F37" si="1">D7/$J$8</f>
+        <v>9.1228070175438589E-3</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>5</v>
       </c>
       <c r="I7" s="6"/>
-      <c r="J7" s="46">
-        <v>60</v>
+      <c r="J7" s="45">
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1866,15 +2945,15 @@
       </c>
       <c r="F8" s="14">
         <f t="shared" si="1"/>
-        <v>9.4541910331384024E-3</v>
+        <v>1.1345029239766082E-2</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>6</v>
       </c>
       <c r="I8" s="8"/>
-      <c r="J8" s="47">
+      <c r="J8" s="46">
         <f>J6*J7</f>
-        <v>20520</v>
+        <v>17100</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -1894,7 +2973,7 @@
       </c>
       <c r="F9" s="14">
         <f t="shared" si="1"/>
-        <v>3.3138401559454189E-2</v>
+        <v>3.9766081871345033E-2</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -1914,13 +2993,13 @@
       </c>
       <c r="F10" s="14">
         <f t="shared" si="1"/>
-        <v>0.05</v>
-      </c>
-      <c r="H10" s="34" t="s">
+        <v>0.06</v>
+      </c>
+      <c r="H10" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="35"/>
-      <c r="J10" s="36"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="35"/>
     </row>
     <row r="11" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="9">
@@ -1939,11 +3018,11 @@
       </c>
       <c r="F11" s="14">
         <f t="shared" si="1"/>
-        <v>8.5526315789473686E-2</v>
-      </c>
-      <c r="H11" s="37"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="39"/>
+        <v>0.10263157894736842</v>
+      </c>
+      <c r="H11" s="36"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="38"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B12" s="9">
@@ -1962,15 +3041,15 @@
       </c>
       <c r="F12" s="14">
         <f t="shared" si="1"/>
-        <v>0.12738791423001949</v>
-      </c>
-      <c r="H12" s="41" t="s">
+        <v>0.1528654970760234</v>
+      </c>
+      <c r="H12" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="I12" s="42"/>
-      <c r="J12" s="48">
+      <c r="I12" s="41"/>
+      <c r="J12" s="47">
         <f>J8-MAX(D6:D27)</f>
-        <v>17799</v>
+        <v>13100</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -1990,40 +3069,47 @@
       </c>
       <c r="F13" s="14">
         <f t="shared" si="1"/>
-        <v>0.13260233918128655</v>
-      </c>
-      <c r="H13" s="40" t="s">
+        <v>0.15912280701754386</v>
+      </c>
+      <c r="H13" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="43"/>
-      <c r="J13" s="48">
-        <f>AVERAGE(C9:C12)</f>
-        <v>605</v>
+      <c r="I13" s="42"/>
+      <c r="J13" s="47">
+        <f>AVERAGE(C9:C14)</f>
+        <v>634.33333333333337</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="10"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="B14" s="9">
+        <v>45148</v>
+      </c>
+      <c r="C14" s="1">
+        <f>D14-D13</f>
+        <v>1279</v>
+      </c>
+      <c r="D14" s="1">
+        <v>4000</v>
+      </c>
       <c r="E14" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>11.695906432748538</v>
       </c>
       <c r="F14" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H14" s="44" t="s">
+        <v>0.23391812865497075</v>
+      </c>
+      <c r="H14" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="I14" s="45"/>
-      <c r="J14" s="49">
+      <c r="I14" s="44"/>
+      <c r="J14" s="48">
         <f>J12/J13</f>
-        <v>29.419834710743803</v>
+        <v>20.651602732527586</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B15" s="10"/>
+      <c r="B15" s="9"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="13">
@@ -2034,12 +3120,18 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="33"/>
+      <c r="H15" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" s="32">
+        <v>24.68</v>
+      </c>
+      <c r="J15" s="52">
+        <v>23.78</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B16" s="10"/>
+      <c r="B16" s="9"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="13">
@@ -2050,9 +3142,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B17" s="10"/>
+      <c r="J16" s="53"/>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B17" s="9"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="13">
@@ -2064,8 +3157,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B18" s="10"/>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B18" s="9"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="13">
@@ -2077,8 +3170,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B19" s="10"/>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B19" s="9"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="13">
@@ -2090,8 +3183,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B20" s="10"/>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B20" s="9"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="13">
@@ -2103,8 +3196,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B21" s="10"/>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B21" s="9"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="13">
@@ -2116,8 +3209,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B22" s="10"/>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B22" s="9"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="13">
@@ -2129,8 +3222,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B23" s="10"/>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B23" s="9"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="13">
@@ -2142,8 +3235,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B24" s="10"/>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B24" s="9"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="13">
@@ -2155,8 +3248,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B25" s="10"/>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B25" s="9"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="13">
@@ -2168,8 +3261,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B26" s="10"/>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B26" s="9"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="13">
@@ -2181,20 +3274,430 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="11"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="15">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B27" s="9"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F27" s="16">
+      <c r="F27" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
+    <row r="28" spans="2:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="10"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F28" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M28" t="s">
+        <v>14</v>
+      </c>
+      <c r="N28" t="s">
+        <v>15</v>
+      </c>
+      <c r="O28" t="s">
+        <v>21</v>
+      </c>
+      <c r="P28" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B29" s="10"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F29" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H29" s="50"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="50"/>
+      <c r="L29" t="s">
+        <v>16</v>
+      </c>
+      <c r="M29" cm="1">
+        <f t="array" ref="M29:M50">_xlfn.SORTBY(C6:C27, C6:C27, -1)</f>
+        <v>1279</v>
+      </c>
+      <c r="N29" s="49" cm="1">
+        <f t="array" ref="N29:N50">_xlfn.SORTBY(B6:B27,C6:C27, -1)</f>
+        <v>45148</v>
+      </c>
+      <c r="O29" t="str">
+        <f ca="1">IF(N29=TODAY(), "Green", "Blue")</f>
+        <v>Green</v>
+      </c>
+      <c r="P29" t="str">
+        <f ca="1">IF(NOT(N29=TODAY()), M29, "")</f>
+        <v/>
+      </c>
+      <c r="Q29">
+        <f ca="1">IF(N29=TODAY(), M29, "")</f>
+        <v>1279</v>
+      </c>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B30" s="10"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F30" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H30" s="50"/>
+      <c r="I30" s="50"/>
+      <c r="J30" s="50"/>
+      <c r="L30" t="s">
+        <v>17</v>
+      </c>
+      <c r="M30">
+        <v>859</v>
+      </c>
+      <c r="N30" s="49">
+        <v>45146</v>
+      </c>
+      <c r="O30" t="str">
+        <f t="shared" ref="O30:O33" ca="1" si="2">IF(N30=TODAY(), "Green", "Blue")</f>
+        <v>Blue</v>
+      </c>
+      <c r="P30">
+        <f t="shared" ref="P30:P33" ca="1" si="3">IF(NOT(N30=TODAY()), M30, "")</f>
+        <v>859</v>
+      </c>
+      <c r="Q30" t="str">
+        <f t="shared" ref="Q30:Q33" ca="1" si="4">IF(N30=TODAY(), M30, "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B31" s="10"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F31" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H31" s="50"/>
+      <c r="I31" s="50"/>
+      <c r="J31" s="50"/>
+      <c r="L31" t="s">
+        <v>18</v>
+      </c>
+      <c r="M31">
+        <v>729</v>
+      </c>
+      <c r="N31" s="49">
+        <v>45145</v>
+      </c>
+      <c r="O31" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Blue</v>
+      </c>
+      <c r="P31">
+        <f t="shared" ca="1" si="3"/>
+        <v>729</v>
+      </c>
+      <c r="Q31" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B32" s="10"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F32" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H32" s="50"/>
+      <c r="I32" s="50"/>
+      <c r="J32" s="50"/>
+      <c r="L32" t="s">
+        <v>19</v>
+      </c>
+      <c r="M32">
+        <v>486</v>
+      </c>
+      <c r="N32" s="49">
+        <v>45141</v>
+      </c>
+      <c r="O32" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Blue</v>
+      </c>
+      <c r="P32">
+        <f t="shared" ca="1" si="3"/>
+        <v>486</v>
+      </c>
+      <c r="Q32" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B33" s="10"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F33" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H33" s="50"/>
+      <c r="I33" s="50"/>
+      <c r="J33" s="50"/>
+      <c r="L33" t="s">
+        <v>20</v>
+      </c>
+      <c r="M33">
+        <v>346</v>
+      </c>
+      <c r="N33" s="49">
+        <v>45142</v>
+      </c>
+      <c r="O33" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Blue</v>
+      </c>
+      <c r="P33">
+        <f t="shared" ca="1" si="3"/>
+        <v>346</v>
+      </c>
+      <c r="Q33" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B34" s="10"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F34" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H34" s="50"/>
+      <c r="I34" s="50"/>
+      <c r="J34" s="50"/>
+      <c r="M34">
+        <v>156</v>
+      </c>
+      <c r="N34" s="49">
+        <v>45139</v>
+      </c>
+    </row>
+    <row r="35" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B35" s="10"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F35" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H35" s="50"/>
+      <c r="I35" s="50"/>
+      <c r="J35" s="50"/>
+      <c r="M35">
+        <v>107</v>
+      </c>
+      <c r="N35" s="49">
+        <v>45147</v>
+      </c>
+    </row>
+    <row r="36" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B36" s="10"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F36" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H36" s="50"/>
+      <c r="I36" s="50"/>
+      <c r="J36" s="50"/>
+      <c r="M36">
+        <v>38</v>
+      </c>
+      <c r="N36" s="49">
+        <v>45140</v>
+      </c>
+    </row>
+    <row r="37" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="11"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F37" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H37" s="50"/>
+      <c r="I37" s="50"/>
+      <c r="J37" s="50"/>
+      <c r="M37">
+        <v>0</v>
+      </c>
+      <c r="N37" s="49">
+        <v>45138</v>
+      </c>
+    </row>
+    <row r="38" spans="2:17" ht="5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M38">
+        <v>0</v>
+      </c>
+      <c r="N38" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="M39">
+        <v>0</v>
+      </c>
+      <c r="N39" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="M40">
+        <v>0</v>
+      </c>
+      <c r="N40" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="M41">
+        <v>0</v>
+      </c>
+      <c r="N41" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="M42">
+        <v>0</v>
+      </c>
+      <c r="N42" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="M43">
+        <v>0</v>
+      </c>
+      <c r="N43" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="M44">
+        <v>0</v>
+      </c>
+      <c r="N44" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="M45">
+        <v>0</v>
+      </c>
+      <c r="N45" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="M46">
+        <v>0</v>
+      </c>
+      <c r="N46" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="M47">
+        <v>0</v>
+      </c>
+      <c r="N47" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="M48">
+        <v>0</v>
+      </c>
+      <c r="N48" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="M49">
+        <v>0</v>
+      </c>
+      <c r="N49" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="M50">
+        <v>0</v>
+      </c>
+      <c r="N50" s="49">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M29:M50">
+    <sortCondition descending="1" ref="M29:M50"/>
+  </sortState>
   <mergeCells count="9">
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="H13:I13"/>

</xml_diff>

<commit_message>
Wrote an above-average amount of words and began data overview plot
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC66F44-71F4-C240-B1BF-AF65E031D799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927FCA2A-F717-D44A-8F3C-A0C2243A590F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14420" windowHeight="17900" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -141,8 +141,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="170" formatCode="0.0"/>
-    <numFmt numFmtId="171" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -400,36 +400,17 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="170" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="4" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="4" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -439,6 +420,75 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -448,35 +498,23 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -496,45 +534,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -671,6 +670,9 @@
                 <c:pt idx="8">
                   <c:v>45148</c:v>
                 </c:pt>
+                <c:pt idx="9">
+                  <c:v>45149</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -706,6 +708,9 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4657</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -754,7 +759,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-3120000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-3120000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -1007,7 +1012,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1279</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>859</c:v>
@@ -1016,10 +1021,10 @@
                   <c:v>729</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>486</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>346</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1076,7 +1081,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1279</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1085,7 +1090,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>657</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2812,72 +2817,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="25"/>
+      <c r="A1" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="31"/>
     </row>
     <row r="2" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="26"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="28"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="34"/>
     </row>
     <row r="3" spans="1:11" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="31"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="37"/>
     </row>
     <row r="4" spans="1:11" ht="5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:11" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="20" t="s">
+      <c r="H5" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="21"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="12"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="40"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B6" s="51">
+      <c r="B6" s="20">
         <v>45138</v>
       </c>
       <c r="C6" s="1">
@@ -2886,24 +2890,24 @@
       <c r="D6" s="1">
         <v>0</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="6">
         <f>D6/$J$6</f>
         <v>0</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="7">
         <f>D6/$J$8</f>
         <v>0</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="3"/>
-      <c r="J6" s="45">
+      <c r="I6" s="42"/>
+      <c r="J6" s="14">
         <v>342</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B7" s="9">
+      <c r="B7" s="3">
         <v>45139</v>
       </c>
       <c r="C7" s="1">
@@ -2912,390 +2916,397 @@
       <c r="D7" s="1">
         <v>156</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="6">
         <f t="shared" ref="E7:E37" si="0">D7/$J$6</f>
         <v>0.45614035087719296</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="7">
         <f t="shared" ref="F7:F37" si="1">D7/$J$8</f>
         <v>9.1228070175438589E-3</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="6"/>
-      <c r="J7" s="45">
+      <c r="I7" s="44"/>
+      <c r="J7" s="14">
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="9">
+      <c r="B8" s="3">
         <v>45140</v>
       </c>
       <c r="C8" s="1">
-        <f>D8-D7</f>
+        <f t="shared" ref="C8:C15" si="2">D8-D7</f>
         <v>38</v>
       </c>
       <c r="D8" s="1">
         <v>194</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="6">
         <f t="shared" si="0"/>
         <v>0.56725146198830412</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="7">
         <f t="shared" si="1"/>
         <v>1.1345029239766082E-2</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="8"/>
-      <c r="J8" s="46">
+      <c r="I8" s="46"/>
+      <c r="J8" s="15">
         <f>J6*J7</f>
         <v>17100</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="9">
+      <c r="B9" s="3">
         <v>45141</v>
       </c>
       <c r="C9" s="1">
-        <f>D9-D8</f>
+        <f t="shared" si="2"/>
         <v>486</v>
       </c>
       <c r="D9" s="1">
         <v>680</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="6">
         <f t="shared" si="0"/>
         <v>1.9883040935672514</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="7">
         <f t="shared" si="1"/>
         <v>3.9766081871345033E-2</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="9">
+      <c r="B10" s="3">
         <v>45142</v>
       </c>
       <c r="C10" s="1">
-        <f>D10-D9</f>
+        <f t="shared" si="2"/>
         <v>346</v>
       </c>
       <c r="D10" s="1">
         <v>1026</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="6">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="7">
         <f t="shared" si="1"/>
         <v>0.06</v>
       </c>
-      <c r="H10" s="33" t="s">
+      <c r="H10" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="34"/>
-      <c r="J10" s="35"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="49"/>
     </row>
     <row r="11" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="9">
+      <c r="B11" s="3">
         <v>45145</v>
       </c>
       <c r="C11" s="1">
-        <f>D11-D10</f>
+        <f t="shared" si="2"/>
         <v>729</v>
       </c>
       <c r="D11" s="1">
         <v>1755</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="6">
         <f t="shared" si="0"/>
         <v>5.1315789473684212</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="7">
         <f t="shared" si="1"/>
         <v>0.10263157894736842</v>
       </c>
-      <c r="H11" s="36"/>
-      <c r="I11" s="37"/>
-      <c r="J11" s="38"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="52"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B12" s="9">
+      <c r="B12" s="3">
         <v>45146</v>
       </c>
       <c r="C12" s="1">
-        <f>D12-D11</f>
+        <f t="shared" si="2"/>
         <v>859</v>
       </c>
       <c r="D12" s="1">
         <v>2614</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="6">
         <f t="shared" si="0"/>
         <v>7.6432748538011692</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12" s="7">
         <f t="shared" si="1"/>
         <v>0.1528654970760234</v>
       </c>
-      <c r="H12" s="40" t="s">
+      <c r="H12" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="I12" s="41"/>
-      <c r="J12" s="47">
+      <c r="I12" s="24"/>
+      <c r="J12" s="16">
         <f>J8-MAX(D6:D27)</f>
-        <v>13100</v>
+        <v>12443</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B13" s="9">
+      <c r="B13" s="3">
         <v>45147</v>
       </c>
       <c r="C13" s="1">
-        <f>D13-D12</f>
+        <f t="shared" si="2"/>
         <v>107</v>
       </c>
       <c r="D13" s="1">
         <v>2721</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="6">
         <f t="shared" si="0"/>
         <v>7.9561403508771926</v>
       </c>
-      <c r="F13" s="14">
+      <c r="F13" s="7">
         <f t="shared" si="1"/>
         <v>0.15912280701754386</v>
       </c>
-      <c r="H13" s="39" t="s">
+      <c r="H13" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="42"/>
-      <c r="J13" s="47">
-        <f>AVERAGE(C9:C14)</f>
-        <v>634.33333333333337</v>
+      <c r="I13" s="26"/>
+      <c r="J13" s="16">
+        <f>AVERAGE(C9:C15)</f>
+        <v>637.57142857142856</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="9">
+      <c r="B14" s="3">
         <v>45148</v>
       </c>
       <c r="C14" s="1">
-        <f>D14-D13</f>
+        <f t="shared" si="2"/>
         <v>1279</v>
       </c>
       <c r="D14" s="1">
         <v>4000</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="6">
         <f t="shared" si="0"/>
         <v>11.695906432748538</v>
       </c>
-      <c r="F14" s="14">
+      <c r="F14" s="7">
         <f t="shared" si="1"/>
         <v>0.23391812865497075</v>
       </c>
-      <c r="H14" s="43" t="s">
+      <c r="H14" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="I14" s="44"/>
-      <c r="J14" s="48">
+      <c r="I14" s="28"/>
+      <c r="J14" s="17">
         <f>J12/J13</f>
-        <v>20.651602732527586</v>
+        <v>19.516244678467398</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B15" s="9"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="13">
+      <c r="B15" s="3">
+        <v>45149</v>
+      </c>
+      <c r="C15" s="1">
+        <f t="shared" si="2"/>
+        <v>657</v>
+      </c>
+      <c r="D15" s="1">
+        <v>4657</v>
+      </c>
+      <c r="E15" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F15" s="14">
+        <v>13.616959064327485</v>
+      </c>
+      <c r="F15" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H15" s="32" t="s">
+        <v>0.27233918128654971</v>
+      </c>
+      <c r="H15" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="I15" s="32">
+      <c r="I15" s="13">
         <v>24.68</v>
       </c>
-      <c r="J15" s="52">
+      <c r="J15" s="21">
         <v>23.78</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B16" s="9"/>
+      <c r="B16" s="3"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="13">
+      <c r="E16" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F16" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J16" s="53"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B17" s="9"/>
+      <c r="B17" s="3"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="13">
+      <c r="E17" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F17" s="14">
+      <c r="F17" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B18" s="9"/>
+      <c r="B18" s="3"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="13">
+      <c r="E18" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F18" s="14">
+      <c r="F18" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B19" s="9"/>
+      <c r="B19" s="3"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="13">
+      <c r="E19" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F19" s="14">
+      <c r="F19" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B20" s="9"/>
+      <c r="B20" s="3"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="13">
+      <c r="E20" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F20" s="14">
+      <c r="F20" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B21" s="9"/>
+      <c r="B21" s="3"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="13">
+      <c r="E21" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F21" s="14">
+      <c r="F21" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B22" s="9"/>
+      <c r="B22" s="3"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="13">
+      <c r="E22" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F22" s="14">
+      <c r="F22" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B23" s="9"/>
+      <c r="B23" s="3"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="13">
+      <c r="E23" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F23" s="14">
+      <c r="F23" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B24" s="9"/>
+      <c r="B24" s="3"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
-      <c r="E24" s="13">
+      <c r="E24" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F24" s="14">
+      <c r="F24" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B25" s="9"/>
+      <c r="B25" s="3"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
-      <c r="E25" s="13">
+      <c r="E25" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F25" s="14">
+      <c r="F25" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B26" s="9"/>
+      <c r="B26" s="3"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
-      <c r="E26" s="13">
+      <c r="E26" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F26" s="14">
+      <c r="F26" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B27" s="9"/>
+      <c r="B27" s="3"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
-      <c r="E27" s="13">
+      <c r="E27" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F27" s="14">
+      <c r="F27" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="10"/>
+      <c r="B28" s="4"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
-      <c r="E28" s="13">
+      <c r="E28" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F28" s="14">
+      <c r="F28" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3316,20 +3327,20 @@
       </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B29" s="10"/>
+      <c r="B29" s="4"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
-      <c r="E29" s="13">
+      <c r="E29" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F29" s="14">
+      <c r="F29" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H29" s="50"/>
-      <c r="I29" s="50"/>
-      <c r="J29" s="50"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
       <c r="L29" t="s">
         <v>16</v>
       </c>
@@ -3337,272 +3348,272 @@
         <f t="array" ref="M29:M50">_xlfn.SORTBY(C6:C27, C6:C27, -1)</f>
         <v>1279</v>
       </c>
-      <c r="N29" s="49" cm="1">
+      <c r="N29" s="18" cm="1">
         <f t="array" ref="N29:N50">_xlfn.SORTBY(B6:B27,C6:C27, -1)</f>
         <v>45148</v>
       </c>
       <c r="O29" t="str">
         <f ca="1">IF(N29=TODAY(), "Green", "Blue")</f>
-        <v>Green</v>
-      </c>
-      <c r="P29" t="str">
+        <v>Blue</v>
+      </c>
+      <c r="P29">
         <f ca="1">IF(NOT(N29=TODAY()), M29, "")</f>
+        <v>1279</v>
+      </c>
+      <c r="Q29" t="str">
+        <f ca="1">IF(N29=TODAY(), M29, "")</f>
         <v/>
       </c>
-      <c r="Q29">
-        <f ca="1">IF(N29=TODAY(), M29, "")</f>
-        <v>1279</v>
-      </c>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B30" s="10"/>
+      <c r="B30" s="4"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
-      <c r="E30" s="13">
+      <c r="E30" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F30" s="14">
+      <c r="F30" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H30" s="50"/>
-      <c r="I30" s="50"/>
-      <c r="J30" s="50"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19"/>
       <c r="L30" t="s">
         <v>17</v>
       </c>
       <c r="M30">
         <v>859</v>
       </c>
-      <c r="N30" s="49">
+      <c r="N30" s="18">
         <v>45146</v>
       </c>
       <c r="O30" t="str">
-        <f t="shared" ref="O30:O33" ca="1" si="2">IF(N30=TODAY(), "Green", "Blue")</f>
+        <f t="shared" ref="O30:O33" ca="1" si="3">IF(N30=TODAY(), "Green", "Blue")</f>
         <v>Blue</v>
       </c>
       <c r="P30">
-        <f t="shared" ref="P30:P33" ca="1" si="3">IF(NOT(N30=TODAY()), M30, "")</f>
+        <f t="shared" ref="P30:P33" ca="1" si="4">IF(NOT(N30=TODAY()), M30, "")</f>
         <v>859</v>
       </c>
       <c r="Q30" t="str">
-        <f t="shared" ref="Q30:Q33" ca="1" si="4">IF(N30=TODAY(), M30, "")</f>
+        <f t="shared" ref="Q30:Q33" ca="1" si="5">IF(N30=TODAY(), M30, "")</f>
         <v/>
       </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B31" s="10"/>
+      <c r="B31" s="4"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
-      <c r="E31" s="13">
+      <c r="E31" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F31" s="14">
+      <c r="F31" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H31" s="50"/>
-      <c r="I31" s="50"/>
-      <c r="J31" s="50"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="19"/>
       <c r="L31" t="s">
         <v>18</v>
       </c>
       <c r="M31">
         <v>729</v>
       </c>
-      <c r="N31" s="49">
+      <c r="N31" s="18">
         <v>45145</v>
       </c>
       <c r="O31" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>Blue</v>
       </c>
       <c r="P31">
+        <f t="shared" ca="1" si="4"/>
+        <v>729</v>
+      </c>
+      <c r="Q31" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B32" s="4"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F32" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="19"/>
+      <c r="L32" t="s">
+        <v>19</v>
+      </c>
+      <c r="M32">
+        <v>657</v>
+      </c>
+      <c r="N32" s="18">
+        <v>45149</v>
+      </c>
+      <c r="O32" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>729</v>
-      </c>
-      <c r="Q31" t="str">
+        <v>Green</v>
+      </c>
+      <c r="P32" t="str">
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
-    </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B32" s="10"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F32" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H32" s="50"/>
-      <c r="I32" s="50"/>
-      <c r="J32" s="50"/>
-      <c r="L32" t="s">
-        <v>19</v>
-      </c>
-      <c r="M32">
-        <v>486</v>
-      </c>
-      <c r="N32" s="49">
-        <v>45141</v>
-      </c>
-      <c r="O32" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Blue</v>
-      </c>
-      <c r="P32">
-        <f t="shared" ca="1" si="3"/>
-        <v>486</v>
-      </c>
-      <c r="Q32" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v/>
+      <c r="Q32">
+        <f t="shared" ca="1" si="5"/>
+        <v>657</v>
       </c>
     </row>
     <row r="33" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B33" s="10"/>
+      <c r="B33" s="4"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
-      <c r="E33" s="13">
+      <c r="E33" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F33" s="14">
+      <c r="F33" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H33" s="50"/>
-      <c r="I33" s="50"/>
-      <c r="J33" s="50"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="19"/>
       <c r="L33" t="s">
         <v>20</v>
       </c>
       <c r="M33">
-        <v>346</v>
-      </c>
-      <c r="N33" s="49">
-        <v>45142</v>
+        <v>486</v>
+      </c>
+      <c r="N33" s="18">
+        <v>45141</v>
       </c>
       <c r="O33" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>Blue</v>
       </c>
       <c r="P33">
-        <f t="shared" ca="1" si="3"/>
-        <v>346</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>486</v>
       </c>
       <c r="Q33" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
     </row>
     <row r="34" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B34" s="10"/>
+      <c r="B34" s="4"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
-      <c r="E34" s="13">
+      <c r="E34" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F34" s="14">
+      <c r="F34" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H34" s="50"/>
-      <c r="I34" s="50"/>
-      <c r="J34" s="50"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19"/>
+      <c r="J34" s="19"/>
       <c r="M34">
-        <v>156</v>
-      </c>
-      <c r="N34" s="49">
-        <v>45139</v>
+        <v>346</v>
+      </c>
+      <c r="N34" s="18">
+        <v>45142</v>
       </c>
     </row>
     <row r="35" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B35" s="10"/>
+      <c r="B35" s="4"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
-      <c r="E35" s="13">
+      <c r="E35" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F35" s="14">
+      <c r="F35" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H35" s="50"/>
-      <c r="I35" s="50"/>
-      <c r="J35" s="50"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="19"/>
       <c r="M35">
-        <v>107</v>
-      </c>
-      <c r="N35" s="49">
-        <v>45147</v>
+        <v>156</v>
+      </c>
+      <c r="N35" s="18">
+        <v>45139</v>
       </c>
     </row>
     <row r="36" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B36" s="10"/>
+      <c r="B36" s="4"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
-      <c r="E36" s="13">
+      <c r="E36" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F36" s="14">
+      <c r="F36" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H36" s="50"/>
-      <c r="I36" s="50"/>
-      <c r="J36" s="50"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="19"/>
       <c r="M36">
-        <v>38</v>
-      </c>
-      <c r="N36" s="49">
-        <v>45140</v>
+        <v>107</v>
+      </c>
+      <c r="N36" s="18">
+        <v>45147</v>
       </c>
     </row>
     <row r="37" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="11"/>
+      <c r="B37" s="5"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
-      <c r="E37" s="15">
+      <c r="E37" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F37" s="16">
+      <c r="F37" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H37" s="50"/>
-      <c r="I37" s="50"/>
-      <c r="J37" s="50"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="19"/>
       <c r="M37">
-        <v>0</v>
-      </c>
-      <c r="N37" s="49">
-        <v>45138</v>
+        <v>38</v>
+      </c>
+      <c r="N37" s="18">
+        <v>45140</v>
       </c>
     </row>
     <row r="38" spans="2:17" ht="5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M38">
         <v>0</v>
       </c>
-      <c r="N38" s="49">
-        <v>0</v>
+      <c r="N38" s="18">
+        <v>45138</v>
       </c>
     </row>
     <row r="39" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M39">
         <v>0</v>
       </c>
-      <c r="N39" s="49">
+      <c r="N39" s="18">
         <v>0</v>
       </c>
     </row>
@@ -3610,7 +3621,7 @@
       <c r="M40">
         <v>0</v>
       </c>
-      <c r="N40" s="49">
+      <c r="N40" s="18">
         <v>0</v>
       </c>
     </row>
@@ -3618,7 +3629,7 @@
       <c r="M41">
         <v>0</v>
       </c>
-      <c r="N41" s="49">
+      <c r="N41" s="18">
         <v>0</v>
       </c>
     </row>
@@ -3626,7 +3637,7 @@
       <c r="M42">
         <v>0</v>
       </c>
-      <c r="N42" s="49">
+      <c r="N42" s="18">
         <v>0</v>
       </c>
     </row>
@@ -3634,7 +3645,7 @@
       <c r="M43">
         <v>0</v>
       </c>
-      <c r="N43" s="49">
+      <c r="N43" s="18">
         <v>0</v>
       </c>
     </row>
@@ -3642,7 +3653,7 @@
       <c r="M44">
         <v>0</v>
       </c>
-      <c r="N44" s="49">
+      <c r="N44" s="18">
         <v>0</v>
       </c>
     </row>
@@ -3650,7 +3661,7 @@
       <c r="M45">
         <v>0</v>
       </c>
-      <c r="N45" s="49">
+      <c r="N45" s="18">
         <v>0</v>
       </c>
     </row>
@@ -3658,7 +3669,7 @@
       <c r="M46">
         <v>0</v>
       </c>
-      <c r="N46" s="49">
+      <c r="N46" s="18">
         <v>0</v>
       </c>
     </row>
@@ -3666,7 +3677,7 @@
       <c r="M47">
         <v>0</v>
       </c>
-      <c r="N47" s="49">
+      <c r="N47" s="18">
         <v>0</v>
       </c>
     </row>
@@ -3674,7 +3685,7 @@
       <c r="M48">
         <v>0</v>
       </c>
-      <c r="N48" s="49">
+      <c r="N48" s="18">
         <v>0</v>
       </c>
     </row>
@@ -3682,7 +3693,7 @@
       <c r="M49">
         <v>0</v>
       </c>
-      <c r="N49" s="49">
+      <c r="N49" s="18">
         <v>0</v>
       </c>
     </row>
@@ -3690,7 +3701,7 @@
       <c r="M50">
         <v>0</v>
       </c>
-      <c r="N50" s="49">
+      <c r="N50" s="18">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
DATA figure, DFT section + coverage sim
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927FCA2A-F717-D44A-8F3C-A0C2243A590F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D96CEC-3736-EC40-A2B7-1E77DEE6C6BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14420" windowHeight="17900" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
@@ -673,6 +673,9 @@
                 <c:pt idx="9">
                   <c:v>45149</c:v>
                 </c:pt>
+                <c:pt idx="10">
+                  <c:v>45152</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -711,6 +714,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>4657</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4803</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1021,7 +1027,7 @@
                   <c:v>729</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>657</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>486</c:v>
@@ -1090,7 +1096,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>657</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2803,7 +2809,7 @@
   <dimension ref="A1:Q50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2937,7 +2943,7 @@
         <v>45140</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" ref="C8:C15" si="2">D8-D7</f>
+        <f t="shared" ref="C8:C16" si="2">D8-D7</f>
         <v>38</v>
       </c>
       <c r="D8" s="1">
@@ -3053,7 +3059,7 @@
       <c r="I12" s="24"/>
       <c r="J12" s="16">
         <f>J8-MAX(D6:D27)</f>
-        <v>12443</v>
+        <v>12297</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -3080,8 +3086,8 @@
       </c>
       <c r="I13" s="26"/>
       <c r="J13" s="16">
-        <f>AVERAGE(C9:C15)</f>
-        <v>637.57142857142856</v>
+        <f>AVERAGE(C9:C16)</f>
+        <v>576.125</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3109,7 +3115,7 @@
       <c r="I14" s="28"/>
       <c r="J14" s="17">
         <f>J12/J13</f>
-        <v>19.516244678467398</v>
+        <v>21.344326318073335</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -3142,16 +3148,23 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B16" s="3"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
+      <c r="B16" s="3">
+        <v>45152</v>
+      </c>
+      <c r="C16" s="1">
+        <f t="shared" si="2"/>
+        <v>146</v>
+      </c>
+      <c r="D16" s="1">
+        <v>4803</v>
+      </c>
       <c r="E16" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>14.043859649122806</v>
       </c>
       <c r="F16" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.28087719298245611</v>
       </c>
       <c r="J16" s="22"/>
     </row>
@@ -3465,15 +3478,15 @@
       </c>
       <c r="O32" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Green</v>
-      </c>
-      <c r="P32" t="str">
+        <v>Blue</v>
+      </c>
+      <c r="P32">
         <f t="shared" ca="1" si="4"/>
+        <v>657</v>
+      </c>
+      <c r="Q32" t="str">
+        <f t="shared" ca="1" si="5"/>
         <v/>
-      </c>
-      <c r="Q32">
-        <f t="shared" ca="1" si="5"/>
-        <v>657</v>
       </c>
     </row>
     <row r="33" spans="2:17" x14ac:dyDescent="0.2">
@@ -3573,10 +3586,10 @@
       <c r="I36" s="19"/>
       <c r="J36" s="19"/>
       <c r="M36">
-        <v>107</v>
+        <v>146</v>
       </c>
       <c r="N36" s="18">
-        <v>45147</v>
+        <v>45152</v>
       </c>
     </row>
     <row r="37" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3595,18 +3608,18 @@
       <c r="I37" s="19"/>
       <c r="J37" s="19"/>
       <c r="M37">
-        <v>38</v>
+        <v>107</v>
       </c>
       <c r="N37" s="18">
-        <v>45140</v>
+        <v>45147</v>
       </c>
     </row>
     <row r="38" spans="2:17" ht="5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M38">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="N38" s="18">
-        <v>45138</v>
+        <v>45140</v>
       </c>
     </row>
     <row r="39" spans="2:17" x14ac:dyDescent="0.2">
@@ -3614,7 +3627,7 @@
         <v>0</v>
       </c>
       <c r="N39" s="18">
-        <v>0</v>
+        <v>45138</v>
       </c>
     </row>
     <row r="40" spans="2:17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Finished DATA figure, made notes, read, thought about FAOR
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D96CEC-3736-EC40-A2B7-1E77DEE6C6BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91BF92BF-1ADC-904B-9C3D-341EFE02529E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14420" windowHeight="17900" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
@@ -676,6 +676,9 @@
                 <c:pt idx="10">
                   <c:v>45152</c:v>
                 </c:pt>
+                <c:pt idx="11">
+                  <c:v>45153</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -717,6 +720,9 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>4803</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4932</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2809,7 +2815,7 @@
   <dimension ref="A1:Q50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2943,7 +2949,7 @@
         <v>45140</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" ref="C8:C16" si="2">D8-D7</f>
+        <f t="shared" ref="C8:C17" si="2">D8-D7</f>
         <v>38</v>
       </c>
       <c r="D8" s="1">
@@ -3059,7 +3065,7 @@
       <c r="I12" s="24"/>
       <c r="J12" s="16">
         <f>J8-MAX(D6:D27)</f>
-        <v>12297</v>
+        <v>12168</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -3086,8 +3092,8 @@
       </c>
       <c r="I13" s="26"/>
       <c r="J13" s="16">
-        <f>AVERAGE(C9:C16)</f>
-        <v>576.125</v>
+        <f>AVERAGE(C9:C17)</f>
+        <v>526.44444444444446</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3115,7 +3121,7 @@
       <c r="I14" s="28"/>
       <c r="J14" s="17">
         <f>J12/J13</f>
-        <v>21.344326318073335</v>
+        <v>23.113550021105951</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -3169,16 +3175,23 @@
       <c r="J16" s="22"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B17" s="3"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
+      <c r="B17" s="3">
+        <v>45153</v>
+      </c>
+      <c r="C17" s="1">
+        <f t="shared" si="2"/>
+        <v>129</v>
+      </c>
+      <c r="D17" s="1">
+        <v>4932</v>
+      </c>
       <c r="E17" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>14.421052631578947</v>
       </c>
       <c r="F17" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.28842105263157897</v>
       </c>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.2">
@@ -3608,26 +3621,26 @@
       <c r="I37" s="19"/>
       <c r="J37" s="19"/>
       <c r="M37">
-        <v>107</v>
+        <v>129</v>
       </c>
       <c r="N37" s="18">
-        <v>45147</v>
+        <v>45153</v>
       </c>
     </row>
     <row r="38" spans="2:17" ht="5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M38">
-        <v>38</v>
+        <v>107</v>
       </c>
       <c r="N38" s="18">
-        <v>45140</v>
+        <v>45147</v>
       </c>
     </row>
     <row r="39" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M39">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="N39" s="18">
-        <v>45138</v>
+        <v>45140</v>
       </c>
     </row>
     <row r="40" spans="2:17" x14ac:dyDescent="0.2">
@@ -3635,7 +3648,7 @@
         <v>0</v>
       </c>
       <c r="N40" s="18">
-        <v>0</v>
+        <v>45138</v>
       </c>
     </row>
     <row r="41" spans="2:17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
FAOR cycle plot, writing about formic acid
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3849B405-295C-534F-9C27-2D02E3624E18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A55DCFD4-A1F0-4B44-A665-DE312D2146EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14420" windowHeight="17900" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
@@ -679,6 +679,9 @@
                 <c:pt idx="11">
                   <c:v>45153</c:v>
                 </c:pt>
+                <c:pt idx="12">
+                  <c:v>45154</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -723,6 +726,9 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>4943</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5410</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2814,8 +2820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4213BD91-B5D1-3B47-8D3F-04331482504C}">
   <dimension ref="A1:Q50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2949,7 +2955,7 @@
         <v>45140</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" ref="C8:C17" si="2">D8-D7</f>
+        <f t="shared" ref="C8:C18" si="2">D8-D7</f>
         <v>38</v>
       </c>
       <c r="D8" s="1">
@@ -3065,7 +3071,7 @@
       <c r="I12" s="24"/>
       <c r="J12" s="16">
         <f>J8-MAX(D6:D27)</f>
-        <v>12157</v>
+        <v>11690</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -3092,8 +3098,8 @@
       </c>
       <c r="I13" s="26"/>
       <c r="J13" s="16">
-        <f>AVERAGE(C9:C17)</f>
-        <v>527.66666666666663</v>
+        <f>AVERAGE(C9:C18)</f>
+        <v>521.6</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3121,7 +3127,7 @@
       <c r="I14" s="28"/>
       <c r="J14" s="17">
         <f>J12/J13</f>
-        <v>23.039166140240052</v>
+        <v>22.411809815950921</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -3195,16 +3201,23 @@
       </c>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B18" s="3"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
+      <c r="B18" s="3">
+        <v>45154</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" si="2"/>
+        <v>467</v>
+      </c>
+      <c r="D18" s="1">
+        <v>5410</v>
+      </c>
       <c r="E18" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15.818713450292398</v>
       </c>
       <c r="F18" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.31637426900584797</v>
       </c>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.2">
@@ -3555,10 +3568,10 @@
       <c r="I34" s="19"/>
       <c r="J34" s="19"/>
       <c r="M34">
-        <v>346</v>
+        <v>467</v>
       </c>
       <c r="N34" s="18">
-        <v>45142</v>
+        <v>45154</v>
       </c>
     </row>
     <row r="35" spans="2:17" x14ac:dyDescent="0.2">
@@ -3577,10 +3590,10 @@
       <c r="I35" s="19"/>
       <c r="J35" s="19"/>
       <c r="M35">
-        <v>156</v>
+        <v>346</v>
       </c>
       <c r="N35" s="18">
-        <v>45139</v>
+        <v>45142</v>
       </c>
     </row>
     <row r="36" spans="2:17" x14ac:dyDescent="0.2">
@@ -3599,10 +3612,10 @@
       <c r="I36" s="19"/>
       <c r="J36" s="19"/>
       <c r="M36">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="N36" s="18">
-        <v>45152</v>
+        <v>45139</v>
       </c>
     </row>
     <row r="37" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3621,34 +3634,34 @@
       <c r="I37" s="19"/>
       <c r="J37" s="19"/>
       <c r="M37">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="N37" s="18">
-        <v>45153</v>
+        <v>45152</v>
       </c>
     </row>
     <row r="38" spans="2:17" ht="5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M38">
-        <v>107</v>
+        <v>140</v>
       </c>
       <c r="N38" s="18">
-        <v>45147</v>
+        <v>45153</v>
       </c>
     </row>
     <row r="39" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M39">
-        <v>38</v>
+        <v>107</v>
       </c>
       <c r="N39" s="18">
-        <v>45140</v>
+        <v>45147</v>
       </c>
     </row>
     <row r="40" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M40">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="N40" s="18">
-        <v>45138</v>
+        <v>45140</v>
       </c>
     </row>
     <row r="41" spans="2:17" x14ac:dyDescent="0.2">
@@ -3656,7 +3669,7 @@
         <v>0</v>
       </c>
       <c r="N41" s="18">
-        <v>0</v>
+        <v>45138</v>
       </c>
     </row>
     <row r="42" spans="2:17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Read relevant articles about single-site catalyst experiments and wrote good words
Read relevant articles about single-site catalyst experiments and wrote good words, cleaned notes up as well though, so the total word-count wasn't stellar
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A55DCFD4-A1F0-4B44-A665-DE312D2146EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77CE30AB-5B4A-2041-8EB5-BA5E41440953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14420" windowHeight="17900" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Keeping up with the thesis</t>
   </si>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>100w change</t>
+  </si>
+  <si>
+    <t>Sixth best</t>
+  </si>
+  <si>
+    <t>Seventh best</t>
   </si>
 </sst>
 </file>
@@ -682,6 +688,9 @@
                 <c:pt idx="12">
                   <c:v>45154</c:v>
                 </c:pt>
+                <c:pt idx="13">
+                  <c:v>45155</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -729,6 +738,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>5410</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5858</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -987,9 +999,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>Not today</c:v>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1002,9 +1011,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$L$29:$L$33</c:f>
+              <c:f>Sheet1!$L$29:$L$35</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>Best day</c:v>
                 </c:pt>
@@ -1019,16 +1028,22 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Fifth best</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sixth best</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Seventh best</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$29:$P$33</c:f>
+              <c:f>Sheet1!$P$29:$P$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1279</c:v>
                 </c:pt>
@@ -1043,6 +1058,12 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>486</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>467</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1056,9 +1077,6 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>Today</c:v>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:schemeClr val="accent6"/>
@@ -1071,9 +1089,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$L$29:$L$33</c:f>
+              <c:f>Sheet1!$L$29:$L$35</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>Best day</c:v>
                 </c:pt>
@@ -1088,16 +1106,22 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>Fifth best</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Sixth best</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Seventh best</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$29:$Q$33</c:f>
+              <c:f>Sheet1!$Q$29:$Q$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1112,6 +1136,12 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>448</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2461,15 +2491,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>31750</xdr:colOff>
+      <xdr:colOff>31752</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>7936</xdr:rowOff>
+      <xdr:rowOff>60854</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>531812</xdr:colOff>
+      <xdr:colOff>531814</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>7936</xdr:rowOff>
+      <xdr:rowOff>60854</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2484,8 +2514,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7310438" y="5667374"/>
-          <a:ext cx="5453062" cy="4627562"/>
+          <a:off x="7323669" y="5585354"/>
+          <a:ext cx="5453062" cy="4508500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2821,7 +2851,7 @@
   <dimension ref="A1:Q50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2955,7 +2985,7 @@
         <v>45140</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" ref="C8:C18" si="2">D8-D7</f>
+        <f t="shared" ref="C8:C19" si="2">D8-D7</f>
         <v>38</v>
       </c>
       <c r="D8" s="1">
@@ -3071,7 +3101,7 @@
       <c r="I12" s="24"/>
       <c r="J12" s="16">
         <f>J8-MAX(D6:D27)</f>
-        <v>11690</v>
+        <v>11242</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -3098,8 +3128,8 @@
       </c>
       <c r="I13" s="26"/>
       <c r="J13" s="16">
-        <f>AVERAGE(C9:C18)</f>
-        <v>521.6</v>
+        <f>AVERAGE(C9:C19)</f>
+        <v>514.90909090909088</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3127,7 +3157,7 @@
       <c r="I14" s="28"/>
       <c r="J14" s="17">
         <f>J12/J13</f>
-        <v>22.411809815950921</v>
+        <v>21.832980225988702</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -3221,16 +3251,23 @@
       </c>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B19" s="3"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+      <c r="B19" s="3">
+        <v>45155</v>
+      </c>
+      <c r="C19" s="1">
+        <f t="shared" si="2"/>
+        <v>448</v>
+      </c>
+      <c r="D19" s="1">
+        <v>5858</v>
+      </c>
       <c r="E19" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>17.128654970760234</v>
       </c>
       <c r="F19" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.3425730994152047</v>
       </c>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.2">
@@ -3429,15 +3466,15 @@
         <v>45146</v>
       </c>
       <c r="O30" t="str">
-        <f t="shared" ref="O30:O33" ca="1" si="3">IF(N30=TODAY(), "Green", "Blue")</f>
+        <f t="shared" ref="O30:O35" ca="1" si="3">IF(N30=TODAY(), "Green", "Blue")</f>
         <v>Blue</v>
       </c>
       <c r="P30">
-        <f t="shared" ref="P30:P33" ca="1" si="4">IF(NOT(N30=TODAY()), M30, "")</f>
+        <f t="shared" ref="P30:P35" ca="1" si="4">IF(NOT(N30=TODAY()), M30, "")</f>
         <v>859</v>
       </c>
       <c r="Q30" t="str">
-        <f t="shared" ref="Q30:Q33" ca="1" si="5">IF(N30=TODAY(), M30, "")</f>
+        <f t="shared" ref="Q30:Q35" ca="1" si="5">IF(N30=TODAY(), M30, "")</f>
         <v/>
       </c>
     </row>
@@ -3567,11 +3604,26 @@
       <c r="H34" s="19"/>
       <c r="I34" s="19"/>
       <c r="J34" s="19"/>
+      <c r="L34" t="s">
+        <v>25</v>
+      </c>
       <c r="M34">
         <v>467</v>
       </c>
       <c r="N34" s="18">
         <v>45154</v>
+      </c>
+      <c r="O34" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>Blue</v>
+      </c>
+      <c r="P34">
+        <f t="shared" ca="1" si="4"/>
+        <v>467</v>
+      </c>
+      <c r="Q34" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
       </c>
     </row>
     <row r="35" spans="2:17" x14ac:dyDescent="0.2">
@@ -3589,11 +3641,26 @@
       <c r="H35" s="19"/>
       <c r="I35" s="19"/>
       <c r="J35" s="19"/>
+      <c r="L35" t="s">
+        <v>26</v>
+      </c>
       <c r="M35">
-        <v>346</v>
+        <v>448</v>
       </c>
       <c r="N35" s="18">
-        <v>45142</v>
+        <v>45155</v>
+      </c>
+      <c r="O35" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>Green</v>
+      </c>
+      <c r="P35" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+      <c r="Q35">
+        <f t="shared" ca="1" si="5"/>
+        <v>448</v>
       </c>
     </row>
     <row r="36" spans="2:17" x14ac:dyDescent="0.2">
@@ -3612,10 +3679,10 @@
       <c r="I36" s="19"/>
       <c r="J36" s="19"/>
       <c r="M36">
-        <v>156</v>
+        <v>346</v>
       </c>
       <c r="N36" s="18">
-        <v>45139</v>
+        <v>45142</v>
       </c>
     </row>
     <row r="37" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3634,42 +3701,42 @@
       <c r="I37" s="19"/>
       <c r="J37" s="19"/>
       <c r="M37">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="N37" s="18">
-        <v>45152</v>
+        <v>45139</v>
       </c>
     </row>
     <row r="38" spans="2:17" ht="5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M38">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="N38" s="18">
-        <v>45153</v>
+        <v>45152</v>
       </c>
     </row>
     <row r="39" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M39">
-        <v>107</v>
+        <v>140</v>
       </c>
       <c r="N39" s="18">
-        <v>45147</v>
+        <v>45153</v>
       </c>
     </row>
     <row r="40" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M40">
-        <v>38</v>
+        <v>107</v>
       </c>
       <c r="N40" s="18">
-        <v>45140</v>
+        <v>45147</v>
       </c>
     </row>
     <row r="41" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M41">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="N41" s="18">
-        <v>45138</v>
+        <v>45140</v>
       </c>
     </row>
     <row r="42" spans="2:17" x14ac:dyDescent="0.2">
@@ -3677,7 +3744,7 @@
         <v>0</v>
       </c>
       <c r="N42" s="18">
-        <v>0</v>
+        <v>45138</v>
       </c>
     </row>
     <row r="43" spans="2:17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Learned a lot about Q mec and DFT. And wrote half
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77CE30AB-5B4A-2041-8EB5-BA5E41440953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D5A471C-B7EC-3B4E-8C10-ACF6902E26AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14420" windowHeight="17900" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
@@ -691,6 +691,9 @@
                 <c:pt idx="13">
                   <c:v>45155</c:v>
                 </c:pt>
+                <c:pt idx="14">
+                  <c:v>45156</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -741,6 +744,9 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>5858</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6277</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -810,6 +816,8 @@
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
+        <c:majorUnit val="3"/>
+        <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
         <c:axId val="656428208"/>
@@ -1063,7 +1071,7 @@
                   <c:v>467</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>448</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1141,7 +1149,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>448</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2851,7 +2859,7 @@
   <dimension ref="A1:Q50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2985,7 +2993,7 @@
         <v>45140</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" ref="C8:C19" si="2">D8-D7</f>
+        <f t="shared" ref="C8:C20" si="2">D8-D7</f>
         <v>38</v>
       </c>
       <c r="D8" s="1">
@@ -3101,7 +3109,7 @@
       <c r="I12" s="24"/>
       <c r="J12" s="16">
         <f>J8-MAX(D6:D27)</f>
-        <v>11242</v>
+        <v>10823</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -3157,7 +3165,7 @@
       <c r="I14" s="28"/>
       <c r="J14" s="17">
         <f>J12/J13</f>
-        <v>21.832980225988702</v>
+        <v>21.019244350282488</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -3271,16 +3279,23 @@
       </c>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B20" s="3"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
+      <c r="B20" s="3">
+        <v>45156</v>
+      </c>
+      <c r="C20" s="1">
+        <f t="shared" si="2"/>
+        <v>419</v>
+      </c>
+      <c r="D20" s="1">
+        <v>6277</v>
+      </c>
       <c r="E20" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18.353801169590643</v>
       </c>
       <c r="F20" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.36707602339181289</v>
       </c>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.2">
@@ -3652,15 +3667,15 @@
       </c>
       <c r="O35" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Green</v>
-      </c>
-      <c r="P35" t="str">
+        <v>Blue</v>
+      </c>
+      <c r="P35">
         <f t="shared" ca="1" si="4"/>
+        <v>448</v>
+      </c>
+      <c r="Q35" t="str">
+        <f t="shared" ca="1" si="5"/>
         <v/>
-      </c>
-      <c r="Q35">
-        <f t="shared" ca="1" si="5"/>
-        <v>448</v>
       </c>
     </row>
     <row r="36" spans="2:17" x14ac:dyDescent="0.2">
@@ -3679,10 +3694,10 @@
       <c r="I36" s="19"/>
       <c r="J36" s="19"/>
       <c r="M36">
-        <v>346</v>
+        <v>419</v>
       </c>
       <c r="N36" s="18">
-        <v>45142</v>
+        <v>45156</v>
       </c>
     </row>
     <row r="37" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3701,50 +3716,50 @@
       <c r="I37" s="19"/>
       <c r="J37" s="19"/>
       <c r="M37">
-        <v>156</v>
+        <v>346</v>
       </c>
       <c r="N37" s="18">
-        <v>45139</v>
+        <v>45142</v>
       </c>
     </row>
     <row r="38" spans="2:17" ht="5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M38">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="N38" s="18">
-        <v>45152</v>
+        <v>45139</v>
       </c>
     </row>
     <row r="39" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M39">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="N39" s="18">
-        <v>45153</v>
+        <v>45152</v>
       </c>
     </row>
     <row r="40" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M40">
-        <v>107</v>
+        <v>140</v>
       </c>
       <c r="N40" s="18">
-        <v>45147</v>
+        <v>45153</v>
       </c>
     </row>
     <row r="41" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M41">
-        <v>38</v>
+        <v>107</v>
       </c>
       <c r="N41" s="18">
-        <v>45140</v>
+        <v>45147</v>
       </c>
     </row>
     <row r="42" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M42">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="N42" s="18">
-        <v>45138</v>
+        <v>45140</v>
       </c>
     </row>
     <row r="43" spans="2:17" x14ac:dyDescent="0.2">
@@ -3752,7 +3767,7 @@
         <v>0</v>
       </c>
       <c r="N43" s="18">
-        <v>0</v>
+        <v>45138</v>
       </c>
     </row>
     <row r="44" spans="2:17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Almost finished DFT section
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D5A471C-B7EC-3B4E-8C10-ACF6902E26AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E28BAE-7D69-CA44-913D-A68057CC5ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14420" windowHeight="17900" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Keeping up with the thesis</t>
   </si>
@@ -139,6 +139,15 @@
   </si>
   <si>
     <t>Seventh best</t>
+  </si>
+  <si>
+    <t>Eight best</t>
+  </si>
+  <si>
+    <t>Ninth best</t>
+  </si>
+  <si>
+    <t>Tenth best</t>
   </si>
 </sst>
 </file>
@@ -694,6 +703,9 @@
                 <c:pt idx="14">
                   <c:v>45156</c:v>
                 </c:pt>
+                <c:pt idx="15">
+                  <c:v>45159</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -747,6 +759,9 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>6277</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6938</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1019,9 +1034,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$L$29:$L$35</c:f>
+              <c:f>Sheet1!$L$29:$L$38</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Best day</c:v>
                 </c:pt>
@@ -1042,16 +1057,25 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Seventh best</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Eight best</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Ninth best</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Tenth best</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$29:$P$35</c:f>
+              <c:f>Sheet1!$P$29:$P$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1279</c:v>
                 </c:pt>
@@ -1062,16 +1086,25 @@
                   <c:v>729</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>661</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>657</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>486</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>467</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>448</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>419</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>346</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1097,9 +1130,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$L$29:$L$35</c:f>
+              <c:f>Sheet1!$L$29:$L$38</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Best day</c:v>
                 </c:pt>
@@ -1120,16 +1153,25 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Seventh best</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Eight best</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Ninth best</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Tenth best</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$29:$Q$35</c:f>
+              <c:f>Sheet1!$Q$29:$Q$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1149,6 +1191,15 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2859,7 +2910,7 @@
   <dimension ref="A1:Q50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2993,7 +3044,7 @@
         <v>45140</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" ref="C8:C20" si="2">D8-D7</f>
+        <f t="shared" ref="C8:C21" si="2">D8-D7</f>
         <v>38</v>
       </c>
       <c r="D8" s="1">
@@ -3109,7 +3160,7 @@
       <c r="I12" s="24"/>
       <c r="J12" s="16">
         <f>J8-MAX(D6:D27)</f>
-        <v>10823</v>
+        <v>10162</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -3136,8 +3187,8 @@
       </c>
       <c r="I13" s="26"/>
       <c r="J13" s="16">
-        <f>AVERAGE(C9:C19)</f>
-        <v>514.90909090909088</v>
+        <f>AVERAGE(C9:C21)</f>
+        <v>518.76923076923072</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3165,7 +3216,7 @@
       <c r="I14" s="28"/>
       <c r="J14" s="17">
         <f>J12/J13</f>
-        <v>21.019244350282488</v>
+        <v>19.58867141162515</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -3299,16 +3350,23 @@
       </c>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B21" s="3"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
+      <c r="B21" s="3">
+        <v>45159</v>
+      </c>
+      <c r="C21" s="1">
+        <f t="shared" si="2"/>
+        <v>661</v>
+      </c>
+      <c r="D21" s="1">
+        <v>6938</v>
+      </c>
       <c r="E21" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>20.28654970760234</v>
       </c>
       <c r="F21" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.40573099415204678</v>
       </c>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.2">
@@ -3481,15 +3539,15 @@
         <v>45146</v>
       </c>
       <c r="O30" t="str">
-        <f t="shared" ref="O30:O35" ca="1" si="3">IF(N30=TODAY(), "Green", "Blue")</f>
+        <f t="shared" ref="O30:O38" ca="1" si="3">IF(N30=TODAY(), "Green", "Blue")</f>
         <v>Blue</v>
       </c>
       <c r="P30">
-        <f t="shared" ref="P30:P35" ca="1" si="4">IF(NOT(N30=TODAY()), M30, "")</f>
+        <f t="shared" ref="P30:P38" ca="1" si="4">IF(NOT(N30=TODAY()), M30, "")</f>
         <v>859</v>
       </c>
       <c r="Q30" t="str">
-        <f t="shared" ref="Q30:Q35" ca="1" si="5">IF(N30=TODAY(), M30, "")</f>
+        <f t="shared" ref="Q30:Q38" ca="1" si="5">IF(N30=TODAY(), M30, "")</f>
         <v/>
       </c>
     </row>
@@ -3549,10 +3607,10 @@
         <v>19</v>
       </c>
       <c r="M32">
-        <v>657</v>
+        <v>661</v>
       </c>
       <c r="N32" s="18">
-        <v>45149</v>
+        <v>45159</v>
       </c>
       <c r="O32" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3560,7 +3618,7 @@
       </c>
       <c r="P32">
         <f t="shared" ca="1" si="4"/>
-        <v>657</v>
+        <v>661</v>
       </c>
       <c r="Q32" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -3586,10 +3644,10 @@
         <v>20</v>
       </c>
       <c r="M33">
-        <v>486</v>
+        <v>657</v>
       </c>
       <c r="N33" s="18">
-        <v>45141</v>
+        <v>45149</v>
       </c>
       <c r="O33" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3597,7 +3655,7 @@
       </c>
       <c r="P33">
         <f t="shared" ca="1" si="4"/>
-        <v>486</v>
+        <v>657</v>
       </c>
       <c r="Q33" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -3623,10 +3681,10 @@
         <v>25</v>
       </c>
       <c r="M34">
-        <v>467</v>
+        <v>486</v>
       </c>
       <c r="N34" s="18">
-        <v>45154</v>
+        <v>45141</v>
       </c>
       <c r="O34" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3634,7 +3692,7 @@
       </c>
       <c r="P34">
         <f t="shared" ca="1" si="4"/>
-        <v>467</v>
+        <v>486</v>
       </c>
       <c r="Q34" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -3660,10 +3718,10 @@
         <v>26</v>
       </c>
       <c r="M35">
-        <v>448</v>
+        <v>467</v>
       </c>
       <c r="N35" s="18">
-        <v>45155</v>
+        <v>45154</v>
       </c>
       <c r="O35" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3671,7 +3729,7 @@
       </c>
       <c r="P35">
         <f t="shared" ca="1" si="4"/>
-        <v>448</v>
+        <v>467</v>
       </c>
       <c r="Q35" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -3693,11 +3751,26 @@
       <c r="H36" s="19"/>
       <c r="I36" s="19"/>
       <c r="J36" s="19"/>
+      <c r="L36" t="s">
+        <v>27</v>
+      </c>
       <c r="M36">
-        <v>419</v>
+        <v>448</v>
       </c>
       <c r="N36" s="18">
-        <v>45156</v>
+        <v>45155</v>
+      </c>
+      <c r="O36" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>Blue</v>
+      </c>
+      <c r="P36">
+        <f t="shared" ca="1" si="4"/>
+        <v>448</v>
+      </c>
+      <c r="Q36" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
       </c>
     </row>
     <row r="37" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3715,59 +3788,89 @@
       <c r="H37" s="19"/>
       <c r="I37" s="19"/>
       <c r="J37" s="19"/>
+      <c r="L37" t="s">
+        <v>28</v>
+      </c>
       <c r="M37">
+        <v>419</v>
+      </c>
+      <c r="N37" s="18">
+        <v>45156</v>
+      </c>
+      <c r="O37" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>Blue</v>
+      </c>
+      <c r="P37">
+        <f t="shared" ca="1" si="4"/>
+        <v>419</v>
+      </c>
+      <c r="Q37" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="2:17" ht="5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L38" t="s">
+        <v>29</v>
+      </c>
+      <c r="M38">
         <v>346</v>
       </c>
-      <c r="N37" s="18">
+      <c r="N38" s="18">
         <v>45142</v>
       </c>
-    </row>
-    <row r="38" spans="2:17" ht="5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="M38">
-        <v>156</v>
-      </c>
-      <c r="N38" s="18">
-        <v>45139</v>
+      <c r="O38" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>Blue</v>
+      </c>
+      <c r="P38">
+        <f t="shared" ca="1" si="4"/>
+        <v>346</v>
+      </c>
+      <c r="Q38" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
       </c>
     </row>
     <row r="39" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M39">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="N39" s="18">
-        <v>45152</v>
+        <v>45139</v>
       </c>
     </row>
     <row r="40" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M40">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="N40" s="18">
-        <v>45153</v>
+        <v>45152</v>
       </c>
     </row>
     <row r="41" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M41">
-        <v>107</v>
+        <v>140</v>
       </c>
       <c r="N41" s="18">
-        <v>45147</v>
+        <v>45153</v>
       </c>
     </row>
     <row r="42" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M42">
-        <v>38</v>
+        <v>107</v>
       </c>
       <c r="N42" s="18">
-        <v>45140</v>
+        <v>45147</v>
       </c>
     </row>
     <row r="43" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M43">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="N43" s="18">
-        <v>45138</v>
+        <v>45140</v>
       </c>
     </row>
     <row r="44" spans="2:17" x14ac:dyDescent="0.2">
@@ -3775,7 +3878,7 @@
         <v>0</v>
       </c>
       <c r="N44" s="18">
-        <v>0</v>
+        <v>45138</v>
       </c>
     </row>
     <row r="45" spans="2:17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Finished DFT, worked on adsorb reacs and CHE
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E28BAE-7D69-CA44-913D-A68057CC5ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03250EAB-0B2B-A64E-9C18-262261FEF0BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14420" windowHeight="17900" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
@@ -706,6 +706,9 @@
                 <c:pt idx="15">
                   <c:v>45159</c:v>
                 </c:pt>
+                <c:pt idx="16">
+                  <c:v>45160</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -762,6 +765,9 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>6938</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7518</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1092,19 +1098,19 @@
                   <c:v>657</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>486</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>467</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>448</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>419</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>346</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1188,7 +1194,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>580</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -2910,7 +2916,7 @@
   <dimension ref="A1:Q50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3010,7 +3016,7 @@
       </c>
       <c r="I6" s="42"/>
       <c r="J6" s="14">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -3025,11 +3031,11 @@
       </c>
       <c r="E7" s="6">
         <f t="shared" ref="E7:E37" si="0">D7/$J$6</f>
-        <v>0.45614035087719296</v>
+        <v>0.45882352941176469</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" ref="F7:F37" si="1">D7/$J$8</f>
-        <v>9.1228070175438589E-3</v>
+        <v>9.1764705882352946E-3</v>
       </c>
       <c r="H7" s="43" t="s">
         <v>5</v>
@@ -3044,7 +3050,7 @@
         <v>45140</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" ref="C8:C21" si="2">D8-D7</f>
+        <f t="shared" ref="C8:C22" si="2">D8-D7</f>
         <v>38</v>
       </c>
       <c r="D8" s="1">
@@ -3052,11 +3058,11 @@
       </c>
       <c r="E8" s="6">
         <f t="shared" si="0"/>
-        <v>0.56725146198830412</v>
+        <v>0.57058823529411762</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="1"/>
-        <v>1.1345029239766082E-2</v>
+        <v>1.1411764705882352E-2</v>
       </c>
       <c r="H8" s="45" t="s">
         <v>6</v>
@@ -3064,7 +3070,7 @@
       <c r="I8" s="46"/>
       <c r="J8" s="15">
         <f>J6*J7</f>
-        <v>17100</v>
+        <v>17000</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3080,11 +3086,11 @@
       </c>
       <c r="E9" s="6">
         <f t="shared" si="0"/>
-        <v>1.9883040935672514</v>
+        <v>2</v>
       </c>
       <c r="F9" s="7">
         <f t="shared" si="1"/>
-        <v>3.9766081871345033E-2</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -3100,11 +3106,11 @@
       </c>
       <c r="E10" s="6">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>3.0176470588235293</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="1"/>
-        <v>0.06</v>
+        <v>6.0352941176470588E-2</v>
       </c>
       <c r="H10" s="47" t="s">
         <v>10</v>
@@ -3125,11 +3131,11 @@
       </c>
       <c r="E11" s="6">
         <f t="shared" si="0"/>
-        <v>5.1315789473684212</v>
+        <v>5.1617647058823533</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="1"/>
-        <v>0.10263157894736842</v>
+        <v>0.10323529411764706</v>
       </c>
       <c r="H11" s="50"/>
       <c r="I11" s="51"/>
@@ -3148,11 +3154,11 @@
       </c>
       <c r="E12" s="6">
         <f t="shared" si="0"/>
-        <v>7.6432748538011692</v>
+        <v>7.6882352941176473</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="1"/>
-        <v>0.1528654970760234</v>
+        <v>0.15376470588235294</v>
       </c>
       <c r="H12" s="23" t="s">
         <v>11</v>
@@ -3160,7 +3166,7 @@
       <c r="I12" s="24"/>
       <c r="J12" s="16">
         <f>J8-MAX(D6:D27)</f>
-        <v>10162</v>
+        <v>9482</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -3176,19 +3182,19 @@
       </c>
       <c r="E13" s="6">
         <f t="shared" si="0"/>
-        <v>7.9561403508771926</v>
+        <v>8.0029411764705891</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="1"/>
-        <v>0.15912280701754386</v>
+        <v>0.16005882352941175</v>
       </c>
       <c r="H13" s="25" t="s">
         <v>12</v>
       </c>
       <c r="I13" s="26"/>
       <c r="J13" s="16">
-        <f>AVERAGE(C9:C21)</f>
-        <v>518.76923076923072</v>
+        <f>AVERAGE(C9:C22)</f>
+        <v>523.14285714285711</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3204,11 +3210,11 @@
       </c>
       <c r="E14" s="6">
         <f t="shared" si="0"/>
-        <v>11.695906432748538</v>
+        <v>11.764705882352942</v>
       </c>
       <c r="F14" s="7">
         <f t="shared" si="1"/>
-        <v>0.23391812865497075</v>
+        <v>0.23529411764705882</v>
       </c>
       <c r="H14" s="27" t="s">
         <v>13</v>
@@ -3216,7 +3222,7 @@
       <c r="I14" s="28"/>
       <c r="J14" s="17">
         <f>J12/J13</f>
-        <v>19.58867141162515</v>
+        <v>18.125068268705625</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -3232,11 +3238,11 @@
       </c>
       <c r="E15" s="6">
         <f t="shared" si="0"/>
-        <v>13.616959064327485</v>
+        <v>13.697058823529412</v>
       </c>
       <c r="F15" s="7">
         <f t="shared" si="1"/>
-        <v>0.27233918128654971</v>
+        <v>0.27394117647058824</v>
       </c>
       <c r="H15" s="13" t="s">
         <v>24</v>
@@ -3261,11 +3267,11 @@
       </c>
       <c r="E16" s="6">
         <f t="shared" si="0"/>
-        <v>14.043859649122806</v>
+        <v>14.126470588235295</v>
       </c>
       <c r="F16" s="7">
         <f t="shared" si="1"/>
-        <v>0.28087719298245611</v>
+        <v>0.28252941176470586</v>
       </c>
       <c r="J16" s="22"/>
     </row>
@@ -3282,11 +3288,11 @@
       </c>
       <c r="E17" s="6">
         <f t="shared" si="0"/>
-        <v>14.453216374269006</v>
+        <v>14.538235294117648</v>
       </c>
       <c r="F17" s="7">
         <f t="shared" si="1"/>
-        <v>0.28906432748538013</v>
+        <v>0.29076470588235293</v>
       </c>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.2">
@@ -3302,11 +3308,11 @@
       </c>
       <c r="E18" s="6">
         <f t="shared" si="0"/>
-        <v>15.818713450292398</v>
+        <v>15.911764705882353</v>
       </c>
       <c r="F18" s="7">
         <f t="shared" si="1"/>
-        <v>0.31637426900584797</v>
+        <v>0.31823529411764706</v>
       </c>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.2">
@@ -3322,11 +3328,11 @@
       </c>
       <c r="E19" s="6">
         <f t="shared" si="0"/>
-        <v>17.128654970760234</v>
+        <v>17.229411764705883</v>
       </c>
       <c r="F19" s="7">
         <f t="shared" si="1"/>
-        <v>0.3425730994152047</v>
+        <v>0.34458823529411764</v>
       </c>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.2">
@@ -3342,11 +3348,11 @@
       </c>
       <c r="E20" s="6">
         <f t="shared" si="0"/>
-        <v>18.353801169590643</v>
+        <v>18.461764705882352</v>
       </c>
       <c r="F20" s="7">
         <f t="shared" si="1"/>
-        <v>0.36707602339181289</v>
+        <v>0.36923529411764705</v>
       </c>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.2">
@@ -3362,24 +3368,31 @@
       </c>
       <c r="E21" s="6">
         <f t="shared" si="0"/>
-        <v>20.28654970760234</v>
+        <v>20.405882352941177</v>
       </c>
       <c r="F21" s="7">
         <f t="shared" si="1"/>
-        <v>0.40573099415204678</v>
+        <v>0.40811764705882353</v>
       </c>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B22" s="3"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
+      <c r="B22" s="3">
+        <v>45160</v>
+      </c>
+      <c r="C22" s="1">
+        <f t="shared" si="2"/>
+        <v>580</v>
+      </c>
+      <c r="D22" s="1">
+        <v>7518</v>
+      </c>
       <c r="E22" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>22.111764705882354</v>
       </c>
       <c r="F22" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.44223529411764706</v>
       </c>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.2">
@@ -3681,22 +3694,22 @@
         <v>25</v>
       </c>
       <c r="M34">
-        <v>486</v>
+        <v>580</v>
       </c>
       <c r="N34" s="18">
-        <v>45141</v>
+        <v>45160</v>
       </c>
       <c r="O34" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Blue</v>
-      </c>
-      <c r="P34">
+        <v>Green</v>
+      </c>
+      <c r="P34" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>486</v>
-      </c>
-      <c r="Q34" t="str">
+        <v/>
+      </c>
+      <c r="Q34">
         <f t="shared" ca="1" si="5"/>
-        <v/>
+        <v>580</v>
       </c>
     </row>
     <row r="35" spans="2:17" x14ac:dyDescent="0.2">
@@ -3718,10 +3731,10 @@
         <v>26</v>
       </c>
       <c r="M35">
-        <v>467</v>
+        <v>486</v>
       </c>
       <c r="N35" s="18">
-        <v>45154</v>
+        <v>45141</v>
       </c>
       <c r="O35" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3729,7 +3742,7 @@
       </c>
       <c r="P35">
         <f t="shared" ca="1" si="4"/>
-        <v>467</v>
+        <v>486</v>
       </c>
       <c r="Q35" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -3755,10 +3768,10 @@
         <v>27</v>
       </c>
       <c r="M36">
-        <v>448</v>
+        <v>467</v>
       </c>
       <c r="N36" s="18">
-        <v>45155</v>
+        <v>45154</v>
       </c>
       <c r="O36" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3766,7 +3779,7 @@
       </c>
       <c r="P36">
         <f t="shared" ca="1" si="4"/>
-        <v>448</v>
+        <v>467</v>
       </c>
       <c r="Q36" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -3792,10 +3805,10 @@
         <v>28</v>
       </c>
       <c r="M37">
-        <v>419</v>
+        <v>448</v>
       </c>
       <c r="N37" s="18">
-        <v>45156</v>
+        <v>45155</v>
       </c>
       <c r="O37" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3803,7 +3816,7 @@
       </c>
       <c r="P37">
         <f t="shared" ca="1" si="4"/>
-        <v>419</v>
+        <v>448</v>
       </c>
       <c r="Q37" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -3815,10 +3828,10 @@
         <v>29</v>
       </c>
       <c r="M38">
-        <v>346</v>
+        <v>419</v>
       </c>
       <c r="N38" s="18">
-        <v>45142</v>
+        <v>45156</v>
       </c>
       <c r="O38" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3826,7 +3839,7 @@
       </c>
       <c r="P38">
         <f t="shared" ca="1" si="4"/>
-        <v>346</v>
+        <v>419</v>
       </c>
       <c r="Q38" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -3835,50 +3848,50 @@
     </row>
     <row r="39" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M39">
-        <v>156</v>
+        <v>346</v>
       </c>
       <c r="N39" s="18">
-        <v>45139</v>
+        <v>45142</v>
       </c>
     </row>
     <row r="40" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M40">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="N40" s="18">
-        <v>45152</v>
+        <v>45139</v>
       </c>
     </row>
     <row r="41" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M41">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="N41" s="18">
-        <v>45153</v>
+        <v>45152</v>
       </c>
     </row>
     <row r="42" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M42">
-        <v>107</v>
+        <v>140</v>
       </c>
       <c r="N42" s="18">
-        <v>45147</v>
+        <v>45153</v>
       </c>
     </row>
     <row r="43" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M43">
-        <v>38</v>
+        <v>107</v>
       </c>
       <c r="N43" s="18">
-        <v>45140</v>
+        <v>45147</v>
       </c>
     </row>
     <row r="44" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M44">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="N44" s="18">
-        <v>45138</v>
+        <v>45140</v>
       </c>
     </row>
     <row r="45" spans="2:17" x14ac:dyDescent="0.2">
@@ -3886,7 +3899,7 @@
         <v>0</v>
       </c>
       <c r="N45" s="18">
-        <v>0</v>
+        <v>45138</v>
       </c>
     </row>
     <row r="46" spans="2:17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Wrote about the SHE, RHE and CHE
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03250EAB-0B2B-A64E-9C18-262261FEF0BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A8059FA-122E-FF4A-987D-AA63F6E49E44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14420" windowHeight="17900" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Keeping up with the thesis</t>
   </si>
@@ -148,6 +148,12 @@
   </si>
   <si>
     <t>Tenth best</t>
+  </si>
+  <si>
+    <t>Eleventh best</t>
+  </si>
+  <si>
+    <t>Twelth best</t>
   </si>
 </sst>
 </file>
@@ -709,6 +715,9 @@
                 <c:pt idx="16">
                   <c:v>45160</c:v>
                 </c:pt>
+                <c:pt idx="17">
+                  <c:v>45161</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -768,6 +777,9 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>7518</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7867</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1040,9 +1052,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$L$29:$L$38</c:f>
+              <c:f>Sheet1!$L$29:$L$40</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>Best day</c:v>
                 </c:pt>
@@ -1072,16 +1084,22 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Tenth best</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Eleventh best</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Twelth best</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$29:$P$38</c:f>
+              <c:f>Sheet1!$P$29:$P$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>1279</c:v>
                 </c:pt>
@@ -1098,7 +1116,7 @@
                   <c:v>657</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>580</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>486</c:v>
@@ -1111,6 +1129,12 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>419</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>346</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1136,9 +1160,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$L$29:$L$38</c:f>
+              <c:f>Sheet1!$L$29:$L$40</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>Best day</c:v>
                 </c:pt>
@@ -1168,16 +1192,22 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Tenth best</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Eleventh best</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Twelth best</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$29:$Q$38</c:f>
+              <c:f>Sheet1!$Q$29:$Q$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1194,7 +1224,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>580</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -1206,6 +1236,12 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>349</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1334,6 +1370,8 @@
         <c:crossAx val="813497808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="340"/>
+        <c:minorUnit val="340"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2556,15 +2594,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>31752</xdr:colOff>
+      <xdr:colOff>31754</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>60854</xdr:rowOff>
+      <xdr:rowOff>60857</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>531814</xdr:colOff>
+      <xdr:colOff>531816</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>60854</xdr:rowOff>
+      <xdr:rowOff>60857</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2579,7 +2617,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7323669" y="5585354"/>
+          <a:off x="7323671" y="5585357"/>
           <a:ext cx="5453062" cy="4508500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2915,8 +2953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4213BD91-B5D1-3B47-8D3F-04331482504C}">
   <dimension ref="A1:Q50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3050,7 +3088,7 @@
         <v>45140</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" ref="C8:C22" si="2">D8-D7</f>
+        <f t="shared" ref="C8:C23" si="2">D8-D7</f>
         <v>38</v>
       </c>
       <c r="D8" s="1">
@@ -3166,7 +3204,7 @@
       <c r="I12" s="24"/>
       <c r="J12" s="16">
         <f>J8-MAX(D6:D27)</f>
-        <v>9482</v>
+        <v>9133</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -3222,7 +3260,7 @@
       <c r="I14" s="28"/>
       <c r="J14" s="17">
         <f>J12/J13</f>
-        <v>18.125068268705625</v>
+        <v>17.45794647733479</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -3396,16 +3434,23 @@
       </c>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B23" s="3"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
+      <c r="B23" s="3">
+        <v>45161</v>
+      </c>
+      <c r="C23" s="1">
+        <f t="shared" si="2"/>
+        <v>349</v>
+      </c>
+      <c r="D23" s="1">
+        <v>7867</v>
+      </c>
       <c r="E23" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23.138235294117646</v>
       </c>
       <c r="F23" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.46276470588235297</v>
       </c>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.2">
@@ -3552,15 +3597,15 @@
         <v>45146</v>
       </c>
       <c r="O30" t="str">
-        <f t="shared" ref="O30:O38" ca="1" si="3">IF(N30=TODAY(), "Green", "Blue")</f>
+        <f t="shared" ref="O30:O40" ca="1" si="3">IF(N30=TODAY(), "Green", "Blue")</f>
         <v>Blue</v>
       </c>
       <c r="P30">
-        <f t="shared" ref="P30:P38" ca="1" si="4">IF(NOT(N30=TODAY()), M30, "")</f>
+        <f t="shared" ref="P30:P40" ca="1" si="4">IF(NOT(N30=TODAY()), M30, "")</f>
         <v>859</v>
       </c>
       <c r="Q30" t="str">
-        <f t="shared" ref="Q30:Q38" ca="1" si="5">IF(N30=TODAY(), M30, "")</f>
+        <f t="shared" ref="Q30:Q40" ca="1" si="5">IF(N30=TODAY(), M30, "")</f>
         <v/>
       </c>
     </row>
@@ -3701,15 +3746,15 @@
       </c>
       <c r="O34" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Green</v>
-      </c>
-      <c r="P34" t="str">
+        <v>Blue</v>
+      </c>
+      <c r="P34">
         <f t="shared" ca="1" si="4"/>
+        <v>580</v>
+      </c>
+      <c r="Q34" t="str">
+        <f t="shared" ca="1" si="5"/>
         <v/>
-      </c>
-      <c r="Q34">
-        <f t="shared" ca="1" si="5"/>
-        <v>580</v>
       </c>
     </row>
     <row r="35" spans="2:17" x14ac:dyDescent="0.2">
@@ -3847,59 +3892,89 @@
       </c>
     </row>
     <row r="39" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="L39" t="s">
+        <v>30</v>
+      </c>
       <c r="M39">
+        <v>349</v>
+      </c>
+      <c r="N39" s="18">
+        <v>45161</v>
+      </c>
+      <c r="O39" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>Green</v>
+      </c>
+      <c r="P39" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+      <c r="Q39">
+        <f t="shared" ca="1" si="5"/>
+        <v>349</v>
+      </c>
+    </row>
+    <row r="40" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="L40" t="s">
+        <v>31</v>
+      </c>
+      <c r="M40">
         <v>346</v>
       </c>
-      <c r="N39" s="18">
+      <c r="N40" s="18">
         <v>45142</v>
       </c>
-    </row>
-    <row r="40" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="M40">
-        <v>156</v>
-      </c>
-      <c r="N40" s="18">
-        <v>45139</v>
+      <c r="O40" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>Blue</v>
+      </c>
+      <c r="P40">
+        <f t="shared" ca="1" si="4"/>
+        <v>346</v>
+      </c>
+      <c r="Q40" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
       </c>
     </row>
     <row r="41" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M41">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="N41" s="18">
-        <v>45152</v>
+        <v>45139</v>
       </c>
     </row>
     <row r="42" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M42">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="N42" s="18">
-        <v>45153</v>
+        <v>45152</v>
       </c>
     </row>
     <row r="43" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M43">
-        <v>107</v>
+        <v>140</v>
       </c>
       <c r="N43" s="18">
-        <v>45147</v>
+        <v>45153</v>
       </c>
     </row>
     <row r="44" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M44">
-        <v>38</v>
+        <v>107</v>
       </c>
       <c r="N44" s="18">
-        <v>45140</v>
+        <v>45147</v>
       </c>
     </row>
     <row r="45" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M45">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="N45" s="18">
-        <v>45138</v>
+        <v>45140</v>
       </c>
     </row>
     <row r="46" spans="2:17" x14ac:dyDescent="0.2">
@@ -3907,7 +3982,7 @@
         <v>0</v>
       </c>
       <c r="N46" s="18">
-        <v>0</v>
+        <v>45138</v>
       </c>
     </row>
     <row r="47" spans="2:17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Finished writing on E -> G and HALFWAY IN WORDCOUNT
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A8059FA-122E-FF4A-987D-AA63F6E49E44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D0368E-9C36-FE41-A648-5F26DA55429E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14420" windowHeight="17900" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Keeping up with the thesis</t>
   </si>
@@ -154,6 +154,15 @@
   </si>
   <si>
     <t>Twelth best</t>
+  </si>
+  <si>
+    <t>Thirteenth best</t>
+  </si>
+  <si>
+    <t>Fourteenth best</t>
+  </si>
+  <si>
+    <t>Fifteen best</t>
   </si>
 </sst>
 </file>
@@ -718,6 +727,12 @@
                 <c:pt idx="17">
                   <c:v>45161</c:v>
                 </c:pt>
+                <c:pt idx="18">
+                  <c:v>45162</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>45163</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -780,6 +795,12 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>7867</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8021</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8632</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1052,9 +1073,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$L$29:$L$40</c:f>
+              <c:f>Sheet1!$L$29:$L$43</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>Best day</c:v>
                 </c:pt>
@@ -1090,16 +1111,25 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>Twelth best</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Thirteenth best</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Fourteenth best</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Fifteen best</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$29:$P$40</c:f>
+              <c:f>Sheet1!$P$29:$P$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>1279</c:v>
                 </c:pt>
@@ -1116,25 +1146,34 @@
                   <c:v>657</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>580</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>486</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>467</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>448</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>419</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="11">
+                  <c:v>349</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>346</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>154</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1160,9 +1199,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$L$29:$L$40</c:f>
+              <c:f>Sheet1!$L$29:$L$43</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>Best day</c:v>
                 </c:pt>
@@ -1198,16 +1237,25 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>Twelth best</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Thirteenth best</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Fourteenth best</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Fifteen best</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$29:$Q$40</c:f>
+              <c:f>Sheet1!$Q$29:$Q$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1224,7 +1272,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>611</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -1239,9 +1287,18 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>349</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1295,7 +1352,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2596,13 +2653,13 @@
       <xdr:col>11</xdr:col>
       <xdr:colOff>31754</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>60857</xdr:rowOff>
+      <xdr:rowOff>50272</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>531816</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>60857</xdr:rowOff>
+      <xdr:rowOff>50272</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2617,7 +2674,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7323671" y="5585357"/>
+          <a:off x="7323671" y="5574772"/>
           <a:ext cx="5453062" cy="4508500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2953,8 +3010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4213BD91-B5D1-3B47-8D3F-04331482504C}">
   <dimension ref="A1:Q50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3088,7 +3145,7 @@
         <v>45140</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" ref="C8:C23" si="2">D8-D7</f>
+        <f t="shared" ref="C8:C25" si="2">D8-D7</f>
         <v>38</v>
       </c>
       <c r="D8" s="1">
@@ -3204,7 +3261,7 @@
       <c r="I12" s="24"/>
       <c r="J12" s="16">
         <f>J8-MAX(D6:D27)</f>
-        <v>9133</v>
+        <v>8368</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -3231,8 +3288,8 @@
       </c>
       <c r="I13" s="26"/>
       <c r="J13" s="16">
-        <f>AVERAGE(C9:C22)</f>
-        <v>523.14285714285711</v>
+        <f>AVERAGE(C9:C25)</f>
+        <v>496.35294117647061</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -3260,7 +3317,7 @@
       <c r="I14" s="28"/>
       <c r="J14" s="17">
         <f>J12/J13</f>
-        <v>17.45794647733479</v>
+        <v>16.85897132021806</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -3454,29 +3511,43 @@
       </c>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B24" s="3"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
+      <c r="B24" s="3">
+        <v>45162</v>
+      </c>
+      <c r="C24" s="1">
+        <f t="shared" si="2"/>
+        <v>154</v>
+      </c>
+      <c r="D24" s="1">
+        <v>8021</v>
+      </c>
       <c r="E24" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>23.591176470588234</v>
       </c>
       <c r="F24" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.4718235294117647</v>
       </c>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B25" s="3"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
+      <c r="B25" s="3">
+        <v>45163</v>
+      </c>
+      <c r="C25" s="1">
+        <f t="shared" si="2"/>
+        <v>611</v>
+      </c>
+      <c r="D25" s="1">
+        <v>8632</v>
+      </c>
       <c r="E25" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>25.388235294117646</v>
       </c>
       <c r="F25" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.5077647058823529</v>
       </c>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.2">
@@ -3597,15 +3668,15 @@
         <v>45146</v>
       </c>
       <c r="O30" t="str">
-        <f t="shared" ref="O30:O40" ca="1" si="3">IF(N30=TODAY(), "Green", "Blue")</f>
+        <f t="shared" ref="O30:O43" ca="1" si="3">IF(N30=TODAY(), "Green", "Blue")</f>
         <v>Blue</v>
       </c>
       <c r="P30">
-        <f t="shared" ref="P30:P40" ca="1" si="4">IF(NOT(N30=TODAY()), M30, "")</f>
+        <f t="shared" ref="P30:P43" ca="1" si="4">IF(NOT(N30=TODAY()), M30, "")</f>
         <v>859</v>
       </c>
       <c r="Q30" t="str">
-        <f t="shared" ref="Q30:Q40" ca="1" si="5">IF(N30=TODAY(), M30, "")</f>
+        <f t="shared" ref="Q30:Q43" ca="1" si="5">IF(N30=TODAY(), M30, "")</f>
         <v/>
       </c>
     </row>
@@ -3739,22 +3810,22 @@
         <v>25</v>
       </c>
       <c r="M34">
-        <v>580</v>
+        <v>611</v>
       </c>
       <c r="N34" s="18">
-        <v>45160</v>
+        <v>45163</v>
       </c>
       <c r="O34" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Blue</v>
-      </c>
-      <c r="P34">
+        <v>Green</v>
+      </c>
+      <c r="P34" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>580</v>
-      </c>
-      <c r="Q34" t="str">
+        <v/>
+      </c>
+      <c r="Q34">
         <f t="shared" ca="1" si="5"/>
-        <v/>
+        <v>611</v>
       </c>
     </row>
     <row r="35" spans="2:17" x14ac:dyDescent="0.2">
@@ -3776,10 +3847,10 @@
         <v>26</v>
       </c>
       <c r="M35">
-        <v>486</v>
+        <v>580</v>
       </c>
       <c r="N35" s="18">
-        <v>45141</v>
+        <v>45160</v>
       </c>
       <c r="O35" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3787,7 +3858,7 @@
       </c>
       <c r="P35">
         <f t="shared" ca="1" si="4"/>
-        <v>486</v>
+        <v>580</v>
       </c>
       <c r="Q35" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -3813,10 +3884,10 @@
         <v>27</v>
       </c>
       <c r="M36">
-        <v>467</v>
+        <v>486</v>
       </c>
       <c r="N36" s="18">
-        <v>45154</v>
+        <v>45141</v>
       </c>
       <c r="O36" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3824,7 +3895,7 @@
       </c>
       <c r="P36">
         <f t="shared" ca="1" si="4"/>
-        <v>467</v>
+        <v>486</v>
       </c>
       <c r="Q36" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -3850,10 +3921,10 @@
         <v>28</v>
       </c>
       <c r="M37">
-        <v>448</v>
+        <v>467</v>
       </c>
       <c r="N37" s="18">
-        <v>45155</v>
+        <v>45154</v>
       </c>
       <c r="O37" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3861,7 +3932,7 @@
       </c>
       <c r="P37">
         <f t="shared" ca="1" si="4"/>
-        <v>448</v>
+        <v>467</v>
       </c>
       <c r="Q37" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -3873,10 +3944,10 @@
         <v>29</v>
       </c>
       <c r="M38">
-        <v>419</v>
+        <v>448</v>
       </c>
       <c r="N38" s="18">
-        <v>45156</v>
+        <v>45155</v>
       </c>
       <c r="O38" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3884,7 +3955,7 @@
       </c>
       <c r="P38">
         <f t="shared" ca="1" si="4"/>
-        <v>419</v>
+        <v>448</v>
       </c>
       <c r="Q38" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -3896,22 +3967,22 @@
         <v>30</v>
       </c>
       <c r="M39">
-        <v>349</v>
+        <v>419</v>
       </c>
       <c r="N39" s="18">
-        <v>45161</v>
+        <v>45156</v>
       </c>
       <c r="O39" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Green</v>
-      </c>
-      <c r="P39" t="str">
+        <v>Blue</v>
+      </c>
+      <c r="P39">
         <f t="shared" ca="1" si="4"/>
+        <v>419</v>
+      </c>
+      <c r="Q39" t="str">
+        <f t="shared" ca="1" si="5"/>
         <v/>
-      </c>
-      <c r="Q39">
-        <f t="shared" ca="1" si="5"/>
-        <v>349</v>
       </c>
     </row>
     <row r="40" spans="2:17" x14ac:dyDescent="0.2">
@@ -3919,10 +3990,10 @@
         <v>31</v>
       </c>
       <c r="M40">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="N40" s="18">
-        <v>45142</v>
+        <v>45161</v>
       </c>
       <c r="O40" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3930,7 +4001,7 @@
       </c>
       <c r="P40">
         <f t="shared" ca="1" si="4"/>
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="Q40" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -3938,59 +4009,104 @@
       </c>
     </row>
     <row r="41" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="L41" t="s">
+        <v>32</v>
+      </c>
       <c r="M41">
+        <v>346</v>
+      </c>
+      <c r="N41" s="18">
+        <v>45142</v>
+      </c>
+      <c r="O41" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>Blue</v>
+      </c>
+      <c r="P41">
+        <f t="shared" ca="1" si="4"/>
+        <v>346</v>
+      </c>
+      <c r="Q41" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="L42" t="s">
+        <v>33</v>
+      </c>
+      <c r="M42">
         <v>156</v>
       </c>
-      <c r="N41" s="18">
+      <c r="N42" s="18">
         <v>45139</v>
       </c>
-    </row>
-    <row r="42" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="M42">
-        <v>146</v>
-      </c>
-      <c r="N42" s="18">
-        <v>45152</v>
+      <c r="O42" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>Blue</v>
+      </c>
+      <c r="P42">
+        <f t="shared" ca="1" si="4"/>
+        <v>156</v>
+      </c>
+      <c r="Q42" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
       </c>
     </row>
     <row r="43" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="L43" t="s">
+        <v>34</v>
+      </c>
       <c r="M43">
-        <v>140</v>
+        <v>154</v>
       </c>
       <c r="N43" s="18">
-        <v>45153</v>
+        <v>45162</v>
+      </c>
+      <c r="O43" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>Blue</v>
+      </c>
+      <c r="P43">
+        <f t="shared" ca="1" si="4"/>
+        <v>154</v>
+      </c>
+      <c r="Q43" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
       </c>
     </row>
     <row r="44" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M44">
-        <v>107</v>
+        <v>146</v>
       </c>
       <c r="N44" s="18">
-        <v>45147</v>
+        <v>45152</v>
       </c>
     </row>
     <row r="45" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M45">
-        <v>38</v>
+        <v>140</v>
       </c>
       <c r="N45" s="18">
-        <v>45140</v>
+        <v>45153</v>
       </c>
     </row>
     <row r="46" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M46">
-        <v>0</v>
+        <v>107</v>
       </c>
       <c r="N46" s="18">
-        <v>45138</v>
+        <v>45147</v>
       </c>
     </row>
     <row r="47" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M47">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="N47" s="18">
-        <v>0</v>
+        <v>45140</v>
       </c>
     </row>
     <row r="48" spans="2:17" x14ac:dyDescent="0.2">
@@ -3998,7 +4114,7 @@
         <v>0</v>
       </c>
       <c r="N48" s="18">
-        <v>0</v>
+        <v>45138</v>
       </c>
     </row>
     <row r="49" spans="13:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Drew a diagram of all the science to show Jan and made notes on HEA
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D0368E-9C36-FE41-A648-5F26DA55429E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC43A7CF-B739-5F46-BA74-81287606EAFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14420" windowHeight="17900" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
@@ -733,6 +733,9 @@
                 <c:pt idx="19">
                   <c:v>45163</c:v>
                 </c:pt>
+                <c:pt idx="20">
+                  <c:v>45164</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -801,6 +804,9 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>8632</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8727</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1146,7 +1152,7 @@
                   <c:v>657</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>611</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>580</c:v>
@@ -1272,7 +1278,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>611</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -3011,7 +3017,7 @@
   <dimension ref="A1:Q50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3145,7 +3151,7 @@
         <v>45140</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" ref="C8:C25" si="2">D8-D7</f>
+        <f t="shared" ref="C8:C26" si="2">D8-D7</f>
         <v>38</v>
       </c>
       <c r="D8" s="1">
@@ -3261,7 +3267,7 @@
       <c r="I12" s="24"/>
       <c r="J12" s="16">
         <f>J8-MAX(D6:D27)</f>
-        <v>8368</v>
+        <v>8273</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -3317,7 +3323,7 @@
       <c r="I14" s="28"/>
       <c r="J14" s="17">
         <f>J12/J13</f>
-        <v>16.85897132021806</v>
+        <v>16.667575254799715</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -3551,16 +3557,23 @@
       </c>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B26" s="3"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
+      <c r="B26" s="3">
+        <v>45164</v>
+      </c>
+      <c r="C26" s="1">
+        <f t="shared" si="2"/>
+        <v>95</v>
+      </c>
+      <c r="D26" s="1">
+        <v>8727</v>
+      </c>
       <c r="E26" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>25.66764705882353</v>
       </c>
       <c r="F26" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.51335294117647057</v>
       </c>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.2">
@@ -3817,15 +3830,15 @@
       </c>
       <c r="O34" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Green</v>
-      </c>
-      <c r="P34" t="str">
+        <v>Blue</v>
+      </c>
+      <c r="P34">
         <f t="shared" ca="1" si="4"/>
+        <v>611</v>
+      </c>
+      <c r="Q34" t="str">
+        <f t="shared" ca="1" si="5"/>
         <v/>
-      </c>
-      <c r="Q34">
-        <f t="shared" ca="1" si="5"/>
-        <v>611</v>
       </c>
     </row>
     <row r="35" spans="2:17" x14ac:dyDescent="0.2">
@@ -4103,18 +4116,18 @@
     </row>
     <row r="47" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M47">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="N47" s="18">
-        <v>45140</v>
+        <v>45164</v>
       </c>
     </row>
     <row r="48" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M48">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="N48" s="18">
-        <v>45138</v>
+        <v>45140</v>
       </c>
     </row>
     <row r="49" spans="13:14" x14ac:dyDescent="0.2">
@@ -4122,7 +4135,7 @@
         <v>0</v>
       </c>
       <c r="N49" s="18">
-        <v>0</v>
+        <v>45138</v>
       </c>
     </row>
     <row r="50" spans="13:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Wrote a 100 words and made 4 figures
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC43A7CF-B739-5F46-BA74-81287606EAFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC310C06-242B-1D47-A17F-537CA70DB6D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14420" windowHeight="17900" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
@@ -736,6 +736,9 @@
                 <c:pt idx="20">
                   <c:v>45164</c:v>
                 </c:pt>
+                <c:pt idx="21">
+                  <c:v>45168</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -807,6 +810,9 @@
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>8727</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8846</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3017,7 +3023,7 @@
   <dimension ref="A1:Q50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3151,7 +3157,7 @@
         <v>45140</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" ref="C8:C26" si="2">D8-D7</f>
+        <f t="shared" ref="C8:C27" si="2">D8-D7</f>
         <v>38</v>
       </c>
       <c r="D8" s="1">
@@ -3267,7 +3273,7 @@
       <c r="I12" s="24"/>
       <c r="J12" s="16">
         <f>J8-MAX(D6:D27)</f>
-        <v>8273</v>
+        <v>8154</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -3323,7 +3329,7 @@
       <c r="I14" s="28"/>
       <c r="J14" s="17">
         <f>J12/J13</f>
-        <v>16.667575254799715</v>
+        <v>16.427826499170418</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -3577,16 +3583,23 @@
       </c>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B27" s="3"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
+      <c r="B27" s="3">
+        <v>45168</v>
+      </c>
+      <c r="C27" s="1">
+        <f t="shared" si="2"/>
+        <v>119</v>
+      </c>
+      <c r="D27" s="1">
+        <v>8846</v>
+      </c>
       <c r="E27" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>26.017647058823531</v>
       </c>
       <c r="F27" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.52035294117647057</v>
       </c>
     </row>
     <row r="28" spans="2:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -4108,34 +4121,34 @@
     </row>
     <row r="46" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M46">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="N46" s="18">
-        <v>45147</v>
+        <v>45168</v>
       </c>
     </row>
     <row r="47" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M47">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="N47" s="18">
-        <v>45164</v>
+        <v>45147</v>
       </c>
     </row>
     <row r="48" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M48">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="N48" s="18">
-        <v>45140</v>
+        <v>45164</v>
       </c>
     </row>
     <row r="49" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M49">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="N49" s="18">
-        <v>45138</v>
+        <v>45140</v>
       </c>
     </row>
     <row r="50" spans="13:14" x14ac:dyDescent="0.2">
@@ -4143,7 +4156,7 @@
         <v>0</v>
       </c>
       <c r="N50" s="18">
-        <v>0</v>
+        <v>45138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved two figures and wrote 200 words about FAOR
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC310C06-242B-1D47-A17F-537CA70DB6D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B5B69C-339B-9C45-9780-25459A4A8618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14420" windowHeight="17900" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -1182,10 +1182,10 @@
                   <c:v>346</c:v>
                 </c:pt>
                 <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>156</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>154</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1308,7 +1308,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>217</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -2663,15 +2663,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>31754</xdr:colOff>
+      <xdr:colOff>31753</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>50272</xdr:rowOff>
+      <xdr:rowOff>39688</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>531816</xdr:colOff>
+      <xdr:colOff>531815</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>50272</xdr:rowOff>
+      <xdr:rowOff>39688</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2686,7 +2686,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7323671" y="5574772"/>
+          <a:off x="7323670" y="5564188"/>
           <a:ext cx="5453062" cy="4508500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3020,10 +3020,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4213BD91-B5D1-3B47-8D3F-04331482504C}">
-  <dimension ref="A1:Q50"/>
+  <dimension ref="A1:Q60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3157,7 +3157,7 @@
         <v>45140</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" ref="C8:C27" si="2">D8-D7</f>
+        <f t="shared" ref="C8:C28" si="2">D8-D7</f>
         <v>38</v>
       </c>
       <c r="D8" s="1">
@@ -3272,8 +3272,8 @@
       </c>
       <c r="I12" s="24"/>
       <c r="J12" s="16">
-        <f>J8-MAX(D6:D27)</f>
-        <v>8154</v>
+        <f>J8-MAX(D6:D37)</f>
+        <v>7937</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -3329,7 +3329,7 @@
       <c r="I14" s="28"/>
       <c r="J14" s="17">
         <f>J12/J13</f>
-        <v>16.427826499170418</v>
+        <v>15.990637591846408</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -3603,16 +3603,23 @@
       </c>
     </row>
     <row r="28" spans="2:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="4"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
+      <c r="B28" s="3">
+        <v>45173</v>
+      </c>
+      <c r="C28" s="1">
+        <f t="shared" si="2"/>
+        <v>217</v>
+      </c>
+      <c r="D28" s="1">
+        <v>9063</v>
+      </c>
       <c r="E28" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>26.655882352941177</v>
       </c>
       <c r="F28" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.53311764705882347</v>
       </c>
       <c r="M28" t="s">
         <v>14</v>
@@ -3649,11 +3656,11 @@
         <v>16</v>
       </c>
       <c r="M29" cm="1">
-        <f t="array" ref="M29:M50">_xlfn.SORTBY(C6:C27, C6:C27, -1)</f>
+        <f t="array" ref="M29:M60">_xlfn.SORTBY(C6:C37, C6:C37, -1)</f>
         <v>1279</v>
       </c>
       <c r="N29" s="18" cm="1">
-        <f t="array" ref="N29:N50">_xlfn.SORTBY(B6:B27,C6:C27, -1)</f>
+        <f t="array" ref="N29:N60">_xlfn.SORTBY(B6:B37,C6:C37, -1)</f>
         <v>45148</v>
       </c>
       <c r="O29" t="str">
@@ -4062,22 +4069,22 @@
         <v>33</v>
       </c>
       <c r="M42">
-        <v>156</v>
+        <v>217</v>
       </c>
       <c r="N42" s="18">
-        <v>45139</v>
+        <v>45173</v>
       </c>
       <c r="O42" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Blue</v>
-      </c>
-      <c r="P42">
+        <v>Green</v>
+      </c>
+      <c r="P42" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>156</v>
-      </c>
-      <c r="Q42" t="str">
+        <v/>
+      </c>
+      <c r="Q42">
         <f t="shared" ca="1" si="5"/>
-        <v/>
+        <v>217</v>
       </c>
     </row>
     <row r="43" spans="2:17" x14ac:dyDescent="0.2">
@@ -4085,10 +4092,10 @@
         <v>34</v>
       </c>
       <c r="M43">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="N43" s="18">
-        <v>45162</v>
+        <v>45139</v>
       </c>
       <c r="O43" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4096,7 +4103,7 @@
       </c>
       <c r="P43">
         <f t="shared" ca="1" si="4"/>
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="Q43" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -4105,58 +4112,138 @@
     </row>
     <row r="44" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M44">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="N44" s="18">
-        <v>45152</v>
+        <v>45162</v>
       </c>
     </row>
     <row r="45" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M45">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="N45" s="18">
-        <v>45153</v>
+        <v>45152</v>
       </c>
     </row>
     <row r="46" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M46">
-        <v>119</v>
+        <v>140</v>
       </c>
       <c r="N46" s="18">
-        <v>45168</v>
+        <v>45153</v>
       </c>
     </row>
     <row r="47" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M47">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="N47" s="18">
-        <v>45147</v>
+        <v>45168</v>
       </c>
     </row>
     <row r="48" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M48">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="N48" s="18">
-        <v>45164</v>
+        <v>45147</v>
       </c>
     </row>
     <row r="49" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M49">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="N49" s="18">
-        <v>45140</v>
+        <v>45164</v>
       </c>
     </row>
     <row r="50" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M50">
+        <v>38</v>
+      </c>
+      <c r="N50" s="18">
+        <v>45140</v>
+      </c>
+    </row>
+    <row r="51" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="M51">
         <v>0</v>
       </c>
-      <c r="N50" s="18">
+      <c r="N51">
         <v>45138</v>
+      </c>
+    </row>
+    <row r="52" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="M52">
+        <v>0</v>
+      </c>
+      <c r="N52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="M53">
+        <v>0</v>
+      </c>
+      <c r="N53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="M54">
+        <v>0</v>
+      </c>
+      <c r="N54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="M55">
+        <v>0</v>
+      </c>
+      <c r="N55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="M56">
+        <v>0</v>
+      </c>
+      <c r="N56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="M57">
+        <v>0</v>
+      </c>
+      <c r="N57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="M58">
+        <v>0</v>
+      </c>
+      <c r="N58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="M59">
+        <v>0</v>
+      </c>
+      <c r="N59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="M60">
+        <v>0</v>
+      </c>
+      <c r="N60">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Calculations on U_cathode and writing
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADACF65E-6854-814C-85EF-267FDEB0B0FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA47A567-A2DB-DB49-8B07-BCCB57310578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14420" windowHeight="17900" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
@@ -430,14 +430,12 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="4" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="4" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -564,6 +562,14 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -669,10 +675,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$6:$B$27</c:f>
+              <c:f>Sheet1!$B$6:$B$30</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>45138</c:v>
                 </c:pt>
@@ -738,16 +744,25 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>45168</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>45173</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>45174</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>45175</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$6:$D$27</c:f>
+              <c:f>Sheet1!$D$6:$D$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="22"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -813,6 +828,15 @@
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>8846</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9063</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9536</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9756</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -865,7 +889,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="700" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
@@ -889,6 +913,7 @@
         <c:axId val="656428208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="17000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -937,6 +962,7 @@
         <c:crossAx val="294074880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="1000"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1167,7 +1193,7 @@
                   <c:v>486</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>473</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>467</c:v>
@@ -1185,7 +1211,7 @@
                   <c:v>346</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>217</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1293,7 +1319,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>473</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -1311,7 +1337,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>220</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2598,8 +2624,8 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>8467</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>220132</xdr:rowOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>10583</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2627,15 +2653,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>10584</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>10584</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>825499</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>206374</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>10583</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>206373</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2670,8 +2696,8 @@
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>531815</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>39688</xdr:rowOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>52916</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2687,7 +2713,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7323670" y="5564188"/>
-          <a:ext cx="5453062" cy="4508500"/>
+          <a:ext cx="5453062" cy="6670145"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3022,8 +3048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4213BD91-B5D1-3B47-8D3F-04331482504C}">
   <dimension ref="A1:Q60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3036,588 +3062,588 @@
     <col min="11" max="11" width="0.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="31"/>
-    </row>
-    <row r="2" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="32"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="34"/>
-    </row>
-    <row r="3" spans="1:11" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35"/>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="37"/>
-    </row>
-    <row r="4" spans="1:11" ht="5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:11" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="11" t="s">
+    <row r="1" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="29"/>
+    </row>
+    <row r="2" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="30"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="32"/>
+    </row>
+    <row r="3" spans="1:17" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="33"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="35"/>
+    </row>
+    <row r="4" spans="1:17" ht="5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:17" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="38" t="s">
+      <c r="H5" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="39"/>
-      <c r="J5" s="40"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B6" s="20">
+      <c r="I5" s="37"/>
+      <c r="J5" s="38"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B6" s="18">
         <v>45138</v>
       </c>
-      <c r="C6" s="1">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0</v>
-      </c>
-      <c r="E6" s="6">
+      <c r="C6" s="53">
+        <v>0</v>
+      </c>
+      <c r="D6" s="54">
+        <v>0</v>
+      </c>
+      <c r="E6" s="55">
         <f>D6/$J$6</f>
         <v>0</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="56">
         <f>D6/$J$8</f>
         <v>0</v>
       </c>
-      <c r="H6" s="41" t="s">
+      <c r="H6" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="42"/>
-      <c r="J6" s="14">
+      <c r="I6" s="40"/>
+      <c r="J6" s="12">
         <v>340</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B7" s="3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B7" s="2">
         <v>45139</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="57">
         <v>156</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="51">
         <v>156</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="52">
         <f t="shared" ref="E7:E37" si="0">D7/$J$6</f>
         <v>0.45882352941176469</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="5">
         <f t="shared" ref="F7:F37" si="1">D7/$J$8</f>
         <v>9.1764705882352946E-3</v>
       </c>
-      <c r="H7" s="43" t="s">
+      <c r="H7" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="44"/>
-      <c r="J7" s="14">
+      <c r="I7" s="42"/>
+      <c r="J7" s="12">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="3">
+    <row r="8" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
         <v>45140</v>
       </c>
-      <c r="C8" s="1">
-        <f t="shared" ref="C8:C29" si="2">D8-D7</f>
+      <c r="C8" s="57">
+        <f t="shared" ref="C8:C30" si="2">D8-D7</f>
         <v>38</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="51">
         <v>194</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="52">
         <f t="shared" si="0"/>
         <v>0.57058823529411762</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="5">
         <f t="shared" si="1"/>
         <v>1.1411764705882352E-2</v>
       </c>
-      <c r="H8" s="45" t="s">
+      <c r="H8" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="46"/>
-      <c r="J8" s="15">
+      <c r="I8" s="44"/>
+      <c r="J8" s="13">
         <f>J6*J7</f>
         <v>17000</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="3">
+    <row r="9" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="2">
         <v>45141</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="57">
         <f t="shared" si="2"/>
         <v>486</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="51">
         <v>680</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="52">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="5">
         <f t="shared" si="1"/>
         <v>0.04</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B10" s="2">
         <v>45142</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="57">
         <f t="shared" si="2"/>
         <v>346</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="51">
         <v>1026</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="52">
         <f t="shared" si="0"/>
         <v>3.0176470588235293</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="5">
         <f t="shared" si="1"/>
         <v>6.0352941176470588E-2</v>
       </c>
-      <c r="H10" s="47" t="s">
+      <c r="H10" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="48"/>
-      <c r="J10" s="49"/>
-    </row>
-    <row r="11" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="3">
+      <c r="I10" s="46"/>
+      <c r="J10" s="47"/>
+    </row>
+    <row r="11" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="2">
         <v>45145</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="57">
         <f t="shared" si="2"/>
         <v>729</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="51">
         <v>1755</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="52">
         <f t="shared" si="0"/>
         <v>5.1617647058823533</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="5">
         <f t="shared" si="1"/>
         <v>0.10323529411764706</v>
       </c>
-      <c r="H11" s="50"/>
-      <c r="I11" s="51"/>
-      <c r="J11" s="52"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B12" s="3">
+      <c r="H11" s="48"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="50"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B12" s="2">
         <v>45146</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="57">
         <f t="shared" si="2"/>
         <v>859</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="51">
         <v>2614</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="52">
         <f t="shared" si="0"/>
         <v>7.6882352941176473</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="5">
         <f t="shared" si="1"/>
         <v>0.15376470588235294</v>
       </c>
-      <c r="H12" s="23" t="s">
+      <c r="H12" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="I12" s="24"/>
-      <c r="J12" s="16">
+      <c r="I12" s="22"/>
+      <c r="J12" s="14">
         <f>J8-MAX(D6:D37)</f>
-        <v>7464</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B13" s="3">
+        <v>7244</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B13" s="2">
         <v>45147</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="57">
         <f t="shared" si="2"/>
         <v>107</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="51">
         <v>2721</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="52">
         <f t="shared" si="0"/>
         <v>8.0029411764705891</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="5">
         <f t="shared" si="1"/>
         <v>0.16005882352941175</v>
       </c>
-      <c r="H13" s="25" t="s">
+      <c r="H13" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="26"/>
-      <c r="J13" s="16">
+      <c r="I13" s="24"/>
+      <c r="J13" s="14">
         <f>AVERAGE(C9:C25)</f>
         <v>496.35294117647061</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="3">
+    <row r="14" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="2">
         <v>45148</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="57">
         <f t="shared" si="2"/>
         <v>1279</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="51">
         <v>4000</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="52">
         <f t="shared" si="0"/>
         <v>11.764705882352942</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="5">
         <f t="shared" si="1"/>
         <v>0.23529411764705882</v>
       </c>
-      <c r="H14" s="27" t="s">
+      <c r="H14" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="I14" s="28"/>
-      <c r="J14" s="17">
+      <c r="I14" s="26"/>
+      <c r="J14" s="15">
         <f>J12/J13</f>
-        <v>15.037686655605594</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B15" s="3">
+        <v>14.594453662005215</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B15" s="2">
         <v>45149</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="57">
         <f t="shared" si="2"/>
         <v>657</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="51">
         <v>4657</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="52">
         <f t="shared" si="0"/>
         <v>13.697058823529412</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="5">
         <f t="shared" si="1"/>
         <v>0.27394117647058824</v>
       </c>
-      <c r="H15" s="13" t="s">
+      <c r="O15" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I15" s="13">
+      <c r="P15" s="11">
         <v>24.68</v>
       </c>
-      <c r="J15" s="21">
+      <c r="Q15" s="19">
         <v>23.78</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B16" s="3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B16" s="2">
         <v>45152</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="57">
         <f t="shared" si="2"/>
         <v>146</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="51">
         <v>4803</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="52">
         <f t="shared" si="0"/>
         <v>14.126470588235295</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="5">
         <f t="shared" si="1"/>
         <v>0.28252941176470586</v>
       </c>
-      <c r="J16" s="22"/>
+      <c r="J16" s="20"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B17" s="3">
+      <c r="B17" s="2">
         <v>45153</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="57">
         <f t="shared" si="2"/>
         <v>140</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="51">
         <v>4943</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="52">
         <f t="shared" si="0"/>
         <v>14.538235294117648</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="5">
         <f t="shared" si="1"/>
         <v>0.29076470588235293</v>
       </c>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B18" s="3">
+      <c r="B18" s="2">
         <v>45154</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="57">
         <f t="shared" si="2"/>
         <v>467</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="51">
         <v>5410</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="52">
         <f t="shared" si="0"/>
         <v>15.911764705882353</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="5">
         <f t="shared" si="1"/>
         <v>0.31823529411764706</v>
       </c>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B19" s="3">
+      <c r="B19" s="2">
         <v>45155</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="57">
         <f t="shared" si="2"/>
         <v>448</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="51">
         <v>5858</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="52">
         <f t="shared" si="0"/>
         <v>17.229411764705883</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="5">
         <f t="shared" si="1"/>
         <v>0.34458823529411764</v>
       </c>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B20" s="3">
+      <c r="B20" s="2">
         <v>45156</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="57">
         <f t="shared" si="2"/>
         <v>419</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="51">
         <v>6277</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="52">
         <f t="shared" si="0"/>
         <v>18.461764705882352</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="5">
         <f t="shared" si="1"/>
         <v>0.36923529411764705</v>
       </c>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B21" s="3">
+      <c r="B21" s="2">
         <v>45159</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="57">
         <f t="shared" si="2"/>
         <v>661</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="51">
         <v>6938</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="52">
         <f t="shared" si="0"/>
         <v>20.405882352941177</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="5">
         <f t="shared" si="1"/>
         <v>0.40811764705882353</v>
       </c>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B22" s="3">
+      <c r="B22" s="2">
         <v>45160</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="57">
         <f t="shared" si="2"/>
         <v>580</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="51">
         <v>7518</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="52">
         <f t="shared" si="0"/>
         <v>22.111764705882354</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F22" s="5">
         <f t="shared" si="1"/>
         <v>0.44223529411764706</v>
       </c>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B23" s="3">
+      <c r="B23" s="2">
         <v>45161</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="57">
         <f t="shared" si="2"/>
         <v>349</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23" s="51">
         <v>7867</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="52">
         <f t="shared" si="0"/>
         <v>23.138235294117646</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="5">
         <f t="shared" si="1"/>
         <v>0.46276470588235297</v>
       </c>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B24" s="3">
+      <c r="B24" s="2">
         <v>45162</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="57">
         <f t="shared" si="2"/>
         <v>154</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24" s="51">
         <v>8021</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="52">
         <f t="shared" si="0"/>
         <v>23.591176470588234</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F24" s="5">
         <f t="shared" si="1"/>
         <v>0.4718235294117647</v>
       </c>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B25" s="3">
+      <c r="B25" s="2">
         <v>45163</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="57">
         <f t="shared" si="2"/>
         <v>611</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25" s="51">
         <v>8632</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="52">
         <f t="shared" si="0"/>
         <v>25.388235294117646</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="5">
         <f t="shared" si="1"/>
         <v>0.5077647058823529</v>
       </c>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B26" s="3">
+      <c r="B26" s="2">
         <v>45164</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="57">
         <f t="shared" si="2"/>
         <v>95</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26" s="51">
         <v>8727</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="52">
         <f t="shared" si="0"/>
         <v>25.66764705882353</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F26" s="5">
         <f t="shared" si="1"/>
         <v>0.51335294117647057</v>
       </c>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B27" s="3">
+      <c r="B27" s="2">
         <v>45168</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="57">
         <f t="shared" si="2"/>
         <v>119</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27" s="51">
         <v>8846</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="52">
         <f t="shared" si="0"/>
         <v>26.017647058823531</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F27" s="5">
         <f t="shared" si="1"/>
         <v>0.52035294117647057</v>
       </c>
     </row>
     <row r="28" spans="2:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="3">
+      <c r="B28" s="2">
         <v>45173</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="57">
         <f t="shared" si="2"/>
         <v>217</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28" s="51">
         <v>9063</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="52">
         <f t="shared" si="0"/>
         <v>26.655882352941177</v>
       </c>
-      <c r="F28" s="7">
+      <c r="F28" s="5">
         <f t="shared" si="1"/>
         <v>0.53311764705882347</v>
       </c>
@@ -3638,27 +3664,27 @@
       </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B29" s="3">
+      <c r="B29" s="2">
         <v>45174</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29" s="57">
         <f t="shared" si="2"/>
         <v>473</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29" s="51">
         <v>9536</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29" s="52">
         <f t="shared" si="0"/>
         <v>28.047058823529412</v>
       </c>
-      <c r="F29" s="7">
+      <c r="F29" s="5">
         <f t="shared" si="1"/>
         <v>0.56094117647058828</v>
       </c>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="17"/>
       <c r="L29" t="s">
         <v>16</v>
       </c>
@@ -3666,7 +3692,7 @@
         <f t="array" ref="M29:M60">_xlfn.SORTBY(C6:C37, C6:C37, -1)</f>
         <v>1279</v>
       </c>
-      <c r="N29" s="18" cm="1">
+      <c r="N29" s="16" cm="1">
         <f t="array" ref="N29:N60">_xlfn.SORTBY(B6:B37,C6:C37, -1)</f>
         <v>45148</v>
       </c>
@@ -3684,27 +3710,34 @@
       </c>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B30" s="4"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="6">
+      <c r="B30" s="2">
+        <v>45175</v>
+      </c>
+      <c r="C30" s="57">
+        <f t="shared" si="2"/>
+        <v>220</v>
+      </c>
+      <c r="D30" s="51">
+        <v>9756</v>
+      </c>
+      <c r="E30" s="52">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F30" s="7">
+        <v>28.694117647058825</v>
+      </c>
+      <c r="F30" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="19"/>
+        <v>0.57388235294117651</v>
+      </c>
+      <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="17"/>
       <c r="L30" t="s">
         <v>17</v>
       </c>
       <c r="M30">
         <v>859</v>
       </c>
-      <c r="N30" s="18">
+      <c r="N30" s="16">
         <v>45146</v>
       </c>
       <c r="O30" t="str">
@@ -3721,27 +3754,27 @@
       </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B31" s="4"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="6">
+      <c r="B31" s="3"/>
+      <c r="C31" s="57"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="52">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F31" s="7">
+      <c r="F31" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H31" s="19"/>
-      <c r="I31" s="19"/>
-      <c r="J31" s="19"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="17"/>
       <c r="L31" t="s">
         <v>18</v>
       </c>
       <c r="M31">
         <v>729</v>
       </c>
-      <c r="N31" s="18">
+      <c r="N31" s="16">
         <v>45145</v>
       </c>
       <c r="O31" t="str">
@@ -3758,27 +3791,27 @@
       </c>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B32" s="4"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="6">
+      <c r="B32" s="3"/>
+      <c r="C32" s="57"/>
+      <c r="D32" s="51"/>
+      <c r="E32" s="52">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F32" s="7">
+      <c r="F32" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="17"/>
       <c r="L32" t="s">
         <v>19</v>
       </c>
       <c r="M32">
         <v>661</v>
       </c>
-      <c r="N32" s="18">
+      <c r="N32" s="16">
         <v>45159</v>
       </c>
       <c r="O32" t="str">
@@ -3795,27 +3828,27 @@
       </c>
     </row>
     <row r="33" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B33" s="4"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="6">
+      <c r="B33" s="3"/>
+      <c r="C33" s="57"/>
+      <c r="D33" s="51"/>
+      <c r="E33" s="52">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F33" s="7">
+      <c r="F33" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
-      <c r="J33" s="19"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="17"/>
+      <c r="J33" s="17"/>
       <c r="L33" t="s">
         <v>20</v>
       </c>
       <c r="M33">
         <v>657</v>
       </c>
-      <c r="N33" s="18">
+      <c r="N33" s="16">
         <v>45149</v>
       </c>
       <c r="O33" t="str">
@@ -3832,27 +3865,27 @@
       </c>
     </row>
     <row r="34" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B34" s="4"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="6">
+      <c r="B34" s="3"/>
+      <c r="C34" s="57"/>
+      <c r="D34" s="51"/>
+      <c r="E34" s="52">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F34" s="7">
+      <c r="F34" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H34" s="19"/>
-      <c r="I34" s="19"/>
-      <c r="J34" s="19"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="17"/>
+      <c r="J34" s="17"/>
       <c r="L34" t="s">
         <v>25</v>
       </c>
       <c r="M34">
         <v>611</v>
       </c>
-      <c r="N34" s="18">
+      <c r="N34" s="16">
         <v>45163</v>
       </c>
       <c r="O34" t="str">
@@ -3869,27 +3902,27 @@
       </c>
     </row>
     <row r="35" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B35" s="4"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="6">
+      <c r="B35" s="3"/>
+      <c r="C35" s="57"/>
+      <c r="D35" s="51"/>
+      <c r="E35" s="52">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F35" s="7">
+      <c r="F35" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H35" s="19"/>
-      <c r="I35" s="19"/>
-      <c r="J35" s="19"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="17"/>
       <c r="L35" t="s">
         <v>26</v>
       </c>
       <c r="M35">
         <v>580</v>
       </c>
-      <c r="N35" s="18">
+      <c r="N35" s="16">
         <v>45160</v>
       </c>
       <c r="O35" t="str">
@@ -3906,27 +3939,27 @@
       </c>
     </row>
     <row r="36" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B36" s="4"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="6">
+      <c r="B36" s="3"/>
+      <c r="C36" s="57"/>
+      <c r="D36" s="51"/>
+      <c r="E36" s="52">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F36" s="7">
+      <c r="F36" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H36" s="19"/>
-      <c r="I36" s="19"/>
-      <c r="J36" s="19"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="17"/>
+      <c r="J36" s="17"/>
       <c r="L36" t="s">
         <v>27</v>
       </c>
       <c r="M36">
         <v>486</v>
       </c>
-      <c r="N36" s="18">
+      <c r="N36" s="16">
         <v>45141</v>
       </c>
       <c r="O36" t="str">
@@ -3942,51 +3975,62 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="5"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="8">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B37" s="3"/>
+      <c r="C37" s="57"/>
+      <c r="D37" s="51"/>
+      <c r="E37" s="52">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F37" s="9">
+      <c r="F37" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H37" s="19"/>
-      <c r="I37" s="19"/>
-      <c r="J37" s="19"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="17"/>
+      <c r="J37" s="17"/>
       <c r="L37" t="s">
         <v>28</v>
       </c>
       <c r="M37">
         <v>473</v>
       </c>
-      <c r="N37" s="18">
+      <c r="N37" s="16">
         <v>45174</v>
       </c>
       <c r="O37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Green</v>
-      </c>
-      <c r="P37" t="str">
+        <v>Blue</v>
+      </c>
+      <c r="P37">
         <f t="shared" ca="1" si="4"/>
+        <v>473</v>
+      </c>
+      <c r="Q37" t="str">
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
-      <c r="Q37">
-        <f t="shared" ca="1" si="5"/>
-        <v>473</v>
-      </c>
-    </row>
-    <row r="38" spans="2:17" ht="5" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="3"/>
+      <c r="C38" s="57"/>
+      <c r="D38" s="51"/>
+      <c r="E38" s="52">
+        <f t="shared" ref="E38:E44" si="6">D38/$J$6</f>
+        <v>0</v>
+      </c>
+      <c r="F38" s="5">
+        <f t="shared" ref="F38:F44" si="7">D38/$J$8</f>
+        <v>0</v>
+      </c>
       <c r="L38" t="s">
         <v>29</v>
       </c>
       <c r="M38">
         <v>467</v>
       </c>
-      <c r="N38" s="18">
+      <c r="N38" s="16">
         <v>45154</v>
       </c>
       <c r="O38" t="str">
@@ -4003,13 +4047,24 @@
       </c>
     </row>
     <row r="39" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B39" s="3"/>
+      <c r="C39" s="57"/>
+      <c r="D39" s="51"/>
+      <c r="E39" s="52">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F39" s="5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
       <c r="L39" t="s">
         <v>30</v>
       </c>
       <c r="M39">
         <v>448</v>
       </c>
-      <c r="N39" s="18">
+      <c r="N39" s="16">
         <v>45155</v>
       </c>
       <c r="O39" t="str">
@@ -4026,13 +4081,24 @@
       </c>
     </row>
     <row r="40" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B40" s="3"/>
+      <c r="C40" s="57"/>
+      <c r="D40" s="51"/>
+      <c r="E40" s="52">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F40" s="5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
       <c r="L40" t="s">
         <v>31</v>
       </c>
       <c r="M40">
         <v>419</v>
       </c>
-      <c r="N40" s="18">
+      <c r="N40" s="16">
         <v>45156</v>
       </c>
       <c r="O40" t="str">
@@ -4049,13 +4115,24 @@
       </c>
     </row>
     <row r="41" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B41" s="3"/>
+      <c r="C41" s="57"/>
+      <c r="D41" s="51"/>
+      <c r="E41" s="52">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F41" s="5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
       <c r="L41" t="s">
         <v>32</v>
       </c>
       <c r="M41">
         <v>349</v>
       </c>
-      <c r="N41" s="18">
+      <c r="N41" s="16">
         <v>45161</v>
       </c>
       <c r="O41" t="str">
@@ -4072,13 +4149,24 @@
       </c>
     </row>
     <row r="42" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B42" s="3"/>
+      <c r="C42" s="57"/>
+      <c r="D42" s="51"/>
+      <c r="E42" s="52">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F42" s="5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
       <c r="L42" t="s">
         <v>33</v>
       </c>
       <c r="M42">
         <v>346</v>
       </c>
-      <c r="N42" s="18">
+      <c r="N42" s="16">
         <v>45142</v>
       </c>
       <c r="O42" t="str">
@@ -4095,98 +4183,120 @@
       </c>
     </row>
     <row r="43" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B43" s="3"/>
+      <c r="C43" s="57"/>
+      <c r="D43" s="51"/>
+      <c r="E43" s="52">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F43" s="5">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
       <c r="L43" t="s">
         <v>34</v>
       </c>
       <c r="M43">
-        <v>217</v>
-      </c>
-      <c r="N43" s="18">
-        <v>45173</v>
+        <v>220</v>
+      </c>
+      <c r="N43" s="16">
+        <v>45175</v>
       </c>
       <c r="O43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Blue</v>
-      </c>
-      <c r="P43">
+        <v>Green</v>
+      </c>
+      <c r="P43" t="str">
         <f t="shared" ca="1" si="4"/>
+        <v/>
+      </c>
+      <c r="Q43">
+        <f t="shared" ca="1" si="5"/>
+        <v>220</v>
+      </c>
+    </row>
+    <row r="44" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="4"/>
+      <c r="C44" s="58"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F44" s="7">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M44">
         <v>217</v>
       </c>
-      <c r="Q43" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="44" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="M44">
-        <v>156</v>
-      </c>
-      <c r="N44" s="18">
-        <v>45139</v>
+      <c r="N44" s="16">
+        <v>45173</v>
       </c>
     </row>
     <row r="45" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M45">
-        <v>154</v>
-      </c>
-      <c r="N45" s="18">
-        <v>45162</v>
+        <v>156</v>
+      </c>
+      <c r="N45" s="16">
+        <v>45139</v>
       </c>
     </row>
     <row r="46" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M46">
-        <v>146</v>
-      </c>
-      <c r="N46" s="18">
-        <v>45152</v>
+        <v>154</v>
+      </c>
+      <c r="N46" s="16">
+        <v>45162</v>
       </c>
     </row>
     <row r="47" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M47">
-        <v>140</v>
-      </c>
-      <c r="N47" s="18">
-        <v>45153</v>
+        <v>146</v>
+      </c>
+      <c r="N47" s="16">
+        <v>45152</v>
       </c>
     </row>
     <row r="48" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M48">
-        <v>119</v>
-      </c>
-      <c r="N48" s="18">
-        <v>45168</v>
+        <v>140</v>
+      </c>
+      <c r="N48" s="16">
+        <v>45153</v>
       </c>
     </row>
     <row r="49" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M49">
-        <v>107</v>
-      </c>
-      <c r="N49" s="18">
-        <v>45147</v>
+        <v>119</v>
+      </c>
+      <c r="N49" s="16">
+        <v>45168</v>
       </c>
     </row>
     <row r="50" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M50">
-        <v>95</v>
-      </c>
-      <c r="N50" s="18">
-        <v>45164</v>
+        <v>107</v>
+      </c>
+      <c r="N50" s="16">
+        <v>45147</v>
       </c>
     </row>
     <row r="51" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M51">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="N51">
-        <v>45140</v>
+        <v>45164</v>
       </c>
     </row>
     <row r="52" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M52">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="N52">
-        <v>45138</v>
+        <v>45140</v>
       </c>
     </row>
     <row r="53" spans="13:14" x14ac:dyDescent="0.2">
@@ -4194,7 +4304,7 @@
         <v>0</v>
       </c>
       <c r="N53">
-        <v>0</v>
+        <v>45138</v>
       </c>
     </row>
     <row r="54" spans="13:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Models trained + plots + 300 words
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA47A567-A2DB-DB49-8B07-BCCB57310578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237EA479-91E9-4F4F-BEE1-394C64B35F73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14420" windowHeight="17900" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -472,6 +472,14 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -562,14 +570,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -675,10 +675,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$6:$B$30</c:f>
+              <c:f>Sheet1!$B$6:$B$44</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="39"/>
                 <c:pt idx="0">
                   <c:v>45138</c:v>
                 </c:pt>
@@ -753,16 +753,19 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>45175</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>45181</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$6:$D$30</c:f>
+              <c:f>Sheet1!$D$6:$D$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="39"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -837,6 +840,9 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>9756</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>10056</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1337,7 +1343,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>220</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3048,8 +3054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4213BD91-B5D1-3B47-8D3F-04331482504C}">
   <dimension ref="A1:Q60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3063,45 +3069,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="29"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="37"/>
     </row>
     <row r="2" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="30"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="32"/>
+      <c r="A2" s="38"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="40"/>
     </row>
     <row r="3" spans="1:17" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="34"/>
-      <c r="K3" s="35"/>
+      <c r="A3" s="41"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="43"/>
     </row>
     <row r="4" spans="1:17" ht="5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:17" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3120,34 +3126,34 @@
       <c r="F5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="36" t="s">
+      <c r="H5" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="37"/>
-      <c r="J5" s="38"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="46"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B6" s="18">
         <v>45138</v>
       </c>
-      <c r="C6" s="53">
+      <c r="C6" s="23">
         <v>0</v>
       </c>
-      <c r="D6" s="54">
+      <c r="D6" s="24">
         <v>0</v>
       </c>
-      <c r="E6" s="55">
+      <c r="E6" s="25">
         <f>D6/$J$6</f>
         <v>0</v>
       </c>
-      <c r="F6" s="56">
+      <c r="F6" s="26">
         <f>D6/$J$8</f>
         <v>0</v>
       </c>
-      <c r="H6" s="39" t="s">
+      <c r="H6" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="40"/>
+      <c r="I6" s="48"/>
       <c r="J6" s="12">
         <v>340</v>
       </c>
@@ -3156,13 +3162,13 @@
       <c r="B7" s="2">
         <v>45139</v>
       </c>
-      <c r="C7" s="57">
+      <c r="C7" s="27">
         <v>156</v>
       </c>
-      <c r="D7" s="51">
+      <c r="D7" s="21">
         <v>156</v>
       </c>
-      <c r="E7" s="52">
+      <c r="E7" s="22">
         <f t="shared" ref="E7:E37" si="0">D7/$J$6</f>
         <v>0.45882352941176469</v>
       </c>
@@ -3170,10 +3176,10 @@
         <f t="shared" ref="F7:F37" si="1">D7/$J$8</f>
         <v>9.1764705882352946E-3</v>
       </c>
-      <c r="H7" s="41" t="s">
+      <c r="H7" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="42"/>
+      <c r="I7" s="50"/>
       <c r="J7" s="12">
         <v>50</v>
       </c>
@@ -3182,14 +3188,14 @@
       <c r="B8" s="2">
         <v>45140</v>
       </c>
-      <c r="C8" s="57">
-        <f t="shared" ref="C8:C30" si="2">D8-D7</f>
+      <c r="C8" s="27">
+        <f t="shared" ref="C8:C31" si="2">D8-D7</f>
         <v>38</v>
       </c>
-      <c r="D8" s="51">
+      <c r="D8" s="21">
         <v>194</v>
       </c>
-      <c r="E8" s="52">
+      <c r="E8" s="22">
         <f t="shared" si="0"/>
         <v>0.57058823529411762</v>
       </c>
@@ -3197,10 +3203,10 @@
         <f t="shared" si="1"/>
         <v>1.1411764705882352E-2</v>
       </c>
-      <c r="H8" s="43" t="s">
+      <c r="H8" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="44"/>
+      <c r="I8" s="52"/>
       <c r="J8" s="13">
         <f>J6*J7</f>
         <v>17000</v>
@@ -3210,14 +3216,14 @@
       <c r="B9" s="2">
         <v>45141</v>
       </c>
-      <c r="C9" s="57">
+      <c r="C9" s="27">
         <f t="shared" si="2"/>
         <v>486</v>
       </c>
-      <c r="D9" s="51">
+      <c r="D9" s="21">
         <v>680</v>
       </c>
-      <c r="E9" s="52">
+      <c r="E9" s="22">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -3230,14 +3236,14 @@
       <c r="B10" s="2">
         <v>45142</v>
       </c>
-      <c r="C10" s="57">
+      <c r="C10" s="27">
         <f t="shared" si="2"/>
         <v>346</v>
       </c>
-      <c r="D10" s="51">
+      <c r="D10" s="21">
         <v>1026</v>
       </c>
-      <c r="E10" s="52">
+      <c r="E10" s="22">
         <f t="shared" si="0"/>
         <v>3.0176470588235293</v>
       </c>
@@ -3245,24 +3251,24 @@
         <f t="shared" si="1"/>
         <v>6.0352941176470588E-2</v>
       </c>
-      <c r="H10" s="45" t="s">
+      <c r="H10" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="46"/>
-      <c r="J10" s="47"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="55"/>
     </row>
     <row r="11" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>45145</v>
       </c>
-      <c r="C11" s="57">
+      <c r="C11" s="27">
         <f t="shared" si="2"/>
         <v>729</v>
       </c>
-      <c r="D11" s="51">
+      <c r="D11" s="21">
         <v>1755</v>
       </c>
-      <c r="E11" s="52">
+      <c r="E11" s="22">
         <f t="shared" si="0"/>
         <v>5.1617647058823533</v>
       </c>
@@ -3270,22 +3276,22 @@
         <f t="shared" si="1"/>
         <v>0.10323529411764706</v>
       </c>
-      <c r="H11" s="48"/>
-      <c r="I11" s="49"/>
-      <c r="J11" s="50"/>
+      <c r="H11" s="56"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="58"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B12" s="2">
         <v>45146</v>
       </c>
-      <c r="C12" s="57">
+      <c r="C12" s="27">
         <f t="shared" si="2"/>
         <v>859</v>
       </c>
-      <c r="D12" s="51">
+      <c r="D12" s="21">
         <v>2614</v>
       </c>
-      <c r="E12" s="52">
+      <c r="E12" s="22">
         <f t="shared" si="0"/>
         <v>7.6882352941176473</v>
       </c>
@@ -3293,27 +3299,27 @@
         <f t="shared" si="1"/>
         <v>0.15376470588235294</v>
       </c>
-      <c r="H12" s="21" t="s">
+      <c r="H12" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="I12" s="22"/>
+      <c r="I12" s="30"/>
       <c r="J12" s="14">
         <f>J8-MAX(D6:D37)</f>
-        <v>7244</v>
+        <v>6944</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B13" s="2">
         <v>45147</v>
       </c>
-      <c r="C13" s="57">
+      <c r="C13" s="27">
         <f t="shared" si="2"/>
         <v>107</v>
       </c>
-      <c r="D13" s="51">
+      <c r="D13" s="21">
         <v>2721</v>
       </c>
-      <c r="E13" s="52">
+      <c r="E13" s="22">
         <f t="shared" si="0"/>
         <v>8.0029411764705891</v>
       </c>
@@ -3321,10 +3327,10 @@
         <f t="shared" si="1"/>
         <v>0.16005882352941175</v>
       </c>
-      <c r="H13" s="23" t="s">
+      <c r="H13" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="24"/>
+      <c r="I13" s="32"/>
       <c r="J13" s="14">
         <f>AVERAGE(C9:C25)</f>
         <v>496.35294117647061</v>
@@ -3334,14 +3340,14 @@
       <c r="B14" s="2">
         <v>45148</v>
       </c>
-      <c r="C14" s="57">
+      <c r="C14" s="27">
         <f t="shared" si="2"/>
         <v>1279</v>
       </c>
-      <c r="D14" s="51">
+      <c r="D14" s="21">
         <v>4000</v>
       </c>
-      <c r="E14" s="52">
+      <c r="E14" s="22">
         <f t="shared" si="0"/>
         <v>11.764705882352942</v>
       </c>
@@ -3349,27 +3355,27 @@
         <f t="shared" si="1"/>
         <v>0.23529411764705882</v>
       </c>
-      <c r="H14" s="25" t="s">
+      <c r="H14" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="I14" s="26"/>
+      <c r="I14" s="34"/>
       <c r="J14" s="15">
         <f>J12/J13</f>
-        <v>14.594453662005215</v>
+        <v>13.990045034368332</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B15" s="2">
         <v>45149</v>
       </c>
-      <c r="C15" s="57">
+      <c r="C15" s="27">
         <f t="shared" si="2"/>
         <v>657</v>
       </c>
-      <c r="D15" s="51">
+      <c r="D15" s="21">
         <v>4657</v>
       </c>
-      <c r="E15" s="52">
+      <c r="E15" s="22">
         <f t="shared" si="0"/>
         <v>13.697058823529412</v>
       </c>
@@ -3391,14 +3397,14 @@
       <c r="B16" s="2">
         <v>45152</v>
       </c>
-      <c r="C16" s="57">
+      <c r="C16" s="27">
         <f t="shared" si="2"/>
         <v>146</v>
       </c>
-      <c r="D16" s="51">
+      <c r="D16" s="21">
         <v>4803</v>
       </c>
-      <c r="E16" s="52">
+      <c r="E16" s="22">
         <f t="shared" si="0"/>
         <v>14.126470588235295</v>
       </c>
@@ -3412,14 +3418,14 @@
       <c r="B17" s="2">
         <v>45153</v>
       </c>
-      <c r="C17" s="57">
+      <c r="C17" s="27">
         <f t="shared" si="2"/>
         <v>140</v>
       </c>
-      <c r="D17" s="51">
+      <c r="D17" s="21">
         <v>4943</v>
       </c>
-      <c r="E17" s="52">
+      <c r="E17" s="22">
         <f t="shared" si="0"/>
         <v>14.538235294117648</v>
       </c>
@@ -3432,14 +3438,14 @@
       <c r="B18" s="2">
         <v>45154</v>
       </c>
-      <c r="C18" s="57">
+      <c r="C18" s="27">
         <f t="shared" si="2"/>
         <v>467</v>
       </c>
-      <c r="D18" s="51">
+      <c r="D18" s="21">
         <v>5410</v>
       </c>
-      <c r="E18" s="52">
+      <c r="E18" s="22">
         <f t="shared" si="0"/>
         <v>15.911764705882353</v>
       </c>
@@ -3452,14 +3458,14 @@
       <c r="B19" s="2">
         <v>45155</v>
       </c>
-      <c r="C19" s="57">
+      <c r="C19" s="27">
         <f t="shared" si="2"/>
         <v>448</v>
       </c>
-      <c r="D19" s="51">
+      <c r="D19" s="21">
         <v>5858</v>
       </c>
-      <c r="E19" s="52">
+      <c r="E19" s="22">
         <f t="shared" si="0"/>
         <v>17.229411764705883</v>
       </c>
@@ -3472,14 +3478,14 @@
       <c r="B20" s="2">
         <v>45156</v>
       </c>
-      <c r="C20" s="57">
+      <c r="C20" s="27">
         <f t="shared" si="2"/>
         <v>419</v>
       </c>
-      <c r="D20" s="51">
+      <c r="D20" s="21">
         <v>6277</v>
       </c>
-      <c r="E20" s="52">
+      <c r="E20" s="22">
         <f t="shared" si="0"/>
         <v>18.461764705882352</v>
       </c>
@@ -3492,14 +3498,14 @@
       <c r="B21" s="2">
         <v>45159</v>
       </c>
-      <c r="C21" s="57">
+      <c r="C21" s="27">
         <f t="shared" si="2"/>
         <v>661</v>
       </c>
-      <c r="D21" s="51">
+      <c r="D21" s="21">
         <v>6938</v>
       </c>
-      <c r="E21" s="52">
+      <c r="E21" s="22">
         <f t="shared" si="0"/>
         <v>20.405882352941177</v>
       </c>
@@ -3512,14 +3518,14 @@
       <c r="B22" s="2">
         <v>45160</v>
       </c>
-      <c r="C22" s="57">
+      <c r="C22" s="27">
         <f t="shared" si="2"/>
         <v>580</v>
       </c>
-      <c r="D22" s="51">
+      <c r="D22" s="21">
         <v>7518</v>
       </c>
-      <c r="E22" s="52">
+      <c r="E22" s="22">
         <f t="shared" si="0"/>
         <v>22.111764705882354</v>
       </c>
@@ -3532,14 +3538,14 @@
       <c r="B23" s="2">
         <v>45161</v>
       </c>
-      <c r="C23" s="57">
+      <c r="C23" s="27">
         <f t="shared" si="2"/>
         <v>349</v>
       </c>
-      <c r="D23" s="51">
+      <c r="D23" s="21">
         <v>7867</v>
       </c>
-      <c r="E23" s="52">
+      <c r="E23" s="22">
         <f t="shared" si="0"/>
         <v>23.138235294117646</v>
       </c>
@@ -3552,14 +3558,14 @@
       <c r="B24" s="2">
         <v>45162</v>
       </c>
-      <c r="C24" s="57">
+      <c r="C24" s="27">
         <f t="shared" si="2"/>
         <v>154</v>
       </c>
-      <c r="D24" s="51">
+      <c r="D24" s="21">
         <v>8021</v>
       </c>
-      <c r="E24" s="52">
+      <c r="E24" s="22">
         <f t="shared" si="0"/>
         <v>23.591176470588234</v>
       </c>
@@ -3572,14 +3578,14 @@
       <c r="B25" s="2">
         <v>45163</v>
       </c>
-      <c r="C25" s="57">
+      <c r="C25" s="27">
         <f t="shared" si="2"/>
         <v>611</v>
       </c>
-      <c r="D25" s="51">
+      <c r="D25" s="21">
         <v>8632</v>
       </c>
-      <c r="E25" s="52">
+      <c r="E25" s="22">
         <f t="shared" si="0"/>
         <v>25.388235294117646</v>
       </c>
@@ -3592,14 +3598,14 @@
       <c r="B26" s="2">
         <v>45164</v>
       </c>
-      <c r="C26" s="57">
+      <c r="C26" s="27">
         <f t="shared" si="2"/>
         <v>95</v>
       </c>
-      <c r="D26" s="51">
+      <c r="D26" s="21">
         <v>8727</v>
       </c>
-      <c r="E26" s="52">
+      <c r="E26" s="22">
         <f t="shared" si="0"/>
         <v>25.66764705882353</v>
       </c>
@@ -3612,14 +3618,14 @@
       <c r="B27" s="2">
         <v>45168</v>
       </c>
-      <c r="C27" s="57">
+      <c r="C27" s="27">
         <f t="shared" si="2"/>
         <v>119</v>
       </c>
-      <c r="D27" s="51">
+      <c r="D27" s="21">
         <v>8846</v>
       </c>
-      <c r="E27" s="52">
+      <c r="E27" s="22">
         <f t="shared" si="0"/>
         <v>26.017647058823531</v>
       </c>
@@ -3632,14 +3638,14 @@
       <c r="B28" s="2">
         <v>45173</v>
       </c>
-      <c r="C28" s="57">
+      <c r="C28" s="27">
         <f t="shared" si="2"/>
         <v>217</v>
       </c>
-      <c r="D28" s="51">
+      <c r="D28" s="21">
         <v>9063</v>
       </c>
-      <c r="E28" s="52">
+      <c r="E28" s="22">
         <f t="shared" si="0"/>
         <v>26.655882352941177</v>
       </c>
@@ -3667,14 +3673,14 @@
       <c r="B29" s="2">
         <v>45174</v>
       </c>
-      <c r="C29" s="57">
+      <c r="C29" s="27">
         <f t="shared" si="2"/>
         <v>473</v>
       </c>
-      <c r="D29" s="51">
+      <c r="D29" s="21">
         <v>9536</v>
       </c>
-      <c r="E29" s="52">
+      <c r="E29" s="22">
         <f t="shared" si="0"/>
         <v>28.047058823529412</v>
       </c>
@@ -3713,14 +3719,14 @@
       <c r="B30" s="2">
         <v>45175</v>
       </c>
-      <c r="C30" s="57">
+      <c r="C30" s="27">
         <f t="shared" si="2"/>
         <v>220</v>
       </c>
-      <c r="D30" s="51">
+      <c r="D30" s="21">
         <v>9756</v>
       </c>
-      <c r="E30" s="52">
+      <c r="E30" s="22">
         <f t="shared" si="0"/>
         <v>28.694117647058825</v>
       </c>
@@ -3754,16 +3760,23 @@
       </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B31" s="3"/>
-      <c r="C31" s="57"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="52">
+      <c r="B31" s="2">
+        <v>45181</v>
+      </c>
+      <c r="C31" s="27">
+        <f t="shared" si="2"/>
+        <v>300</v>
+      </c>
+      <c r="D31" s="21">
+        <v>10056</v>
+      </c>
+      <c r="E31" s="22">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>29.576470588235296</v>
       </c>
       <c r="F31" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.59152941176470586</v>
       </c>
       <c r="H31" s="17"/>
       <c r="I31" s="17"/>
@@ -3792,9 +3805,9 @@
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B32" s="3"/>
-      <c r="C32" s="57"/>
-      <c r="D32" s="51"/>
-      <c r="E32" s="52">
+      <c r="C32" s="27"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3829,9 +3842,9 @@
     </row>
     <row r="33" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B33" s="3"/>
-      <c r="C33" s="57"/>
-      <c r="D33" s="51"/>
-      <c r="E33" s="52">
+      <c r="C33" s="27"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3866,9 +3879,9 @@
     </row>
     <row r="34" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B34" s="3"/>
-      <c r="C34" s="57"/>
-      <c r="D34" s="51"/>
-      <c r="E34" s="52">
+      <c r="C34" s="27"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3903,9 +3916,9 @@
     </row>
     <row r="35" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B35" s="3"/>
-      <c r="C35" s="57"/>
-      <c r="D35" s="51"/>
-      <c r="E35" s="52">
+      <c r="C35" s="27"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3940,9 +3953,9 @@
     </row>
     <row r="36" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B36" s="3"/>
-      <c r="C36" s="57"/>
-      <c r="D36" s="51"/>
-      <c r="E36" s="52">
+      <c r="C36" s="27"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3977,9 +3990,9 @@
     </row>
     <row r="37" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B37" s="3"/>
-      <c r="C37" s="57"/>
-      <c r="D37" s="51"/>
-      <c r="E37" s="52">
+      <c r="C37" s="27"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4014,9 +4027,9 @@
     </row>
     <row r="38" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="3"/>
-      <c r="C38" s="57"/>
-      <c r="D38" s="51"/>
-      <c r="E38" s="52">
+      <c r="C38" s="27"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="22">
         <f t="shared" ref="E38:E44" si="6">D38/$J$6</f>
         <v>0</v>
       </c>
@@ -4048,9 +4061,9 @@
     </row>
     <row r="39" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B39" s="3"/>
-      <c r="C39" s="57"/>
-      <c r="D39" s="51"/>
-      <c r="E39" s="52">
+      <c r="C39" s="27"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="22">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -4082,9 +4095,9 @@
     </row>
     <row r="40" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B40" s="3"/>
-      <c r="C40" s="57"/>
-      <c r="D40" s="51"/>
-      <c r="E40" s="52">
+      <c r="C40" s="27"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="22">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -4116,9 +4129,9 @@
     </row>
     <row r="41" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B41" s="3"/>
-      <c r="C41" s="57"/>
-      <c r="D41" s="51"/>
-      <c r="E41" s="52">
+      <c r="C41" s="27"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="22">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -4150,9 +4163,9 @@
     </row>
     <row r="42" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B42" s="3"/>
-      <c r="C42" s="57"/>
-      <c r="D42" s="51"/>
-      <c r="E42" s="52">
+      <c r="C42" s="27"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="22">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -4184,9 +4197,9 @@
     </row>
     <row r="43" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B43" s="3"/>
-      <c r="C43" s="57"/>
-      <c r="D43" s="51"/>
-      <c r="E43" s="52">
+      <c r="C43" s="27"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="22">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -4198,10 +4211,10 @@
         <v>34</v>
       </c>
       <c r="M43">
-        <v>220</v>
+        <v>300</v>
       </c>
       <c r="N43" s="16">
-        <v>45175</v>
+        <v>45181</v>
       </c>
       <c r="O43" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4213,12 +4226,12 @@
       </c>
       <c r="Q43">
         <f t="shared" ca="1" si="5"/>
-        <v>220</v>
+        <v>300</v>
       </c>
     </row>
     <row r="44" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B44" s="4"/>
-      <c r="C44" s="58"/>
+      <c r="C44" s="28"/>
       <c r="D44" s="1"/>
       <c r="E44" s="6">
         <f t="shared" si="6"/>
@@ -4229,82 +4242,82 @@
         <v>0</v>
       </c>
       <c r="M44">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="N44" s="16">
-        <v>45173</v>
+        <v>45175</v>
       </c>
     </row>
     <row r="45" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M45">
-        <v>156</v>
+        <v>217</v>
       </c>
       <c r="N45" s="16">
-        <v>45139</v>
+        <v>45173</v>
       </c>
     </row>
     <row r="46" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M46">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="N46" s="16">
-        <v>45162</v>
+        <v>45139</v>
       </c>
     </row>
     <row r="47" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M47">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="N47" s="16">
-        <v>45152</v>
+        <v>45162</v>
       </c>
     </row>
     <row r="48" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M48">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="N48" s="16">
-        <v>45153</v>
+        <v>45152</v>
       </c>
     </row>
     <row r="49" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M49">
-        <v>119</v>
+        <v>140</v>
       </c>
       <c r="N49" s="16">
-        <v>45168</v>
+        <v>45153</v>
       </c>
     </row>
     <row r="50" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M50">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="N50" s="16">
-        <v>45147</v>
+        <v>45168</v>
       </c>
     </row>
     <row r="51" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M51">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="N51">
-        <v>45164</v>
+        <v>45147</v>
       </c>
     </row>
     <row r="52" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M52">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="N52">
-        <v>45140</v>
+        <v>45164</v>
       </c>
     </row>
     <row r="53" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M53">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="N53">
-        <v>45138</v>
+        <v>45140</v>
       </c>
     </row>
     <row r="54" spans="13:14" x14ac:dyDescent="0.2">
@@ -4312,7 +4325,7 @@
         <v>0</v>
       </c>
       <c r="N54">
-        <v>0</v>
+        <v>45138</v>
       </c>
     </row>
     <row r="55" spans="13:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Writing about the models and looking at data
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237EA479-91E9-4F4F-BEE1-394C64B35F73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8DD93D-0FA6-A14E-8E6B-1009187653FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14420" windowHeight="17900" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
@@ -757,6 +757,9 @@
                 <c:pt idx="25">
                   <c:v>45181</c:v>
                 </c:pt>
+                <c:pt idx="26">
+                  <c:v>45182</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -843,6 +846,9 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>10056</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>10215</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1217,7 +1223,7 @@
                   <c:v>346</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1343,7 +1349,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>300</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3055,7 +3061,7 @@
   <dimension ref="A1:Q60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3189,7 +3195,7 @@
         <v>45140</v>
       </c>
       <c r="C8" s="27">
-        <f t="shared" ref="C8:C31" si="2">D8-D7</f>
+        <f t="shared" ref="C8:C32" si="2">D8-D7</f>
         <v>38</v>
       </c>
       <c r="D8" s="21">
@@ -3305,7 +3311,7 @@
       <c r="I12" s="30"/>
       <c r="J12" s="14">
         <f>J8-MAX(D6:D37)</f>
-        <v>6944</v>
+        <v>6785</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
@@ -3361,7 +3367,7 @@
       <c r="I14" s="34"/>
       <c r="J14" s="15">
         <f>J12/J13</f>
-        <v>13.990045034368332</v>
+        <v>13.669708461720786</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
@@ -3804,16 +3810,23 @@
       </c>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B32" s="3"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="21"/>
+      <c r="B32" s="2">
+        <v>45182</v>
+      </c>
+      <c r="C32" s="27">
+        <f t="shared" si="2"/>
+        <v>159</v>
+      </c>
+      <c r="D32" s="21">
+        <v>10215</v>
+      </c>
       <c r="E32" s="22">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>30.044117647058822</v>
       </c>
       <c r="F32" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.60088235294117642</v>
       </c>
       <c r="H32" s="17"/>
       <c r="I32" s="17"/>
@@ -4218,15 +4231,15 @@
       </c>
       <c r="O43" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Green</v>
-      </c>
-      <c r="P43" t="str">
+        <v>Blue</v>
+      </c>
+      <c r="P43">
         <f t="shared" ca="1" si="4"/>
+        <v>300</v>
+      </c>
+      <c r="Q43" t="str">
+        <f t="shared" ca="1" si="5"/>
         <v/>
-      </c>
-      <c r="Q43">
-        <f t="shared" ca="1" si="5"/>
-        <v>300</v>
       </c>
     </row>
     <row r="44" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4258,74 +4271,74 @@
     </row>
     <row r="46" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M46">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="N46" s="16">
-        <v>45139</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="47" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M47">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="N47" s="16">
-        <v>45162</v>
+        <v>45139</v>
       </c>
     </row>
     <row r="48" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M48">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="N48" s="16">
-        <v>45152</v>
+        <v>45162</v>
       </c>
     </row>
     <row r="49" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M49">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="N49" s="16">
-        <v>45153</v>
+        <v>45152</v>
       </c>
     </row>
     <row r="50" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M50">
-        <v>119</v>
+        <v>140</v>
       </c>
       <c r="N50" s="16">
-        <v>45168</v>
+        <v>45153</v>
       </c>
     </row>
     <row r="51" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M51">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="N51">
-        <v>45147</v>
+        <v>45168</v>
       </c>
     </row>
     <row r="52" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M52">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="N52">
-        <v>45164</v>
+        <v>45147</v>
       </c>
     </row>
     <row r="53" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M53">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="N53">
-        <v>45140</v>
+        <v>45164</v>
       </c>
     </row>
     <row r="54" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M54">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="N54">
-        <v>45138</v>
+        <v>45140</v>
       </c>
     </row>
     <row r="55" spans="13:14" x14ac:dyDescent="0.2">
@@ -4333,7 +4346,7 @@
         <v>0</v>
       </c>
       <c r="N55">
-        <v>0</v>
+        <v>45138</v>
       </c>
     </row>
     <row r="56" spans="13:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Lots of good plots and 1.5 pages written!
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD64258-0B1F-6541-950F-C77367671ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F71CFB-B44F-9345-BBA4-84A67CA292D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14420" windowHeight="17500" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
@@ -769,6 +769,9 @@
                 <c:pt idx="29">
                   <c:v>45188</c:v>
                 </c:pt>
+                <c:pt idx="30">
+                  <c:v>45191</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -867,6 +870,9 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>10709</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>11224</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1220,28 +1226,28 @@
                   <c:v>580</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>515</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>486</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>473</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>467</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>448</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>419</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>349</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>346</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3078,8 +3084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4213BD91-B5D1-3B47-8D3F-04331482504C}">
   <dimension ref="A1:Q60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3213,7 +3219,7 @@
         <v>45140</v>
       </c>
       <c r="C8" s="27">
-        <f t="shared" ref="C8:C35" si="2">D8-D7</f>
+        <f t="shared" ref="C8:C36" si="2">D8-D7</f>
         <v>38</v>
       </c>
       <c r="D8" s="21">
@@ -3329,7 +3335,7 @@
       <c r="I12" s="30"/>
       <c r="J12" s="14">
         <f>J8-MAX(D6:D37)</f>
-        <v>6291</v>
+        <v>5776</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
@@ -3385,7 +3391,7 @@
       <c r="I14" s="34"/>
       <c r="J14" s="15">
         <f>J12/J13</f>
-        <v>12.674448921545389</v>
+        <v>11.63688077743541</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
@@ -4004,16 +4010,23 @@
       </c>
     </row>
     <row r="36" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B36" s="3"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="21"/>
+      <c r="B36" s="2">
+        <v>45191</v>
+      </c>
+      <c r="C36" s="27">
+        <f t="shared" si="2"/>
+        <v>515</v>
+      </c>
+      <c r="D36" s="21">
+        <v>11224</v>
+      </c>
       <c r="E36" s="22">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>33.011764705882356</v>
       </c>
       <c r="F36" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.66023529411764703</v>
       </c>
       <c r="H36" s="17"/>
       <c r="I36" s="17"/>
@@ -4022,10 +4035,10 @@
         <v>27</v>
       </c>
       <c r="M36">
-        <v>486</v>
+        <v>515</v>
       </c>
       <c r="N36" s="16">
-        <v>45141</v>
+        <v>45191</v>
       </c>
       <c r="O36" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4033,7 +4046,7 @@
       </c>
       <c r="P36">
         <f t="shared" ca="1" si="4"/>
-        <v>486</v>
+        <v>515</v>
       </c>
       <c r="Q36" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -4059,10 +4072,10 @@
         <v>28</v>
       </c>
       <c r="M37">
-        <v>473</v>
+        <v>486</v>
       </c>
       <c r="N37" s="16">
-        <v>45174</v>
+        <v>45141</v>
       </c>
       <c r="O37" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4070,7 +4083,7 @@
       </c>
       <c r="P37">
         <f t="shared" ca="1" si="4"/>
-        <v>473</v>
+        <v>486</v>
       </c>
       <c r="Q37" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -4093,10 +4106,10 @@
         <v>29</v>
       </c>
       <c r="M38">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="N38" s="16">
-        <v>45154</v>
+        <v>45174</v>
       </c>
       <c r="O38" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4104,7 +4117,7 @@
       </c>
       <c r="P38">
         <f t="shared" ca="1" si="4"/>
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="Q38" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -4127,10 +4140,10 @@
         <v>30</v>
       </c>
       <c r="M39">
-        <v>448</v>
+        <v>467</v>
       </c>
       <c r="N39" s="16">
-        <v>45155</v>
+        <v>45154</v>
       </c>
       <c r="O39" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4138,7 +4151,7 @@
       </c>
       <c r="P39">
         <f t="shared" ca="1" si="4"/>
-        <v>448</v>
+        <v>467</v>
       </c>
       <c r="Q39" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -4161,10 +4174,10 @@
         <v>31</v>
       </c>
       <c r="M40">
-        <v>419</v>
+        <v>448</v>
       </c>
       <c r="N40" s="16">
-        <v>45156</v>
+        <v>45155</v>
       </c>
       <c r="O40" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4172,7 +4185,7 @@
       </c>
       <c r="P40">
         <f t="shared" ca="1" si="4"/>
-        <v>419</v>
+        <v>448</v>
       </c>
       <c r="Q40" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -4195,10 +4208,10 @@
         <v>32</v>
       </c>
       <c r="M41">
-        <v>349</v>
+        <v>419</v>
       </c>
       <c r="N41" s="16">
-        <v>45161</v>
+        <v>45156</v>
       </c>
       <c r="O41" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4206,7 +4219,7 @@
       </c>
       <c r="P41">
         <f t="shared" ca="1" si="4"/>
-        <v>349</v>
+        <v>419</v>
       </c>
       <c r="Q41" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -4229,10 +4242,10 @@
         <v>33</v>
       </c>
       <c r="M42">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="N42" s="16">
-        <v>45142</v>
+        <v>45161</v>
       </c>
       <c r="O42" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4240,7 +4253,7 @@
       </c>
       <c r="P42">
         <f t="shared" ca="1" si="4"/>
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="Q42" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -4263,10 +4276,10 @@
         <v>34</v>
       </c>
       <c r="M43">
-        <v>300</v>
+        <v>346</v>
       </c>
       <c r="N43" s="16">
-        <v>45181</v>
+        <v>45142</v>
       </c>
       <c r="O43" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4274,7 +4287,7 @@
       </c>
       <c r="P43">
         <f t="shared" ca="1" si="4"/>
-        <v>300</v>
+        <v>346</v>
       </c>
       <c r="Q43" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -4294,122 +4307,122 @@
         <v>0</v>
       </c>
       <c r="M44">
-        <v>272</v>
+        <v>300</v>
       </c>
       <c r="N44" s="16">
-        <v>45188</v>
+        <v>45181</v>
       </c>
     </row>
     <row r="45" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M45">
-        <v>220</v>
+        <v>272</v>
       </c>
       <c r="N45" s="16">
-        <v>45175</v>
+        <v>45188</v>
       </c>
     </row>
     <row r="46" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M46">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="N46" s="16">
-        <v>45173</v>
+        <v>45175</v>
       </c>
     </row>
     <row r="47" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M47">
-        <v>159</v>
+        <v>217</v>
       </c>
       <c r="N47" s="16">
-        <v>45182</v>
+        <v>45173</v>
       </c>
     </row>
     <row r="48" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M48">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="N48" s="16">
-        <v>45139</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="49" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M49">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="N49" s="16">
-        <v>45162</v>
+        <v>45139</v>
       </c>
     </row>
     <row r="50" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M50">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="N50" s="16">
-        <v>45152</v>
+        <v>45162</v>
       </c>
     </row>
     <row r="51" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M51">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="N51">
-        <v>45153</v>
+        <v>45152</v>
       </c>
     </row>
     <row r="52" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M52">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="N52">
-        <v>45187</v>
+        <v>45153</v>
       </c>
     </row>
     <row r="53" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M53">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="N53">
-        <v>45168</v>
+        <v>45187</v>
       </c>
     </row>
     <row r="54" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M54">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="N54">
-        <v>45147</v>
+        <v>45168</v>
       </c>
     </row>
     <row r="55" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M55">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="N55">
-        <v>45183</v>
+        <v>45147</v>
       </c>
     </row>
     <row r="56" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M56">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="N56">
-        <v>45164</v>
+        <v>45183</v>
       </c>
     </row>
     <row r="57" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M57">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="N57">
-        <v>45140</v>
+        <v>45164</v>
       </c>
     </row>
     <row r="58" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M58">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="N58">
-        <v>45138</v>
+        <v>45140</v>
       </c>
     </row>
     <row r="59" spans="13:14" x14ac:dyDescent="0.2">
@@ -4417,7 +4430,7 @@
         <v>0</v>
       </c>
       <c r="N59">
-        <v>0</v>
+        <v>45138</v>
       </c>
     </row>
     <row r="60" spans="13:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Improving plots and writing
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F71CFB-B44F-9345-BBA4-84A67CA292D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4BFD1DA-2C90-E747-A896-BAC7E6590C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14420" windowHeight="17500" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
@@ -772,6 +772,9 @@
                 <c:pt idx="30">
                   <c:v>45191</c:v>
                 </c:pt>
+                <c:pt idx="31">
+                  <c:v>45193</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -873,6 +876,9 @@
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>11224</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>11593</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1244,10 +1250,10 @@
                   <c:v>419</c:v>
                 </c:pt>
                 <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>349</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>346</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1370,7 +1376,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>369</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -3084,8 +3090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4213BD91-B5D1-3B47-8D3F-04331482504C}">
   <dimension ref="A1:Q60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3219,7 +3225,7 @@
         <v>45140</v>
       </c>
       <c r="C8" s="27">
-        <f t="shared" ref="C8:C36" si="2">D8-D7</f>
+        <f t="shared" ref="C8:C37" si="2">D8-D7</f>
         <v>38</v>
       </c>
       <c r="D8" s="21">
@@ -3335,7 +3341,7 @@
       <c r="I12" s="30"/>
       <c r="J12" s="14">
         <f>J8-MAX(D6:D37)</f>
-        <v>5776</v>
+        <v>5407</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
@@ -3391,7 +3397,7 @@
       <c r="I14" s="34"/>
       <c r="J14" s="15">
         <f>J12/J13</f>
-        <v>11.63688077743541</v>
+        <v>10.893458165442047</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
@@ -4054,16 +4060,23 @@
       </c>
     </row>
     <row r="37" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B37" s="3"/>
-      <c r="C37" s="27"/>
-      <c r="D37" s="21"/>
+      <c r="B37" s="2">
+        <v>45193</v>
+      </c>
+      <c r="C37" s="27">
+        <f t="shared" si="2"/>
+        <v>369</v>
+      </c>
+      <c r="D37" s="21">
+        <v>11593</v>
+      </c>
       <c r="E37" s="22">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>34.097058823529409</v>
       </c>
       <c r="F37" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.68194117647058827</v>
       </c>
       <c r="H37" s="17"/>
       <c r="I37" s="17"/>
@@ -4242,22 +4255,22 @@
         <v>33</v>
       </c>
       <c r="M42">
-        <v>349</v>
+        <v>369</v>
       </c>
       <c r="N42" s="16">
-        <v>45161</v>
+        <v>45193</v>
       </c>
       <c r="O42" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Blue</v>
-      </c>
-      <c r="P42">
+        <v>Green</v>
+      </c>
+      <c r="P42" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>349</v>
-      </c>
-      <c r="Q42" t="str">
+        <v/>
+      </c>
+      <c r="Q42">
         <f t="shared" ca="1" si="5"/>
-        <v/>
+        <v>369</v>
       </c>
     </row>
     <row r="43" spans="2:17" x14ac:dyDescent="0.2">
@@ -4276,10 +4289,10 @@
         <v>34</v>
       </c>
       <c r="M43">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="N43" s="16">
-        <v>45142</v>
+        <v>45161</v>
       </c>
       <c r="O43" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4287,7 +4300,7 @@
       </c>
       <c r="P43">
         <f t="shared" ca="1" si="4"/>
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="Q43" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -4307,130 +4320,130 @@
         <v>0</v>
       </c>
       <c r="M44">
-        <v>300</v>
+        <v>346</v>
       </c>
       <c r="N44" s="16">
-        <v>45181</v>
+        <v>45142</v>
       </c>
     </row>
     <row r="45" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M45">
-        <v>272</v>
+        <v>300</v>
       </c>
       <c r="N45" s="16">
-        <v>45188</v>
+        <v>45181</v>
       </c>
     </row>
     <row r="46" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M46">
-        <v>220</v>
+        <v>272</v>
       </c>
       <c r="N46" s="16">
-        <v>45175</v>
+        <v>45188</v>
       </c>
     </row>
     <row r="47" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M47">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="N47" s="16">
-        <v>45173</v>
+        <v>45175</v>
       </c>
     </row>
     <row r="48" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M48">
-        <v>159</v>
+        <v>217</v>
       </c>
       <c r="N48" s="16">
-        <v>45182</v>
+        <v>45173</v>
       </c>
     </row>
     <row r="49" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M49">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="N49" s="16">
-        <v>45139</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="50" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M50">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="N50" s="16">
-        <v>45162</v>
+        <v>45139</v>
       </c>
     </row>
     <row r="51" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M51">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="N51">
-        <v>45152</v>
+        <v>45162</v>
       </c>
     </row>
     <row r="52" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M52">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="N52">
-        <v>45153</v>
+        <v>45152</v>
       </c>
     </row>
     <row r="53" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M53">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="N53">
-        <v>45187</v>
+        <v>45153</v>
       </c>
     </row>
     <row r="54" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M54">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="N54">
-        <v>45168</v>
+        <v>45187</v>
       </c>
     </row>
     <row r="55" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M55">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="N55">
-        <v>45147</v>
+        <v>45168</v>
       </c>
     </row>
     <row r="56" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M56">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="N56">
-        <v>45183</v>
+        <v>45147</v>
       </c>
     </row>
     <row r="57" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M57">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="N57">
-        <v>45164</v>
+        <v>45183</v>
       </c>
     </row>
     <row r="58" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M58">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="N58">
-        <v>45140</v>
+        <v>45164</v>
       </c>
     </row>
     <row r="59" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M59">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="N59">
-        <v>45138</v>
+        <v>45140</v>
       </c>
     </row>
     <row r="60" spans="13:14" x14ac:dyDescent="0.2">
@@ -4438,7 +4451,7 @@
         <v>0</v>
       </c>
       <c r="N60">
-        <v>0</v>
+        <v>45138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Writing about COOH given H energies
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4BFD1DA-2C90-E747-A896-BAC7E6590C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03CF9BEA-F9ED-894F-B9CD-BC1BF1F6CB40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="14420" windowHeight="17500" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="14380" windowHeight="17500" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -878,7 +878,7 @@
                   <c:v>11224</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>11593</c:v>
+                  <c:v>11827</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1229,28 +1229,28 @@
                   <c:v>611</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>603</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>580</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>515</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>486</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>473</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>467</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>448</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>419</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>349</c:v>
@@ -1376,7 +1376,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>369</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -3090,7 +3090,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4213BD91-B5D1-3B47-8D3F-04331482504C}">
   <dimension ref="A1:Q60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
@@ -3341,7 +3341,7 @@
       <c r="I12" s="30"/>
       <c r="J12" s="14">
         <f>J8-MAX(D6:D37)</f>
-        <v>5407</v>
+        <v>5173</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
@@ -3397,7 +3397,7 @@
       <c r="I14" s="34"/>
       <c r="J14" s="15">
         <f>J12/J13</f>
-        <v>10.893458165442047</v>
+        <v>10.42201943588528</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
@@ -3997,10 +3997,10 @@
         <v>26</v>
       </c>
       <c r="M35">
-        <v>580</v>
+        <v>603</v>
       </c>
       <c r="N35" s="16">
-        <v>45160</v>
+        <v>45193</v>
       </c>
       <c r="O35" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4008,7 +4008,7 @@
       </c>
       <c r="P35">
         <f t="shared" ca="1" si="4"/>
-        <v>580</v>
+        <v>603</v>
       </c>
       <c r="Q35" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -4041,10 +4041,10 @@
         <v>27</v>
       </c>
       <c r="M36">
-        <v>515</v>
+        <v>580</v>
       </c>
       <c r="N36" s="16">
-        <v>45191</v>
+        <v>45160</v>
       </c>
       <c r="O36" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4052,7 +4052,7 @@
       </c>
       <c r="P36">
         <f t="shared" ca="1" si="4"/>
-        <v>515</v>
+        <v>580</v>
       </c>
       <c r="Q36" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -4065,18 +4065,18 @@
       </c>
       <c r="C37" s="27">
         <f t="shared" si="2"/>
-        <v>369</v>
+        <v>603</v>
       </c>
       <c r="D37" s="21">
-        <v>11593</v>
+        <v>11827</v>
       </c>
       <c r="E37" s="22">
         <f t="shared" si="0"/>
-        <v>34.097058823529409</v>
+        <v>34.785294117647062</v>
       </c>
       <c r="F37" s="5">
         <f t="shared" si="1"/>
-        <v>0.68194117647058827</v>
+        <v>0.69570588235294117</v>
       </c>
       <c r="H37" s="17"/>
       <c r="I37" s="17"/>
@@ -4085,10 +4085,10 @@
         <v>28</v>
       </c>
       <c r="M37">
-        <v>486</v>
+        <v>515</v>
       </c>
       <c r="N37" s="16">
-        <v>45141</v>
+        <v>45191</v>
       </c>
       <c r="O37" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4096,7 +4096,7 @@
       </c>
       <c r="P37">
         <f t="shared" ca="1" si="4"/>
-        <v>486</v>
+        <v>515</v>
       </c>
       <c r="Q37" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -4119,10 +4119,10 @@
         <v>29</v>
       </c>
       <c r="M38">
-        <v>473</v>
+        <v>486</v>
       </c>
       <c r="N38" s="16">
-        <v>45174</v>
+        <v>45141</v>
       </c>
       <c r="O38" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4130,7 +4130,7 @@
       </c>
       <c r="P38">
         <f t="shared" ca="1" si="4"/>
-        <v>473</v>
+        <v>486</v>
       </c>
       <c r="Q38" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -4153,10 +4153,10 @@
         <v>30</v>
       </c>
       <c r="M39">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="N39" s="16">
-        <v>45154</v>
+        <v>45174</v>
       </c>
       <c r="O39" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4164,7 +4164,7 @@
       </c>
       <c r="P39">
         <f t="shared" ca="1" si="4"/>
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="Q39" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -4187,10 +4187,10 @@
         <v>31</v>
       </c>
       <c r="M40">
-        <v>448</v>
+        <v>467</v>
       </c>
       <c r="N40" s="16">
-        <v>45155</v>
+        <v>45154</v>
       </c>
       <c r="O40" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4198,7 +4198,7 @@
       </c>
       <c r="P40">
         <f t="shared" ca="1" si="4"/>
-        <v>448</v>
+        <v>467</v>
       </c>
       <c r="Q40" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -4221,10 +4221,10 @@
         <v>32</v>
       </c>
       <c r="M41">
-        <v>419</v>
+        <v>448</v>
       </c>
       <c r="N41" s="16">
-        <v>45156</v>
+        <v>45155</v>
       </c>
       <c r="O41" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4232,7 +4232,7 @@
       </c>
       <c r="P41">
         <f t="shared" ca="1" si="4"/>
-        <v>419</v>
+        <v>448</v>
       </c>
       <c r="Q41" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -4255,22 +4255,22 @@
         <v>33</v>
       </c>
       <c r="M42">
-        <v>369</v>
+        <v>419</v>
       </c>
       <c r="N42" s="16">
-        <v>45193</v>
+        <v>45156</v>
       </c>
       <c r="O42" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Green</v>
-      </c>
-      <c r="P42" t="str">
+        <v>Blue</v>
+      </c>
+      <c r="P42">
         <f t="shared" ca="1" si="4"/>
+        <v>419</v>
+      </c>
+      <c r="Q42" t="str">
+        <f t="shared" ca="1" si="5"/>
         <v/>
-      </c>
-      <c r="Q42">
-        <f t="shared" ca="1" si="5"/>
-        <v>369</v>
       </c>
     </row>
     <row r="43" spans="2:17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
H given COOH plot + writing + calculations
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03CF9BEA-F9ED-894F-B9CD-BC1BF1F6CB40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE4F9DE-CDE2-8B42-9D0D-36210659CE81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14380" windowHeight="17500" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -174,7 +174,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -200,6 +200,14 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -430,7 +438,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -570,6 +578,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -775,6 +784,9 @@
                 <c:pt idx="31">
                   <c:v>45193</c:v>
                 </c:pt>
+                <c:pt idx="32">
+                  <c:v>45194</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -879,6 +891,9 @@
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>11827</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>12202</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1253,7 +1268,7 @@
                   <c:v>419</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>349</c:v>
+                  <c:v>375</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2731,15 +2746,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>31753</xdr:colOff>
+      <xdr:colOff>31754</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>39688</xdr:rowOff>
+      <xdr:rowOff>60857</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>531815</xdr:colOff>
+      <xdr:colOff>531816</xdr:colOff>
       <xdr:row>60</xdr:row>
-      <xdr:rowOff>52916</xdr:rowOff>
+      <xdr:rowOff>74085</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2754,7 +2769,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7323670" y="5564188"/>
+          <a:off x="7323671" y="5585357"/>
           <a:ext cx="5453062" cy="6670145"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3088,10 +3103,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4213BD91-B5D1-3B47-8D3F-04331482504C}">
-  <dimension ref="A1:Q60"/>
+  <dimension ref="A1:Q67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3225,7 +3240,7 @@
         <v>45140</v>
       </c>
       <c r="C8" s="27">
-        <f t="shared" ref="C8:C37" si="2">D8-D7</f>
+        <f t="shared" ref="C8:C38" si="2">D8-D7</f>
         <v>38</v>
       </c>
       <c r="D8" s="21">
@@ -3340,8 +3355,8 @@
       </c>
       <c r="I12" s="30"/>
       <c r="J12" s="14">
-        <f>J8-MAX(D6:D37)</f>
-        <v>5173</v>
+        <f>J8-MAX(D6:D44)</f>
+        <v>4798</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
@@ -3397,7 +3412,7 @@
       <c r="I14" s="34"/>
       <c r="J14" s="15">
         <f>J12/J13</f>
-        <v>10.42201943588528</v>
+        <v>9.6665086513391802</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
@@ -3731,11 +3746,11 @@
         <v>16</v>
       </c>
       <c r="M29" cm="1">
-        <f t="array" ref="M29:M60">_xlfn.SORTBY(C6:C37, C6:C37, -1)</f>
+        <f t="array" ref="M29:M67">_xlfn.SORTBY(C6:C44, C6:C44, -1)</f>
         <v>1279</v>
       </c>
       <c r="N29" s="16" cm="1">
-        <f t="array" ref="N29:N60">_xlfn.SORTBY(B6:B37,C6:C37, -1)</f>
+        <f t="array" ref="N29:N67">_xlfn.SORTBY(B6:B44,C6:C44, -1)</f>
         <v>45148</v>
       </c>
       <c r="O29" t="str">
@@ -4104,16 +4119,23 @@
       </c>
     </row>
     <row r="38" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="3"/>
-      <c r="C38" s="27"/>
-      <c r="D38" s="21"/>
+      <c r="B38" s="2">
+        <v>45194</v>
+      </c>
+      <c r="C38" s="27">
+        <f t="shared" si="2"/>
+        <v>375</v>
+      </c>
+      <c r="D38" s="21">
+        <v>12202</v>
+      </c>
       <c r="E38" s="22">
         <f t="shared" ref="E38:E44" si="6">D38/$J$6</f>
-        <v>0</v>
+        <v>35.888235294117649</v>
       </c>
       <c r="F38" s="5">
         <f t="shared" ref="F38:F44" si="7">D38/$J$8</f>
-        <v>0</v>
+        <v>0.71776470588235297</v>
       </c>
       <c r="L38" t="s">
         <v>29</v>
@@ -4140,7 +4162,7 @@
     <row r="39" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B39" s="3"/>
       <c r="C39" s="27"/>
-      <c r="D39" s="21"/>
+      <c r="D39" s="59"/>
       <c r="E39" s="22">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -4289,10 +4311,10 @@
         <v>34</v>
       </c>
       <c r="M43">
-        <v>349</v>
+        <v>375</v>
       </c>
       <c r="N43" s="16">
-        <v>45161</v>
+        <v>45194</v>
       </c>
       <c r="O43" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4300,7 +4322,7 @@
       </c>
       <c r="P43">
         <f t="shared" ca="1" si="4"/>
-        <v>349</v>
+        <v>375</v>
       </c>
       <c r="Q43" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -4320,138 +4342,194 @@
         <v>0</v>
       </c>
       <c r="M44">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="N44" s="16">
-        <v>45142</v>
+        <v>45161</v>
       </c>
     </row>
     <row r="45" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M45">
-        <v>300</v>
+        <v>346</v>
       </c>
       <c r="N45" s="16">
-        <v>45181</v>
+        <v>45142</v>
       </c>
     </row>
     <row r="46" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M46">
-        <v>272</v>
+        <v>300</v>
       </c>
       <c r="N46" s="16">
-        <v>45188</v>
+        <v>45181</v>
       </c>
     </row>
     <row r="47" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M47">
-        <v>220</v>
+        <v>272</v>
       </c>
       <c r="N47" s="16">
-        <v>45175</v>
+        <v>45188</v>
       </c>
     </row>
     <row r="48" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M48">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="N48" s="16">
-        <v>45173</v>
+        <v>45175</v>
       </c>
     </row>
     <row r="49" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M49">
-        <v>159</v>
+        <v>217</v>
       </c>
       <c r="N49" s="16">
-        <v>45182</v>
+        <v>45173</v>
       </c>
     </row>
     <row r="50" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M50">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="N50" s="16">
-        <v>45139</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="51" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M51">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="N51">
-        <v>45162</v>
+        <v>45139</v>
       </c>
     </row>
     <row r="52" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M52">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="N52">
-        <v>45152</v>
+        <v>45162</v>
       </c>
     </row>
     <row r="53" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M53">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="N53">
-        <v>45153</v>
+        <v>45152</v>
       </c>
     </row>
     <row r="54" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M54">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="N54">
-        <v>45187</v>
+        <v>45153</v>
       </c>
     </row>
     <row r="55" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M55">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="N55">
-        <v>45168</v>
+        <v>45187</v>
       </c>
     </row>
     <row r="56" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M56">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="N56">
-        <v>45147</v>
+        <v>45168</v>
       </c>
     </row>
     <row r="57" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M57">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="N57">
-        <v>45183</v>
+        <v>45147</v>
       </c>
     </row>
     <row r="58" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M58">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="N58">
-        <v>45164</v>
+        <v>45183</v>
       </c>
     </row>
     <row r="59" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M59">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="N59">
-        <v>45140</v>
+        <v>45164</v>
       </c>
     </row>
     <row r="60" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M60">
+        <v>38</v>
+      </c>
+      <c r="N60">
+        <v>45140</v>
+      </c>
+    </row>
+    <row r="61" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="M61">
         <v>0</v>
       </c>
-      <c r="N60">
+      <c r="N61">
         <v>45138</v>
+      </c>
+    </row>
+    <row r="62" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="M62">
+        <v>0</v>
+      </c>
+      <c r="N62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="M63">
+        <v>0</v>
+      </c>
+      <c r="N63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="M64">
+        <v>0</v>
+      </c>
+      <c r="N64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="M65">
+        <v>0</v>
+      </c>
+      <c r="N65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="M66">
+        <v>0</v>
+      </c>
+      <c r="N66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="M67">
+        <v>0</v>
+      </c>
+      <c r="N67">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mostly wrote on paper
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE4F9DE-CDE2-8B42-9D0D-36210659CE81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB8132A-6A56-014A-A00F-CE55EA9AF7DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14380" windowHeight="17500" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
@@ -3105,7 +3105,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4213BD91-B5D1-3B47-8D3F-04331482504C}">
   <dimension ref="A1:Q67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
GOOD plots and 12345 total wordcount
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB8132A-6A56-014A-A00F-CE55EA9AF7DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D6F9133-EA00-F749-953E-14169DB3FD3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14380" windowHeight="17500" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
@@ -174,7 +174,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -200,14 +200,6 @@
     <font>
       <b/>
       <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -578,7 +570,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -787,6 +779,9 @@
                 <c:pt idx="32">
                   <c:v>45194</c:v>
                 </c:pt>
+                <c:pt idx="33">
+                  <c:v>45195</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -894,6 +889,9 @@
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>12202</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>12345</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3106,7 +3104,7 @@
   <dimension ref="A1:Q67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3240,7 +3238,7 @@
         <v>45140</v>
       </c>
       <c r="C8" s="27">
-        <f t="shared" ref="C8:C38" si="2">D8-D7</f>
+        <f t="shared" ref="C8:C39" si="2">D8-D7</f>
         <v>38</v>
       </c>
       <c r="D8" s="21">
@@ -3356,7 +3354,7 @@
       <c r="I12" s="30"/>
       <c r="J12" s="14">
         <f>J8-MAX(D6:D44)</f>
-        <v>4798</v>
+        <v>4655</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
@@ -3412,7 +3410,7 @@
       <c r="I14" s="34"/>
       <c r="J14" s="15">
         <f>J12/J13</f>
-        <v>9.6665086513391802</v>
+        <v>9.3784072054989327</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
@@ -4160,16 +4158,23 @@
       </c>
     </row>
     <row r="39" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B39" s="3"/>
-      <c r="C39" s="27"/>
-      <c r="D39" s="59"/>
+      <c r="B39" s="2">
+        <v>45195</v>
+      </c>
+      <c r="C39" s="27">
+        <f t="shared" si="2"/>
+        <v>143</v>
+      </c>
+      <c r="D39" s="59">
+        <v>12345</v>
+      </c>
       <c r="E39" s="22">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>36.308823529411768</v>
       </c>
       <c r="F39" s="5">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>0.72617647058823531</v>
       </c>
       <c r="L39" t="s">
         <v>30</v>
@@ -4422,66 +4427,66 @@
     </row>
     <row r="54" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M54">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="N54">
-        <v>45153</v>
+        <v>45195</v>
       </c>
     </row>
     <row r="55" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M55">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="N55">
-        <v>45187</v>
+        <v>45153</v>
       </c>
     </row>
     <row r="56" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M56">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="N56">
-        <v>45168</v>
+        <v>45187</v>
       </c>
     </row>
     <row r="57" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M57">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="N57">
-        <v>45147</v>
+        <v>45168</v>
       </c>
     </row>
     <row r="58" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M58">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="N58">
-        <v>45183</v>
+        <v>45147</v>
       </c>
     </row>
     <row r="59" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M59">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="N59">
-        <v>45164</v>
+        <v>45183</v>
       </c>
     </row>
     <row r="60" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M60">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="N60">
-        <v>45140</v>
+        <v>45164</v>
       </c>
     </row>
     <row r="61" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M61">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="N61">
-        <v>45138</v>
+        <v>45140</v>
       </c>
     </row>
     <row r="62" spans="13:14" x14ac:dyDescent="0.2">
@@ -4489,7 +4494,7 @@
         <v>0</v>
       </c>
       <c r="N62">
-        <v>0</v>
+        <v>45138</v>
       </c>
     </row>
     <row r="63" spans="13:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Presented progress to Satellite meeting
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D6F9133-EA00-F749-953E-14169DB3FD3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4CFE72C-044C-794B-89E7-EA0983080DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14380" windowHeight="17500" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
@@ -782,6 +782,9 @@
                 <c:pt idx="33">
                   <c:v>45195</c:v>
                 </c:pt>
+                <c:pt idx="34">
+                  <c:v>45196</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -892,6 +895,9 @@
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>12345</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>12496</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3103,8 +3109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4213BD91-B5D1-3B47-8D3F-04331482504C}">
   <dimension ref="A1:Q67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3238,7 +3244,7 @@
         <v>45140</v>
       </c>
       <c r="C8" s="27">
-        <f t="shared" ref="C8:C39" si="2">D8-D7</f>
+        <f t="shared" ref="C8:C40" si="2">D8-D7</f>
         <v>38</v>
       </c>
       <c r="D8" s="21">
@@ -3354,7 +3360,7 @@
       <c r="I12" s="30"/>
       <c r="J12" s="14">
         <f>J8-MAX(D6:D44)</f>
-        <v>4655</v>
+        <v>4504</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
@@ -3410,7 +3416,7 @@
       <c r="I14" s="34"/>
       <c r="J14" s="15">
         <f>J12/J13</f>
-        <v>9.3784072054989327</v>
+        <v>9.0741881962550366</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
@@ -4199,16 +4205,23 @@
       </c>
     </row>
     <row r="40" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B40" s="3"/>
-      <c r="C40" s="27"/>
-      <c r="D40" s="21"/>
+      <c r="B40" s="2">
+        <v>45196</v>
+      </c>
+      <c r="C40" s="27">
+        <f t="shared" si="2"/>
+        <v>151</v>
+      </c>
+      <c r="D40" s="21">
+        <v>12496</v>
+      </c>
       <c r="E40" s="22">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>36.752941176470586</v>
       </c>
       <c r="F40" s="5">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>0.73505882352941176</v>
       </c>
       <c r="L40" t="s">
         <v>31</v>
@@ -4419,82 +4432,82 @@
     </row>
     <row r="53" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M53">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="N53">
-        <v>45152</v>
+        <v>45196</v>
       </c>
     </row>
     <row r="54" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M54">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="N54">
-        <v>45195</v>
+        <v>45152</v>
       </c>
     </row>
     <row r="55" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M55">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="N55">
-        <v>45153</v>
+        <v>45195</v>
       </c>
     </row>
     <row r="56" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M56">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="N56">
-        <v>45187</v>
+        <v>45153</v>
       </c>
     </row>
     <row r="57" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M57">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="N57">
-        <v>45168</v>
+        <v>45187</v>
       </c>
     </row>
     <row r="58" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M58">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="N58">
-        <v>45147</v>
+        <v>45168</v>
       </c>
     </row>
     <row r="59" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M59">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="N59">
-        <v>45183</v>
+        <v>45147</v>
       </c>
     </row>
     <row r="60" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M60">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="N60">
-        <v>45164</v>
+        <v>45183</v>
       </c>
     </row>
     <row r="61" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M61">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="N61">
-        <v>45140</v>
+        <v>45164</v>
       </c>
     </row>
     <row r="62" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M62">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="N62">
-        <v>45138</v>
+        <v>45140</v>
       </c>
     </row>
     <row r="63" spans="13:14" x14ac:dyDescent="0.2">
@@ -4502,7 +4515,7 @@
         <v>0</v>
       </c>
       <c r="N63">
-        <v>0</v>
+        <v>45138</v>
       </c>
     </row>
     <row r="64" spans="13:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Lots of triangles and 500 words
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4CFE72C-044C-794B-89E7-EA0983080DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C924CD6-AB71-A144-9219-3E3CE7325BA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="14380" windowHeight="17500" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="14380" windowHeight="17040" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -430,7 +430,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -570,7 +570,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -785,6 +784,9 @@
                 <c:pt idx="34">
                   <c:v>45196</c:v>
                 </c:pt>
+                <c:pt idx="35">
+                  <c:v>45208</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -898,6 +900,9 @@
                 </c:pt>
                 <c:pt idx="34">
                   <c:v>12496</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>13044</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1254,25 +1259,25 @@
                   <c:v>580</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>548</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>515</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>486</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>473</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>467</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>448</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>419</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>375</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3109,8 +3114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4213BD91-B5D1-3B47-8D3F-04331482504C}">
   <dimension ref="A1:Q67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3360,7 +3365,7 @@
       <c r="I12" s="30"/>
       <c r="J12" s="14">
         <f>J8-MAX(D6:D44)</f>
-        <v>4504</v>
+        <v>3956</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
@@ -3416,7 +3421,7 @@
       <c r="I14" s="34"/>
       <c r="J14" s="15">
         <f>J12/J13</f>
-        <v>9.0741881962550366</v>
+        <v>7.970135103105001</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
@@ -4104,10 +4109,10 @@
         <v>28</v>
       </c>
       <c r="M37">
-        <v>515</v>
+        <v>548</v>
       </c>
       <c r="N37" s="16">
-        <v>45191</v>
+        <v>45208</v>
       </c>
       <c r="O37" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4115,7 +4120,7 @@
       </c>
       <c r="P37">
         <f t="shared" ca="1" si="4"/>
-        <v>515</v>
+        <v>548</v>
       </c>
       <c r="Q37" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -4145,10 +4150,10 @@
         <v>29</v>
       </c>
       <c r="M38">
-        <v>486</v>
+        <v>515</v>
       </c>
       <c r="N38" s="16">
-        <v>45141</v>
+        <v>45191</v>
       </c>
       <c r="O38" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4156,7 +4161,7 @@
       </c>
       <c r="P38">
         <f t="shared" ca="1" si="4"/>
-        <v>486</v>
+        <v>515</v>
       </c>
       <c r="Q38" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -4171,7 +4176,7 @@
         <f t="shared" si="2"/>
         <v>143</v>
       </c>
-      <c r="D39" s="59">
+      <c r="D39" s="21">
         <v>12345</v>
       </c>
       <c r="E39" s="22">
@@ -4186,10 +4191,10 @@
         <v>30</v>
       </c>
       <c r="M39">
-        <v>473</v>
+        <v>486</v>
       </c>
       <c r="N39" s="16">
-        <v>45174</v>
+        <v>45141</v>
       </c>
       <c r="O39" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4197,7 +4202,7 @@
       </c>
       <c r="P39">
         <f t="shared" ca="1" si="4"/>
-        <v>473</v>
+        <v>486</v>
       </c>
       <c r="Q39" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -4227,10 +4232,10 @@
         <v>31</v>
       </c>
       <c r="M40">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="N40" s="16">
-        <v>45154</v>
+        <v>45174</v>
       </c>
       <c r="O40" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4238,7 +4243,7 @@
       </c>
       <c r="P40">
         <f t="shared" ca="1" si="4"/>
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="Q40" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -4246,25 +4251,32 @@
       </c>
     </row>
     <row r="41" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B41" s="3"/>
-      <c r="C41" s="27"/>
-      <c r="D41" s="21"/>
+      <c r="B41" s="2">
+        <v>45208</v>
+      </c>
+      <c r="C41" s="27">
+        <f>D41-D40</f>
+        <v>548</v>
+      </c>
+      <c r="D41" s="21">
+        <v>13044</v>
+      </c>
       <c r="E41" s="22">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f>D41/$J$6</f>
+        <v>38.364705882352943</v>
       </c>
       <c r="F41" s="5">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f>D41/$J$8</f>
+        <v>0.76729411764705879</v>
       </c>
       <c r="L41" t="s">
         <v>32</v>
       </c>
       <c r="M41">
-        <v>448</v>
+        <v>467</v>
       </c>
       <c r="N41" s="16">
-        <v>45155</v>
+        <v>45154</v>
       </c>
       <c r="O41" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4272,7 +4284,7 @@
       </c>
       <c r="P41">
         <f t="shared" ca="1" si="4"/>
-        <v>448</v>
+        <v>467</v>
       </c>
       <c r="Q41" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -4284,21 +4296,21 @@
       <c r="C42" s="27"/>
       <c r="D42" s="21"/>
       <c r="E42" s="22">
-        <f t="shared" si="6"/>
+        <f>D42/$J$6</f>
         <v>0</v>
       </c>
       <c r="F42" s="5">
-        <f t="shared" si="7"/>
+        <f>D42/$J$8</f>
         <v>0</v>
       </c>
       <c r="L42" t="s">
         <v>33</v>
       </c>
       <c r="M42">
-        <v>419</v>
+        <v>448</v>
       </c>
       <c r="N42" s="16">
-        <v>45156</v>
+        <v>45155</v>
       </c>
       <c r="O42" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4306,7 +4318,7 @@
       </c>
       <c r="P42">
         <f t="shared" ca="1" si="4"/>
-        <v>419</v>
+        <v>448</v>
       </c>
       <c r="Q42" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -4329,10 +4341,10 @@
         <v>34</v>
       </c>
       <c r="M43">
-        <v>375</v>
+        <v>419</v>
       </c>
       <c r="N43" s="16">
-        <v>45194</v>
+        <v>45156</v>
       </c>
       <c r="O43" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4340,7 +4352,7 @@
       </c>
       <c r="P43">
         <f t="shared" ca="1" si="4"/>
-        <v>375</v>
+        <v>419</v>
       </c>
       <c r="Q43" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -4360,162 +4372,162 @@
         <v>0</v>
       </c>
       <c r="M44">
-        <v>349</v>
+        <v>375</v>
       </c>
       <c r="N44" s="16">
-        <v>45161</v>
+        <v>45194</v>
       </c>
     </row>
     <row r="45" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M45">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="N45" s="16">
-        <v>45142</v>
+        <v>45161</v>
       </c>
     </row>
     <row r="46" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M46">
-        <v>300</v>
+        <v>346</v>
       </c>
       <c r="N46" s="16">
-        <v>45181</v>
+        <v>45142</v>
       </c>
     </row>
     <row r="47" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M47">
-        <v>272</v>
+        <v>300</v>
       </c>
       <c r="N47" s="16">
-        <v>45188</v>
+        <v>45181</v>
       </c>
     </row>
     <row r="48" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M48">
-        <v>220</v>
+        <v>272</v>
       </c>
       <c r="N48" s="16">
-        <v>45175</v>
+        <v>45188</v>
       </c>
     </row>
     <row r="49" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M49">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="N49" s="16">
-        <v>45173</v>
+        <v>45175</v>
       </c>
     </row>
     <row r="50" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M50">
-        <v>159</v>
+        <v>217</v>
       </c>
       <c r="N50" s="16">
-        <v>45182</v>
+        <v>45173</v>
       </c>
     </row>
     <row r="51" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M51">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="N51">
-        <v>45139</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="52" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M52">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="N52">
-        <v>45162</v>
+        <v>45139</v>
       </c>
     </row>
     <row r="53" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M53">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="N53">
-        <v>45196</v>
+        <v>45162</v>
       </c>
     </row>
     <row r="54" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M54">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="N54">
-        <v>45152</v>
+        <v>45196</v>
       </c>
     </row>
     <row r="55" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M55">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="N55">
-        <v>45195</v>
+        <v>45152</v>
       </c>
     </row>
     <row r="56" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M56">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="N56">
-        <v>45153</v>
+        <v>45195</v>
       </c>
     </row>
     <row r="57" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M57">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="N57">
-        <v>45187</v>
+        <v>45153</v>
       </c>
     </row>
     <row r="58" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M58">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="N58">
-        <v>45168</v>
+        <v>45187</v>
       </c>
     </row>
     <row r="59" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M59">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="N59">
-        <v>45147</v>
+        <v>45168</v>
       </c>
     </row>
     <row r="60" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M60">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="N60">
-        <v>45183</v>
+        <v>45147</v>
       </c>
     </row>
     <row r="61" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M61">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="N61">
-        <v>45164</v>
+        <v>45183</v>
       </c>
     </row>
     <row r="62" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M62">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="N62">
-        <v>45140</v>
+        <v>45164</v>
       </c>
     </row>
     <row r="63" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M63">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="N63">
-        <v>45138</v>
+        <v>45140</v>
       </c>
     </row>
     <row r="64" spans="13:14" x14ac:dyDescent="0.2">
@@ -4523,7 +4535,7 @@
         <v>0</v>
       </c>
       <c r="N64">
-        <v>0</v>
+        <v>45138</v>
       </c>
     </row>
     <row r="65" spans="13:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Talking w. Mads, thinking and writing
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C924CD6-AB71-A144-9219-3E3CE7325BA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC48E35D-B1B2-9544-AAF2-898B47653BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="14380" windowHeight="17040" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
@@ -787,6 +787,9 @@
                 <c:pt idx="35">
                   <c:v>45208</c:v>
                 </c:pt>
+                <c:pt idx="36">
+                  <c:v>45209</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -903,6 +906,9 @@
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>13044</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>13454</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3114,8 +3120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4213BD91-B5D1-3B47-8D3F-04331482504C}">
   <dimension ref="A1:Q67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3365,7 +3371,7 @@
       <c r="I12" s="30"/>
       <c r="J12" s="14">
         <f>J8-MAX(D6:D44)</f>
-        <v>3956</v>
+        <v>3546</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
@@ -3421,7 +3427,7 @@
       <c r="I14" s="34"/>
       <c r="J14" s="15">
         <f>J12/J13</f>
-        <v>7.970135103105001</v>
+        <v>7.1441099786679301</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
@@ -4292,16 +4298,23 @@
       </c>
     </row>
     <row r="42" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B42" s="3"/>
-      <c r="C42" s="27"/>
-      <c r="D42" s="21"/>
+      <c r="B42" s="2">
+        <v>45209</v>
+      </c>
+      <c r="C42" s="27">
+        <f>D42-D41</f>
+        <v>410</v>
+      </c>
+      <c r="D42" s="21">
+        <v>13454</v>
+      </c>
       <c r="E42" s="22">
         <f>D42/$J$6</f>
-        <v>0</v>
+        <v>39.570588235294117</v>
       </c>
       <c r="F42" s="5">
         <f>D42/$J$8</f>
-        <v>0</v>
+        <v>0.79141176470588237</v>
       </c>
       <c r="L42" t="s">
         <v>33</v>
@@ -4372,170 +4385,170 @@
         <v>0</v>
       </c>
       <c r="M44">
-        <v>375</v>
+        <v>410</v>
       </c>
       <c r="N44" s="16">
-        <v>45194</v>
+        <v>45209</v>
       </c>
     </row>
     <row r="45" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M45">
-        <v>349</v>
+        <v>375</v>
       </c>
       <c r="N45" s="16">
-        <v>45161</v>
+        <v>45194</v>
       </c>
     </row>
     <row r="46" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M46">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="N46" s="16">
-        <v>45142</v>
+        <v>45161</v>
       </c>
     </row>
     <row r="47" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M47">
-        <v>300</v>
+        <v>346</v>
       </c>
       <c r="N47" s="16">
-        <v>45181</v>
+        <v>45142</v>
       </c>
     </row>
     <row r="48" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M48">
-        <v>272</v>
+        <v>300</v>
       </c>
       <c r="N48" s="16">
-        <v>45188</v>
+        <v>45181</v>
       </c>
     </row>
     <row r="49" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M49">
-        <v>220</v>
+        <v>272</v>
       </c>
       <c r="N49" s="16">
-        <v>45175</v>
+        <v>45188</v>
       </c>
     </row>
     <row r="50" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M50">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="N50" s="16">
-        <v>45173</v>
+        <v>45175</v>
       </c>
     </row>
     <row r="51" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M51">
-        <v>159</v>
+        <v>217</v>
       </c>
       <c r="N51">
-        <v>45182</v>
+        <v>45173</v>
       </c>
     </row>
     <row r="52" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M52">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="N52">
-        <v>45139</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="53" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M53">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="N53">
-        <v>45162</v>
+        <v>45139</v>
       </c>
     </row>
     <row r="54" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M54">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="N54">
-        <v>45196</v>
+        <v>45162</v>
       </c>
     </row>
     <row r="55" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M55">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="N55">
-        <v>45152</v>
+        <v>45196</v>
       </c>
     </row>
     <row r="56" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M56">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="N56">
-        <v>45195</v>
+        <v>45152</v>
       </c>
     </row>
     <row r="57" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M57">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="N57">
-        <v>45153</v>
+        <v>45195</v>
       </c>
     </row>
     <row r="58" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M58">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="N58">
-        <v>45187</v>
+        <v>45153</v>
       </c>
     </row>
     <row r="59" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M59">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="N59">
-        <v>45168</v>
+        <v>45187</v>
       </c>
     </row>
     <row r="60" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M60">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="N60">
-        <v>45147</v>
+        <v>45168</v>
       </c>
     </row>
     <row r="61" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M61">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="N61">
-        <v>45183</v>
+        <v>45147</v>
       </c>
     </row>
     <row r="62" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M62">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="N62">
-        <v>45164</v>
+        <v>45183</v>
       </c>
     </row>
     <row r="63" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M63">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="N63">
-        <v>45140</v>
+        <v>45164</v>
       </c>
     </row>
     <row r="64" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M64">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="N64">
-        <v>45138</v>
+        <v>45140</v>
       </c>
     </row>
     <row r="65" spans="13:14" x14ac:dyDescent="0.2">
@@ -4543,7 +4556,7 @@
         <v>0</v>
       </c>
       <c r="N65">
-        <v>0</v>
+        <v>45138</v>
       </c>
     </row>
     <row r="66" spans="13:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Corrections final + writing about corrections
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -1,20 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7173A40A-7A07-164E-9D7D-989717D83A12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42EE2ED4-3747-A24D-AC09-3323C4DA872D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="15020" windowHeight="17040" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
+    <workbookView xWindow="2180" yWindow="1300" windowWidth="15820" windowHeight="19800" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$C$7:$C$44</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$C$7:$C$44</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$C$7:$C$44</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$C$7:$C$44</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$C$7:$C$44</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -58,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Keeping up with the thesis</t>
   </si>
@@ -163,6 +170,21 @@
   </si>
   <si>
     <t>Fifteen best</t>
+  </si>
+  <si>
+    <t>Twentieth best</t>
+  </si>
+  <si>
+    <t>Sixteenth best</t>
+  </si>
+  <si>
+    <t>Seventeenth best</t>
+  </si>
+  <si>
+    <t>Eightteenth best</t>
+  </si>
+  <si>
+    <t>Nineteenth best</t>
   </si>
 </sst>
 </file>
@@ -430,7 +452,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -438,15 +460,6 @@
     <xf numFmtId="165" fontId="0" fillId="4" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="4" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -471,8 +484,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -569,6 +580,18 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -577,6 +600,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF71A3E7"/>
+      <color rgb="FFFF9300"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -792,6 +821,9 @@
                 <c:pt idx="37">
                   <c:v>45210</c:v>
                 </c:pt>
+                <c:pt idx="38">
+                  <c:v>45211</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -914,6 +946,9 @@
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>13609</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>14169</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1188,9 +1223,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$L$29:$L$43</c:f>
+              <c:f>Sheet1!$L$29:$L$48</c:f>
               <c:strCache>
-                <c:ptCount val="15"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>Best day</c:v>
                 </c:pt>
@@ -1235,16 +1270,31 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>Fifteen best</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Sixteenth best</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Seventeenth best</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Eightteenth best</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Nineteenth best</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Twentieth best</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$29:$P$43</c:f>
+              <c:f>Sheet1!$P$29:$P$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>1279</c:v>
                 </c:pt>
@@ -1270,25 +1320,40 @@
                   <c:v>580</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>548</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>515</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>486</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>473</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>467</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>448</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>419</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>375</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>349</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>346</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1314,9 +1379,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$L$29:$L$43</c:f>
+              <c:f>Sheet1!$L$29:$L$48</c:f>
               <c:strCache>
-                <c:ptCount val="15"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>Best day</c:v>
                 </c:pt>
@@ -1361,16 +1426,31 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>Fifteen best</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Sixteenth best</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Seventeenth best</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Eightteenth best</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Nineteenth best</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Twentieth best</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$29:$Q$43</c:f>
+              <c:f>Sheet1!$Q$29:$Q$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1396,7 +1476,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>560</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -1414,6 +1494,21 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1467,7 +1562,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="700" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1590,6 +1685,450 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Words per day</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-DK"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$7:$C$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="38"/>
+                <c:pt idx="0">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>486</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>346</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>729</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>859</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1279</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>657</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>467</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>448</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>419</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>661</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>580</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>349</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>611</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>217</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>473</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>272</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>515</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>603</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>375</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>548</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>560</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D259-2745-A5D4-802DDA42F194}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="173250656"/>
+        <c:axId val="173252928"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="173250656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Day</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-DK"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="173252928"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="173252928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="173250656"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="340"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="71A3E7"/>
+    </a:solidFill>
+    <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-DK"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1670,6 +2209,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -2670,6 +3249,522 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -2737,8 +3832,8 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>10583</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>206373</xdr:rowOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>74084</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2766,15 +3861,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>31754</xdr:colOff>
+      <xdr:colOff>21171</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>60857</xdr:rowOff>
+      <xdr:rowOff>7941</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>531816</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>74085</xdr:rowOff>
+      <xdr:colOff>521233</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>127001</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2789,8 +3884,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7323671" y="5585357"/>
-          <a:ext cx="5453062" cy="6670145"/>
+          <a:off x="8022171" y="5532441"/>
+          <a:ext cx="5453062" cy="8183560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2821,6 +3916,42 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>10582</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>201083</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D49185D-672F-3EFE-2E9C-833218C38623}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3125,8 +4256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4213BD91-B5D1-3B47-8D3F-04331482504C}">
   <dimension ref="A1:Q67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3137,96 +4268,97 @@
     <col min="4" max="4" width="12.33203125" customWidth="1"/>
     <col min="5" max="6" width="12.1640625" customWidth="1"/>
     <col min="7" max="7" width="1" customWidth="1"/>
-    <col min="11" max="11" width="0.83203125" customWidth="1"/>
+    <col min="10" max="10" width="16.1640625" customWidth="1"/>
+    <col min="11" max="11" width="3.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="36"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="31"/>
     </row>
     <row r="2" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="37"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="39"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="34"/>
     </row>
     <row r="3" spans="1:17" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="40"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="42"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="37"/>
     </row>
     <row r="4" spans="1:17" ht="5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:17" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="43" t="s">
+      <c r="H5" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="44"/>
-      <c r="J5" s="45"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="40"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B6" s="17">
+      <c r="B6" s="14">
         <v>45138</v>
       </c>
-      <c r="C6" s="22">
+      <c r="C6" s="17">
         <v>0</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="18">
         <v>0</v>
       </c>
-      <c r="E6" s="24">
+      <c r="E6" s="19">
         <f>D6/$J$6</f>
         <v>0</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="20">
         <f>D6/$J$8</f>
         <v>0</v>
       </c>
-      <c r="H6" s="46" t="s">
+      <c r="H6" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="47"/>
-      <c r="J6" s="11">
+      <c r="I6" s="42"/>
+      <c r="J6" s="8">
         <v>340</v>
       </c>
     </row>
@@ -3234,13 +4366,13 @@
       <c r="B7" s="2">
         <v>45139</v>
       </c>
-      <c r="C7" s="26">
+      <c r="C7" s="21">
         <v>156</v>
       </c>
-      <c r="D7" s="20">
+      <c r="D7" s="53">
         <v>156</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="54">
         <f t="shared" ref="E7:E37" si="0">D7/$J$6</f>
         <v>0.45882352941176469</v>
       </c>
@@ -3248,11 +4380,11 @@
         <f t="shared" ref="F7:F37" si="1">D7/$J$8</f>
         <v>9.1764705882352946E-3</v>
       </c>
-      <c r="H7" s="48" t="s">
+      <c r="H7" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="49"/>
-      <c r="J7" s="11">
+      <c r="I7" s="44"/>
+      <c r="J7" s="8">
         <v>50</v>
       </c>
     </row>
@@ -3260,14 +4392,14 @@
       <c r="B8" s="2">
         <v>45140</v>
       </c>
-      <c r="C8" s="26">
+      <c r="C8" s="21">
         <f t="shared" ref="C8:C40" si="2">D8-D7</f>
         <v>38</v>
       </c>
-      <c r="D8" s="20">
+      <c r="D8" s="53">
         <v>194</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="54">
         <f t="shared" si="0"/>
         <v>0.57058823529411762</v>
       </c>
@@ -3275,11 +4407,11 @@
         <f t="shared" si="1"/>
         <v>1.1411764705882352E-2</v>
       </c>
-      <c r="H8" s="50" t="s">
+      <c r="H8" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="51"/>
-      <c r="J8" s="12">
+      <c r="I8" s="46"/>
+      <c r="J8" s="9">
         <f>J6*J7</f>
         <v>17000</v>
       </c>
@@ -3288,14 +4420,14 @@
       <c r="B9" s="2">
         <v>45141</v>
       </c>
-      <c r="C9" s="26">
+      <c r="C9" s="21">
         <f t="shared" si="2"/>
         <v>486</v>
       </c>
-      <c r="D9" s="20">
+      <c r="D9" s="53">
         <v>680</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="54">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -3308,14 +4440,14 @@
       <c r="B10" s="2">
         <v>45142</v>
       </c>
-      <c r="C10" s="26">
+      <c r="C10" s="21">
         <f t="shared" si="2"/>
         <v>346</v>
       </c>
-      <c r="D10" s="20">
+      <c r="D10" s="53">
         <v>1026</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="54">
         <f t="shared" si="0"/>
         <v>3.0176470588235293</v>
       </c>
@@ -3323,24 +4455,24 @@
         <f t="shared" si="1"/>
         <v>6.0352941176470588E-2</v>
       </c>
-      <c r="H10" s="52" t="s">
+      <c r="H10" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="53"/>
-      <c r="J10" s="54"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="49"/>
     </row>
     <row r="11" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>45145</v>
       </c>
-      <c r="C11" s="26">
+      <c r="C11" s="21">
         <f t="shared" si="2"/>
         <v>729</v>
       </c>
-      <c r="D11" s="20">
+      <c r="D11" s="53">
         <v>1755</v>
       </c>
-      <c r="E11" s="21">
+      <c r="E11" s="54">
         <f t="shared" si="0"/>
         <v>5.1617647058823533</v>
       </c>
@@ -3348,22 +4480,22 @@
         <f t="shared" si="1"/>
         <v>0.10323529411764706</v>
       </c>
-      <c r="H11" s="55"/>
-      <c r="I11" s="56"/>
-      <c r="J11" s="57"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="52"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B12" s="2">
         <v>45146</v>
       </c>
-      <c r="C12" s="26">
+      <c r="C12" s="21">
         <f t="shared" si="2"/>
         <v>859</v>
       </c>
-      <c r="D12" s="20">
+      <c r="D12" s="53">
         <v>2614</v>
       </c>
-      <c r="E12" s="21">
+      <c r="E12" s="54">
         <f t="shared" si="0"/>
         <v>7.6882352941176473</v>
       </c>
@@ -3371,27 +4503,27 @@
         <f t="shared" si="1"/>
         <v>0.15376470588235294</v>
       </c>
-      <c r="H12" s="28" t="s">
+      <c r="H12" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="I12" s="29"/>
-      <c r="J12" s="13">
+      <c r="I12" s="24"/>
+      <c r="J12" s="10">
         <f>J8-MAX(D6:D44)</f>
-        <v>3391</v>
+        <v>2831</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B13" s="2">
         <v>45147</v>
       </c>
-      <c r="C13" s="26">
+      <c r="C13" s="21">
         <f t="shared" si="2"/>
         <v>107</v>
       </c>
-      <c r="D13" s="20">
+      <c r="D13" s="53">
         <v>2721</v>
       </c>
-      <c r="E13" s="21">
+      <c r="E13" s="54">
         <f t="shared" si="0"/>
         <v>8.0029411764705891</v>
       </c>
@@ -3399,11 +4531,11 @@
         <f t="shared" si="1"/>
         <v>0.16005882352941175</v>
       </c>
-      <c r="H13" s="30" t="s">
+      <c r="H13" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="31"/>
-      <c r="J13" s="13">
+      <c r="I13" s="26"/>
+      <c r="J13" s="10">
         <f>AVERAGE(C9:C25)</f>
         <v>496.35294117647061</v>
       </c>
@@ -3412,14 +4544,14 @@
       <c r="B14" s="2">
         <v>45148</v>
       </c>
-      <c r="C14" s="26">
+      <c r="C14" s="21">
         <f t="shared" si="2"/>
         <v>1279</v>
       </c>
-      <c r="D14" s="20">
+      <c r="D14" s="53">
         <v>4000</v>
       </c>
-      <c r="E14" s="21">
+      <c r="E14" s="54">
         <f t="shared" si="0"/>
         <v>11.764705882352942</v>
       </c>
@@ -3427,27 +4559,27 @@
         <f t="shared" si="1"/>
         <v>0.23529411764705882</v>
       </c>
-      <c r="H14" s="32" t="s">
+      <c r="H14" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="I14" s="33"/>
-      <c r="J14" s="14">
+      <c r="I14" s="28"/>
+      <c r="J14" s="11">
         <f>J12/J13</f>
-        <v>6.8318321877222088</v>
+        <v>5.7036027494666977</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B15" s="2">
         <v>45149</v>
       </c>
-      <c r="C15" s="26">
+      <c r="C15" s="21">
         <f t="shared" si="2"/>
         <v>657</v>
       </c>
-      <c r="D15" s="20">
+      <c r="D15" s="53">
         <v>4657</v>
       </c>
-      <c r="E15" s="21">
+      <c r="E15" s="54">
         <f t="shared" si="0"/>
         <v>13.697058823529412</v>
       </c>
@@ -3455,13 +4587,13 @@
         <f t="shared" si="1"/>
         <v>0.27394117647058824</v>
       </c>
-      <c r="O15" s="10" t="s">
+      <c r="O15" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="P15" s="10">
+      <c r="P15" s="7">
         <v>24.68</v>
       </c>
-      <c r="Q15" s="18">
+      <c r="Q15" s="15">
         <v>23.78</v>
       </c>
     </row>
@@ -3469,14 +4601,14 @@
       <c r="B16" s="2">
         <v>45152</v>
       </c>
-      <c r="C16" s="26">
+      <c r="C16" s="21">
         <f t="shared" si="2"/>
         <v>146</v>
       </c>
-      <c r="D16" s="20">
+      <c r="D16" s="53">
         <v>4803</v>
       </c>
-      <c r="E16" s="21">
+      <c r="E16" s="54">
         <f t="shared" si="0"/>
         <v>14.126470588235295</v>
       </c>
@@ -3484,20 +4616,20 @@
         <f t="shared" si="1"/>
         <v>0.28252941176470586</v>
       </c>
-      <c r="J16" s="19"/>
+      <c r="J16" s="16"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B17" s="2">
         <v>45153</v>
       </c>
-      <c r="C17" s="26">
+      <c r="C17" s="21">
         <f t="shared" si="2"/>
         <v>140</v>
       </c>
-      <c r="D17" s="20">
+      <c r="D17" s="53">
         <v>4943</v>
       </c>
-      <c r="E17" s="21">
+      <c r="E17" s="54">
         <f t="shared" si="0"/>
         <v>14.538235294117648</v>
       </c>
@@ -3510,14 +4642,14 @@
       <c r="B18" s="2">
         <v>45154</v>
       </c>
-      <c r="C18" s="26">
+      <c r="C18" s="21">
         <f t="shared" si="2"/>
         <v>467</v>
       </c>
-      <c r="D18" s="20">
+      <c r="D18" s="53">
         <v>5410</v>
       </c>
-      <c r="E18" s="21">
+      <c r="E18" s="54">
         <f t="shared" si="0"/>
         <v>15.911764705882353</v>
       </c>
@@ -3530,14 +4662,14 @@
       <c r="B19" s="2">
         <v>45155</v>
       </c>
-      <c r="C19" s="26">
+      <c r="C19" s="21">
         <f t="shared" si="2"/>
         <v>448</v>
       </c>
-      <c r="D19" s="20">
+      <c r="D19" s="53">
         <v>5858</v>
       </c>
-      <c r="E19" s="21">
+      <c r="E19" s="54">
         <f t="shared" si="0"/>
         <v>17.229411764705883</v>
       </c>
@@ -3550,14 +4682,14 @@
       <c r="B20" s="2">
         <v>45156</v>
       </c>
-      <c r="C20" s="26">
+      <c r="C20" s="21">
         <f t="shared" si="2"/>
         <v>419</v>
       </c>
-      <c r="D20" s="20">
+      <c r="D20" s="53">
         <v>6277</v>
       </c>
-      <c r="E20" s="21">
+      <c r="E20" s="54">
         <f t="shared" si="0"/>
         <v>18.461764705882352</v>
       </c>
@@ -3570,14 +4702,14 @@
       <c r="B21" s="2">
         <v>45159</v>
       </c>
-      <c r="C21" s="26">
+      <c r="C21" s="21">
         <f t="shared" si="2"/>
         <v>661</v>
       </c>
-      <c r="D21" s="20">
+      <c r="D21" s="53">
         <v>6938</v>
       </c>
-      <c r="E21" s="21">
+      <c r="E21" s="54">
         <f t="shared" si="0"/>
         <v>20.405882352941177</v>
       </c>
@@ -3590,14 +4722,14 @@
       <c r="B22" s="2">
         <v>45160</v>
       </c>
-      <c r="C22" s="26">
+      <c r="C22" s="21">
         <f t="shared" si="2"/>
         <v>580</v>
       </c>
-      <c r="D22" s="20">
+      <c r="D22" s="53">
         <v>7518</v>
       </c>
-      <c r="E22" s="21">
+      <c r="E22" s="54">
         <f t="shared" si="0"/>
         <v>22.111764705882354</v>
       </c>
@@ -3610,14 +4742,14 @@
       <c r="B23" s="2">
         <v>45161</v>
       </c>
-      <c r="C23" s="26">
+      <c r="C23" s="21">
         <f t="shared" si="2"/>
         <v>349</v>
       </c>
-      <c r="D23" s="20">
+      <c r="D23" s="53">
         <v>7867</v>
       </c>
-      <c r="E23" s="21">
+      <c r="E23" s="54">
         <f t="shared" si="0"/>
         <v>23.138235294117646</v>
       </c>
@@ -3630,14 +4762,14 @@
       <c r="B24" s="2">
         <v>45162</v>
       </c>
-      <c r="C24" s="26">
+      <c r="C24" s="21">
         <f t="shared" si="2"/>
         <v>154</v>
       </c>
-      <c r="D24" s="20">
+      <c r="D24" s="53">
         <v>8021</v>
       </c>
-      <c r="E24" s="21">
+      <c r="E24" s="54">
         <f t="shared" si="0"/>
         <v>23.591176470588234</v>
       </c>
@@ -3650,14 +4782,14 @@
       <c r="B25" s="2">
         <v>45163</v>
       </c>
-      <c r="C25" s="26">
+      <c r="C25" s="21">
         <f t="shared" si="2"/>
         <v>611</v>
       </c>
-      <c r="D25" s="20">
+      <c r="D25" s="53">
         <v>8632</v>
       </c>
-      <c r="E25" s="21">
+      <c r="E25" s="54">
         <f t="shared" si="0"/>
         <v>25.388235294117646</v>
       </c>
@@ -3670,14 +4802,14 @@
       <c r="B26" s="2">
         <v>45164</v>
       </c>
-      <c r="C26" s="26">
+      <c r="C26" s="21">
         <f t="shared" si="2"/>
         <v>95</v>
       </c>
-      <c r="D26" s="20">
+      <c r="D26" s="53">
         <v>8727</v>
       </c>
-      <c r="E26" s="21">
+      <c r="E26" s="54">
         <f t="shared" si="0"/>
         <v>25.66764705882353</v>
       </c>
@@ -3690,14 +4822,14 @@
       <c r="B27" s="2">
         <v>45168</v>
       </c>
-      <c r="C27" s="26">
+      <c r="C27" s="21">
         <f t="shared" si="2"/>
         <v>119</v>
       </c>
-      <c r="D27" s="20">
+      <c r="D27" s="53">
         <v>8846</v>
       </c>
-      <c r="E27" s="21">
+      <c r="E27" s="54">
         <f t="shared" si="0"/>
         <v>26.017647058823531</v>
       </c>
@@ -3710,14 +4842,14 @@
       <c r="B28" s="2">
         <v>45173</v>
       </c>
-      <c r="C28" s="26">
+      <c r="C28" s="21">
         <f t="shared" si="2"/>
         <v>217</v>
       </c>
-      <c r="D28" s="20">
+      <c r="D28" s="53">
         <v>9063</v>
       </c>
-      <c r="E28" s="21">
+      <c r="E28" s="54">
         <f t="shared" si="0"/>
         <v>26.655882352941177</v>
       </c>
@@ -3745,14 +4877,14 @@
       <c r="B29" s="2">
         <v>45174</v>
       </c>
-      <c r="C29" s="26">
+      <c r="C29" s="21">
         <f t="shared" si="2"/>
         <v>473</v>
       </c>
-      <c r="D29" s="20">
+      <c r="D29" s="53">
         <v>9536</v>
       </c>
-      <c r="E29" s="21">
+      <c r="E29" s="54">
         <f t="shared" si="0"/>
         <v>28.047058823529412</v>
       </c>
@@ -3760,9 +4892,9 @@
         <f t="shared" si="1"/>
         <v>0.56094117647058828</v>
       </c>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
       <c r="L29" t="s">
         <v>16</v>
       </c>
@@ -3770,7 +4902,7 @@
         <f t="array" ref="M29:M67">_xlfn.SORTBY(C6:C44, C6:C44, -1)</f>
         <v>1279</v>
       </c>
-      <c r="N29" s="15" cm="1">
+      <c r="N29" s="12" cm="1">
         <f t="array" ref="N29:N67">_xlfn.SORTBY(B6:B44,C6:C44, -1)</f>
         <v>45148</v>
       </c>
@@ -3791,14 +4923,14 @@
       <c r="B30" s="2">
         <v>45175</v>
       </c>
-      <c r="C30" s="26">
+      <c r="C30" s="21">
         <f t="shared" si="2"/>
         <v>220</v>
       </c>
-      <c r="D30" s="20">
+      <c r="D30" s="53">
         <v>9756</v>
       </c>
-      <c r="E30" s="21">
+      <c r="E30" s="54">
         <f t="shared" si="0"/>
         <v>28.694117647058825</v>
       </c>
@@ -3806,28 +4938,28 @@
         <f t="shared" si="1"/>
         <v>0.57388235294117651</v>
       </c>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="16"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
       <c r="L30" t="s">
         <v>17</v>
       </c>
       <c r="M30">
         <v>859</v>
       </c>
-      <c r="N30" s="15">
+      <c r="N30" s="12">
         <v>45146</v>
       </c>
       <c r="O30" t="str">
-        <f t="shared" ref="O30:O43" ca="1" si="3">IF(N30=TODAY(), "Green", "Blue")</f>
+        <f t="shared" ref="O30:O48" ca="1" si="3">IF(N30=TODAY(), "Green", "Blue")</f>
         <v>Blue</v>
       </c>
       <c r="P30">
-        <f t="shared" ref="P30:P43" ca="1" si="4">IF(NOT(N30=TODAY()), M30, "")</f>
+        <f t="shared" ref="P30:P48" ca="1" si="4">IF(NOT(N30=TODAY()), M30, "")</f>
         <v>859</v>
       </c>
       <c r="Q30" t="str">
-        <f t="shared" ref="Q30:Q43" ca="1" si="5">IF(N30=TODAY(), M30, "")</f>
+        <f t="shared" ref="Q30:Q48" ca="1" si="5">IF(N30=TODAY(), M30, "")</f>
         <v/>
       </c>
     </row>
@@ -3835,14 +4967,14 @@
       <c r="B31" s="2">
         <v>45181</v>
       </c>
-      <c r="C31" s="26">
+      <c r="C31" s="21">
         <f t="shared" si="2"/>
         <v>300</v>
       </c>
-      <c r="D31" s="20">
+      <c r="D31" s="53">
         <v>10056</v>
       </c>
-      <c r="E31" s="21">
+      <c r="E31" s="54">
         <f t="shared" si="0"/>
         <v>29.576470588235296</v>
       </c>
@@ -3850,16 +4982,16 @@
         <f t="shared" si="1"/>
         <v>0.59152941176470586</v>
       </c>
-      <c r="H31" s="16"/>
-      <c r="I31" s="16"/>
-      <c r="J31" s="16"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
       <c r="L31" t="s">
         <v>18</v>
       </c>
       <c r="M31">
         <v>729</v>
       </c>
-      <c r="N31" s="15">
+      <c r="N31" s="12">
         <v>45145</v>
       </c>
       <c r="O31" t="str">
@@ -3879,14 +5011,14 @@
       <c r="B32" s="2">
         <v>45182</v>
       </c>
-      <c r="C32" s="26">
+      <c r="C32" s="21">
         <f t="shared" si="2"/>
         <v>159</v>
       </c>
-      <c r="D32" s="20">
+      <c r="D32" s="53">
         <v>10215</v>
       </c>
-      <c r="E32" s="21">
+      <c r="E32" s="54">
         <f t="shared" si="0"/>
         <v>30.044117647058822</v>
       </c>
@@ -3894,16 +5026,16 @@
         <f t="shared" si="1"/>
         <v>0.60088235294117642</v>
       </c>
-      <c r="H32" s="16"/>
-      <c r="I32" s="16"/>
-      <c r="J32" s="16"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
       <c r="L32" t="s">
         <v>19</v>
       </c>
       <c r="M32">
         <v>661</v>
       </c>
-      <c r="N32" s="15">
+      <c r="N32" s="12">
         <v>45159</v>
       </c>
       <c r="O32" t="str">
@@ -3923,14 +5055,14 @@
       <c r="B33" s="2">
         <v>45183</v>
       </c>
-      <c r="C33" s="26">
+      <c r="C33" s="21">
         <f t="shared" si="2"/>
         <v>97</v>
       </c>
-      <c r="D33" s="20">
+      <c r="D33" s="53">
         <v>10312</v>
       </c>
-      <c r="E33" s="21">
+      <c r="E33" s="54">
         <f t="shared" si="0"/>
         <v>30.329411764705881</v>
       </c>
@@ -3938,16 +5070,16 @@
         <f t="shared" si="1"/>
         <v>0.60658823529411765</v>
       </c>
-      <c r="H33" s="16"/>
-      <c r="I33" s="16"/>
-      <c r="J33" s="16"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
       <c r="L33" t="s">
         <v>20</v>
       </c>
       <c r="M33">
         <v>657</v>
       </c>
-      <c r="N33" s="15">
+      <c r="N33" s="12">
         <v>45149</v>
       </c>
       <c r="O33" t="str">
@@ -3967,14 +5099,14 @@
       <c r="B34" s="2">
         <v>45187</v>
       </c>
-      <c r="C34" s="26">
+      <c r="C34" s="21">
         <f t="shared" si="2"/>
         <v>125</v>
       </c>
-      <c r="D34" s="20">
+      <c r="D34" s="53">
         <v>10437</v>
       </c>
-      <c r="E34" s="21">
+      <c r="E34" s="54">
         <f t="shared" si="0"/>
         <v>30.69705882352941</v>
       </c>
@@ -3982,16 +5114,16 @@
         <f t="shared" si="1"/>
         <v>0.61394117647058821</v>
       </c>
-      <c r="H34" s="16"/>
-      <c r="I34" s="16"/>
-      <c r="J34" s="16"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
       <c r="L34" t="s">
         <v>25</v>
       </c>
       <c r="M34">
         <v>611</v>
       </c>
-      <c r="N34" s="15">
+      <c r="N34" s="12">
         <v>45163</v>
       </c>
       <c r="O34" t="str">
@@ -4011,14 +5143,14 @@
       <c r="B35" s="2">
         <v>45188</v>
       </c>
-      <c r="C35" s="26">
+      <c r="C35" s="21">
         <f t="shared" si="2"/>
         <v>272</v>
       </c>
-      <c r="D35" s="20">
+      <c r="D35" s="53">
         <v>10709</v>
       </c>
-      <c r="E35" s="21">
+      <c r="E35" s="54">
         <f t="shared" si="0"/>
         <v>31.497058823529411</v>
       </c>
@@ -4026,16 +5158,16 @@
         <f t="shared" si="1"/>
         <v>0.62994117647058823</v>
       </c>
-      <c r="H35" s="16"/>
-      <c r="I35" s="16"/>
-      <c r="J35" s="16"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
       <c r="L35" t="s">
         <v>26</v>
       </c>
       <c r="M35">
         <v>603</v>
       </c>
-      <c r="N35" s="15">
+      <c r="N35" s="12">
         <v>45193</v>
       </c>
       <c r="O35" t="str">
@@ -4055,14 +5187,14 @@
       <c r="B36" s="2">
         <v>45191</v>
       </c>
-      <c r="C36" s="26">
+      <c r="C36" s="21">
         <f t="shared" si="2"/>
         <v>515</v>
       </c>
-      <c r="D36" s="20">
+      <c r="D36" s="53">
         <v>11224</v>
       </c>
-      <c r="E36" s="21">
+      <c r="E36" s="54">
         <f t="shared" si="0"/>
         <v>33.011764705882356</v>
       </c>
@@ -4070,16 +5202,16 @@
         <f t="shared" si="1"/>
         <v>0.66023529411764703</v>
       </c>
-      <c r="H36" s="16"/>
-      <c r="I36" s="16"/>
-      <c r="J36" s="16"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
       <c r="L36" t="s">
         <v>27</v>
       </c>
       <c r="M36">
         <v>580</v>
       </c>
-      <c r="N36" s="15">
+      <c r="N36" s="12">
         <v>45160</v>
       </c>
       <c r="O36" t="str">
@@ -4099,14 +5231,14 @@
       <c r="B37" s="2">
         <v>45193</v>
       </c>
-      <c r="C37" s="26">
+      <c r="C37" s="21">
         <f t="shared" si="2"/>
         <v>603</v>
       </c>
-      <c r="D37" s="20">
+      <c r="D37" s="53">
         <v>11827</v>
       </c>
-      <c r="E37" s="21">
+      <c r="E37" s="54">
         <f t="shared" si="0"/>
         <v>34.785294117647062</v>
       </c>
@@ -4114,58 +5246,58 @@
         <f t="shared" si="1"/>
         <v>0.69570588235294117</v>
       </c>
-      <c r="H37" s="16"/>
-      <c r="I37" s="16"/>
-      <c r="J37" s="16"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
       <c r="L37" t="s">
         <v>28</v>
       </c>
       <c r="M37">
-        <v>548</v>
-      </c>
-      <c r="N37" s="15">
-        <v>45208</v>
+        <v>560</v>
+      </c>
+      <c r="N37" s="12">
+        <v>45211</v>
       </c>
       <c r="O37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Blue</v>
-      </c>
-      <c r="P37">
+        <v>Green</v>
+      </c>
+      <c r="P37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>548</v>
-      </c>
-      <c r="Q37" t="str">
+        <v/>
+      </c>
+      <c r="Q37">
         <f t="shared" ca="1" si="5"/>
-        <v/>
+        <v>560</v>
       </c>
     </row>
     <row r="38" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="2">
         <v>45194</v>
       </c>
-      <c r="C38" s="26">
+      <c r="C38" s="21">
         <f t="shared" si="2"/>
         <v>375</v>
       </c>
-      <c r="D38" s="20">
+      <c r="D38" s="53">
         <v>12202</v>
       </c>
-      <c r="E38" s="21">
-        <f t="shared" ref="E38:E44" si="6">D38/$J$6</f>
+      <c r="E38" s="54">
+        <f t="shared" ref="E38:E63" si="6">D38/$J$6</f>
         <v>35.888235294117649</v>
       </c>
       <c r="F38" s="4">
-        <f t="shared" ref="F38:F44" si="7">D38/$J$8</f>
+        <f t="shared" ref="F38:F63" si="7">D38/$J$8</f>
         <v>0.71776470588235297</v>
       </c>
       <c r="L38" t="s">
         <v>29</v>
       </c>
       <c r="M38">
-        <v>515</v>
-      </c>
-      <c r="N38" s="15">
-        <v>45191</v>
+        <v>548</v>
+      </c>
+      <c r="N38" s="12">
+        <v>45208</v>
       </c>
       <c r="O38" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4173,7 +5305,7 @@
       </c>
       <c r="P38">
         <f t="shared" ca="1" si="4"/>
-        <v>515</v>
+        <v>548</v>
       </c>
       <c r="Q38" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -4184,14 +5316,14 @@
       <c r="B39" s="2">
         <v>45195</v>
       </c>
-      <c r="C39" s="26">
+      <c r="C39" s="21">
         <f t="shared" si="2"/>
         <v>143</v>
       </c>
-      <c r="D39" s="20">
+      <c r="D39" s="53">
         <v>12345</v>
       </c>
-      <c r="E39" s="21">
+      <c r="E39" s="54">
         <f t="shared" si="6"/>
         <v>36.308823529411768</v>
       </c>
@@ -4203,10 +5335,10 @@
         <v>30</v>
       </c>
       <c r="M39">
-        <v>486</v>
-      </c>
-      <c r="N39" s="15">
-        <v>45141</v>
+        <v>515</v>
+      </c>
+      <c r="N39" s="12">
+        <v>45191</v>
       </c>
       <c r="O39" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4214,7 +5346,7 @@
       </c>
       <c r="P39">
         <f t="shared" ca="1" si="4"/>
-        <v>486</v>
+        <v>515</v>
       </c>
       <c r="Q39" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -4225,14 +5357,14 @@
       <c r="B40" s="2">
         <v>45196</v>
       </c>
-      <c r="C40" s="26">
+      <c r="C40" s="21">
         <f t="shared" si="2"/>
         <v>151</v>
       </c>
-      <c r="D40" s="20">
+      <c r="D40" s="53">
         <v>12496</v>
       </c>
-      <c r="E40" s="21">
+      <c r="E40" s="54">
         <f t="shared" si="6"/>
         <v>36.752941176470586</v>
       </c>
@@ -4244,10 +5376,10 @@
         <v>31</v>
       </c>
       <c r="M40">
-        <v>473</v>
-      </c>
-      <c r="N40" s="15">
-        <v>45174</v>
+        <v>486</v>
+      </c>
+      <c r="N40" s="12">
+        <v>45141</v>
       </c>
       <c r="O40" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4255,7 +5387,7 @@
       </c>
       <c r="P40">
         <f t="shared" ca="1" si="4"/>
-        <v>473</v>
+        <v>486</v>
       </c>
       <c r="Q40" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -4266,14 +5398,14 @@
       <c r="B41" s="2">
         <v>45208</v>
       </c>
-      <c r="C41" s="26">
+      <c r="C41" s="21">
         <f>D41-D40</f>
         <v>548</v>
       </c>
-      <c r="D41" s="20">
+      <c r="D41" s="53">
         <v>13044</v>
       </c>
-      <c r="E41" s="21">
+      <c r="E41" s="54">
         <f>D41/$J$6</f>
         <v>38.364705882352943</v>
       </c>
@@ -4285,10 +5417,10 @@
         <v>32</v>
       </c>
       <c r="M41">
-        <v>467</v>
-      </c>
-      <c r="N41" s="15">
-        <v>45154</v>
+        <v>473</v>
+      </c>
+      <c r="N41" s="12">
+        <v>45174</v>
       </c>
       <c r="O41" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4296,7 +5428,7 @@
       </c>
       <c r="P41">
         <f t="shared" ca="1" si="4"/>
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="Q41" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -4307,14 +5439,14 @@
       <c r="B42" s="2">
         <v>45209</v>
       </c>
-      <c r="C42" s="26">
+      <c r="C42" s="21">
         <f>D42-D41</f>
         <v>410</v>
       </c>
-      <c r="D42" s="20">
+      <c r="D42" s="53">
         <v>13454</v>
       </c>
-      <c r="E42" s="21">
+      <c r="E42" s="54">
         <f>D42/$J$6</f>
         <v>39.570588235294117</v>
       </c>
@@ -4326,10 +5458,10 @@
         <v>33</v>
       </c>
       <c r="M42">
-        <v>448</v>
-      </c>
-      <c r="N42" s="15">
-        <v>45155</v>
+        <v>467</v>
+      </c>
+      <c r="N42" s="12">
+        <v>45154</v>
       </c>
       <c r="O42" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4337,7 +5469,7 @@
       </c>
       <c r="P42">
         <f t="shared" ca="1" si="4"/>
-        <v>448</v>
+        <v>467</v>
       </c>
       <c r="Q42" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -4348,14 +5480,14 @@
       <c r="B43" s="2">
         <v>45210</v>
       </c>
-      <c r="C43" s="26">
+      <c r="C43" s="21">
         <f>D43-D42</f>
         <v>155</v>
       </c>
-      <c r="D43" s="20">
+      <c r="D43" s="53">
         <v>13609</v>
       </c>
-      <c r="E43" s="21">
+      <c r="E43" s="54">
         <f t="shared" si="6"/>
         <v>40.026470588235291</v>
       </c>
@@ -4367,10 +5499,10 @@
         <v>34</v>
       </c>
       <c r="M43">
-        <v>419</v>
-      </c>
-      <c r="N43" s="15">
-        <v>45156</v>
+        <v>448</v>
+      </c>
+      <c r="N43" s="12">
+        <v>45155</v>
       </c>
       <c r="O43" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4378,206 +5510,497 @@
       </c>
       <c r="P43">
         <f t="shared" ca="1" si="4"/>
-        <v>419</v>
+        <v>448</v>
       </c>
       <c r="Q43" t="str">
         <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="44" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="3"/>
-      <c r="C44" s="27"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="5">
+    <row r="44" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B44" s="2">
+        <v>45211</v>
+      </c>
+      <c r="C44" s="21">
+        <f>D44-D43</f>
+        <v>560</v>
+      </c>
+      <c r="D44" s="53">
+        <v>14169</v>
+      </c>
+      <c r="E44" s="54">
+        <f t="shared" si="6"/>
+        <v>41.673529411764704</v>
+      </c>
+      <c r="F44" s="4">
+        <f t="shared" si="7"/>
+        <v>0.83347058823529407</v>
+      </c>
+      <c r="L44" t="s">
+        <v>36</v>
+      </c>
+      <c r="M44">
+        <v>419</v>
+      </c>
+      <c r="N44" s="12">
+        <v>45156</v>
+      </c>
+      <c r="O44" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>Blue</v>
+      </c>
+      <c r="P44">
+        <f t="shared" ca="1" si="4"/>
+        <v>419</v>
+      </c>
+      <c r="Q44" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B45" s="58"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="53"/>
+      <c r="E45" s="54">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F44" s="6">
+      <c r="F45" s="4">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="M44">
+      <c r="L45" t="s">
+        <v>37</v>
+      </c>
+      <c r="M45">
         <v>410</v>
       </c>
-      <c r="N44" s="15">
+      <c r="N45" s="12">
         <v>45209</v>
       </c>
-    </row>
-    <row r="45" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="M45">
+      <c r="O45" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>Blue</v>
+      </c>
+      <c r="P45">
+        <f t="shared" ca="1" si="4"/>
+        <v>410</v>
+      </c>
+      <c r="Q45" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B46" s="58"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="53"/>
+      <c r="E46" s="54">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F46" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L46" t="s">
+        <v>38</v>
+      </c>
+      <c r="M46">
         <v>375</v>
       </c>
-      <c r="N45" s="15">
+      <c r="N46" s="12">
         <v>45194</v>
       </c>
-    </row>
-    <row r="46" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="M46">
+      <c r="O46" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>Blue</v>
+      </c>
+      <c r="P46">
+        <f t="shared" ca="1" si="4"/>
+        <v>375</v>
+      </c>
+      <c r="Q46" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B47" s="58"/>
+      <c r="C47" s="21"/>
+      <c r="D47" s="53"/>
+      <c r="E47" s="54">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F47" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L47" t="s">
+        <v>39</v>
+      </c>
+      <c r="M47">
         <v>349</v>
       </c>
-      <c r="N46" s="15">
+      <c r="N47" s="12">
         <v>45161</v>
       </c>
-    </row>
-    <row r="47" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="M47">
+      <c r="O47" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>Blue</v>
+      </c>
+      <c r="P47">
+        <f t="shared" ca="1" si="4"/>
+        <v>349</v>
+      </c>
+      <c r="Q47" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B48" s="58"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="53"/>
+      <c r="E48" s="54">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F48" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="L48" t="s">
+        <v>35</v>
+      </c>
+      <c r="M48">
         <v>346</v>
       </c>
-      <c r="N47" s="15">
+      <c r="N48" s="12">
         <v>45142</v>
       </c>
-    </row>
-    <row r="48" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="M48">
+      <c r="O48" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>Blue</v>
+      </c>
+      <c r="P48">
+        <f t="shared" ca="1" si="4"/>
+        <v>346</v>
+      </c>
+      <c r="Q48" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B49" s="58"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="53"/>
+      <c r="E49" s="54">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F49" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M49">
         <v>300</v>
       </c>
-      <c r="N48" s="15">
+      <c r="N49" s="12">
         <v>45181</v>
       </c>
     </row>
-    <row r="49" spans="13:14" x14ac:dyDescent="0.2">
-      <c r="M49">
+    <row r="50" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B50" s="58"/>
+      <c r="C50" s="21"/>
+      <c r="D50" s="53"/>
+      <c r="E50" s="54">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F50" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M50">
         <v>272</v>
       </c>
-      <c r="N49" s="15">
+      <c r="N50" s="12">
         <v>45188</v>
       </c>
     </row>
-    <row r="50" spans="13:14" x14ac:dyDescent="0.2">
-      <c r="M50">
+    <row r="51" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B51" s="58"/>
+      <c r="C51" s="21"/>
+      <c r="D51" s="53"/>
+      <c r="E51" s="54">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F51" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M51">
         <v>220</v>
       </c>
-      <c r="N50" s="15">
+      <c r="N51">
         <v>45175</v>
       </c>
     </row>
-    <row r="51" spans="13:14" x14ac:dyDescent="0.2">
-      <c r="M51">
+    <row r="52" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B52" s="58"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="53"/>
+      <c r="E52" s="54">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F52" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M52">
         <v>217</v>
       </c>
-      <c r="N51">
+      <c r="N52">
         <v>45173</v>
       </c>
     </row>
-    <row r="52" spans="13:14" x14ac:dyDescent="0.2">
-      <c r="M52">
+    <row r="53" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B53" s="58"/>
+      <c r="C53" s="21"/>
+      <c r="D53" s="53"/>
+      <c r="E53" s="54">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F53" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M53">
         <v>159</v>
       </c>
-      <c r="N52">
+      <c r="N53">
         <v>45182</v>
       </c>
     </row>
-    <row r="53" spans="13:14" x14ac:dyDescent="0.2">
-      <c r="M53">
+    <row r="54" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B54" s="58"/>
+      <c r="C54" s="21"/>
+      <c r="D54" s="53"/>
+      <c r="E54" s="54">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F54" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M54">
         <v>156</v>
       </c>
-      <c r="N53">
+      <c r="N54">
         <v>45139</v>
       </c>
     </row>
-    <row r="54" spans="13:14" x14ac:dyDescent="0.2">
-      <c r="M54">
+    <row r="55" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B55" s="58"/>
+      <c r="C55" s="21"/>
+      <c r="D55" s="53"/>
+      <c r="E55" s="54">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F55" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M55">
         <v>155</v>
       </c>
-      <c r="N54">
+      <c r="N55">
         <v>45210</v>
       </c>
     </row>
-    <row r="55" spans="13:14" x14ac:dyDescent="0.2">
-      <c r="M55">
+    <row r="56" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B56" s="58"/>
+      <c r="C56" s="21"/>
+      <c r="D56" s="53"/>
+      <c r="E56" s="54">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F56" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M56">
         <v>154</v>
       </c>
-      <c r="N55">
+      <c r="N56">
         <v>45162</v>
       </c>
     </row>
-    <row r="56" spans="13:14" x14ac:dyDescent="0.2">
-      <c r="M56">
+    <row r="57" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B57" s="58"/>
+      <c r="C57" s="21"/>
+      <c r="D57" s="53"/>
+      <c r="E57" s="54">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F57" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M57">
         <v>151</v>
       </c>
-      <c r="N56">
+      <c r="N57">
         <v>45196</v>
       </c>
     </row>
-    <row r="57" spans="13:14" x14ac:dyDescent="0.2">
-      <c r="M57">
+    <row r="58" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B58" s="58"/>
+      <c r="C58" s="21"/>
+      <c r="D58" s="53"/>
+      <c r="E58" s="54">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F58" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M58">
         <v>146</v>
       </c>
-      <c r="N57">
+      <c r="N58">
         <v>45152</v>
       </c>
     </row>
-    <row r="58" spans="13:14" x14ac:dyDescent="0.2">
-      <c r="M58">
+    <row r="59" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B59" s="58"/>
+      <c r="C59" s="21"/>
+      <c r="D59" s="53"/>
+      <c r="E59" s="54">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F59" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M59">
         <v>143</v>
       </c>
-      <c r="N58">
+      <c r="N59">
         <v>45195</v>
       </c>
     </row>
-    <row r="59" spans="13:14" x14ac:dyDescent="0.2">
-      <c r="M59">
+    <row r="60" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B60" s="58"/>
+      <c r="C60" s="21"/>
+      <c r="D60" s="53"/>
+      <c r="E60" s="54">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F60" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M60">
         <v>140</v>
       </c>
-      <c r="N59">
+      <c r="N60">
         <v>45153</v>
       </c>
     </row>
-    <row r="60" spans="13:14" x14ac:dyDescent="0.2">
-      <c r="M60">
+    <row r="61" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B61" s="58"/>
+      <c r="C61" s="21"/>
+      <c r="D61" s="53"/>
+      <c r="E61" s="54">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F61" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M61">
         <v>125</v>
       </c>
-      <c r="N60">
+      <c r="N61">
         <v>45187</v>
       </c>
     </row>
-    <row r="61" spans="13:14" x14ac:dyDescent="0.2">
-      <c r="M61">
+    <row r="62" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B62" s="58"/>
+      <c r="C62" s="21"/>
+      <c r="D62" s="53"/>
+      <c r="E62" s="54">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F62" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M62">
         <v>119</v>
       </c>
-      <c r="N61">
+      <c r="N62">
         <v>45168</v>
       </c>
     </row>
-    <row r="62" spans="13:14" x14ac:dyDescent="0.2">
-      <c r="M62">
+    <row r="63" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="3"/>
+      <c r="C63" s="22"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F63" s="6">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="M63">
         <v>107</v>
       </c>
-      <c r="N62">
+      <c r="N63">
         <v>45147</v>
       </c>
     </row>
-    <row r="63" spans="13:14" x14ac:dyDescent="0.2">
-      <c r="M63">
+    <row r="64" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="M64">
         <v>97</v>
       </c>
-      <c r="N63">
+      <c r="N64">
         <v>45183</v>
-      </c>
-    </row>
-    <row r="64" spans="13:14" x14ac:dyDescent="0.2">
-      <c r="M64">
-        <v>95</v>
-      </c>
-      <c r="N64">
-        <v>45164</v>
       </c>
     </row>
     <row r="65" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M65">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="N65">
-        <v>45140</v>
+        <v>45164</v>
       </c>
     </row>
     <row r="66" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M66">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="N66">
-        <v>45138</v>
+        <v>45140</v>
       </c>
     </row>
     <row r="67" spans="13:14" x14ac:dyDescent="0.2">
@@ -4585,7 +6008,7 @@
         <v>0</v>
       </c>
       <c r="N67">
-        <v>0</v>
+        <v>45138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Plotting correction lines with eU and writing
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42EE2ED4-3747-A24D-AC09-3323C4DA872D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89518B14-5723-0E49-B3B2-7EAC8A5B01C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2180" yWindow="1300" windowWidth="15820" windowHeight="19800" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="15020" windowHeight="17040" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -948,7 +948,7 @@
                   <c:v>13609</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>14169</c:v>
+                  <c:v>14423</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1302,25 +1302,25 @@
                   <c:v>859</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>814</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>729</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>661</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>657</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>611</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>603</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>580</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>548</c:v>
@@ -1476,7 +1476,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>560</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -1901,7 +1901,7 @@
                   <c:v>155</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>560</c:v>
+                  <c:v>814</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4256,8 +4256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4213BD91-B5D1-3B47-8D3F-04331482504C}">
   <dimension ref="A1:Q67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4509,7 +4509,7 @@
       <c r="I12" s="24"/>
       <c r="J12" s="10">
         <f>J8-MAX(D6:D44)</f>
-        <v>2831</v>
+        <v>2577</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
@@ -4565,7 +4565,7 @@
       <c r="I14" s="28"/>
       <c r="J14" s="11">
         <f>J12/J13</f>
-        <v>5.7036027494666977</v>
+        <v>5.1918701114008057</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
@@ -4989,10 +4989,10 @@
         <v>18</v>
       </c>
       <c r="M31">
-        <v>729</v>
+        <v>814</v>
       </c>
       <c r="N31" s="12">
-        <v>45145</v>
+        <v>45211</v>
       </c>
       <c r="O31" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5000,7 +5000,7 @@
       </c>
       <c r="P31">
         <f t="shared" ca="1" si="4"/>
-        <v>729</v>
+        <v>814</v>
       </c>
       <c r="Q31" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5033,10 +5033,10 @@
         <v>19</v>
       </c>
       <c r="M32">
-        <v>661</v>
+        <v>729</v>
       </c>
       <c r="N32" s="12">
-        <v>45159</v>
+        <v>45145</v>
       </c>
       <c r="O32" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5044,7 +5044,7 @@
       </c>
       <c r="P32">
         <f t="shared" ca="1" si="4"/>
-        <v>661</v>
+        <v>729</v>
       </c>
       <c r="Q32" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5077,10 +5077,10 @@
         <v>20</v>
       </c>
       <c r="M33">
-        <v>657</v>
+        <v>661</v>
       </c>
       <c r="N33" s="12">
-        <v>45149</v>
+        <v>45159</v>
       </c>
       <c r="O33" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5088,7 +5088,7 @@
       </c>
       <c r="P33">
         <f t="shared" ca="1" si="4"/>
-        <v>657</v>
+        <v>661</v>
       </c>
       <c r="Q33" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5121,10 +5121,10 @@
         <v>25</v>
       </c>
       <c r="M34">
-        <v>611</v>
+        <v>657</v>
       </c>
       <c r="N34" s="12">
-        <v>45163</v>
+        <v>45149</v>
       </c>
       <c r="O34" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5132,7 +5132,7 @@
       </c>
       <c r="P34">
         <f t="shared" ca="1" si="4"/>
-        <v>611</v>
+        <v>657</v>
       </c>
       <c r="Q34" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5165,10 +5165,10 @@
         <v>26</v>
       </c>
       <c r="M35">
-        <v>603</v>
+        <v>611</v>
       </c>
       <c r="N35" s="12">
-        <v>45193</v>
+        <v>45163</v>
       </c>
       <c r="O35" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5176,7 +5176,7 @@
       </c>
       <c r="P35">
         <f t="shared" ca="1" si="4"/>
-        <v>603</v>
+        <v>611</v>
       </c>
       <c r="Q35" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5209,10 +5209,10 @@
         <v>27</v>
       </c>
       <c r="M36">
-        <v>580</v>
+        <v>603</v>
       </c>
       <c r="N36" s="12">
-        <v>45160</v>
+        <v>45193</v>
       </c>
       <c r="O36" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5220,7 +5220,7 @@
       </c>
       <c r="P36">
         <f t="shared" ca="1" si="4"/>
-        <v>580</v>
+        <v>603</v>
       </c>
       <c r="Q36" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5253,22 +5253,22 @@
         <v>28</v>
       </c>
       <c r="M37">
-        <v>560</v>
+        <v>580</v>
       </c>
       <c r="N37" s="12">
-        <v>45211</v>
+        <v>45160</v>
       </c>
       <c r="O37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Green</v>
-      </c>
-      <c r="P37" t="str">
+        <v>Blue</v>
+      </c>
+      <c r="P37">
         <f t="shared" ca="1" si="4"/>
+        <v>580</v>
+      </c>
+      <c r="Q37" t="str">
+        <f t="shared" ca="1" si="5"/>
         <v/>
-      </c>
-      <c r="Q37">
-        <f t="shared" ca="1" si="5"/>
-        <v>560</v>
       </c>
     </row>
     <row r="38" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -5523,18 +5523,18 @@
       </c>
       <c r="C44" s="21">
         <f>D44-D43</f>
-        <v>560</v>
+        <v>814</v>
       </c>
       <c r="D44" s="53">
-        <v>14169</v>
+        <v>14423</v>
       </c>
       <c r="E44" s="54">
         <f t="shared" si="6"/>
-        <v>41.673529411764704</v>
+        <v>42.420588235294119</v>
       </c>
       <c r="F44" s="4">
         <f t="shared" si="7"/>
-        <v>0.83347058823529407</v>
+        <v>0.84841176470588231</v>
       </c>
       <c r="L44" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
Counting activity estimate + tested on all significant surfaces
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89518B14-5723-0E49-B3B2-7EAC8A5B01C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{784DD6EA-0897-384E-9074-413DF661D622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="15020" windowHeight="17040" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
@@ -1785,10 +1785,10 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$7:$C$44</c:f>
+              <c:f>Sheet1!$C$7:$C$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="38"/>
+                <c:ptCount val="39"/>
                 <c:pt idx="0">
                   <c:v>156</c:v>
                 </c:pt>
@@ -1902,6 +1902,9 @@
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>814</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>143</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4256,14 +4259,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4213BD91-B5D1-3B47-8D3F-04331482504C}">
   <dimension ref="A1:Q67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="0.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" customWidth="1"/>
     <col min="5" max="6" width="12.1640625" customWidth="1"/>
@@ -4737,6 +4740,10 @@
         <f t="shared" si="1"/>
         <v>0.44223529411764706</v>
       </c>
+      <c r="M22">
+        <f>AVERAGE(C7:C44)</f>
+        <v>379.55263157894734</v>
+      </c>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B23" s="2">
@@ -5559,16 +5566,23 @@
       </c>
     </row>
     <row r="45" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B45" s="58"/>
-      <c r="C45" s="21"/>
-      <c r="D45" s="53"/>
+      <c r="B45" s="2">
+        <v>45212</v>
+      </c>
+      <c r="C45" s="21">
+        <f>D45-D44</f>
+        <v>143</v>
+      </c>
+      <c r="D45" s="53">
+        <v>14566</v>
+      </c>
       <c r="E45" s="54">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>42.841176470588238</v>
       </c>
       <c r="F45" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>0.85682352941176465</v>
       </c>
       <c r="L45" t="s">
         <v>37</v>
@@ -5593,16 +5607,23 @@
       </c>
     </row>
     <row r="46" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B46" s="58"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="53"/>
+      <c r="B46" s="2">
+        <v>45213</v>
+      </c>
+      <c r="C46" s="21">
+        <f>D46-D45</f>
+        <v>0</v>
+      </c>
+      <c r="D46" s="53">
+        <v>14566</v>
+      </c>
       <c r="E46" s="54">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>42.841176470588238</v>
       </c>
       <c r="F46" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>0.85682352941176465</v>
       </c>
       <c r="L46" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
GREAT plot for best molar fraction at each potential
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{784DD6EA-0897-384E-9074-413DF661D622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233212E3-B0C1-D043-9F71-7C5150939DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="15020" windowHeight="17040" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
@@ -4259,8 +4259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4213BD91-B5D1-3B47-8D3F-04331482504C}">
   <dimension ref="A1:Q67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5608,22 +5608,22 @@
     </row>
     <row r="46" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B46" s="2">
-        <v>45213</v>
+        <v>45216</v>
       </c>
       <c r="C46" s="21">
         <f>D46-D45</f>
-        <v>0</v>
+        <v>1434</v>
       </c>
       <c r="D46" s="53">
-        <v>14566</v>
+        <v>16000</v>
       </c>
       <c r="E46" s="54">
         <f t="shared" si="6"/>
-        <v>42.841176470588238</v>
+        <v>47.058823529411768</v>
       </c>
       <c r="F46" s="4">
         <f t="shared" si="7"/>
-        <v>0.85682352941176465</v>
+        <v>0.94117647058823528</v>
       </c>
       <c r="L46" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
Fixed everything + writing up to page 7
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,20 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63929FB6-32DE-B84C-BF61-E62B66381EB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D705B43-64F1-DB4D-AA4E-8867CC160B87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="15420" windowHeight="17040" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="15420" windowHeight="16940" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$C$7:$C$44</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$C$7:$C$44</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$C$7:$C$44</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$C$7:$C$44</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$C$7:$C$44</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -490,6 +483,18 @@
     <xf numFmtId="165" fontId="0" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -580,18 +585,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -703,10 +696,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$6:$B$44</c:f>
+              <c:f>Sheet1!$B$6:$B$63</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="0">
                   <c:v>45138</c:v>
                 </c:pt>
@@ -823,16 +816,25 @@
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>45211</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>45212</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>45218</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>45219</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$6:$D$44</c:f>
+              <c:f>Sheet1!$D$6:$D$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="58"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -949,6 +951,15 @@
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>14423</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>14566</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>13793</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>14035</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4259,7 +4270,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4213BD91-B5D1-3B47-8D3F-04331482504C}">
   <dimension ref="A1:Q67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
@@ -4276,68 +4287,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="31"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="37"/>
     </row>
     <row r="2" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="32"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="34"/>
+      <c r="A2" s="38"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="40"/>
     </row>
     <row r="3" spans="1:17" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35"/>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="37"/>
+      <c r="A3" s="41"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="43"/>
     </row>
     <row r="4" spans="1:17" ht="5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:17" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="56" t="s">
+      <c r="D5" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="56" t="s">
+      <c r="E5" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="57" t="s">
+      <c r="F5" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="38" t="s">
+      <c r="H5" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="39"/>
-      <c r="J5" s="40"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="46"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B6" s="14">
@@ -4357,10 +4368,10 @@
         <f>D6/$J$8</f>
         <v>0</v>
       </c>
-      <c r="H6" s="41" t="s">
+      <c r="H6" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="42"/>
+      <c r="I6" s="48"/>
       <c r="J6" s="8">
         <v>340</v>
       </c>
@@ -4372,10 +4383,10 @@
       <c r="C7" s="21">
         <v>156</v>
       </c>
-      <c r="D7" s="53">
+      <c r="D7" s="23">
         <v>156</v>
       </c>
-      <c r="E7" s="54">
+      <c r="E7" s="24">
         <f t="shared" ref="E7:E37" si="0">D7/$J$6</f>
         <v>0.45882352941176469</v>
       </c>
@@ -4383,10 +4394,10 @@
         <f t="shared" ref="F7:F37" si="1">D7/$J$8</f>
         <v>9.1764705882352946E-3</v>
       </c>
-      <c r="H7" s="43" t="s">
+      <c r="H7" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="44"/>
+      <c r="I7" s="50"/>
       <c r="J7" s="8">
         <v>50</v>
       </c>
@@ -4399,10 +4410,10 @@
         <f t="shared" ref="C8:C40" si="2">D8-D7</f>
         <v>38</v>
       </c>
-      <c r="D8" s="53">
+      <c r="D8" s="23">
         <v>194</v>
       </c>
-      <c r="E8" s="54">
+      <c r="E8" s="24">
         <f t="shared" si="0"/>
         <v>0.57058823529411762</v>
       </c>
@@ -4410,10 +4421,10 @@
         <f t="shared" si="1"/>
         <v>1.1411764705882352E-2</v>
       </c>
-      <c r="H8" s="45" t="s">
+      <c r="H8" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="46"/>
+      <c r="I8" s="52"/>
       <c r="J8" s="9">
         <f>J6*J7</f>
         <v>17000</v>
@@ -4427,10 +4438,10 @@
         <f t="shared" si="2"/>
         <v>486</v>
       </c>
-      <c r="D9" s="53">
+      <c r="D9" s="23">
         <v>680</v>
       </c>
-      <c r="E9" s="54">
+      <c r="E9" s="24">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -4447,10 +4458,10 @@
         <f t="shared" si="2"/>
         <v>346</v>
       </c>
-      <c r="D10" s="53">
+      <c r="D10" s="23">
         <v>1026</v>
       </c>
-      <c r="E10" s="54">
+      <c r="E10" s="24">
         <f t="shared" si="0"/>
         <v>3.0176470588235293</v>
       </c>
@@ -4458,11 +4469,11 @@
         <f t="shared" si="1"/>
         <v>6.0352941176470588E-2</v>
       </c>
-      <c r="H10" s="47" t="s">
+      <c r="H10" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="48"/>
-      <c r="J10" s="49"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="55"/>
     </row>
     <row r="11" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
@@ -4472,10 +4483,10 @@
         <f t="shared" si="2"/>
         <v>729</v>
       </c>
-      <c r="D11" s="53">
+      <c r="D11" s="23">
         <v>1755</v>
       </c>
-      <c r="E11" s="54">
+      <c r="E11" s="24">
         <f t="shared" si="0"/>
         <v>5.1617647058823533</v>
       </c>
@@ -4483,9 +4494,9 @@
         <f t="shared" si="1"/>
         <v>0.10323529411764706</v>
       </c>
-      <c r="H11" s="50"/>
-      <c r="I11" s="51"/>
-      <c r="J11" s="52"/>
+      <c r="H11" s="56"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="58"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B12" s="2">
@@ -4495,10 +4506,10 @@
         <f t="shared" si="2"/>
         <v>859</v>
       </c>
-      <c r="D12" s="53">
+      <c r="D12" s="23">
         <v>2614</v>
       </c>
-      <c r="E12" s="54">
+      <c r="E12" s="24">
         <f t="shared" si="0"/>
         <v>7.6882352941176473</v>
       </c>
@@ -4506,10 +4517,10 @@
         <f t="shared" si="1"/>
         <v>0.15376470588235294</v>
       </c>
-      <c r="H12" s="23" t="s">
+      <c r="H12" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="I12" s="24"/>
+      <c r="I12" s="30"/>
       <c r="J12" s="10">
         <f>J8-MAX(D6:D44)</f>
         <v>2577</v>
@@ -4523,10 +4534,10 @@
         <f t="shared" si="2"/>
         <v>107</v>
       </c>
-      <c r="D13" s="53">
+      <c r="D13" s="23">
         <v>2721</v>
       </c>
-      <c r="E13" s="54">
+      <c r="E13" s="24">
         <f t="shared" si="0"/>
         <v>8.0029411764705891</v>
       </c>
@@ -4534,10 +4545,10 @@
         <f t="shared" si="1"/>
         <v>0.16005882352941175</v>
       </c>
-      <c r="H13" s="25" t="s">
+      <c r="H13" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="26"/>
+      <c r="I13" s="32"/>
       <c r="J13" s="10">
         <f>AVERAGE(C9:C25)</f>
         <v>496.35294117647061</v>
@@ -4551,10 +4562,10 @@
         <f t="shared" si="2"/>
         <v>1279</v>
       </c>
-      <c r="D14" s="53">
+      <c r="D14" s="23">
         <v>4000</v>
       </c>
-      <c r="E14" s="54">
+      <c r="E14" s="24">
         <f t="shared" si="0"/>
         <v>11.764705882352942</v>
       </c>
@@ -4562,10 +4573,10 @@
         <f t="shared" si="1"/>
         <v>0.23529411764705882</v>
       </c>
-      <c r="H14" s="27" t="s">
+      <c r="H14" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="I14" s="28"/>
+      <c r="I14" s="34"/>
       <c r="J14" s="11">
         <f>J12/J13</f>
         <v>5.1918701114008057</v>
@@ -4579,10 +4590,10 @@
         <f t="shared" si="2"/>
         <v>657</v>
       </c>
-      <c r="D15" s="53">
+      <c r="D15" s="23">
         <v>4657</v>
       </c>
-      <c r="E15" s="54">
+      <c r="E15" s="24">
         <f t="shared" si="0"/>
         <v>13.697058823529412</v>
       </c>
@@ -4608,10 +4619,10 @@
         <f t="shared" si="2"/>
         <v>146</v>
       </c>
-      <c r="D16" s="53">
+      <c r="D16" s="23">
         <v>4803</v>
       </c>
-      <c r="E16" s="54">
+      <c r="E16" s="24">
         <f t="shared" si="0"/>
         <v>14.126470588235295</v>
       </c>
@@ -4629,10 +4640,10 @@
         <f t="shared" si="2"/>
         <v>140</v>
       </c>
-      <c r="D17" s="53">
+      <c r="D17" s="23">
         <v>4943</v>
       </c>
-      <c r="E17" s="54">
+      <c r="E17" s="24">
         <f t="shared" si="0"/>
         <v>14.538235294117648</v>
       </c>
@@ -4649,10 +4660,10 @@
         <f t="shared" si="2"/>
         <v>467</v>
       </c>
-      <c r="D18" s="53">
+      <c r="D18" s="23">
         <v>5410</v>
       </c>
-      <c r="E18" s="54">
+      <c r="E18" s="24">
         <f t="shared" si="0"/>
         <v>15.911764705882353</v>
       </c>
@@ -4669,10 +4680,10 @@
         <f t="shared" si="2"/>
         <v>448</v>
       </c>
-      <c r="D19" s="53">
+      <c r="D19" s="23">
         <v>5858</v>
       </c>
-      <c r="E19" s="54">
+      <c r="E19" s="24">
         <f t="shared" si="0"/>
         <v>17.229411764705883</v>
       </c>
@@ -4689,10 +4700,10 @@
         <f t="shared" si="2"/>
         <v>419</v>
       </c>
-      <c r="D20" s="53">
+      <c r="D20" s="23">
         <v>6277</v>
       </c>
-      <c r="E20" s="54">
+      <c r="E20" s="24">
         <f t="shared" si="0"/>
         <v>18.461764705882352</v>
       </c>
@@ -4709,10 +4720,10 @@
         <f t="shared" si="2"/>
         <v>661</v>
       </c>
-      <c r="D21" s="53">
+      <c r="D21" s="23">
         <v>6938</v>
       </c>
-      <c r="E21" s="54">
+      <c r="E21" s="24">
         <f t="shared" si="0"/>
         <v>20.405882352941177</v>
       </c>
@@ -4729,10 +4740,10 @@
         <f t="shared" si="2"/>
         <v>580</v>
       </c>
-      <c r="D22" s="53">
+      <c r="D22" s="23">
         <v>7518</v>
       </c>
-      <c r="E22" s="54">
+      <c r="E22" s="24">
         <f t="shared" si="0"/>
         <v>22.111764705882354</v>
       </c>
@@ -4753,10 +4764,10 @@
         <f t="shared" si="2"/>
         <v>349</v>
       </c>
-      <c r="D23" s="53">
+      <c r="D23" s="23">
         <v>7867</v>
       </c>
-      <c r="E23" s="54">
+      <c r="E23" s="24">
         <f t="shared" si="0"/>
         <v>23.138235294117646</v>
       </c>
@@ -4773,10 +4784,10 @@
         <f t="shared" si="2"/>
         <v>154</v>
       </c>
-      <c r="D24" s="53">
+      <c r="D24" s="23">
         <v>8021</v>
       </c>
-      <c r="E24" s="54">
+      <c r="E24" s="24">
         <f t="shared" si="0"/>
         <v>23.591176470588234</v>
       </c>
@@ -4793,10 +4804,10 @@
         <f t="shared" si="2"/>
         <v>611</v>
       </c>
-      <c r="D25" s="53">
+      <c r="D25" s="23">
         <v>8632</v>
       </c>
-      <c r="E25" s="54">
+      <c r="E25" s="24">
         <f t="shared" si="0"/>
         <v>25.388235294117646</v>
       </c>
@@ -4813,10 +4824,10 @@
         <f t="shared" si="2"/>
         <v>95</v>
       </c>
-      <c r="D26" s="53">
+      <c r="D26" s="23">
         <v>8727</v>
       </c>
-      <c r="E26" s="54">
+      <c r="E26" s="24">
         <f t="shared" si="0"/>
         <v>25.66764705882353</v>
       </c>
@@ -4833,10 +4844,10 @@
         <f t="shared" si="2"/>
         <v>119</v>
       </c>
-      <c r="D27" s="53">
+      <c r="D27" s="23">
         <v>8846</v>
       </c>
-      <c r="E27" s="54">
+      <c r="E27" s="24">
         <f t="shared" si="0"/>
         <v>26.017647058823531</v>
       </c>
@@ -4853,10 +4864,10 @@
         <f t="shared" si="2"/>
         <v>217</v>
       </c>
-      <c r="D28" s="53">
+      <c r="D28" s="23">
         <v>9063</v>
       </c>
-      <c r="E28" s="54">
+      <c r="E28" s="24">
         <f t="shared" si="0"/>
         <v>26.655882352941177</v>
       </c>
@@ -4888,10 +4899,10 @@
         <f t="shared" si="2"/>
         <v>473</v>
       </c>
-      <c r="D29" s="53">
+      <c r="D29" s="23">
         <v>9536</v>
       </c>
-      <c r="E29" s="54">
+      <c r="E29" s="24">
         <f t="shared" si="0"/>
         <v>28.047058823529412</v>
       </c>
@@ -4934,10 +4945,10 @@
         <f t="shared" si="2"/>
         <v>220</v>
       </c>
-      <c r="D30" s="53">
+      <c r="D30" s="23">
         <v>9756</v>
       </c>
-      <c r="E30" s="54">
+      <c r="E30" s="24">
         <f t="shared" si="0"/>
         <v>28.694117647058825</v>
       </c>
@@ -4978,10 +4989,10 @@
         <f t="shared" si="2"/>
         <v>300</v>
       </c>
-      <c r="D31" s="53">
+      <c r="D31" s="23">
         <v>10056</v>
       </c>
-      <c r="E31" s="54">
+      <c r="E31" s="24">
         <f t="shared" si="0"/>
         <v>29.576470588235296</v>
       </c>
@@ -5022,10 +5033,10 @@
         <f t="shared" si="2"/>
         <v>159</v>
       </c>
-      <c r="D32" s="53">
+      <c r="D32" s="23">
         <v>10215</v>
       </c>
-      <c r="E32" s="54">
+      <c r="E32" s="24">
         <f t="shared" si="0"/>
         <v>30.044117647058822</v>
       </c>
@@ -5066,10 +5077,10 @@
         <f t="shared" si="2"/>
         <v>97</v>
       </c>
-      <c r="D33" s="53">
+      <c r="D33" s="23">
         <v>10312</v>
       </c>
-      <c r="E33" s="54">
+      <c r="E33" s="24">
         <f t="shared" si="0"/>
         <v>30.329411764705881</v>
       </c>
@@ -5110,10 +5121,10 @@
         <f t="shared" si="2"/>
         <v>125</v>
       </c>
-      <c r="D34" s="53">
+      <c r="D34" s="23">
         <v>10437</v>
       </c>
-      <c r="E34" s="54">
+      <c r="E34" s="24">
         <f t="shared" si="0"/>
         <v>30.69705882352941</v>
       </c>
@@ -5154,10 +5165,10 @@
         <f t="shared" si="2"/>
         <v>272</v>
       </c>
-      <c r="D35" s="53">
+      <c r="D35" s="23">
         <v>10709</v>
       </c>
-      <c r="E35" s="54">
+      <c r="E35" s="24">
         <f t="shared" si="0"/>
         <v>31.497058823529411</v>
       </c>
@@ -5198,10 +5209,10 @@
         <f t="shared" si="2"/>
         <v>515</v>
       </c>
-      <c r="D36" s="53">
+      <c r="D36" s="23">
         <v>11224</v>
       </c>
-      <c r="E36" s="54">
+      <c r="E36" s="24">
         <f t="shared" si="0"/>
         <v>33.011764705882356</v>
       </c>
@@ -5242,10 +5253,10 @@
         <f t="shared" si="2"/>
         <v>603</v>
       </c>
-      <c r="D37" s="53">
+      <c r="D37" s="23">
         <v>11827</v>
       </c>
-      <c r="E37" s="54">
+      <c r="E37" s="24">
         <f t="shared" si="0"/>
         <v>34.785294117647062</v>
       </c>
@@ -5286,10 +5297,10 @@
         <f t="shared" si="2"/>
         <v>375</v>
       </c>
-      <c r="D38" s="53">
+      <c r="D38" s="23">
         <v>12202</v>
       </c>
-      <c r="E38" s="54">
+      <c r="E38" s="24">
         <f t="shared" ref="E38:E63" si="6">D38/$J$6</f>
         <v>35.888235294117649</v>
       </c>
@@ -5327,10 +5338,10 @@
         <f t="shared" si="2"/>
         <v>143</v>
       </c>
-      <c r="D39" s="53">
+      <c r="D39" s="23">
         <v>12345</v>
       </c>
-      <c r="E39" s="54">
+      <c r="E39" s="24">
         <f t="shared" si="6"/>
         <v>36.308823529411768</v>
       </c>
@@ -5368,10 +5379,10 @@
         <f t="shared" si="2"/>
         <v>151</v>
       </c>
-      <c r="D40" s="53">
+      <c r="D40" s="23">
         <v>12496</v>
       </c>
-      <c r="E40" s="54">
+      <c r="E40" s="24">
         <f t="shared" si="6"/>
         <v>36.752941176470586</v>
       </c>
@@ -5406,13 +5417,13 @@
         <v>45208</v>
       </c>
       <c r="C41" s="21">
-        <f>D41-D40</f>
+        <f t="shared" ref="C41:C47" si="8">D41-D40</f>
         <v>548</v>
       </c>
-      <c r="D41" s="53">
+      <c r="D41" s="23">
         <v>13044</v>
       </c>
-      <c r="E41" s="54">
+      <c r="E41" s="24">
         <f>D41/$J$6</f>
         <v>38.364705882352943</v>
       </c>
@@ -5447,13 +5458,13 @@
         <v>45209</v>
       </c>
       <c r="C42" s="21">
-        <f>D42-D41</f>
+        <f t="shared" si="8"/>
         <v>410</v>
       </c>
-      <c r="D42" s="53">
+      <c r="D42" s="23">
         <v>13454</v>
       </c>
-      <c r="E42" s="54">
+      <c r="E42" s="24">
         <f>D42/$J$6</f>
         <v>39.570588235294117</v>
       </c>
@@ -5488,13 +5499,13 @@
         <v>45210</v>
       </c>
       <c r="C43" s="21">
-        <f>D43-D42</f>
+        <f t="shared" si="8"/>
         <v>155</v>
       </c>
-      <c r="D43" s="53">
+      <c r="D43" s="23">
         <v>13609</v>
       </c>
-      <c r="E43" s="54">
+      <c r="E43" s="24">
         <f t="shared" si="6"/>
         <v>40.026470588235291</v>
       </c>
@@ -5529,13 +5540,13 @@
         <v>45211</v>
       </c>
       <c r="C44" s="21">
-        <f>D44-D43</f>
+        <f t="shared" si="8"/>
         <v>814</v>
       </c>
-      <c r="D44" s="53">
+      <c r="D44" s="23">
         <v>14423</v>
       </c>
-      <c r="E44" s="54">
+      <c r="E44" s="24">
         <f t="shared" si="6"/>
         <v>42.420588235294119</v>
       </c>
@@ -5570,13 +5581,13 @@
         <v>45212</v>
       </c>
       <c r="C45" s="21">
-        <f>D45-D44</f>
+        <f t="shared" si="8"/>
         <v>143</v>
       </c>
-      <c r="D45" s="53">
+      <c r="D45" s="23">
         <v>14566</v>
       </c>
-      <c r="E45" s="54">
+      <c r="E45" s="24">
         <f t="shared" si="6"/>
         <v>42.841176470588238</v>
       </c>
@@ -5608,22 +5619,22 @@
     </row>
     <row r="46" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B46" s="2">
-        <v>45216</v>
+        <v>45218</v>
       </c>
       <c r="C46" s="21">
-        <f>D46-D45</f>
-        <v>-89</v>
-      </c>
-      <c r="D46" s="53">
-        <v>14477</v>
-      </c>
-      <c r="E46" s="54">
+        <f t="shared" si="8"/>
+        <v>-773</v>
+      </c>
+      <c r="D46" s="23">
+        <v>13793</v>
+      </c>
+      <c r="E46" s="24">
         <f t="shared" si="6"/>
-        <v>42.579411764705881</v>
+        <v>40.567647058823532</v>
       </c>
       <c r="F46" s="4">
         <f t="shared" si="7"/>
-        <v>0.85158823529411765</v>
+        <v>0.81135294117647061</v>
       </c>
       <c r="L46" t="s">
         <v>38</v>
@@ -5648,16 +5659,23 @@
       </c>
     </row>
     <row r="47" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B47" s="58"/>
-      <c r="C47" s="21"/>
-      <c r="D47" s="53"/>
-      <c r="E47" s="54">
+      <c r="B47" s="2">
+        <v>45219</v>
+      </c>
+      <c r="C47" s="21">
+        <f t="shared" si="8"/>
+        <v>242</v>
+      </c>
+      <c r="D47" s="23">
+        <v>14035</v>
+      </c>
+      <c r="E47" s="24">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>41.279411764705884</v>
       </c>
       <c r="F47" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>0.82558823529411762</v>
       </c>
       <c r="L47" t="s">
         <v>39</v>
@@ -5682,10 +5700,10 @@
       </c>
     </row>
     <row r="48" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B48" s="58"/>
+      <c r="B48" s="28"/>
       <c r="C48" s="21"/>
-      <c r="D48" s="53"/>
-      <c r="E48" s="54">
+      <c r="D48" s="23"/>
+      <c r="E48" s="24">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -5716,10 +5734,10 @@
       </c>
     </row>
     <row r="49" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B49" s="58"/>
+      <c r="B49" s="28"/>
       <c r="C49" s="21"/>
-      <c r="D49" s="53"/>
-      <c r="E49" s="54">
+      <c r="D49" s="23"/>
+      <c r="E49" s="24">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -5735,10 +5753,10 @@
       </c>
     </row>
     <row r="50" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B50" s="58"/>
+      <c r="B50" s="28"/>
       <c r="C50" s="21"/>
-      <c r="D50" s="53"/>
-      <c r="E50" s="54">
+      <c r="D50" s="23"/>
+      <c r="E50" s="24">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -5754,10 +5772,10 @@
       </c>
     </row>
     <row r="51" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B51" s="58"/>
+      <c r="B51" s="28"/>
       <c r="C51" s="21"/>
-      <c r="D51" s="53"/>
-      <c r="E51" s="54">
+      <c r="D51" s="23"/>
+      <c r="E51" s="24">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -5773,10 +5791,10 @@
       </c>
     </row>
     <row r="52" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B52" s="58"/>
+      <c r="B52" s="28"/>
       <c r="C52" s="21"/>
-      <c r="D52" s="53"/>
-      <c r="E52" s="54">
+      <c r="D52" s="23"/>
+      <c r="E52" s="24">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -5792,10 +5810,10 @@
       </c>
     </row>
     <row r="53" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B53" s="58"/>
+      <c r="B53" s="28"/>
       <c r="C53" s="21"/>
-      <c r="D53" s="53"/>
-      <c r="E53" s="54">
+      <c r="D53" s="23"/>
+      <c r="E53" s="24">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -5811,10 +5829,10 @@
       </c>
     </row>
     <row r="54" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B54" s="58"/>
+      <c r="B54" s="28"/>
       <c r="C54" s="21"/>
-      <c r="D54" s="53"/>
-      <c r="E54" s="54">
+      <c r="D54" s="23"/>
+      <c r="E54" s="24">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -5830,10 +5848,10 @@
       </c>
     </row>
     <row r="55" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B55" s="58"/>
+      <c r="B55" s="28"/>
       <c r="C55" s="21"/>
-      <c r="D55" s="53"/>
-      <c r="E55" s="54">
+      <c r="D55" s="23"/>
+      <c r="E55" s="24">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -5849,10 +5867,10 @@
       </c>
     </row>
     <row r="56" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B56" s="58"/>
+      <c r="B56" s="28"/>
       <c r="C56" s="21"/>
-      <c r="D56" s="53"/>
-      <c r="E56" s="54">
+      <c r="D56" s="23"/>
+      <c r="E56" s="24">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -5868,10 +5886,10 @@
       </c>
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B57" s="58"/>
+      <c r="B57" s="28"/>
       <c r="C57" s="21"/>
-      <c r="D57" s="53"/>
-      <c r="E57" s="54">
+      <c r="D57" s="23"/>
+      <c r="E57" s="24">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -5887,10 +5905,10 @@
       </c>
     </row>
     <row r="58" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B58" s="58"/>
+      <c r="B58" s="28"/>
       <c r="C58" s="21"/>
-      <c r="D58" s="53"/>
-      <c r="E58" s="54">
+      <c r="D58" s="23"/>
+      <c r="E58" s="24">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -5906,10 +5924,10 @@
       </c>
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B59" s="58"/>
+      <c r="B59" s="28"/>
       <c r="C59" s="21"/>
-      <c r="D59" s="53"/>
-      <c r="E59" s="54">
+      <c r="D59" s="23"/>
+      <c r="E59" s="24">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -5925,10 +5943,10 @@
       </c>
     </row>
     <row r="60" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B60" s="58"/>
+      <c r="B60" s="28"/>
       <c r="C60" s="21"/>
-      <c r="D60" s="53"/>
-      <c r="E60" s="54">
+      <c r="D60" s="23"/>
+      <c r="E60" s="24">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -5944,10 +5962,10 @@
       </c>
     </row>
     <row r="61" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B61" s="58"/>
+      <c r="B61" s="28"/>
       <c r="C61" s="21"/>
-      <c r="D61" s="53"/>
-      <c r="E61" s="54">
+      <c r="D61" s="23"/>
+      <c r="E61" s="24">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -5963,10 +5981,10 @@
       </c>
     </row>
     <row r="62" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B62" s="58"/>
+      <c r="B62" s="28"/>
       <c r="C62" s="21"/>
-      <c r="D62" s="53"/>
-      <c r="E62" s="54">
+      <c r="D62" s="23"/>
+      <c r="E62" s="24">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Fixed "Fuel Cells" section, halfway through "Formic Acid"
It took me half a day, and I got through 11 pages and I even wrote 1.5 page and fixed 2 figures. This pace seems to be satisfactory, even though I have 16 sections left for 10 days
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D705B43-64F1-DB4D-AA4E-8867CC160B87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18512928-91AC-934E-A187-5082891673A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="15420" windowHeight="16940" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="15080" windowHeight="16940" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -959,7 +959,7 @@
                   <c:v>13793</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>14035</c:v>
+                  <c:v>14368</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1334,37 +1334,37 @@
                   <c:v>580</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>575</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>548</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>515</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>486</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>473</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>467</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>448</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>419</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>410</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>375</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>349</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>346</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1796,10 +1796,10 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$7:$C$45</c:f>
+              <c:f>Sheet1!$C$7:$C$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>156</c:v>
                 </c:pt>
@@ -1916,6 +1916,12 @@
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-773</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>575</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3875,15 +3881,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>21171</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>7941</xdr:rowOff>
+      <xdr:colOff>42337</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>145523</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>521233</xdr:colOff>
+      <xdr:colOff>542399</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>127001</xdr:rowOff>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3898,7 +3904,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8022171" y="5532441"/>
+          <a:off x="7852837" y="5468940"/>
           <a:ext cx="5453062" cy="8183560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4268,9 +4274,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4213BD91-B5D1-3B47-8D3F-04331482504C}">
-  <dimension ref="A1:Q67"/>
+  <dimension ref="A1:Q86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
@@ -4917,11 +4923,11 @@
         <v>16</v>
       </c>
       <c r="M29" cm="1">
-        <f t="array" ref="M29:M67">_xlfn.SORTBY(C6:C44, C6:C44, -1)</f>
+        <f t="array" ref="M29:M86">_xlfn.SORTBY(C6:C63, C6:C63, -1)</f>
         <v>1279</v>
       </c>
       <c r="N29" s="12" cm="1">
-        <f t="array" ref="N29:N67">_xlfn.SORTBY(B6:B44,C6:C44, -1)</f>
+        <f t="array" ref="N29:N70">_xlfn.SORTBY(B6:B47,C6:C47, -1)</f>
         <v>45148</v>
       </c>
       <c r="O29" t="str">
@@ -5312,10 +5318,10 @@
         <v>29</v>
       </c>
       <c r="M38">
-        <v>548</v>
+        <v>575</v>
       </c>
       <c r="N38" s="12">
-        <v>45208</v>
+        <v>45219</v>
       </c>
       <c r="O38" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5323,7 +5329,7 @@
       </c>
       <c r="P38">
         <f t="shared" ca="1" si="4"/>
-        <v>548</v>
+        <v>575</v>
       </c>
       <c r="Q38" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5353,10 +5359,10 @@
         <v>30</v>
       </c>
       <c r="M39">
-        <v>515</v>
+        <v>548</v>
       </c>
       <c r="N39" s="12">
-        <v>45191</v>
+        <v>45208</v>
       </c>
       <c r="O39" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5364,7 +5370,7 @@
       </c>
       <c r="P39">
         <f t="shared" ca="1" si="4"/>
-        <v>515</v>
+        <v>548</v>
       </c>
       <c r="Q39" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5394,10 +5400,10 @@
         <v>31</v>
       </c>
       <c r="M40">
-        <v>486</v>
+        <v>515</v>
       </c>
       <c r="N40" s="12">
-        <v>45141</v>
+        <v>45191</v>
       </c>
       <c r="O40" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5405,7 +5411,7 @@
       </c>
       <c r="P40">
         <f t="shared" ca="1" si="4"/>
-        <v>486</v>
+        <v>515</v>
       </c>
       <c r="Q40" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5435,10 +5441,10 @@
         <v>32</v>
       </c>
       <c r="M41">
-        <v>473</v>
+        <v>486</v>
       </c>
       <c r="N41" s="12">
-        <v>45174</v>
+        <v>45141</v>
       </c>
       <c r="O41" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5446,7 +5452,7 @@
       </c>
       <c r="P41">
         <f t="shared" ca="1" si="4"/>
-        <v>473</v>
+        <v>486</v>
       </c>
       <c r="Q41" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5476,10 +5482,10 @@
         <v>33</v>
       </c>
       <c r="M42">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="N42" s="12">
-        <v>45154</v>
+        <v>45174</v>
       </c>
       <c r="O42" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5487,7 +5493,7 @@
       </c>
       <c r="P42">
         <f t="shared" ca="1" si="4"/>
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="Q42" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5517,10 +5523,10 @@
         <v>34</v>
       </c>
       <c r="M43">
-        <v>448</v>
+        <v>467</v>
       </c>
       <c r="N43" s="12">
-        <v>45155</v>
+        <v>45154</v>
       </c>
       <c r="O43" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5528,7 +5534,7 @@
       </c>
       <c r="P43">
         <f t="shared" ca="1" si="4"/>
-        <v>448</v>
+        <v>467</v>
       </c>
       <c r="Q43" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5558,10 +5564,10 @@
         <v>36</v>
       </c>
       <c r="M44">
-        <v>419</v>
+        <v>448</v>
       </c>
       <c r="N44" s="12">
-        <v>45156</v>
+        <v>45155</v>
       </c>
       <c r="O44" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5569,7 +5575,7 @@
       </c>
       <c r="P44">
         <f t="shared" ca="1" si="4"/>
-        <v>419</v>
+        <v>448</v>
       </c>
       <c r="Q44" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5599,10 +5605,10 @@
         <v>37</v>
       </c>
       <c r="M45">
-        <v>410</v>
+        <v>419</v>
       </c>
       <c r="N45" s="12">
-        <v>45209</v>
+        <v>45156</v>
       </c>
       <c r="O45" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5610,7 +5616,7 @@
       </c>
       <c r="P45">
         <f t="shared" ca="1" si="4"/>
-        <v>410</v>
+        <v>419</v>
       </c>
       <c r="Q45" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5640,10 +5646,10 @@
         <v>38</v>
       </c>
       <c r="M46">
-        <v>375</v>
+        <v>410</v>
       </c>
       <c r="N46" s="12">
-        <v>45194</v>
+        <v>45209</v>
       </c>
       <c r="O46" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5651,7 +5657,7 @@
       </c>
       <c r="P46">
         <f t="shared" ca="1" si="4"/>
-        <v>375</v>
+        <v>410</v>
       </c>
       <c r="Q46" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5664,27 +5670,27 @@
       </c>
       <c r="C47" s="21">
         <f t="shared" si="8"/>
-        <v>242</v>
+        <v>575</v>
       </c>
       <c r="D47" s="23">
-        <v>14035</v>
+        <v>14368</v>
       </c>
       <c r="E47" s="24">
         <f t="shared" si="6"/>
-        <v>41.279411764705884</v>
+        <v>42.258823529411764</v>
       </c>
       <c r="F47" s="4">
         <f t="shared" si="7"/>
-        <v>0.82558823529411762</v>
+        <v>0.84517647058823531</v>
       </c>
       <c r="L47" t="s">
         <v>39</v>
       </c>
       <c r="M47">
-        <v>349</v>
+        <v>375</v>
       </c>
       <c r="N47" s="12">
-        <v>45161</v>
+        <v>45194</v>
       </c>
       <c r="O47" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5692,7 +5698,7 @@
       </c>
       <c r="P47">
         <f t="shared" ca="1" si="4"/>
-        <v>349</v>
+        <v>375</v>
       </c>
       <c r="Q47" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5715,10 +5721,10 @@
         <v>35</v>
       </c>
       <c r="M48">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="N48" s="12">
-        <v>45142</v>
+        <v>45161</v>
       </c>
       <c r="O48" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5726,7 +5732,7 @@
       </c>
       <c r="P48">
         <f t="shared" ca="1" si="4"/>
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="Q48" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5746,10 +5752,10 @@
         <v>0</v>
       </c>
       <c r="M49">
-        <v>300</v>
+        <v>346</v>
       </c>
       <c r="N49" s="12">
-        <v>45181</v>
+        <v>45142</v>
       </c>
     </row>
     <row r="50" spans="2:14" x14ac:dyDescent="0.2">
@@ -5765,10 +5771,10 @@
         <v>0</v>
       </c>
       <c r="M50">
-        <v>272</v>
+        <v>300</v>
       </c>
       <c r="N50" s="12">
-        <v>45188</v>
+        <v>45181</v>
       </c>
     </row>
     <row r="51" spans="2:14" x14ac:dyDescent="0.2">
@@ -5784,10 +5790,10 @@
         <v>0</v>
       </c>
       <c r="M51">
-        <v>220</v>
+        <v>272</v>
       </c>
       <c r="N51">
-        <v>45175</v>
+        <v>45188</v>
       </c>
     </row>
     <row r="52" spans="2:14" x14ac:dyDescent="0.2">
@@ -5803,10 +5809,10 @@
         <v>0</v>
       </c>
       <c r="M52">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="N52">
-        <v>45173</v>
+        <v>45175</v>
       </c>
     </row>
     <row r="53" spans="2:14" x14ac:dyDescent="0.2">
@@ -5822,10 +5828,10 @@
         <v>0</v>
       </c>
       <c r="M53">
-        <v>159</v>
+        <v>217</v>
       </c>
       <c r="N53">
-        <v>45182</v>
+        <v>45173</v>
       </c>
     </row>
     <row r="54" spans="2:14" x14ac:dyDescent="0.2">
@@ -5841,10 +5847,10 @@
         <v>0</v>
       </c>
       <c r="M54">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="N54">
-        <v>45139</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="55" spans="2:14" x14ac:dyDescent="0.2">
@@ -5860,10 +5866,10 @@
         <v>0</v>
       </c>
       <c r="M55">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="N55">
-        <v>45210</v>
+        <v>45139</v>
       </c>
     </row>
     <row r="56" spans="2:14" x14ac:dyDescent="0.2">
@@ -5879,10 +5885,10 @@
         <v>0</v>
       </c>
       <c r="M56">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="N56">
-        <v>45162</v>
+        <v>45210</v>
       </c>
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.2">
@@ -5898,10 +5904,10 @@
         <v>0</v>
       </c>
       <c r="M57">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="N57">
-        <v>45196</v>
+        <v>45162</v>
       </c>
     </row>
     <row r="58" spans="2:14" x14ac:dyDescent="0.2">
@@ -5917,10 +5923,10 @@
         <v>0</v>
       </c>
       <c r="M58">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="N58">
-        <v>45152</v>
+        <v>45196</v>
       </c>
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.2">
@@ -5936,10 +5942,10 @@
         <v>0</v>
       </c>
       <c r="M59">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="N59">
-        <v>45195</v>
+        <v>45152</v>
       </c>
     </row>
     <row r="60" spans="2:14" x14ac:dyDescent="0.2">
@@ -5955,10 +5961,10 @@
         <v>0</v>
       </c>
       <c r="M60">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="N60">
-        <v>45153</v>
+        <v>45195</v>
       </c>
     </row>
     <row r="61" spans="2:14" x14ac:dyDescent="0.2">
@@ -5974,10 +5980,10 @@
         <v>0</v>
       </c>
       <c r="M61">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="N61">
-        <v>45187</v>
+        <v>45212</v>
       </c>
     </row>
     <row r="62" spans="2:14" x14ac:dyDescent="0.2">
@@ -5993,10 +5999,10 @@
         <v>0</v>
       </c>
       <c r="M62">
-        <v>119</v>
+        <v>140</v>
       </c>
       <c r="N62">
-        <v>45168</v>
+        <v>45153</v>
       </c>
     </row>
     <row r="63" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -6012,42 +6018,146 @@
         <v>0</v>
       </c>
       <c r="M63">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="N63">
-        <v>45147</v>
+        <v>45187</v>
       </c>
     </row>
     <row r="64" spans="2:14" x14ac:dyDescent="0.2">
       <c r="M64">
-        <v>97</v>
+        <v>119</v>
       </c>
       <c r="N64">
-        <v>45183</v>
+        <v>45168</v>
       </c>
     </row>
     <row r="65" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M65">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="N65">
-        <v>45164</v>
+        <v>45147</v>
       </c>
     </row>
     <row r="66" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M66">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="N66">
-        <v>45140</v>
+        <v>45183</v>
       </c>
     </row>
     <row r="67" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M67">
+        <v>95</v>
+      </c>
+      <c r="N67">
+        <v>45164</v>
+      </c>
+    </row>
+    <row r="68" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="M68">
+        <v>38</v>
+      </c>
+      <c r="N68">
+        <v>45140</v>
+      </c>
+    </row>
+    <row r="69" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="M69">
         <v>0</v>
       </c>
-      <c r="N67">
+      <c r="N69">
         <v>45138</v>
+      </c>
+    </row>
+    <row r="70" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="M70">
+        <v>-773</v>
+      </c>
+      <c r="N70">
+        <v>45218</v>
+      </c>
+    </row>
+    <row r="71" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="M71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="M72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="M73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="M74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="M75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="M76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="M77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="M78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="M79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="13:14" x14ac:dyDescent="0.2">
+      <c r="M80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M86">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Second best writing ever - wrote catalysis section
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18512928-91AC-934E-A187-5082891673A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA1A950-AFC7-A348-984F-09677FA4B505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="15080" windowHeight="16940" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
@@ -826,6 +826,9 @@
                 <c:pt idx="41">
                   <c:v>45219</c:v>
                 </c:pt>
+                <c:pt idx="42">
+                  <c:v>45221</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -956,10 +959,13 @@
                   <c:v>14566</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>13793</c:v>
+                  <c:v>13604</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>14368</c:v>
+                  <c:v>14179</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>15201</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1310,61 +1316,61 @@
                   <c:v>1279</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>859</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>814</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>729</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>661</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>657</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>611</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>603</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>580</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>575</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>548</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>515</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>486</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>473</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>467</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>448</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>419</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>410</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>375</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>349</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1466,7 +1472,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1022</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1796,10 +1802,10 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$7:$C$47</c:f>
+              <c:f>Sheet1!$C$7:$C$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="41"/>
+                <c:ptCount val="42"/>
                 <c:pt idx="0">
                   <c:v>156</c:v>
                 </c:pt>
@@ -1918,10 +1924,13 @@
                   <c:v>143</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>-773</c:v>
+                  <c:v>-962</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>575</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1022</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3881,15 +3890,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>42337</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>145523</xdr:rowOff>
+      <xdr:colOff>31755</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>18524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>542399</xdr:colOff>
+      <xdr:colOff>531817</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:rowOff>137584</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3904,7 +3913,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7852837" y="5468940"/>
+          <a:off x="7842255" y="5543024"/>
           <a:ext cx="5453062" cy="8183560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4276,8 +4285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4213BD91-B5D1-3B47-8D3F-04331482504C}">
   <dimension ref="A1:Q86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4528,8 +4537,8 @@
       </c>
       <c r="I12" s="30"/>
       <c r="J12" s="10">
-        <f>J8-MAX(D6:D44)</f>
-        <v>2577</v>
+        <f>J8-MAX(D6:D48)</f>
+        <v>1799</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
@@ -4585,7 +4594,7 @@
       <c r="I14" s="34"/>
       <c r="J14" s="11">
         <f>J12/J13</f>
-        <v>5.1918701114008057</v>
+        <v>3.6244370703958282</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
@@ -4927,7 +4936,7 @@
         <v>1279</v>
       </c>
       <c r="N29" s="12" cm="1">
-        <f t="array" ref="N29:N70">_xlfn.SORTBY(B6:B47,C6:C47, -1)</f>
+        <f t="array" ref="N29:N71">_xlfn.SORTBY(B6:B48,C6:C48, -1)</f>
         <v>45148</v>
       </c>
       <c r="O29" t="str">
@@ -4969,22 +4978,22 @@
         <v>17</v>
       </c>
       <c r="M30">
-        <v>859</v>
+        <v>1022</v>
       </c>
       <c r="N30" s="12">
-        <v>45146</v>
+        <v>45221</v>
       </c>
       <c r="O30" t="str">
         <f t="shared" ref="O30:O48" ca="1" si="3">IF(N30=TODAY(), "Green", "Blue")</f>
-        <v>Blue</v>
-      </c>
-      <c r="P30">
+        <v>Green</v>
+      </c>
+      <c r="P30" t="str">
         <f t="shared" ref="P30:P48" ca="1" si="4">IF(NOT(N30=TODAY()), M30, "")</f>
-        <v>859</v>
-      </c>
-      <c r="Q30" t="str">
+        <v/>
+      </c>
+      <c r="Q30">
         <f t="shared" ref="Q30:Q48" ca="1" si="5">IF(N30=TODAY(), M30, "")</f>
-        <v/>
+        <v>1022</v>
       </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.2">
@@ -5013,10 +5022,10 @@
         <v>18</v>
       </c>
       <c r="M31">
-        <v>814</v>
+        <v>859</v>
       </c>
       <c r="N31" s="12">
-        <v>45211</v>
+        <v>45146</v>
       </c>
       <c r="O31" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5024,7 +5033,7 @@
       </c>
       <c r="P31">
         <f t="shared" ca="1" si="4"/>
-        <v>814</v>
+        <v>859</v>
       </c>
       <c r="Q31" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5057,10 +5066,10 @@
         <v>19</v>
       </c>
       <c r="M32">
-        <v>729</v>
+        <v>814</v>
       </c>
       <c r="N32" s="12">
-        <v>45145</v>
+        <v>45211</v>
       </c>
       <c r="O32" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5068,7 +5077,7 @@
       </c>
       <c r="P32">
         <f t="shared" ca="1" si="4"/>
-        <v>729</v>
+        <v>814</v>
       </c>
       <c r="Q32" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5101,10 +5110,10 @@
         <v>20</v>
       </c>
       <c r="M33">
-        <v>661</v>
+        <v>729</v>
       </c>
       <c r="N33" s="12">
-        <v>45159</v>
+        <v>45145</v>
       </c>
       <c r="O33" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5112,7 +5121,7 @@
       </c>
       <c r="P33">
         <f t="shared" ca="1" si="4"/>
-        <v>661</v>
+        <v>729</v>
       </c>
       <c r="Q33" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5145,10 +5154,10 @@
         <v>25</v>
       </c>
       <c r="M34">
-        <v>657</v>
+        <v>661</v>
       </c>
       <c r="N34" s="12">
-        <v>45149</v>
+        <v>45159</v>
       </c>
       <c r="O34" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5156,7 +5165,7 @@
       </c>
       <c r="P34">
         <f t="shared" ca="1" si="4"/>
-        <v>657</v>
+        <v>661</v>
       </c>
       <c r="Q34" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5189,10 +5198,10 @@
         <v>26</v>
       </c>
       <c r="M35">
-        <v>611</v>
+        <v>657</v>
       </c>
       <c r="N35" s="12">
-        <v>45163</v>
+        <v>45149</v>
       </c>
       <c r="O35" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5200,7 +5209,7 @@
       </c>
       <c r="P35">
         <f t="shared" ca="1" si="4"/>
-        <v>611</v>
+        <v>657</v>
       </c>
       <c r="Q35" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5233,10 +5242,10 @@
         <v>27</v>
       </c>
       <c r="M36">
-        <v>603</v>
+        <v>611</v>
       </c>
       <c r="N36" s="12">
-        <v>45193</v>
+        <v>45163</v>
       </c>
       <c r="O36" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5244,7 +5253,7 @@
       </c>
       <c r="P36">
         <f t="shared" ca="1" si="4"/>
-        <v>603</v>
+        <v>611</v>
       </c>
       <c r="Q36" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5277,10 +5286,10 @@
         <v>28</v>
       </c>
       <c r="M37">
-        <v>580</v>
+        <v>603</v>
       </c>
       <c r="N37" s="12">
-        <v>45160</v>
+        <v>45193</v>
       </c>
       <c r="O37" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5288,7 +5297,7 @@
       </c>
       <c r="P37">
         <f t="shared" ca="1" si="4"/>
-        <v>580</v>
+        <v>603</v>
       </c>
       <c r="Q37" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5318,10 +5327,10 @@
         <v>29</v>
       </c>
       <c r="M38">
-        <v>575</v>
+        <v>580</v>
       </c>
       <c r="N38" s="12">
-        <v>45219</v>
+        <v>45160</v>
       </c>
       <c r="O38" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5329,7 +5338,7 @@
       </c>
       <c r="P38">
         <f t="shared" ca="1" si="4"/>
-        <v>575</v>
+        <v>580</v>
       </c>
       <c r="Q38" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5359,10 +5368,10 @@
         <v>30</v>
       </c>
       <c r="M39">
-        <v>548</v>
+        <v>575</v>
       </c>
       <c r="N39" s="12">
-        <v>45208</v>
+        <v>45219</v>
       </c>
       <c r="O39" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5370,7 +5379,7 @@
       </c>
       <c r="P39">
         <f t="shared" ca="1" si="4"/>
-        <v>548</v>
+        <v>575</v>
       </c>
       <c r="Q39" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5400,10 +5409,10 @@
         <v>31</v>
       </c>
       <c r="M40">
-        <v>515</v>
+        <v>548</v>
       </c>
       <c r="N40" s="12">
-        <v>45191</v>
+        <v>45208</v>
       </c>
       <c r="O40" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5411,7 +5420,7 @@
       </c>
       <c r="P40">
         <f t="shared" ca="1" si="4"/>
-        <v>515</v>
+        <v>548</v>
       </c>
       <c r="Q40" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5423,7 +5432,7 @@
         <v>45208</v>
       </c>
       <c r="C41" s="21">
-        <f t="shared" ref="C41:C47" si="8">D41-D40</f>
+        <f t="shared" ref="C41:C48" si="8">D41-D40</f>
         <v>548</v>
       </c>
       <c r="D41" s="23">
@@ -5441,10 +5450,10 @@
         <v>32</v>
       </c>
       <c r="M41">
-        <v>486</v>
+        <v>515</v>
       </c>
       <c r="N41" s="12">
-        <v>45141</v>
+        <v>45191</v>
       </c>
       <c r="O41" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5452,7 +5461,7 @@
       </c>
       <c r="P41">
         <f t="shared" ca="1" si="4"/>
-        <v>486</v>
+        <v>515</v>
       </c>
       <c r="Q41" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5482,10 +5491,10 @@
         <v>33</v>
       </c>
       <c r="M42">
-        <v>473</v>
+        <v>486</v>
       </c>
       <c r="N42" s="12">
-        <v>45174</v>
+        <v>45141</v>
       </c>
       <c r="O42" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5493,7 +5502,7 @@
       </c>
       <c r="P42">
         <f t="shared" ca="1" si="4"/>
-        <v>473</v>
+        <v>486</v>
       </c>
       <c r="Q42" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5523,10 +5532,10 @@
         <v>34</v>
       </c>
       <c r="M43">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="N43" s="12">
-        <v>45154</v>
+        <v>45174</v>
       </c>
       <c r="O43" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5534,7 +5543,7 @@
       </c>
       <c r="P43">
         <f t="shared" ca="1" si="4"/>
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="Q43" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5564,10 +5573,10 @@
         <v>36</v>
       </c>
       <c r="M44">
-        <v>448</v>
+        <v>467</v>
       </c>
       <c r="N44" s="12">
-        <v>45155</v>
+        <v>45154</v>
       </c>
       <c r="O44" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5575,7 +5584,7 @@
       </c>
       <c r="P44">
         <f t="shared" ca="1" si="4"/>
-        <v>448</v>
+        <v>467</v>
       </c>
       <c r="Q44" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5605,10 +5614,10 @@
         <v>37</v>
       </c>
       <c r="M45">
-        <v>419</v>
+        <v>448</v>
       </c>
       <c r="N45" s="12">
-        <v>45156</v>
+        <v>45155</v>
       </c>
       <c r="O45" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5616,7 +5625,7 @@
       </c>
       <c r="P45">
         <f t="shared" ca="1" si="4"/>
-        <v>419</v>
+        <v>448</v>
       </c>
       <c r="Q45" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5629,27 +5638,28 @@
       </c>
       <c r="C46" s="21">
         <f t="shared" si="8"/>
-        <v>-773</v>
+        <v>-962</v>
       </c>
       <c r="D46" s="23">
-        <v>13793</v>
+        <f>13793-105-84</f>
+        <v>13604</v>
       </c>
       <c r="E46" s="24">
         <f t="shared" si="6"/>
-        <v>40.567647058823532</v>
+        <v>40.011764705882356</v>
       </c>
       <c r="F46" s="4">
         <f t="shared" si="7"/>
-        <v>0.81135294117647061</v>
+        <v>0.80023529411764704</v>
       </c>
       <c r="L46" t="s">
         <v>38</v>
       </c>
       <c r="M46">
-        <v>410</v>
+        <v>419</v>
       </c>
       <c r="N46" s="12">
-        <v>45209</v>
+        <v>45156</v>
       </c>
       <c r="O46" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5657,7 +5667,7 @@
       </c>
       <c r="P46">
         <f t="shared" ca="1" si="4"/>
-        <v>410</v>
+        <v>419</v>
       </c>
       <c r="Q46" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5673,24 +5683,25 @@
         <v>575</v>
       </c>
       <c r="D47" s="23">
-        <v>14368</v>
+        <f>14368-105-84</f>
+        <v>14179</v>
       </c>
       <c r="E47" s="24">
         <f t="shared" si="6"/>
-        <v>42.258823529411764</v>
+        <v>41.702941176470588</v>
       </c>
       <c r="F47" s="4">
         <f t="shared" si="7"/>
-        <v>0.84517647058823531</v>
+        <v>0.83405882352941174</v>
       </c>
       <c r="L47" t="s">
         <v>39</v>
       </c>
       <c r="M47">
-        <v>375</v>
+        <v>410</v>
       </c>
       <c r="N47" s="12">
-        <v>45194</v>
+        <v>45209</v>
       </c>
       <c r="O47" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5698,7 +5709,7 @@
       </c>
       <c r="P47">
         <f t="shared" ca="1" si="4"/>
-        <v>375</v>
+        <v>410</v>
       </c>
       <c r="Q47" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5706,25 +5717,32 @@
       </c>
     </row>
     <row r="48" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B48" s="28"/>
-      <c r="C48" s="21"/>
-      <c r="D48" s="23"/>
+      <c r="B48" s="2">
+        <v>45221</v>
+      </c>
+      <c r="C48" s="21">
+        <f t="shared" si="8"/>
+        <v>1022</v>
+      </c>
+      <c r="D48" s="23">
+        <v>15201</v>
+      </c>
       <c r="E48" s="24">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>44.708823529411767</v>
       </c>
       <c r="F48" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>0.89417647058823524</v>
       </c>
       <c r="L48" t="s">
         <v>35</v>
       </c>
       <c r="M48">
-        <v>349</v>
+        <v>375</v>
       </c>
       <c r="N48" s="12">
-        <v>45161</v>
+        <v>45194</v>
       </c>
       <c r="O48" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5732,7 +5750,7 @@
       </c>
       <c r="P48">
         <f t="shared" ca="1" si="4"/>
-        <v>349</v>
+        <v>375</v>
       </c>
       <c r="Q48" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5752,10 +5770,10 @@
         <v>0</v>
       </c>
       <c r="M49">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="N49" s="12">
-        <v>45142</v>
+        <v>45161</v>
       </c>
     </row>
     <row r="50" spans="2:14" x14ac:dyDescent="0.2">
@@ -5771,10 +5789,10 @@
         <v>0</v>
       </c>
       <c r="M50">
-        <v>300</v>
+        <v>346</v>
       </c>
       <c r="N50" s="12">
-        <v>45181</v>
+        <v>45142</v>
       </c>
     </row>
     <row r="51" spans="2:14" x14ac:dyDescent="0.2">
@@ -5790,10 +5808,10 @@
         <v>0</v>
       </c>
       <c r="M51">
-        <v>272</v>
+        <v>300</v>
       </c>
       <c r="N51">
-        <v>45188</v>
+        <v>45181</v>
       </c>
     </row>
     <row r="52" spans="2:14" x14ac:dyDescent="0.2">
@@ -5809,10 +5827,10 @@
         <v>0</v>
       </c>
       <c r="M52">
-        <v>220</v>
+        <v>272</v>
       </c>
       <c r="N52">
-        <v>45175</v>
+        <v>45188</v>
       </c>
     </row>
     <row r="53" spans="2:14" x14ac:dyDescent="0.2">
@@ -5828,10 +5846,10 @@
         <v>0</v>
       </c>
       <c r="M53">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="N53">
-        <v>45173</v>
+        <v>45175</v>
       </c>
     </row>
     <row r="54" spans="2:14" x14ac:dyDescent="0.2">
@@ -5847,10 +5865,10 @@
         <v>0</v>
       </c>
       <c r="M54">
-        <v>159</v>
+        <v>217</v>
       </c>
       <c r="N54">
-        <v>45182</v>
+        <v>45173</v>
       </c>
     </row>
     <row r="55" spans="2:14" x14ac:dyDescent="0.2">
@@ -5866,10 +5884,10 @@
         <v>0</v>
       </c>
       <c r="M55">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="N55">
-        <v>45139</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="56" spans="2:14" x14ac:dyDescent="0.2">
@@ -5885,10 +5903,10 @@
         <v>0</v>
       </c>
       <c r="M56">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="N56">
-        <v>45210</v>
+        <v>45139</v>
       </c>
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.2">
@@ -5904,10 +5922,10 @@
         <v>0</v>
       </c>
       <c r="M57">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="N57">
-        <v>45162</v>
+        <v>45210</v>
       </c>
     </row>
     <row r="58" spans="2:14" x14ac:dyDescent="0.2">
@@ -5923,10 +5941,10 @@
         <v>0</v>
       </c>
       <c r="M58">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="N58">
-        <v>45196</v>
+        <v>45162</v>
       </c>
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.2">
@@ -5942,10 +5960,10 @@
         <v>0</v>
       </c>
       <c r="M59">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="N59">
-        <v>45152</v>
+        <v>45196</v>
       </c>
     </row>
     <row r="60" spans="2:14" x14ac:dyDescent="0.2">
@@ -5961,10 +5979,10 @@
         <v>0</v>
       </c>
       <c r="M60">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="N60">
-        <v>45195</v>
+        <v>45152</v>
       </c>
     </row>
     <row r="61" spans="2:14" x14ac:dyDescent="0.2">
@@ -5983,7 +6001,7 @@
         <v>143</v>
       </c>
       <c r="N61">
-        <v>45212</v>
+        <v>45195</v>
       </c>
     </row>
     <row r="62" spans="2:14" x14ac:dyDescent="0.2">
@@ -5999,10 +6017,10 @@
         <v>0</v>
       </c>
       <c r="M62">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="N62">
-        <v>45153</v>
+        <v>45212</v>
       </c>
     </row>
     <row r="63" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -6018,71 +6036,74 @@
         <v>0</v>
       </c>
       <c r="M63">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="N63">
-        <v>45187</v>
+        <v>45153</v>
       </c>
     </row>
     <row r="64" spans="2:14" x14ac:dyDescent="0.2">
       <c r="M64">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="N64">
-        <v>45168</v>
+        <v>45187</v>
       </c>
     </row>
     <row r="65" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M65">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="N65">
-        <v>45147</v>
+        <v>45168</v>
       </c>
     </row>
     <row r="66" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M66">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="N66">
-        <v>45183</v>
+        <v>45147</v>
       </c>
     </row>
     <row r="67" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M67">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="N67">
-        <v>45164</v>
+        <v>45183</v>
       </c>
     </row>
     <row r="68" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M68">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="N68">
-        <v>45140</v>
+        <v>45164</v>
       </c>
     </row>
     <row r="69" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M69">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="N69">
-        <v>45138</v>
+        <v>45140</v>
       </c>
     </row>
     <row r="70" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M70">
-        <v>-773</v>
+        <v>0</v>
       </c>
       <c r="N70">
-        <v>45218</v>
+        <v>45138</v>
       </c>
     </row>
     <row r="71" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M71">
-        <v>0</v>
+        <v>-962</v>
+      </c>
+      <c r="N71">
+        <v>45218</v>
       </c>
     </row>
     <row r="72" spans="13:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Tons of writing! Finished Catalysis, HEA and SS
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA1A950-AFC7-A348-984F-09677FA4B505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2459B431-0274-D74D-8D9F-4165843CA785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="15080" windowHeight="16940" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
@@ -827,7 +827,10 @@
                   <c:v>45219</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>45221</c:v>
+                  <c:v>45220</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>45222</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -959,13 +962,16 @@
                   <c:v>14566</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>13604</c:v>
+                  <c:v>13470</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>14179</c:v>
+                  <c:v>14045</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>15201</c:v>
+                  <c:v>15067</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>16092</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1319,58 +1325,58 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>1022</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>859</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>814</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>729</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>661</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>657</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>611</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>603</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>580</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>575</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>548</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>515</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>486</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>473</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>467</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>448</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>419</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>410</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>375</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1472,7 +1478,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1022</c:v>
+                  <c:v>1025</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1802,10 +1808,10 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$7:$C$48</c:f>
+              <c:f>Sheet1!$C$7:$C$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="42"/>
+                <c:ptCount val="48"/>
                 <c:pt idx="0">
                   <c:v>156</c:v>
                 </c:pt>
@@ -1924,13 +1930,16 @@
                   <c:v>143</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>-962</c:v>
+                  <c:v>-1096</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>575</c:v>
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>1022</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1025</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3890,15 +3899,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>31755</xdr:colOff>
+      <xdr:colOff>21595</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>18524</xdr:rowOff>
+      <xdr:rowOff>111234</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>531817</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>137584</xdr:rowOff>
+      <xdr:colOff>521657</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>27094</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3913,8 +3922,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7842255" y="5543024"/>
-          <a:ext cx="5453062" cy="8183560"/>
+          <a:off x="7834635" y="5714474"/>
+          <a:ext cx="5468302" cy="8277540"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4285,8 +4294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4213BD91-B5D1-3B47-8D3F-04331482504C}">
   <dimension ref="A1:Q86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4537,8 +4546,8 @@
       </c>
       <c r="I12" s="30"/>
       <c r="J12" s="10">
-        <f>J8-MAX(D6:D48)</f>
-        <v>1799</v>
+        <f>J8-MAX(D6:D63)</f>
+        <v>908</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
@@ -4594,7 +4603,7 @@
       <c r="I14" s="34"/>
       <c r="J14" s="11">
         <f>J12/J13</f>
-        <v>3.6244370703958282</v>
+        <v>1.8293434463142924</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
@@ -4767,8 +4776,8 @@
         <v>0.44223529411764706</v>
       </c>
       <c r="M22">
-        <f>AVERAGE(C7:C44)</f>
-        <v>379.55263157894734</v>
+        <f>(AVERAGE(C7:C45)+AVERAGE(C47:C49))/2</f>
+        <v>623.74358974358972</v>
       </c>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.2">
@@ -4936,7 +4945,7 @@
         <v>1279</v>
       </c>
       <c r="N29" s="12" cm="1">
-        <f t="array" ref="N29:N71">_xlfn.SORTBY(B6:B48,C6:C48, -1)</f>
+        <f t="array" ref="N29:N72">_xlfn.SORTBY(B6:B49,C6:C49, -1)</f>
         <v>45148</v>
       </c>
       <c r="O29" t="str">
@@ -4978,10 +4987,10 @@
         <v>17</v>
       </c>
       <c r="M30">
-        <v>1022</v>
+        <v>1025</v>
       </c>
       <c r="N30" s="12">
-        <v>45221</v>
+        <v>45222</v>
       </c>
       <c r="O30" t="str">
         <f t="shared" ref="O30:O48" ca="1" si="3">IF(N30=TODAY(), "Green", "Blue")</f>
@@ -4993,7 +5002,7 @@
       </c>
       <c r="Q30">
         <f t="shared" ref="Q30:Q48" ca="1" si="5">IF(N30=TODAY(), M30, "")</f>
-        <v>1022</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.2">
@@ -5022,10 +5031,10 @@
         <v>18</v>
       </c>
       <c r="M31">
-        <v>859</v>
+        <v>1022</v>
       </c>
       <c r="N31" s="12">
-        <v>45146</v>
+        <v>45220</v>
       </c>
       <c r="O31" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5033,7 +5042,7 @@
       </c>
       <c r="P31">
         <f t="shared" ca="1" si="4"/>
-        <v>859</v>
+        <v>1022</v>
       </c>
       <c r="Q31" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5066,10 +5075,10 @@
         <v>19</v>
       </c>
       <c r="M32">
-        <v>814</v>
+        <v>859</v>
       </c>
       <c r="N32" s="12">
-        <v>45211</v>
+        <v>45146</v>
       </c>
       <c r="O32" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5077,7 +5086,7 @@
       </c>
       <c r="P32">
         <f t="shared" ca="1" si="4"/>
-        <v>814</v>
+        <v>859</v>
       </c>
       <c r="Q32" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5110,10 +5119,10 @@
         <v>20</v>
       </c>
       <c r="M33">
-        <v>729</v>
+        <v>814</v>
       </c>
       <c r="N33" s="12">
-        <v>45145</v>
+        <v>45211</v>
       </c>
       <c r="O33" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5121,7 +5130,7 @@
       </c>
       <c r="P33">
         <f t="shared" ca="1" si="4"/>
-        <v>729</v>
+        <v>814</v>
       </c>
       <c r="Q33" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5154,10 +5163,10 @@
         <v>25</v>
       </c>
       <c r="M34">
-        <v>661</v>
+        <v>729</v>
       </c>
       <c r="N34" s="12">
-        <v>45159</v>
+        <v>45145</v>
       </c>
       <c r="O34" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5165,7 +5174,7 @@
       </c>
       <c r="P34">
         <f t="shared" ca="1" si="4"/>
-        <v>661</v>
+        <v>729</v>
       </c>
       <c r="Q34" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5198,10 +5207,10 @@
         <v>26</v>
       </c>
       <c r="M35">
-        <v>657</v>
+        <v>661</v>
       </c>
       <c r="N35" s="12">
-        <v>45149</v>
+        <v>45159</v>
       </c>
       <c r="O35" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5209,7 +5218,7 @@
       </c>
       <c r="P35">
         <f t="shared" ca="1" si="4"/>
-        <v>657</v>
+        <v>661</v>
       </c>
       <c r="Q35" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5242,10 +5251,10 @@
         <v>27</v>
       </c>
       <c r="M36">
-        <v>611</v>
+        <v>657</v>
       </c>
       <c r="N36" s="12">
-        <v>45163</v>
+        <v>45149</v>
       </c>
       <c r="O36" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5253,7 +5262,7 @@
       </c>
       <c r="P36">
         <f t="shared" ca="1" si="4"/>
-        <v>611</v>
+        <v>657</v>
       </c>
       <c r="Q36" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5286,10 +5295,10 @@
         <v>28</v>
       </c>
       <c r="M37">
-        <v>603</v>
+        <v>611</v>
       </c>
       <c r="N37" s="12">
-        <v>45193</v>
+        <v>45163</v>
       </c>
       <c r="O37" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5297,7 +5306,7 @@
       </c>
       <c r="P37">
         <f t="shared" ca="1" si="4"/>
-        <v>603</v>
+        <v>611</v>
       </c>
       <c r="Q37" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5327,10 +5336,10 @@
         <v>29</v>
       </c>
       <c r="M38">
-        <v>580</v>
+        <v>603</v>
       </c>
       <c r="N38" s="12">
-        <v>45160</v>
+        <v>45193</v>
       </c>
       <c r="O38" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5338,7 +5347,7 @@
       </c>
       <c r="P38">
         <f t="shared" ca="1" si="4"/>
-        <v>580</v>
+        <v>603</v>
       </c>
       <c r="Q38" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5368,10 +5377,10 @@
         <v>30</v>
       </c>
       <c r="M39">
-        <v>575</v>
+        <v>580</v>
       </c>
       <c r="N39" s="12">
-        <v>45219</v>
+        <v>45160</v>
       </c>
       <c r="O39" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5379,7 +5388,7 @@
       </c>
       <c r="P39">
         <f t="shared" ca="1" si="4"/>
-        <v>575</v>
+        <v>580</v>
       </c>
       <c r="Q39" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5409,10 +5418,10 @@
         <v>31</v>
       </c>
       <c r="M40">
-        <v>548</v>
+        <v>575</v>
       </c>
       <c r="N40" s="12">
-        <v>45208</v>
+        <v>45219</v>
       </c>
       <c r="O40" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5420,7 +5429,7 @@
       </c>
       <c r="P40">
         <f t="shared" ca="1" si="4"/>
-        <v>548</v>
+        <v>575</v>
       </c>
       <c r="Q40" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5432,7 +5441,7 @@
         <v>45208</v>
       </c>
       <c r="C41" s="21">
-        <f t="shared" ref="C41:C48" si="8">D41-D40</f>
+        <f t="shared" ref="C41:C49" si="8">D41-D40</f>
         <v>548</v>
       </c>
       <c r="D41" s="23">
@@ -5450,10 +5459,10 @@
         <v>32</v>
       </c>
       <c r="M41">
-        <v>515</v>
+        <v>548</v>
       </c>
       <c r="N41" s="12">
-        <v>45191</v>
+        <v>45208</v>
       </c>
       <c r="O41" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5461,7 +5470,7 @@
       </c>
       <c r="P41">
         <f t="shared" ca="1" si="4"/>
-        <v>515</v>
+        <v>548</v>
       </c>
       <c r="Q41" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5491,10 +5500,10 @@
         <v>33</v>
       </c>
       <c r="M42">
-        <v>486</v>
+        <v>515</v>
       </c>
       <c r="N42" s="12">
-        <v>45141</v>
+        <v>45191</v>
       </c>
       <c r="O42" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5502,7 +5511,7 @@
       </c>
       <c r="P42">
         <f t="shared" ca="1" si="4"/>
-        <v>486</v>
+        <v>515</v>
       </c>
       <c r="Q42" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5532,10 +5541,10 @@
         <v>34</v>
       </c>
       <c r="M43">
-        <v>473</v>
+        <v>486</v>
       </c>
       <c r="N43" s="12">
-        <v>45174</v>
+        <v>45141</v>
       </c>
       <c r="O43" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5543,7 +5552,7 @@
       </c>
       <c r="P43">
         <f t="shared" ca="1" si="4"/>
-        <v>473</v>
+        <v>486</v>
       </c>
       <c r="Q43" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5573,10 +5582,10 @@
         <v>36</v>
       </c>
       <c r="M44">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="N44" s="12">
-        <v>45154</v>
+        <v>45174</v>
       </c>
       <c r="O44" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5584,7 +5593,7 @@
       </c>
       <c r="P44">
         <f t="shared" ca="1" si="4"/>
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="Q44" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5614,10 +5623,10 @@
         <v>37</v>
       </c>
       <c r="M45">
-        <v>448</v>
+        <v>467</v>
       </c>
       <c r="N45" s="12">
-        <v>45155</v>
+        <v>45154</v>
       </c>
       <c r="O45" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5625,7 +5634,7 @@
       </c>
       <c r="P45">
         <f t="shared" ca="1" si="4"/>
-        <v>448</v>
+        <v>467</v>
       </c>
       <c r="Q45" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5638,28 +5647,28 @@
       </c>
       <c r="C46" s="21">
         <f t="shared" si="8"/>
-        <v>-962</v>
+        <v>-1096</v>
       </c>
       <c r="D46" s="23">
-        <f>13793-105-84</f>
-        <v>13604</v>
+        <f>13793-105-84-134</f>
+        <v>13470</v>
       </c>
       <c r="E46" s="24">
         <f t="shared" si="6"/>
-        <v>40.011764705882356</v>
+        <v>39.617647058823529</v>
       </c>
       <c r="F46" s="4">
         <f t="shared" si="7"/>
-        <v>0.80023529411764704</v>
+        <v>0.79235294117647059</v>
       </c>
       <c r="L46" t="s">
         <v>38</v>
       </c>
       <c r="M46">
-        <v>419</v>
+        <v>448</v>
       </c>
       <c r="N46" s="12">
-        <v>45156</v>
+        <v>45155</v>
       </c>
       <c r="O46" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5667,7 +5676,7 @@
       </c>
       <c r="P46">
         <f t="shared" ca="1" si="4"/>
-        <v>419</v>
+        <v>448</v>
       </c>
       <c r="Q46" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5683,25 +5692,25 @@
         <v>575</v>
       </c>
       <c r="D47" s="23">
-        <f>14368-105-84</f>
-        <v>14179</v>
+        <f>14368-105-84-134</f>
+        <v>14045</v>
       </c>
       <c r="E47" s="24">
         <f t="shared" si="6"/>
-        <v>41.702941176470588</v>
+        <v>41.308823529411768</v>
       </c>
       <c r="F47" s="4">
         <f t="shared" si="7"/>
-        <v>0.83405882352941174</v>
+        <v>0.82617647058823529</v>
       </c>
       <c r="L47" t="s">
         <v>39</v>
       </c>
       <c r="M47">
-        <v>410</v>
+        <v>419</v>
       </c>
       <c r="N47" s="12">
-        <v>45209</v>
+        <v>45156</v>
       </c>
       <c r="O47" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5709,7 +5718,7 @@
       </c>
       <c r="P47">
         <f t="shared" ca="1" si="4"/>
-        <v>410</v>
+        <v>419</v>
       </c>
       <c r="Q47" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5718,31 +5727,32 @@
     </row>
     <row r="48" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B48" s="2">
-        <v>45221</v>
+        <v>45220</v>
       </c>
       <c r="C48" s="21">
         <f t="shared" si="8"/>
         <v>1022</v>
       </c>
       <c r="D48" s="23">
-        <v>15201</v>
+        <f>15201-134</f>
+        <v>15067</v>
       </c>
       <c r="E48" s="24">
         <f t="shared" si="6"/>
-        <v>44.708823529411767</v>
+        <v>44.314705882352939</v>
       </c>
       <c r="F48" s="4">
         <f t="shared" si="7"/>
-        <v>0.89417647058823524</v>
+        <v>0.88629411764705879</v>
       </c>
       <c r="L48" t="s">
         <v>35</v>
       </c>
       <c r="M48">
-        <v>375</v>
+        <v>410</v>
       </c>
       <c r="N48" s="12">
-        <v>45194</v>
+        <v>45209</v>
       </c>
       <c r="O48" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5750,7 +5760,7 @@
       </c>
       <c r="P48">
         <f t="shared" ca="1" si="4"/>
-        <v>375</v>
+        <v>410</v>
       </c>
       <c r="Q48" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5758,22 +5768,29 @@
       </c>
     </row>
     <row r="49" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B49" s="28"/>
-      <c r="C49" s="21"/>
-      <c r="D49" s="23"/>
+      <c r="B49" s="2">
+        <v>45222</v>
+      </c>
+      <c r="C49" s="21">
+        <f t="shared" si="8"/>
+        <v>1025</v>
+      </c>
+      <c r="D49" s="23">
+        <v>16092</v>
+      </c>
       <c r="E49" s="24">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>47.329411764705881</v>
       </c>
       <c r="F49" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>0.94658823529411762</v>
       </c>
       <c r="M49">
-        <v>349</v>
+        <v>375</v>
       </c>
       <c r="N49" s="12">
-        <v>45161</v>
+        <v>45194</v>
       </c>
     </row>
     <row r="50" spans="2:14" x14ac:dyDescent="0.2">
@@ -5789,10 +5806,10 @@
         <v>0</v>
       </c>
       <c r="M50">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="N50" s="12">
-        <v>45142</v>
+        <v>45161</v>
       </c>
     </row>
     <row r="51" spans="2:14" x14ac:dyDescent="0.2">
@@ -5808,10 +5825,10 @@
         <v>0</v>
       </c>
       <c r="M51">
-        <v>300</v>
+        <v>346</v>
       </c>
       <c r="N51">
-        <v>45181</v>
+        <v>45142</v>
       </c>
     </row>
     <row r="52" spans="2:14" x14ac:dyDescent="0.2">
@@ -5827,10 +5844,10 @@
         <v>0</v>
       </c>
       <c r="M52">
-        <v>272</v>
+        <v>300</v>
       </c>
       <c r="N52">
-        <v>45188</v>
+        <v>45181</v>
       </c>
     </row>
     <row r="53" spans="2:14" x14ac:dyDescent="0.2">
@@ -5846,10 +5863,10 @@
         <v>0</v>
       </c>
       <c r="M53">
-        <v>220</v>
+        <v>272</v>
       </c>
       <c r="N53">
-        <v>45175</v>
+        <v>45188</v>
       </c>
     </row>
     <row r="54" spans="2:14" x14ac:dyDescent="0.2">
@@ -5865,10 +5882,10 @@
         <v>0</v>
       </c>
       <c r="M54">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="N54">
-        <v>45173</v>
+        <v>45175</v>
       </c>
     </row>
     <row r="55" spans="2:14" x14ac:dyDescent="0.2">
@@ -5884,10 +5901,10 @@
         <v>0</v>
       </c>
       <c r="M55">
-        <v>159</v>
+        <v>217</v>
       </c>
       <c r="N55">
-        <v>45182</v>
+        <v>45173</v>
       </c>
     </row>
     <row r="56" spans="2:14" x14ac:dyDescent="0.2">
@@ -5903,10 +5920,10 @@
         <v>0</v>
       </c>
       <c r="M56">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="N56">
-        <v>45139</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.2">
@@ -5922,10 +5939,10 @@
         <v>0</v>
       </c>
       <c r="M57">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="N57">
-        <v>45210</v>
+        <v>45139</v>
       </c>
     </row>
     <row r="58" spans="2:14" x14ac:dyDescent="0.2">
@@ -5941,10 +5958,10 @@
         <v>0</v>
       </c>
       <c r="M58">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="N58">
-        <v>45162</v>
+        <v>45210</v>
       </c>
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.2">
@@ -5960,10 +5977,10 @@
         <v>0</v>
       </c>
       <c r="M59">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="N59">
-        <v>45196</v>
+        <v>45162</v>
       </c>
     </row>
     <row r="60" spans="2:14" x14ac:dyDescent="0.2">
@@ -5979,10 +5996,10 @@
         <v>0</v>
       </c>
       <c r="M60">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="N60">
-        <v>45152</v>
+        <v>45196</v>
       </c>
     </row>
     <row r="61" spans="2:14" x14ac:dyDescent="0.2">
@@ -5998,10 +6015,10 @@
         <v>0</v>
       </c>
       <c r="M61">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="N61">
-        <v>45195</v>
+        <v>45152</v>
       </c>
     </row>
     <row r="62" spans="2:14" x14ac:dyDescent="0.2">
@@ -6020,7 +6037,7 @@
         <v>143</v>
       </c>
       <c r="N62">
-        <v>45212</v>
+        <v>45195</v>
       </c>
     </row>
     <row r="63" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -6036,79 +6053,82 @@
         <v>0</v>
       </c>
       <c r="M63">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="N63">
-        <v>45153</v>
+        <v>45212</v>
       </c>
     </row>
     <row r="64" spans="2:14" x14ac:dyDescent="0.2">
       <c r="M64">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="N64">
-        <v>45187</v>
+        <v>45153</v>
       </c>
     </row>
     <row r="65" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M65">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="N65">
-        <v>45168</v>
+        <v>45187</v>
       </c>
     </row>
     <row r="66" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M66">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="N66">
-        <v>45147</v>
+        <v>45168</v>
       </c>
     </row>
     <row r="67" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M67">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="N67">
-        <v>45183</v>
+        <v>45147</v>
       </c>
     </row>
     <row r="68" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M68">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="N68">
-        <v>45164</v>
+        <v>45183</v>
       </c>
     </row>
     <row r="69" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M69">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="N69">
-        <v>45140</v>
+        <v>45164</v>
       </c>
     </row>
     <row r="70" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M70">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="N70">
-        <v>45138</v>
+        <v>45140</v>
       </c>
     </row>
     <row r="71" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M71">
-        <v>-962</v>
+        <v>0</v>
       </c>
       <c r="N71">
-        <v>45218</v>
+        <v>45138</v>
       </c>
     </row>
     <row r="72" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M72">
-        <v>0</v>
+        <v>-1096</v>
+      </c>
+      <c r="N72">
+        <v>45218</v>
       </c>
     </row>
     <row r="73" spans="13:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Biggest writing day ever
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2459B431-0274-D74D-8D9F-4165843CA785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD386CEF-F89E-2540-8E2D-E952FFFE4FD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="15080" windowHeight="16940" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
@@ -830,7 +830,10 @@
                   <c:v>45220</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>45222</c:v>
+                  <c:v>45221</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45223</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -962,16 +965,19 @@
                   <c:v>14566</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>13470</c:v>
+                  <c:v>13156</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>14045</c:v>
+                  <c:v>13731</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>15067</c:v>
+                  <c:v>14753</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>16092</c:v>
+                  <c:v>15778</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>17163</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1319,64 +1325,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1279</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="2">
+                  <c:v>1025</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>1022</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>859</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>814</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>729</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>661</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>657</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>611</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>603</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>580</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>575</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>548</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>515</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>486</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>473</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>467</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>448</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>419</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>410</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1475,10 +1481,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
+                  <c:v>1385</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1025</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1930,7 +1936,7 @@
                   <c:v>143</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>-1096</c:v>
+                  <c:v>-1410</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>575</c:v>
@@ -1940,6 +1946,9 @@
                 </c:pt>
                 <c:pt idx="42">
                   <c:v>1025</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1385</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3898,16 +3907,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>21595</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>111234</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>635654</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>160215</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>521657</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>27094</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>315273</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>82426</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3922,8 +3931,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7834635" y="5714474"/>
-          <a:ext cx="5468302" cy="8277540"/>
+          <a:off x="10922654" y="5483632"/>
+          <a:ext cx="5458119" cy="8187794"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4294,8 +4303,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4213BD91-B5D1-3B47-8D3F-04331482504C}">
   <dimension ref="A1:Q86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="B14" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4547,7 +4556,7 @@
       <c r="I12" s="30"/>
       <c r="J12" s="10">
         <f>J8-MAX(D6:D63)</f>
-        <v>908</v>
+        <v>-163</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
@@ -4574,8 +4583,8 @@
       </c>
       <c r="I13" s="32"/>
       <c r="J13" s="10">
-        <f>AVERAGE(C9:C25)</f>
-        <v>496.35294117647061</v>
+        <f>(AVERAGE(C7:C45)+AVERAGE(C47:C50))/2</f>
+        <v>687.61858974358972</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4603,7 +4612,7 @@
       <c r="I14" s="34"/>
       <c r="J14" s="11">
         <f>J12/J13</f>
-        <v>1.8293434463142924</v>
+        <v>-0.23705001934398262</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
@@ -4776,8 +4785,8 @@
         <v>0.44223529411764706</v>
       </c>
       <c r="M22">
-        <f>(AVERAGE(C7:C45)+AVERAGE(C47:C49))/2</f>
-        <v>623.74358974358972</v>
+        <f>(AVERAGE(C7:C45)+AVERAGE(C47:C50))/2</f>
+        <v>687.61858974358972</v>
       </c>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.2">
@@ -4942,23 +4951,23 @@
       </c>
       <c r="M29" cm="1">
         <f t="array" ref="M29:M86">_xlfn.SORTBY(C6:C63, C6:C63, -1)</f>
-        <v>1279</v>
+        <v>1385</v>
       </c>
       <c r="N29" s="12" cm="1">
-        <f t="array" ref="N29:N72">_xlfn.SORTBY(B6:B49,C6:C49, -1)</f>
-        <v>45148</v>
+        <f t="array" ref="N29:N73">_xlfn.SORTBY(B6:B50,C6:C50, -1)</f>
+        <v>45223</v>
       </c>
       <c r="O29" t="str">
         <f ca="1">IF(N29=TODAY(), "Green", "Blue")</f>
-        <v>Blue</v>
-      </c>
-      <c r="P29">
+        <v>Green</v>
+      </c>
+      <c r="P29" t="str">
         <f ca="1">IF(NOT(N29=TODAY()), M29, "")</f>
-        <v>1279</v>
-      </c>
-      <c r="Q29" t="str">
+        <v/>
+      </c>
+      <c r="Q29">
         <f ca="1">IF(N29=TODAY(), M29, "")</f>
-        <v/>
+        <v>1385</v>
       </c>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.2">
@@ -4987,22 +4996,22 @@
         <v>17</v>
       </c>
       <c r="M30">
-        <v>1025</v>
+        <v>1279</v>
       </c>
       <c r="N30" s="12">
-        <v>45222</v>
+        <v>45148</v>
       </c>
       <c r="O30" t="str">
         <f t="shared" ref="O30:O48" ca="1" si="3">IF(N30=TODAY(), "Green", "Blue")</f>
-        <v>Green</v>
-      </c>
-      <c r="P30" t="str">
+        <v>Blue</v>
+      </c>
+      <c r="P30">
         <f t="shared" ref="P30:P48" ca="1" si="4">IF(NOT(N30=TODAY()), M30, "")</f>
+        <v>1279</v>
+      </c>
+      <c r="Q30" t="str">
+        <f t="shared" ref="Q30:Q48" ca="1" si="5">IF(N30=TODAY(), M30, "")</f>
         <v/>
-      </c>
-      <c r="Q30">
-        <f t="shared" ref="Q30:Q48" ca="1" si="5">IF(N30=TODAY(), M30, "")</f>
-        <v>1025</v>
       </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.2">
@@ -5031,10 +5040,10 @@
         <v>18</v>
       </c>
       <c r="M31">
-        <v>1022</v>
+        <v>1025</v>
       </c>
       <c r="N31" s="12">
-        <v>45220</v>
+        <v>45221</v>
       </c>
       <c r="O31" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5042,7 +5051,7 @@
       </c>
       <c r="P31">
         <f t="shared" ca="1" si="4"/>
-        <v>1022</v>
+        <v>1025</v>
       </c>
       <c r="Q31" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5075,10 +5084,10 @@
         <v>19</v>
       </c>
       <c r="M32">
-        <v>859</v>
+        <v>1022</v>
       </c>
       <c r="N32" s="12">
-        <v>45146</v>
+        <v>45220</v>
       </c>
       <c r="O32" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5086,7 +5095,7 @@
       </c>
       <c r="P32">
         <f t="shared" ca="1" si="4"/>
-        <v>859</v>
+        <v>1022</v>
       </c>
       <c r="Q32" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5119,10 +5128,10 @@
         <v>20</v>
       </c>
       <c r="M33">
-        <v>814</v>
+        <v>859</v>
       </c>
       <c r="N33" s="12">
-        <v>45211</v>
+        <v>45146</v>
       </c>
       <c r="O33" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5130,7 +5139,7 @@
       </c>
       <c r="P33">
         <f t="shared" ca="1" si="4"/>
-        <v>814</v>
+        <v>859</v>
       </c>
       <c r="Q33" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5163,10 +5172,10 @@
         <v>25</v>
       </c>
       <c r="M34">
-        <v>729</v>
+        <v>814</v>
       </c>
       <c r="N34" s="12">
-        <v>45145</v>
+        <v>45211</v>
       </c>
       <c r="O34" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5174,7 +5183,7 @@
       </c>
       <c r="P34">
         <f t="shared" ca="1" si="4"/>
-        <v>729</v>
+        <v>814</v>
       </c>
       <c r="Q34" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5207,10 +5216,10 @@
         <v>26</v>
       </c>
       <c r="M35">
-        <v>661</v>
+        <v>729</v>
       </c>
       <c r="N35" s="12">
-        <v>45159</v>
+        <v>45145</v>
       </c>
       <c r="O35" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5218,7 +5227,7 @@
       </c>
       <c r="P35">
         <f t="shared" ca="1" si="4"/>
-        <v>661</v>
+        <v>729</v>
       </c>
       <c r="Q35" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5251,10 +5260,10 @@
         <v>27</v>
       </c>
       <c r="M36">
-        <v>657</v>
+        <v>661</v>
       </c>
       <c r="N36" s="12">
-        <v>45149</v>
+        <v>45159</v>
       </c>
       <c r="O36" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5262,7 +5271,7 @@
       </c>
       <c r="P36">
         <f t="shared" ca="1" si="4"/>
-        <v>657</v>
+        <v>661</v>
       </c>
       <c r="Q36" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5295,10 +5304,10 @@
         <v>28</v>
       </c>
       <c r="M37">
-        <v>611</v>
+        <v>657</v>
       </c>
       <c r="N37" s="12">
-        <v>45163</v>
+        <v>45149</v>
       </c>
       <c r="O37" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5306,7 +5315,7 @@
       </c>
       <c r="P37">
         <f t="shared" ca="1" si="4"/>
-        <v>611</v>
+        <v>657</v>
       </c>
       <c r="Q37" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5336,10 +5345,10 @@
         <v>29</v>
       </c>
       <c r="M38">
-        <v>603</v>
+        <v>611</v>
       </c>
       <c r="N38" s="12">
-        <v>45193</v>
+        <v>45163</v>
       </c>
       <c r="O38" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5347,7 +5356,7 @@
       </c>
       <c r="P38">
         <f t="shared" ca="1" si="4"/>
-        <v>603</v>
+        <v>611</v>
       </c>
       <c r="Q38" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5377,10 +5386,10 @@
         <v>30</v>
       </c>
       <c r="M39">
-        <v>580</v>
+        <v>603</v>
       </c>
       <c r="N39" s="12">
-        <v>45160</v>
+        <v>45193</v>
       </c>
       <c r="O39" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5388,7 +5397,7 @@
       </c>
       <c r="P39">
         <f t="shared" ca="1" si="4"/>
-        <v>580</v>
+        <v>603</v>
       </c>
       <c r="Q39" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5418,10 +5427,10 @@
         <v>31</v>
       </c>
       <c r="M40">
-        <v>575</v>
+        <v>580</v>
       </c>
       <c r="N40" s="12">
-        <v>45219</v>
+        <v>45160</v>
       </c>
       <c r="O40" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5429,7 +5438,7 @@
       </c>
       <c r="P40">
         <f t="shared" ca="1" si="4"/>
-        <v>575</v>
+        <v>580</v>
       </c>
       <c r="Q40" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5441,7 +5450,7 @@
         <v>45208</v>
       </c>
       <c r="C41" s="21">
-        <f t="shared" ref="C41:C49" si="8">D41-D40</f>
+        <f t="shared" ref="C41:C50" si="8">D41-D40</f>
         <v>548</v>
       </c>
       <c r="D41" s="23">
@@ -5459,10 +5468,10 @@
         <v>32</v>
       </c>
       <c r="M41">
-        <v>548</v>
+        <v>575</v>
       </c>
       <c r="N41" s="12">
-        <v>45208</v>
+        <v>45219</v>
       </c>
       <c r="O41" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5470,7 +5479,7 @@
       </c>
       <c r="P41">
         <f t="shared" ca="1" si="4"/>
-        <v>548</v>
+        <v>575</v>
       </c>
       <c r="Q41" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5500,10 +5509,10 @@
         <v>33</v>
       </c>
       <c r="M42">
-        <v>515</v>
+        <v>548</v>
       </c>
       <c r="N42" s="12">
-        <v>45191</v>
+        <v>45208</v>
       </c>
       <c r="O42" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5511,7 +5520,7 @@
       </c>
       <c r="P42">
         <f t="shared" ca="1" si="4"/>
-        <v>515</v>
+        <v>548</v>
       </c>
       <c r="Q42" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5541,10 +5550,10 @@
         <v>34</v>
       </c>
       <c r="M43">
-        <v>486</v>
+        <v>515</v>
       </c>
       <c r="N43" s="12">
-        <v>45141</v>
+        <v>45191</v>
       </c>
       <c r="O43" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5552,7 +5561,7 @@
       </c>
       <c r="P43">
         <f t="shared" ca="1" si="4"/>
-        <v>486</v>
+        <v>515</v>
       </c>
       <c r="Q43" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5582,10 +5591,10 @@
         <v>36</v>
       </c>
       <c r="M44">
-        <v>473</v>
+        <v>486</v>
       </c>
       <c r="N44" s="12">
-        <v>45174</v>
+        <v>45141</v>
       </c>
       <c r="O44" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5593,7 +5602,7 @@
       </c>
       <c r="P44">
         <f t="shared" ca="1" si="4"/>
-        <v>473</v>
+        <v>486</v>
       </c>
       <c r="Q44" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5623,10 +5632,10 @@
         <v>37</v>
       </c>
       <c r="M45">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="N45" s="12">
-        <v>45154</v>
+        <v>45174</v>
       </c>
       <c r="O45" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5634,7 +5643,7 @@
       </c>
       <c r="P45">
         <f t="shared" ca="1" si="4"/>
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="Q45" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5647,28 +5656,28 @@
       </c>
       <c r="C46" s="21">
         <f t="shared" si="8"/>
-        <v>-1096</v>
+        <v>-1410</v>
       </c>
       <c r="D46" s="23">
-        <f>13793-105-84-134</f>
-        <v>13470</v>
+        <f>13793-105-84-134-144-170</f>
+        <v>13156</v>
       </c>
       <c r="E46" s="24">
         <f t="shared" si="6"/>
-        <v>39.617647058823529</v>
+        <v>38.694117647058825</v>
       </c>
       <c r="F46" s="4">
         <f t="shared" si="7"/>
-        <v>0.79235294117647059</v>
+        <v>0.77388235294117647</v>
       </c>
       <c r="L46" t="s">
         <v>38</v>
       </c>
       <c r="M46">
-        <v>448</v>
+        <v>467</v>
       </c>
       <c r="N46" s="12">
-        <v>45155</v>
+        <v>45154</v>
       </c>
       <c r="O46" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5676,7 +5685,7 @@
       </c>
       <c r="P46">
         <f t="shared" ca="1" si="4"/>
-        <v>448</v>
+        <v>467</v>
       </c>
       <c r="Q46" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5692,25 +5701,25 @@
         <v>575</v>
       </c>
       <c r="D47" s="23">
-        <f>14368-105-84-134</f>
-        <v>14045</v>
+        <f>14368-105-84-134-144-170</f>
+        <v>13731</v>
       </c>
       <c r="E47" s="24">
         <f t="shared" si="6"/>
-        <v>41.308823529411768</v>
+        <v>40.385294117647057</v>
       </c>
       <c r="F47" s="4">
         <f t="shared" si="7"/>
-        <v>0.82617647058823529</v>
+        <v>0.80770588235294116</v>
       </c>
       <c r="L47" t="s">
         <v>39</v>
       </c>
       <c r="M47">
-        <v>419</v>
+        <v>448</v>
       </c>
       <c r="N47" s="12">
-        <v>45156</v>
+        <v>45155</v>
       </c>
       <c r="O47" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5718,7 +5727,7 @@
       </c>
       <c r="P47">
         <f t="shared" ca="1" si="4"/>
-        <v>419</v>
+        <v>448</v>
       </c>
       <c r="Q47" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5734,25 +5743,25 @@
         <v>1022</v>
       </c>
       <c r="D48" s="23">
-        <f>15201-134</f>
-        <v>15067</v>
+        <f>15201-134-144-170</f>
+        <v>14753</v>
       </c>
       <c r="E48" s="24">
         <f t="shared" si="6"/>
-        <v>44.314705882352939</v>
+        <v>43.391176470588235</v>
       </c>
       <c r="F48" s="4">
         <f t="shared" si="7"/>
-        <v>0.88629411764705879</v>
+        <v>0.86782352941176466</v>
       </c>
       <c r="L48" t="s">
         <v>35</v>
       </c>
       <c r="M48">
-        <v>410</v>
+        <v>419</v>
       </c>
       <c r="N48" s="12">
-        <v>45209</v>
+        <v>45156</v>
       </c>
       <c r="O48" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5760,7 +5769,7 @@
       </c>
       <c r="P48">
         <f t="shared" ca="1" si="4"/>
-        <v>410</v>
+        <v>419</v>
       </c>
       <c r="Q48" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5769,47 +5778,55 @@
     </row>
     <row r="49" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B49" s="2">
-        <v>45222</v>
+        <v>45221</v>
       </c>
       <c r="C49" s="21">
         <f t="shared" si="8"/>
         <v>1025</v>
       </c>
       <c r="D49" s="23">
-        <v>16092</v>
+        <f>16092-144-170</f>
+        <v>15778</v>
       </c>
       <c r="E49" s="24">
         <f t="shared" si="6"/>
-        <v>47.329411764705881</v>
+        <v>46.405882352941177</v>
       </c>
       <c r="F49" s="4">
         <f t="shared" si="7"/>
-        <v>0.94658823529411762</v>
+        <v>0.92811764705882349</v>
       </c>
       <c r="M49">
-        <v>375</v>
+        <v>410</v>
       </c>
       <c r="N49" s="12">
-        <v>45194</v>
+        <v>45209</v>
       </c>
     </row>
     <row r="50" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B50" s="28"/>
-      <c r="C50" s="21"/>
-      <c r="D50" s="23"/>
+      <c r="B50" s="2">
+        <v>45223</v>
+      </c>
+      <c r="C50" s="21">
+        <f t="shared" si="8"/>
+        <v>1385</v>
+      </c>
+      <c r="D50" s="23">
+        <v>17163</v>
+      </c>
       <c r="E50" s="24">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>50.47941176470588</v>
       </c>
       <c r="F50" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1.0095882352941177</v>
       </c>
       <c r="M50">
-        <v>349</v>
+        <v>375</v>
       </c>
       <c r="N50" s="12">
-        <v>45161</v>
+        <v>45194</v>
       </c>
     </row>
     <row r="51" spans="2:14" x14ac:dyDescent="0.2">
@@ -5825,10 +5842,10 @@
         <v>0</v>
       </c>
       <c r="M51">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="N51">
-        <v>45142</v>
+        <v>45161</v>
       </c>
     </row>
     <row r="52" spans="2:14" x14ac:dyDescent="0.2">
@@ -5844,10 +5861,10 @@
         <v>0</v>
       </c>
       <c r="M52">
-        <v>300</v>
+        <v>346</v>
       </c>
       <c r="N52">
-        <v>45181</v>
+        <v>45142</v>
       </c>
     </row>
     <row r="53" spans="2:14" x14ac:dyDescent="0.2">
@@ -5863,10 +5880,10 @@
         <v>0</v>
       </c>
       <c r="M53">
-        <v>272</v>
+        <v>300</v>
       </c>
       <c r="N53">
-        <v>45188</v>
+        <v>45181</v>
       </c>
     </row>
     <row r="54" spans="2:14" x14ac:dyDescent="0.2">
@@ -5882,10 +5899,10 @@
         <v>0</v>
       </c>
       <c r="M54">
-        <v>220</v>
+        <v>272</v>
       </c>
       <c r="N54">
-        <v>45175</v>
+        <v>45188</v>
       </c>
     </row>
     <row r="55" spans="2:14" x14ac:dyDescent="0.2">
@@ -5901,10 +5918,10 @@
         <v>0</v>
       </c>
       <c r="M55">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="N55">
-        <v>45173</v>
+        <v>45175</v>
       </c>
     </row>
     <row r="56" spans="2:14" x14ac:dyDescent="0.2">
@@ -5920,10 +5937,10 @@
         <v>0</v>
       </c>
       <c r="M56">
-        <v>159</v>
+        <v>217</v>
       </c>
       <c r="N56">
-        <v>45182</v>
+        <v>45173</v>
       </c>
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.2">
@@ -5939,10 +5956,10 @@
         <v>0</v>
       </c>
       <c r="M57">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="N57">
-        <v>45139</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="58" spans="2:14" x14ac:dyDescent="0.2">
@@ -5958,10 +5975,10 @@
         <v>0</v>
       </c>
       <c r="M58">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="N58">
-        <v>45210</v>
+        <v>45139</v>
       </c>
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.2">
@@ -5977,10 +5994,10 @@
         <v>0</v>
       </c>
       <c r="M59">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="N59">
-        <v>45162</v>
+        <v>45210</v>
       </c>
     </row>
     <row r="60" spans="2:14" x14ac:dyDescent="0.2">
@@ -5996,10 +6013,10 @@
         <v>0</v>
       </c>
       <c r="M60">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="N60">
-        <v>45196</v>
+        <v>45162</v>
       </c>
     </row>
     <row r="61" spans="2:14" x14ac:dyDescent="0.2">
@@ -6015,10 +6032,10 @@
         <v>0</v>
       </c>
       <c r="M61">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="N61">
-        <v>45152</v>
+        <v>45196</v>
       </c>
     </row>
     <row r="62" spans="2:14" x14ac:dyDescent="0.2">
@@ -6034,10 +6051,10 @@
         <v>0</v>
       </c>
       <c r="M62">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="N62">
-        <v>45195</v>
+        <v>45152</v>
       </c>
     </row>
     <row r="63" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -6056,84 +6073,87 @@
         <v>143</v>
       </c>
       <c r="N63">
-        <v>45212</v>
+        <v>45195</v>
       </c>
     </row>
     <row r="64" spans="2:14" x14ac:dyDescent="0.2">
       <c r="M64">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="N64">
-        <v>45153</v>
+        <v>45212</v>
       </c>
     </row>
     <row r="65" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M65">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="N65">
-        <v>45187</v>
+        <v>45153</v>
       </c>
     </row>
     <row r="66" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M66">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="N66">
-        <v>45168</v>
+        <v>45187</v>
       </c>
     </row>
     <row r="67" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M67">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="N67">
-        <v>45147</v>
+        <v>45168</v>
       </c>
     </row>
     <row r="68" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M68">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="N68">
-        <v>45183</v>
+        <v>45147</v>
       </c>
     </row>
     <row r="69" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M69">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="N69">
-        <v>45164</v>
+        <v>45183</v>
       </c>
     </row>
     <row r="70" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M70">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="N70">
-        <v>45140</v>
+        <v>45164</v>
       </c>
     </row>
     <row r="71" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M71">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="N71">
-        <v>45138</v>
+        <v>45140</v>
       </c>
     </row>
     <row r="72" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M72">
-        <v>-1096</v>
+        <v>0</v>
       </c>
       <c r="N72">
-        <v>45218</v>
+        <v>45138</v>
       </c>
     </row>
     <row r="73" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M73">
-        <v>0</v>
+        <v>-1410</v>
+      </c>
+      <c r="N73">
+        <v>45218</v>
       </c>
     </row>
     <row r="74" spans="13:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Great writing day, almost at results!
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD386CEF-F89E-2540-8E2D-E952FFFE4FD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CDCC65-B589-F340-B4AD-77A7B9539D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="15080" windowHeight="16940" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
@@ -833,6 +833,9 @@
                   <c:v>45221</c:v>
                 </c:pt>
                 <c:pt idx="44">
+                  <c:v>45222</c:v>
+                </c:pt>
+                <c:pt idx="45">
                   <c:v>45223</c:v>
                 </c:pt>
               </c:numCache>
@@ -978,6 +981,9 @@
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>17163</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>17872</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1325,7 +1331,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1385</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1279</c:v>
@@ -1346,43 +1352,43 @@
                   <c:v>729</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>661</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>657</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>611</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>603</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>580</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>575</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>548</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>515</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>486</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>473</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>467</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>448</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>419</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1481,7 +1487,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1385</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1502,7 +1508,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>709</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -1949,6 +1955,9 @@
                 </c:pt>
                 <c:pt idx="43">
                   <c:v>1385</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>709</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4303,8 +4312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4213BD91-B5D1-3B47-8D3F-04331482504C}">
   <dimension ref="A1:Q86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B14" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4317,6 +4326,7 @@
     <col min="7" max="7" width="1" customWidth="1"/>
     <col min="10" max="10" width="16.1640625" customWidth="1"/>
     <col min="11" max="11" width="3.33203125" customWidth="1"/>
+    <col min="14" max="14" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -4556,7 +4566,7 @@
       <c r="I12" s="30"/>
       <c r="J12" s="10">
         <f>J8-MAX(D6:D63)</f>
-        <v>-163</v>
+        <v>-872</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
@@ -4583,8 +4593,8 @@
       </c>
       <c r="I13" s="32"/>
       <c r="J13" s="10">
-        <f>(AVERAGE(C7:C45)+AVERAGE(C47:C50))/2</f>
-        <v>687.61858974358972</v>
+        <f>(AVERAGE(C7:C45)+AVERAGE(C47:C51))/2</f>
+        <v>658.34358974358975</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4612,7 +4622,7 @@
       <c r="I14" s="34"/>
       <c r="J14" s="11">
         <f>J12/J13</f>
-        <v>-0.23705001934398262</v>
+        <v>-1.3245363266005592</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
@@ -4954,20 +4964,20 @@
         <v>1385</v>
       </c>
       <c r="N29" s="12" cm="1">
-        <f t="array" ref="N29:N73">_xlfn.SORTBY(B6:B50,C6:C50, -1)</f>
-        <v>45223</v>
+        <f t="array" ref="N29:N74">_xlfn.SORTBY(B6:B51,C6:C51, -1)</f>
+        <v>45222</v>
       </c>
       <c r="O29" t="str">
         <f ca="1">IF(N29=TODAY(), "Green", "Blue")</f>
-        <v>Green</v>
-      </c>
-      <c r="P29" t="str">
+        <v>Blue</v>
+      </c>
+      <c r="P29">
         <f ca="1">IF(NOT(N29=TODAY()), M29, "")</f>
+        <v>1385</v>
+      </c>
+      <c r="Q29" t="str">
+        <f ca="1">IF(N29=TODAY(), M29, "")</f>
         <v/>
-      </c>
-      <c r="Q29">
-        <f ca="1">IF(N29=TODAY(), M29, "")</f>
-        <v>1385</v>
       </c>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.2">
@@ -5260,22 +5270,22 @@
         <v>27</v>
       </c>
       <c r="M36">
-        <v>661</v>
+        <v>709</v>
       </c>
       <c r="N36" s="12">
-        <v>45159</v>
+        <v>45223</v>
       </c>
       <c r="O36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Blue</v>
-      </c>
-      <c r="P36">
+        <v>Green</v>
+      </c>
+      <c r="P36" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>661</v>
-      </c>
-      <c r="Q36" t="str">
+        <v/>
+      </c>
+      <c r="Q36">
         <f t="shared" ca="1" si="5"/>
-        <v/>
+        <v>709</v>
       </c>
     </row>
     <row r="37" spans="2:17" x14ac:dyDescent="0.2">
@@ -5304,10 +5314,10 @@
         <v>28</v>
       </c>
       <c r="M37">
-        <v>657</v>
+        <v>661</v>
       </c>
       <c r="N37" s="12">
-        <v>45149</v>
+        <v>45159</v>
       </c>
       <c r="O37" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5315,7 +5325,7 @@
       </c>
       <c r="P37">
         <f t="shared" ca="1" si="4"/>
-        <v>657</v>
+        <v>661</v>
       </c>
       <c r="Q37" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5345,10 +5355,10 @@
         <v>29</v>
       </c>
       <c r="M38">
-        <v>611</v>
+        <v>657</v>
       </c>
       <c r="N38" s="12">
-        <v>45163</v>
+        <v>45149</v>
       </c>
       <c r="O38" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5356,7 +5366,7 @@
       </c>
       <c r="P38">
         <f t="shared" ca="1" si="4"/>
-        <v>611</v>
+        <v>657</v>
       </c>
       <c r="Q38" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5386,10 +5396,10 @@
         <v>30</v>
       </c>
       <c r="M39">
-        <v>603</v>
+        <v>611</v>
       </c>
       <c r="N39" s="12">
-        <v>45193</v>
+        <v>45163</v>
       </c>
       <c r="O39" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5397,7 +5407,7 @@
       </c>
       <c r="P39">
         <f t="shared" ca="1" si="4"/>
-        <v>603</v>
+        <v>611</v>
       </c>
       <c r="Q39" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5427,10 +5437,10 @@
         <v>31</v>
       </c>
       <c r="M40">
-        <v>580</v>
+        <v>603</v>
       </c>
       <c r="N40" s="12">
-        <v>45160</v>
+        <v>45193</v>
       </c>
       <c r="O40" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5438,7 +5448,7 @@
       </c>
       <c r="P40">
         <f t="shared" ca="1" si="4"/>
-        <v>580</v>
+        <v>603</v>
       </c>
       <c r="Q40" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5450,7 +5460,7 @@
         <v>45208</v>
       </c>
       <c r="C41" s="21">
-        <f t="shared" ref="C41:C50" si="8">D41-D40</f>
+        <f t="shared" ref="C41:C51" si="8">D41-D40</f>
         <v>548</v>
       </c>
       <c r="D41" s="23">
@@ -5468,10 +5478,10 @@
         <v>32</v>
       </c>
       <c r="M41">
-        <v>575</v>
+        <v>580</v>
       </c>
       <c r="N41" s="12">
-        <v>45219</v>
+        <v>45160</v>
       </c>
       <c r="O41" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5479,7 +5489,7 @@
       </c>
       <c r="P41">
         <f t="shared" ca="1" si="4"/>
-        <v>575</v>
+        <v>580</v>
       </c>
       <c r="Q41" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5509,10 +5519,10 @@
         <v>33</v>
       </c>
       <c r="M42">
-        <v>548</v>
+        <v>575</v>
       </c>
       <c r="N42" s="12">
-        <v>45208</v>
+        <v>45219</v>
       </c>
       <c r="O42" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5520,7 +5530,7 @@
       </c>
       <c r="P42">
         <f t="shared" ca="1" si="4"/>
-        <v>548</v>
+        <v>575</v>
       </c>
       <c r="Q42" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5550,10 +5560,10 @@
         <v>34</v>
       </c>
       <c r="M43">
-        <v>515</v>
+        <v>548</v>
       </c>
       <c r="N43" s="12">
-        <v>45191</v>
+        <v>45208</v>
       </c>
       <c r="O43" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5561,7 +5571,7 @@
       </c>
       <c r="P43">
         <f t="shared" ca="1" si="4"/>
-        <v>515</v>
+        <v>548</v>
       </c>
       <c r="Q43" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5591,10 +5601,10 @@
         <v>36</v>
       </c>
       <c r="M44">
-        <v>486</v>
+        <v>515</v>
       </c>
       <c r="N44" s="12">
-        <v>45141</v>
+        <v>45191</v>
       </c>
       <c r="O44" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5602,7 +5612,7 @@
       </c>
       <c r="P44">
         <f t="shared" ca="1" si="4"/>
-        <v>486</v>
+        <v>515</v>
       </c>
       <c r="Q44" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5632,10 +5642,10 @@
         <v>37</v>
       </c>
       <c r="M45">
-        <v>473</v>
+        <v>486</v>
       </c>
       <c r="N45" s="12">
-        <v>45174</v>
+        <v>45141</v>
       </c>
       <c r="O45" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5643,7 +5653,7 @@
       </c>
       <c r="P45">
         <f t="shared" ca="1" si="4"/>
-        <v>473</v>
+        <v>486</v>
       </c>
       <c r="Q45" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5674,10 +5684,10 @@
         <v>38</v>
       </c>
       <c r="M46">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="N46" s="12">
-        <v>45154</v>
+        <v>45174</v>
       </c>
       <c r="O46" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5685,7 +5695,7 @@
       </c>
       <c r="P46">
         <f t="shared" ca="1" si="4"/>
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="Q46" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5716,10 +5726,10 @@
         <v>39</v>
       </c>
       <c r="M47">
-        <v>448</v>
+        <v>467</v>
       </c>
       <c r="N47" s="12">
-        <v>45155</v>
+        <v>45154</v>
       </c>
       <c r="O47" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5727,7 +5737,7 @@
       </c>
       <c r="P47">
         <f t="shared" ca="1" si="4"/>
-        <v>448</v>
+        <v>467</v>
       </c>
       <c r="Q47" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5758,10 +5768,10 @@
         <v>35</v>
       </c>
       <c r="M48">
-        <v>419</v>
+        <v>448</v>
       </c>
       <c r="N48" s="12">
-        <v>45156</v>
+        <v>45155</v>
       </c>
       <c r="O48" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5769,7 +5779,7 @@
       </c>
       <c r="P48">
         <f t="shared" ca="1" si="4"/>
-        <v>419</v>
+        <v>448</v>
       </c>
       <c r="Q48" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5797,15 +5807,15 @@
         <v>0.92811764705882349</v>
       </c>
       <c r="M49">
-        <v>410</v>
+        <v>419</v>
       </c>
       <c r="N49" s="12">
-        <v>45209</v>
+        <v>45156</v>
       </c>
     </row>
     <row r="50" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B50" s="2">
-        <v>45223</v>
+        <v>45222</v>
       </c>
       <c r="C50" s="21">
         <f t="shared" si="8"/>
@@ -5823,29 +5833,36 @@
         <v>1.0095882352941177</v>
       </c>
       <c r="M50">
-        <v>375</v>
+        <v>410</v>
       </c>
       <c r="N50" s="12">
-        <v>45194</v>
+        <v>45209</v>
       </c>
     </row>
     <row r="51" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B51" s="28"/>
-      <c r="C51" s="21"/>
-      <c r="D51" s="23"/>
+      <c r="B51" s="2">
+        <v>45223</v>
+      </c>
+      <c r="C51" s="21">
+        <f t="shared" si="8"/>
+        <v>709</v>
+      </c>
+      <c r="D51" s="23">
+        <v>17872</v>
+      </c>
       <c r="E51" s="24">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>52.564705882352939</v>
       </c>
       <c r="F51" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1.0512941176470589</v>
       </c>
       <c r="M51">
-        <v>349</v>
-      </c>
-      <c r="N51">
-        <v>45161</v>
+        <v>375</v>
+      </c>
+      <c r="N51" s="12">
+        <v>45194</v>
       </c>
     </row>
     <row r="52" spans="2:14" x14ac:dyDescent="0.2">
@@ -5861,10 +5878,10 @@
         <v>0</v>
       </c>
       <c r="M52">
-        <v>346</v>
-      </c>
-      <c r="N52">
-        <v>45142</v>
+        <v>349</v>
+      </c>
+      <c r="N52" s="12">
+        <v>45161</v>
       </c>
     </row>
     <row r="53" spans="2:14" x14ac:dyDescent="0.2">
@@ -5880,10 +5897,10 @@
         <v>0</v>
       </c>
       <c r="M53">
-        <v>300</v>
-      </c>
-      <c r="N53">
-        <v>45181</v>
+        <v>346</v>
+      </c>
+      <c r="N53" s="12">
+        <v>45142</v>
       </c>
     </row>
     <row r="54" spans="2:14" x14ac:dyDescent="0.2">
@@ -5899,10 +5916,10 @@
         <v>0</v>
       </c>
       <c r="M54">
-        <v>272</v>
-      </c>
-      <c r="N54">
-        <v>45188</v>
+        <v>300</v>
+      </c>
+      <c r="N54" s="12">
+        <v>45181</v>
       </c>
     </row>
     <row r="55" spans="2:14" x14ac:dyDescent="0.2">
@@ -5918,10 +5935,10 @@
         <v>0</v>
       </c>
       <c r="M55">
-        <v>220</v>
-      </c>
-      <c r="N55">
-        <v>45175</v>
+        <v>272</v>
+      </c>
+      <c r="N55" s="12">
+        <v>45188</v>
       </c>
     </row>
     <row r="56" spans="2:14" x14ac:dyDescent="0.2">
@@ -5937,10 +5954,10 @@
         <v>0</v>
       </c>
       <c r="M56">
-        <v>217</v>
-      </c>
-      <c r="N56">
-        <v>45173</v>
+        <v>220</v>
+      </c>
+      <c r="N56" s="12">
+        <v>45175</v>
       </c>
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.2">
@@ -5956,10 +5973,10 @@
         <v>0</v>
       </c>
       <c r="M57">
-        <v>159</v>
-      </c>
-      <c r="N57">
-        <v>45182</v>
+        <v>217</v>
+      </c>
+      <c r="N57" s="12">
+        <v>45173</v>
       </c>
     </row>
     <row r="58" spans="2:14" x14ac:dyDescent="0.2">
@@ -5975,10 +5992,10 @@
         <v>0</v>
       </c>
       <c r="M58">
-        <v>156</v>
-      </c>
-      <c r="N58">
-        <v>45139</v>
+        <v>159</v>
+      </c>
+      <c r="N58" s="12">
+        <v>45182</v>
       </c>
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.2">
@@ -5994,10 +6011,10 @@
         <v>0</v>
       </c>
       <c r="M59">
-        <v>155</v>
-      </c>
-      <c r="N59">
-        <v>45210</v>
+        <v>156</v>
+      </c>
+      <c r="N59" s="12">
+        <v>45139</v>
       </c>
     </row>
     <row r="60" spans="2:14" x14ac:dyDescent="0.2">
@@ -6013,10 +6030,10 @@
         <v>0</v>
       </c>
       <c r="M60">
-        <v>154</v>
-      </c>
-      <c r="N60">
-        <v>45162</v>
+        <v>155</v>
+      </c>
+      <c r="N60" s="12">
+        <v>45210</v>
       </c>
     </row>
     <row r="61" spans="2:14" x14ac:dyDescent="0.2">
@@ -6032,10 +6049,10 @@
         <v>0</v>
       </c>
       <c r="M61">
-        <v>151</v>
-      </c>
-      <c r="N61">
-        <v>45196</v>
+        <v>154</v>
+      </c>
+      <c r="N61" s="12">
+        <v>45162</v>
       </c>
     </row>
     <row r="62" spans="2:14" x14ac:dyDescent="0.2">
@@ -6051,10 +6068,10 @@
         <v>0</v>
       </c>
       <c r="M62">
-        <v>146</v>
-      </c>
-      <c r="N62">
-        <v>45152</v>
+        <v>151</v>
+      </c>
+      <c r="N62" s="12">
+        <v>45196</v>
       </c>
     </row>
     <row r="63" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -6070,95 +6087,98 @@
         <v>0</v>
       </c>
       <c r="M63">
-        <v>143</v>
-      </c>
-      <c r="N63">
-        <v>45195</v>
+        <v>146</v>
+      </c>
+      <c r="N63" s="12">
+        <v>45152</v>
       </c>
     </row>
     <row r="64" spans="2:14" x14ac:dyDescent="0.2">
       <c r="M64">
         <v>143</v>
       </c>
-      <c r="N64">
-        <v>45212</v>
+      <c r="N64" s="12">
+        <v>45195</v>
       </c>
     </row>
     <row r="65" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M65">
-        <v>140</v>
-      </c>
-      <c r="N65">
-        <v>45153</v>
+        <v>143</v>
+      </c>
+      <c r="N65" s="12">
+        <v>45212</v>
       </c>
     </row>
     <row r="66" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M66">
-        <v>125</v>
-      </c>
-      <c r="N66">
-        <v>45187</v>
+        <v>140</v>
+      </c>
+      <c r="N66" s="12">
+        <v>45153</v>
       </c>
     </row>
     <row r="67" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M67">
-        <v>119</v>
-      </c>
-      <c r="N67">
-        <v>45168</v>
+        <v>125</v>
+      </c>
+      <c r="N67" s="12">
+        <v>45187</v>
       </c>
     </row>
     <row r="68" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M68">
-        <v>107</v>
-      </c>
-      <c r="N68">
-        <v>45147</v>
+        <v>119</v>
+      </c>
+      <c r="N68" s="12">
+        <v>45168</v>
       </c>
     </row>
     <row r="69" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M69">
-        <v>97</v>
-      </c>
-      <c r="N69">
-        <v>45183</v>
+        <v>107</v>
+      </c>
+      <c r="N69" s="12">
+        <v>45147</v>
       </c>
     </row>
     <row r="70" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M70">
-        <v>95</v>
-      </c>
-      <c r="N70">
-        <v>45164</v>
+        <v>97</v>
+      </c>
+      <c r="N70" s="12">
+        <v>45183</v>
       </c>
     </row>
     <row r="71" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M71">
-        <v>38</v>
-      </c>
-      <c r="N71">
-        <v>45140</v>
+        <v>95</v>
+      </c>
+      <c r="N71" s="12">
+        <v>45164</v>
       </c>
     </row>
     <row r="72" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M72">
-        <v>0</v>
-      </c>
-      <c r="N72">
-        <v>45138</v>
+        <v>38</v>
+      </c>
+      <c r="N72" s="12">
+        <v>45140</v>
       </c>
     </row>
     <row r="73" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M73">
-        <v>-1410</v>
-      </c>
-      <c r="N73">
-        <v>45218</v>
+        <v>0</v>
+      </c>
+      <c r="N73" s="12">
+        <v>45138</v>
       </c>
     </row>
     <row r="74" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M74">
-        <v>0</v>
+        <v>-1410</v>
+      </c>
+      <c r="N74" s="12">
+        <v>45218</v>
       </c>
     </row>
     <row r="75" spans="13:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Another record day - only need optimization criteria and results now
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CDCC65-B589-F340-B4AD-77A7B9539D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65C36B5-E1DD-E340-9A8C-5D981DBEFA4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="15080" windowHeight="16940" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
@@ -836,7 +836,7 @@
                   <c:v>45222</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>45223</c:v>
+                  <c:v>45224</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -983,7 +983,7 @@
                   <c:v>17163</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>17872</c:v>
+                  <c:v>18198</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1060,7 +1060,8 @@
         <c:axId val="656428208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="17000"/>
+          <c:max val="20400"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1337,22 +1338,22 @@
                   <c:v>1279</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>1025</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>1022</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>859</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>814</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>729</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>661</c:v>
@@ -1493,7 +1494,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1035</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1508,7 +1509,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>709</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -1957,7 +1958,7 @@
                   <c:v>1385</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>709</c:v>
+                  <c:v>1035</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4312,7 +4313,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4213BD91-B5D1-3B47-8D3F-04331482504C}">
   <dimension ref="A1:Q86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
@@ -4566,7 +4567,7 @@
       <c r="I12" s="30"/>
       <c r="J12" s="10">
         <f>J8-MAX(D6:D63)</f>
-        <v>-872</v>
+        <v>-1198</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
@@ -4594,7 +4595,7 @@
       <c r="I13" s="32"/>
       <c r="J13" s="10">
         <f>(AVERAGE(C7:C45)+AVERAGE(C47:C51))/2</f>
-        <v>658.34358974358975</v>
+        <v>690.94358974358977</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4622,7 +4623,7 @@
       <c r="I14" s="34"/>
       <c r="J14" s="11">
         <f>J12/J13</f>
-        <v>-1.3245363266005592</v>
+        <v>-1.7338607923760891</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
@@ -5050,22 +5051,22 @@
         <v>18</v>
       </c>
       <c r="M31">
-        <v>1025</v>
+        <v>1035</v>
       </c>
       <c r="N31" s="12">
-        <v>45221</v>
+        <v>45224</v>
       </c>
       <c r="O31" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Blue</v>
-      </c>
-      <c r="P31">
+        <v>Green</v>
+      </c>
+      <c r="P31" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1025</v>
-      </c>
-      <c r="Q31" t="str">
+        <v/>
+      </c>
+      <c r="Q31">
         <f t="shared" ca="1" si="5"/>
-        <v/>
+        <v>1035</v>
       </c>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.2">
@@ -5094,10 +5095,10 @@
         <v>19</v>
       </c>
       <c r="M32">
-        <v>1022</v>
+        <v>1025</v>
       </c>
       <c r="N32" s="12">
-        <v>45220</v>
+        <v>45221</v>
       </c>
       <c r="O32" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5105,7 +5106,7 @@
       </c>
       <c r="P32">
         <f t="shared" ca="1" si="4"/>
-        <v>1022</v>
+        <v>1025</v>
       </c>
       <c r="Q32" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5138,10 +5139,10 @@
         <v>20</v>
       </c>
       <c r="M33">
-        <v>859</v>
+        <v>1022</v>
       </c>
       <c r="N33" s="12">
-        <v>45146</v>
+        <v>45220</v>
       </c>
       <c r="O33" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5149,7 +5150,7 @@
       </c>
       <c r="P33">
         <f t="shared" ca="1" si="4"/>
-        <v>859</v>
+        <v>1022</v>
       </c>
       <c r="Q33" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5182,10 +5183,10 @@
         <v>25</v>
       </c>
       <c r="M34">
-        <v>814</v>
+        <v>859</v>
       </c>
       <c r="N34" s="12">
-        <v>45211</v>
+        <v>45146</v>
       </c>
       <c r="O34" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5193,7 +5194,7 @@
       </c>
       <c r="P34">
         <f t="shared" ca="1" si="4"/>
-        <v>814</v>
+        <v>859</v>
       </c>
       <c r="Q34" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5226,10 +5227,10 @@
         <v>26</v>
       </c>
       <c r="M35">
-        <v>729</v>
+        <v>814</v>
       </c>
       <c r="N35" s="12">
-        <v>45145</v>
+        <v>45211</v>
       </c>
       <c r="O35" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5237,7 +5238,7 @@
       </c>
       <c r="P35">
         <f t="shared" ca="1" si="4"/>
-        <v>729</v>
+        <v>814</v>
       </c>
       <c r="Q35" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5270,22 +5271,22 @@
         <v>27</v>
       </c>
       <c r="M36">
-        <v>709</v>
+        <v>729</v>
       </c>
       <c r="N36" s="12">
-        <v>45223</v>
+        <v>45145</v>
       </c>
       <c r="O36" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Green</v>
-      </c>
-      <c r="P36" t="str">
+        <v>Blue</v>
+      </c>
+      <c r="P36">
         <f t="shared" ca="1" si="4"/>
+        <v>729</v>
+      </c>
+      <c r="Q36" t="str">
+        <f t="shared" ca="1" si="5"/>
         <v/>
-      </c>
-      <c r="Q36">
-        <f t="shared" ca="1" si="5"/>
-        <v>709</v>
       </c>
     </row>
     <row r="37" spans="2:17" x14ac:dyDescent="0.2">
@@ -5841,22 +5842,22 @@
     </row>
     <row r="51" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B51" s="2">
-        <v>45223</v>
+        <v>45224</v>
       </c>
       <c r="C51" s="21">
         <f t="shared" si="8"/>
-        <v>709</v>
+        <v>1035</v>
       </c>
       <c r="D51" s="23">
-        <v>17872</v>
+        <v>18198</v>
       </c>
       <c r="E51" s="24">
         <f t="shared" si="6"/>
-        <v>52.564705882352939</v>
+        <v>53.523529411764706</v>
       </c>
       <c r="F51" s="4">
         <f t="shared" si="7"/>
-        <v>1.0512941176470589</v>
+        <v>1.0704705882352941</v>
       </c>
       <c r="M51">
         <v>375</v>

</xml_diff>

<commit_message>
Methods finished! Moved into nice template, almost done with figures
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65C36B5-E1DD-E340-9A8C-5D981DBEFA4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E520FD5E-C5BC-E044-BEA8-0D337763FEBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="15080" windowHeight="16940" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
@@ -836,7 +836,10 @@
                   <c:v>45222</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>45224</c:v>
+                  <c:v>45223</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>45225</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -968,22 +971,25 @@
                   <c:v>14566</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>13156</c:v>
+                  <c:v>12356</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>13731</c:v>
+                  <c:v>12931</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>14753</c:v>
+                  <c:v>13953</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>15778</c:v>
+                  <c:v>14978</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>17163</c:v>
+                  <c:v>16363</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>18198</c:v>
+                  <c:v>17398</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>18051</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1338,7 +1344,7 @@
                   <c:v>1279</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1035</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1025</c:v>
@@ -1362,34 +1368,34 @@
                   <c:v>657</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>611</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>603</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>580</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>575</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>548</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>515</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>486</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>473</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>467</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>448</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1494,7 +1500,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1035</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1518,7 +1524,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>653</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
@@ -1943,7 +1949,7 @@
                   <c:v>143</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>-1410</c:v>
+                  <c:v>-2210</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>575</c:v>
@@ -1959,6 +1965,9 @@
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>1035</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>653</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3918,13 +3927,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>635654</xdr:colOff>
+      <xdr:colOff>730904</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>160215</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>315273</xdr:colOff>
+      <xdr:colOff>410523</xdr:colOff>
       <xdr:row>67</xdr:row>
       <xdr:rowOff>82426</xdr:rowOff>
     </xdr:to>
@@ -3941,7 +3950,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10922654" y="5483632"/>
+          <a:off x="11134321" y="5483632"/>
           <a:ext cx="5458119" cy="8187794"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4313,8 +4322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4213BD91-B5D1-3B47-8D3F-04331482504C}">
   <dimension ref="A1:Q86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4567,7 +4576,7 @@
       <c r="I12" s="30"/>
       <c r="J12" s="10">
         <f>J8-MAX(D6:D63)</f>
-        <v>-1198</v>
+        <v>-1051</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
@@ -4623,7 +4632,7 @@
       <c r="I14" s="34"/>
       <c r="J14" s="11">
         <f>J12/J13</f>
-        <v>-1.7338607923760891</v>
+        <v>-1.5211082577523118</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
@@ -4965,7 +4974,7 @@
         <v>1385</v>
       </c>
       <c r="N29" s="12" cm="1">
-        <f t="array" ref="N29:N74">_xlfn.SORTBY(B6:B51,C6:C51, -1)</f>
+        <f t="array" ref="N29:N75">_xlfn.SORTBY(B6:B52,C6:C52, -1)</f>
         <v>45222</v>
       </c>
       <c r="O29" t="str">
@@ -5054,19 +5063,19 @@
         <v>1035</v>
       </c>
       <c r="N31" s="12">
-        <v>45224</v>
+        <v>45223</v>
       </c>
       <c r="O31" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Green</v>
-      </c>
-      <c r="P31" t="str">
+        <v>Blue</v>
+      </c>
+      <c r="P31">
         <f t="shared" ca="1" si="4"/>
+        <v>1035</v>
+      </c>
+      <c r="Q31" t="str">
+        <f t="shared" ca="1" si="5"/>
         <v/>
-      </c>
-      <c r="Q31">
-        <f t="shared" ca="1" si="5"/>
-        <v>1035</v>
       </c>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.2">
@@ -5397,22 +5406,22 @@
         <v>30</v>
       </c>
       <c r="M39">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="N39" s="12">
-        <v>45163</v>
+        <v>45225</v>
       </c>
       <c r="O39" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Blue</v>
-      </c>
-      <c r="P39">
+        <v>Green</v>
+      </c>
+      <c r="P39" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>611</v>
-      </c>
-      <c r="Q39" t="str">
+        <v/>
+      </c>
+      <c r="Q39">
         <f t="shared" ca="1" si="5"/>
-        <v/>
+        <v>653</v>
       </c>
     </row>
     <row r="40" spans="2:17" x14ac:dyDescent="0.2">
@@ -5438,10 +5447,10 @@
         <v>31</v>
       </c>
       <c r="M40">
-        <v>603</v>
+        <v>611</v>
       </c>
       <c r="N40" s="12">
-        <v>45193</v>
+        <v>45163</v>
       </c>
       <c r="O40" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5449,7 +5458,7 @@
       </c>
       <c r="P40">
         <f t="shared" ca="1" si="4"/>
-        <v>603</v>
+        <v>611</v>
       </c>
       <c r="Q40" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5461,7 +5470,7 @@
         <v>45208</v>
       </c>
       <c r="C41" s="21">
-        <f t="shared" ref="C41:C51" si="8">D41-D40</f>
+        <f t="shared" ref="C41:C52" si="8">D41-D40</f>
         <v>548</v>
       </c>
       <c r="D41" s="23">
@@ -5479,10 +5488,10 @@
         <v>32</v>
       </c>
       <c r="M41">
-        <v>580</v>
+        <v>603</v>
       </c>
       <c r="N41" s="12">
-        <v>45160</v>
+        <v>45193</v>
       </c>
       <c r="O41" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5490,7 +5499,7 @@
       </c>
       <c r="P41">
         <f t="shared" ca="1" si="4"/>
-        <v>580</v>
+        <v>603</v>
       </c>
       <c r="Q41" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5520,10 +5529,10 @@
         <v>33</v>
       </c>
       <c r="M42">
-        <v>575</v>
+        <v>580</v>
       </c>
       <c r="N42" s="12">
-        <v>45219</v>
+        <v>45160</v>
       </c>
       <c r="O42" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5531,7 +5540,7 @@
       </c>
       <c r="P42">
         <f t="shared" ca="1" si="4"/>
-        <v>575</v>
+        <v>580</v>
       </c>
       <c r="Q42" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5561,10 +5570,10 @@
         <v>34</v>
       </c>
       <c r="M43">
-        <v>548</v>
+        <v>575</v>
       </c>
       <c r="N43" s="12">
-        <v>45208</v>
+        <v>45219</v>
       </c>
       <c r="O43" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5572,7 +5581,7 @@
       </c>
       <c r="P43">
         <f t="shared" ca="1" si="4"/>
-        <v>548</v>
+        <v>575</v>
       </c>
       <c r="Q43" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5602,10 +5611,10 @@
         <v>36</v>
       </c>
       <c r="M44">
-        <v>515</v>
+        <v>548</v>
       </c>
       <c r="N44" s="12">
-        <v>45191</v>
+        <v>45208</v>
       </c>
       <c r="O44" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5613,7 +5622,7 @@
       </c>
       <c r="P44">
         <f t="shared" ca="1" si="4"/>
-        <v>515</v>
+        <v>548</v>
       </c>
       <c r="Q44" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5643,10 +5652,10 @@
         <v>37</v>
       </c>
       <c r="M45">
-        <v>486</v>
+        <v>515</v>
       </c>
       <c r="N45" s="12">
-        <v>45141</v>
+        <v>45191</v>
       </c>
       <c r="O45" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5654,7 +5663,7 @@
       </c>
       <c r="P45">
         <f t="shared" ca="1" si="4"/>
-        <v>486</v>
+        <v>515</v>
       </c>
       <c r="Q45" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5667,28 +5676,28 @@
       </c>
       <c r="C46" s="21">
         <f t="shared" si="8"/>
-        <v>-1410</v>
+        <v>-2210</v>
       </c>
       <c r="D46" s="23">
-        <f>13793-105-84-134-144-170</f>
-        <v>13156</v>
+        <f>13793-105-84-134-144-170-800</f>
+        <v>12356</v>
       </c>
       <c r="E46" s="24">
         <f t="shared" si="6"/>
-        <v>38.694117647058825</v>
+        <v>36.341176470588238</v>
       </c>
       <c r="F46" s="4">
         <f t="shared" si="7"/>
-        <v>0.77388235294117647</v>
+        <v>0.72682352941176476</v>
       </c>
       <c r="L46" t="s">
         <v>38</v>
       </c>
       <c r="M46">
-        <v>473</v>
+        <v>486</v>
       </c>
       <c r="N46" s="12">
-        <v>45174</v>
+        <v>45141</v>
       </c>
       <c r="O46" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5696,7 +5705,7 @@
       </c>
       <c r="P46">
         <f t="shared" ca="1" si="4"/>
-        <v>473</v>
+        <v>486</v>
       </c>
       <c r="Q46" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5712,25 +5721,25 @@
         <v>575</v>
       </c>
       <c r="D47" s="23">
-        <f>14368-105-84-134-144-170</f>
-        <v>13731</v>
+        <f>14368-105-84-134-144-170-800</f>
+        <v>12931</v>
       </c>
       <c r="E47" s="24">
         <f t="shared" si="6"/>
-        <v>40.385294117647057</v>
+        <v>38.03235294117647</v>
       </c>
       <c r="F47" s="4">
         <f t="shared" si="7"/>
-        <v>0.80770588235294116</v>
+        <v>0.76064705882352945</v>
       </c>
       <c r="L47" t="s">
         <v>39</v>
       </c>
       <c r="M47">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="N47" s="12">
-        <v>45154</v>
+        <v>45174</v>
       </c>
       <c r="O47" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5738,7 +5747,7 @@
       </c>
       <c r="P47">
         <f t="shared" ca="1" si="4"/>
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="Q47" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5754,25 +5763,25 @@
         <v>1022</v>
       </c>
       <c r="D48" s="23">
-        <f>15201-134-144-170</f>
-        <v>14753</v>
+        <f>15201-134-144-170-800</f>
+        <v>13953</v>
       </c>
       <c r="E48" s="24">
         <f t="shared" si="6"/>
-        <v>43.391176470588235</v>
+        <v>41.038235294117648</v>
       </c>
       <c r="F48" s="4">
         <f t="shared" si="7"/>
-        <v>0.86782352941176466</v>
+        <v>0.82076470588235295</v>
       </c>
       <c r="L48" t="s">
         <v>35</v>
       </c>
       <c r="M48">
-        <v>448</v>
+        <v>467</v>
       </c>
       <c r="N48" s="12">
-        <v>45155</v>
+        <v>45154</v>
       </c>
       <c r="O48" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5780,7 +5789,7 @@
       </c>
       <c r="P48">
         <f t="shared" ca="1" si="4"/>
-        <v>448</v>
+        <v>467</v>
       </c>
       <c r="Q48" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5796,22 +5805,22 @@
         <v>1025</v>
       </c>
       <c r="D49" s="23">
-        <f>16092-144-170</f>
-        <v>15778</v>
+        <f>16092-144-170-800</f>
+        <v>14978</v>
       </c>
       <c r="E49" s="24">
         <f t="shared" si="6"/>
-        <v>46.405882352941177</v>
+        <v>44.05294117647059</v>
       </c>
       <c r="F49" s="4">
         <f t="shared" si="7"/>
-        <v>0.92811764705882349</v>
+        <v>0.88105882352941178</v>
       </c>
       <c r="M49">
-        <v>419</v>
+        <v>448</v>
       </c>
       <c r="N49" s="12">
-        <v>45156</v>
+        <v>45155</v>
       </c>
     </row>
     <row r="50" spans="2:14" x14ac:dyDescent="0.2">
@@ -5823,66 +5832,75 @@
         <v>1385</v>
       </c>
       <c r="D50" s="23">
-        <v>17163</v>
+        <f>17163-800</f>
+        <v>16363</v>
       </c>
       <c r="E50" s="24">
         <f t="shared" si="6"/>
-        <v>50.47941176470588</v>
+        <v>48.126470588235293</v>
       </c>
       <c r="F50" s="4">
         <f t="shared" si="7"/>
-        <v>1.0095882352941177</v>
+        <v>0.96252941176470586</v>
       </c>
       <c r="M50">
-        <v>410</v>
+        <v>419</v>
       </c>
       <c r="N50" s="12">
-        <v>45209</v>
+        <v>45156</v>
       </c>
     </row>
     <row r="51" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B51" s="2">
-        <v>45224</v>
+        <v>45223</v>
       </c>
       <c r="C51" s="21">
         <f t="shared" si="8"/>
         <v>1035</v>
       </c>
       <c r="D51" s="23">
-        <v>18198</v>
+        <f>18198-800</f>
+        <v>17398</v>
       </c>
       <c r="E51" s="24">
         <f t="shared" si="6"/>
-        <v>53.523529411764706</v>
+        <v>51.170588235294119</v>
       </c>
       <c r="F51" s="4">
         <f t="shared" si="7"/>
-        <v>1.0704705882352941</v>
+        <v>1.0234117647058822</v>
       </c>
       <c r="M51">
-        <v>375</v>
+        <v>410</v>
       </c>
       <c r="N51" s="12">
-        <v>45194</v>
+        <v>45209</v>
       </c>
     </row>
     <row r="52" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B52" s="28"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="23"/>
+      <c r="B52" s="2">
+        <v>45225</v>
+      </c>
+      <c r="C52" s="21">
+        <f t="shared" si="8"/>
+        <v>653</v>
+      </c>
+      <c r="D52" s="23">
+        <v>18051</v>
+      </c>
       <c r="E52" s="24">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>53.091176470588238</v>
       </c>
       <c r="F52" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1.0618235294117646</v>
       </c>
       <c r="M52">
-        <v>349</v>
+        <v>375</v>
       </c>
       <c r="N52" s="12">
-        <v>45161</v>
+        <v>45194</v>
       </c>
     </row>
     <row r="53" spans="2:14" x14ac:dyDescent="0.2">
@@ -5898,10 +5916,10 @@
         <v>0</v>
       </c>
       <c r="M53">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="N53" s="12">
-        <v>45142</v>
+        <v>45161</v>
       </c>
     </row>
     <row r="54" spans="2:14" x14ac:dyDescent="0.2">
@@ -5917,10 +5935,10 @@
         <v>0</v>
       </c>
       <c r="M54">
-        <v>300</v>
+        <v>346</v>
       </c>
       <c r="N54" s="12">
-        <v>45181</v>
+        <v>45142</v>
       </c>
     </row>
     <row r="55" spans="2:14" x14ac:dyDescent="0.2">
@@ -5936,10 +5954,10 @@
         <v>0</v>
       </c>
       <c r="M55">
-        <v>272</v>
+        <v>300</v>
       </c>
       <c r="N55" s="12">
-        <v>45188</v>
+        <v>45181</v>
       </c>
     </row>
     <row r="56" spans="2:14" x14ac:dyDescent="0.2">
@@ -5955,10 +5973,10 @@
         <v>0</v>
       </c>
       <c r="M56">
-        <v>220</v>
+        <v>272</v>
       </c>
       <c r="N56" s="12">
-        <v>45175</v>
+        <v>45188</v>
       </c>
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.2">
@@ -5974,10 +5992,10 @@
         <v>0</v>
       </c>
       <c r="M57">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="N57" s="12">
-        <v>45173</v>
+        <v>45175</v>
       </c>
     </row>
     <row r="58" spans="2:14" x14ac:dyDescent="0.2">
@@ -5993,10 +6011,10 @@
         <v>0</v>
       </c>
       <c r="M58">
-        <v>159</v>
+        <v>217</v>
       </c>
       <c r="N58" s="12">
-        <v>45182</v>
+        <v>45173</v>
       </c>
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.2">
@@ -6012,10 +6030,10 @@
         <v>0</v>
       </c>
       <c r="M59">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="N59" s="12">
-        <v>45139</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="60" spans="2:14" x14ac:dyDescent="0.2">
@@ -6031,10 +6049,10 @@
         <v>0</v>
       </c>
       <c r="M60">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="N60" s="12">
-        <v>45210</v>
+        <v>45139</v>
       </c>
     </row>
     <row r="61" spans="2:14" x14ac:dyDescent="0.2">
@@ -6050,10 +6068,10 @@
         <v>0</v>
       </c>
       <c r="M61">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="N61" s="12">
-        <v>45162</v>
+        <v>45210</v>
       </c>
     </row>
     <row r="62" spans="2:14" x14ac:dyDescent="0.2">
@@ -6069,10 +6087,10 @@
         <v>0</v>
       </c>
       <c r="M62">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="N62" s="12">
-        <v>45196</v>
+        <v>45162</v>
       </c>
     </row>
     <row r="63" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -6088,18 +6106,18 @@
         <v>0</v>
       </c>
       <c r="M63">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="N63" s="12">
-        <v>45152</v>
+        <v>45196</v>
       </c>
     </row>
     <row r="64" spans="2:14" x14ac:dyDescent="0.2">
       <c r="M64">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="N64" s="12">
-        <v>45195</v>
+        <v>45152</v>
       </c>
     </row>
     <row r="65" spans="13:14" x14ac:dyDescent="0.2">
@@ -6107,84 +6125,87 @@
         <v>143</v>
       </c>
       <c r="N65" s="12">
-        <v>45212</v>
+        <v>45195</v>
       </c>
     </row>
     <row r="66" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M66">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="N66" s="12">
-        <v>45153</v>
+        <v>45212</v>
       </c>
     </row>
     <row r="67" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M67">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="N67" s="12">
-        <v>45187</v>
+        <v>45153</v>
       </c>
     </row>
     <row r="68" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M68">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="N68" s="12">
-        <v>45168</v>
+        <v>45187</v>
       </c>
     </row>
     <row r="69" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M69">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="N69" s="12">
-        <v>45147</v>
+        <v>45168</v>
       </c>
     </row>
     <row r="70" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M70">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="N70" s="12">
-        <v>45183</v>
+        <v>45147</v>
       </c>
     </row>
     <row r="71" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M71">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="N71" s="12">
-        <v>45164</v>
+        <v>45183</v>
       </c>
     </row>
     <row r="72" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M72">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="N72" s="12">
-        <v>45140</v>
+        <v>45164</v>
       </c>
     </row>
     <row r="73" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M73">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="N73" s="12">
-        <v>45138</v>
+        <v>45140</v>
       </c>
     </row>
     <row r="74" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M74">
-        <v>-1410</v>
+        <v>0</v>
       </c>
       <c r="N74" s="12">
-        <v>45218</v>
+        <v>45138</v>
       </c>
     </row>
     <row r="75" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M75">
-        <v>0</v>
+        <v>-2210</v>
+      </c>
+      <c r="N75">
+        <v>45218</v>
       </c>
     </row>
     <row r="76" spans="13:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
FINAL PLOTS DONE DONE + Wrote all result figure texts
Tomorrow I absolutely will write ALL missing results text
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E520FD5E-C5BC-E044-BEA8-0D337763FEBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D9D373-0038-FD42-8F87-E1EE118484CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="15080" windowHeight="16940" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
@@ -839,6 +839,9 @@
                   <c:v>45223</c:v>
                 </c:pt>
                 <c:pt idx="46">
+                  <c:v>45224</c:v>
+                </c:pt>
+                <c:pt idx="47">
                   <c:v>45225</c:v>
                 </c:pt>
               </c:numCache>
@@ -990,6 +993,9 @@
                 </c:pt>
                 <c:pt idx="46">
                   <c:v>18051</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>18776</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1362,40 +1368,40 @@
                   <c:v>729</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>725</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>661</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>657</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="11">
+                  <c:v>653</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>611</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>603</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>580</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>575</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>548</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>515</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>486</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>473</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>467</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1524,7 +1530,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>653</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
@@ -1968,6 +1974,9 @@
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>653</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>725</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4322,8 +4331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4213BD91-B5D1-3B47-8D3F-04331482504C}">
   <dimension ref="A1:Q86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4576,7 +4585,7 @@
       <c r="I12" s="30"/>
       <c r="J12" s="10">
         <f>J8-MAX(D6:D63)</f>
-        <v>-1051</v>
+        <v>-1776</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
@@ -4632,7 +4641,7 @@
       <c r="I14" s="34"/>
       <c r="J14" s="11">
         <f>J12/J13</f>
-        <v>-1.5211082577523118</v>
+        <v>-2.5703979693321655</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
@@ -4974,7 +4983,7 @@
         <v>1385</v>
       </c>
       <c r="N29" s="12" cm="1">
-        <f t="array" ref="N29:N75">_xlfn.SORTBY(B6:B52,C6:C52, -1)</f>
+        <f t="array" ref="N29:N76">_xlfn.SORTBY(B6:B53,C6:C53, -1)</f>
         <v>45222</v>
       </c>
       <c r="O29" t="str">
@@ -5324,10 +5333,10 @@
         <v>28</v>
       </c>
       <c r="M37">
-        <v>661</v>
+        <v>725</v>
       </c>
       <c r="N37" s="12">
-        <v>45159</v>
+        <v>45225</v>
       </c>
       <c r="O37" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5335,7 +5344,7 @@
       </c>
       <c r="P37">
         <f t="shared" ca="1" si="4"/>
-        <v>661</v>
+        <v>725</v>
       </c>
       <c r="Q37" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5365,10 +5374,10 @@
         <v>29</v>
       </c>
       <c r="M38">
-        <v>657</v>
+        <v>661</v>
       </c>
       <c r="N38" s="12">
-        <v>45149</v>
+        <v>45159</v>
       </c>
       <c r="O38" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5376,7 +5385,7 @@
       </c>
       <c r="P38">
         <f t="shared" ca="1" si="4"/>
-        <v>657</v>
+        <v>661</v>
       </c>
       <c r="Q38" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5406,22 +5415,22 @@
         <v>30</v>
       </c>
       <c r="M39">
-        <v>653</v>
+        <v>657</v>
       </c>
       <c r="N39" s="12">
-        <v>45225</v>
+        <v>45149</v>
       </c>
       <c r="O39" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Green</v>
-      </c>
-      <c r="P39" t="str">
+        <v>Blue</v>
+      </c>
+      <c r="P39">
         <f t="shared" ca="1" si="4"/>
+        <v>657</v>
+      </c>
+      <c r="Q39" t="str">
+        <f t="shared" ca="1" si="5"/>
         <v/>
-      </c>
-      <c r="Q39">
-        <f t="shared" ca="1" si="5"/>
-        <v>653</v>
       </c>
     </row>
     <row r="40" spans="2:17" x14ac:dyDescent="0.2">
@@ -5447,10 +5456,10 @@
         <v>31</v>
       </c>
       <c r="M40">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="N40" s="12">
-        <v>45163</v>
+        <v>45224</v>
       </c>
       <c r="O40" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5458,7 +5467,7 @@
       </c>
       <c r="P40">
         <f t="shared" ca="1" si="4"/>
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="Q40" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5470,7 +5479,7 @@
         <v>45208</v>
       </c>
       <c r="C41" s="21">
-        <f t="shared" ref="C41:C52" si="8">D41-D40</f>
+        <f t="shared" ref="C41:C53" si="8">D41-D40</f>
         <v>548</v>
       </c>
       <c r="D41" s="23">
@@ -5488,10 +5497,10 @@
         <v>32</v>
       </c>
       <c r="M41">
-        <v>603</v>
+        <v>611</v>
       </c>
       <c r="N41" s="12">
-        <v>45193</v>
+        <v>45163</v>
       </c>
       <c r="O41" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5499,7 +5508,7 @@
       </c>
       <c r="P41">
         <f t="shared" ca="1" si="4"/>
-        <v>603</v>
+        <v>611</v>
       </c>
       <c r="Q41" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5529,10 +5538,10 @@
         <v>33</v>
       </c>
       <c r="M42">
-        <v>580</v>
+        <v>603</v>
       </c>
       <c r="N42" s="12">
-        <v>45160</v>
+        <v>45193</v>
       </c>
       <c r="O42" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5540,7 +5549,7 @@
       </c>
       <c r="P42">
         <f t="shared" ca="1" si="4"/>
-        <v>580</v>
+        <v>603</v>
       </c>
       <c r="Q42" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5570,10 +5579,10 @@
         <v>34</v>
       </c>
       <c r="M43">
-        <v>575</v>
+        <v>580</v>
       </c>
       <c r="N43" s="12">
-        <v>45219</v>
+        <v>45160</v>
       </c>
       <c r="O43" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5581,7 +5590,7 @@
       </c>
       <c r="P43">
         <f t="shared" ca="1" si="4"/>
-        <v>575</v>
+        <v>580</v>
       </c>
       <c r="Q43" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5611,10 +5620,10 @@
         <v>36</v>
       </c>
       <c r="M44">
-        <v>548</v>
+        <v>575</v>
       </c>
       <c r="N44" s="12">
-        <v>45208</v>
+        <v>45219</v>
       </c>
       <c r="O44" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5622,7 +5631,7 @@
       </c>
       <c r="P44">
         <f t="shared" ca="1" si="4"/>
-        <v>548</v>
+        <v>575</v>
       </c>
       <c r="Q44" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5652,10 +5661,10 @@
         <v>37</v>
       </c>
       <c r="M45">
-        <v>515</v>
+        <v>548</v>
       </c>
       <c r="N45" s="12">
-        <v>45191</v>
+        <v>45208</v>
       </c>
       <c r="O45" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5663,7 +5672,7 @@
       </c>
       <c r="P45">
         <f t="shared" ca="1" si="4"/>
-        <v>515</v>
+        <v>548</v>
       </c>
       <c r="Q45" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5694,10 +5703,10 @@
         <v>38</v>
       </c>
       <c r="M46">
-        <v>486</v>
+        <v>515</v>
       </c>
       <c r="N46" s="12">
-        <v>45141</v>
+        <v>45191</v>
       </c>
       <c r="O46" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5705,7 +5714,7 @@
       </c>
       <c r="P46">
         <f t="shared" ca="1" si="4"/>
-        <v>486</v>
+        <v>515</v>
       </c>
       <c r="Q46" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5736,10 +5745,10 @@
         <v>39</v>
       </c>
       <c r="M47">
-        <v>473</v>
+        <v>486</v>
       </c>
       <c r="N47" s="12">
-        <v>45174</v>
+        <v>45141</v>
       </c>
       <c r="O47" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5747,7 +5756,7 @@
       </c>
       <c r="P47">
         <f t="shared" ca="1" si="4"/>
-        <v>473</v>
+        <v>486</v>
       </c>
       <c r="Q47" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5778,10 +5787,10 @@
         <v>35</v>
       </c>
       <c r="M48">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="N48" s="12">
-        <v>45154</v>
+        <v>45174</v>
       </c>
       <c r="O48" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5789,7 +5798,7 @@
       </c>
       <c r="P48">
         <f t="shared" ca="1" si="4"/>
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="Q48" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5817,10 +5826,10 @@
         <v>0.88105882352941178</v>
       </c>
       <c r="M49">
-        <v>448</v>
+        <v>467</v>
       </c>
       <c r="N49" s="12">
-        <v>45155</v>
+        <v>45154</v>
       </c>
     </row>
     <row r="50" spans="2:14" x14ac:dyDescent="0.2">
@@ -5844,10 +5853,10 @@
         <v>0.96252941176470586</v>
       </c>
       <c r="M50">
-        <v>419</v>
+        <v>448</v>
       </c>
       <c r="N50" s="12">
-        <v>45156</v>
+        <v>45155</v>
       </c>
     </row>
     <row r="51" spans="2:14" x14ac:dyDescent="0.2">
@@ -5871,15 +5880,15 @@
         <v>1.0234117647058822</v>
       </c>
       <c r="M51">
-        <v>410</v>
+        <v>419</v>
       </c>
       <c r="N51" s="12">
-        <v>45209</v>
+        <v>45156</v>
       </c>
     </row>
     <row r="52" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B52" s="2">
-        <v>45225</v>
+        <v>45224</v>
       </c>
       <c r="C52" s="21">
         <f t="shared" si="8"/>
@@ -5897,29 +5906,36 @@
         <v>1.0618235294117646</v>
       </c>
       <c r="M52">
-        <v>375</v>
+        <v>410</v>
       </c>
       <c r="N52" s="12">
-        <v>45194</v>
+        <v>45209</v>
       </c>
     </row>
     <row r="53" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B53" s="28"/>
-      <c r="C53" s="21"/>
-      <c r="D53" s="23"/>
+      <c r="B53" s="2">
+        <v>45225</v>
+      </c>
+      <c r="C53" s="21">
+        <f t="shared" si="8"/>
+        <v>725</v>
+      </c>
+      <c r="D53" s="23">
+        <v>18776</v>
+      </c>
       <c r="E53" s="24">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>55.223529411764709</v>
       </c>
       <c r="F53" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1.1044705882352941</v>
       </c>
       <c r="M53">
-        <v>349</v>
+        <v>375</v>
       </c>
       <c r="N53" s="12">
-        <v>45161</v>
+        <v>45194</v>
       </c>
     </row>
     <row r="54" spans="2:14" x14ac:dyDescent="0.2">
@@ -5935,10 +5951,10 @@
         <v>0</v>
       </c>
       <c r="M54">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="N54" s="12">
-        <v>45142</v>
+        <v>45161</v>
       </c>
     </row>
     <row r="55" spans="2:14" x14ac:dyDescent="0.2">
@@ -5954,10 +5970,10 @@
         <v>0</v>
       </c>
       <c r="M55">
-        <v>300</v>
+        <v>346</v>
       </c>
       <c r="N55" s="12">
-        <v>45181</v>
+        <v>45142</v>
       </c>
     </row>
     <row r="56" spans="2:14" x14ac:dyDescent="0.2">
@@ -5973,10 +5989,10 @@
         <v>0</v>
       </c>
       <c r="M56">
-        <v>272</v>
+        <v>300</v>
       </c>
       <c r="N56" s="12">
-        <v>45188</v>
+        <v>45181</v>
       </c>
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.2">
@@ -5992,10 +6008,10 @@
         <v>0</v>
       </c>
       <c r="M57">
-        <v>220</v>
+        <v>272</v>
       </c>
       <c r="N57" s="12">
-        <v>45175</v>
+        <v>45188</v>
       </c>
     </row>
     <row r="58" spans="2:14" x14ac:dyDescent="0.2">
@@ -6011,10 +6027,10 @@
         <v>0</v>
       </c>
       <c r="M58">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="N58" s="12">
-        <v>45173</v>
+        <v>45175</v>
       </c>
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.2">
@@ -6030,10 +6046,10 @@
         <v>0</v>
       </c>
       <c r="M59">
-        <v>159</v>
+        <v>217</v>
       </c>
       <c r="N59" s="12">
-        <v>45182</v>
+        <v>45173</v>
       </c>
     </row>
     <row r="60" spans="2:14" x14ac:dyDescent="0.2">
@@ -6049,10 +6065,10 @@
         <v>0</v>
       </c>
       <c r="M60">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="N60" s="12">
-        <v>45139</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="61" spans="2:14" x14ac:dyDescent="0.2">
@@ -6068,10 +6084,10 @@
         <v>0</v>
       </c>
       <c r="M61">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="N61" s="12">
-        <v>45210</v>
+        <v>45139</v>
       </c>
     </row>
     <row r="62" spans="2:14" x14ac:dyDescent="0.2">
@@ -6087,10 +6103,10 @@
         <v>0</v>
       </c>
       <c r="M62">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="N62" s="12">
-        <v>45162</v>
+        <v>45210</v>
       </c>
     </row>
     <row r="63" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -6106,26 +6122,26 @@
         <v>0</v>
       </c>
       <c r="M63">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="N63" s="12">
-        <v>45196</v>
+        <v>45162</v>
       </c>
     </row>
     <row r="64" spans="2:14" x14ac:dyDescent="0.2">
       <c r="M64">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="N64" s="12">
-        <v>45152</v>
+        <v>45196</v>
       </c>
     </row>
     <row r="65" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M65">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="N65" s="12">
-        <v>45195</v>
+        <v>45152</v>
       </c>
     </row>
     <row r="66" spans="13:14" x14ac:dyDescent="0.2">
@@ -6133,84 +6149,87 @@
         <v>143</v>
       </c>
       <c r="N66" s="12">
-        <v>45212</v>
+        <v>45195</v>
       </c>
     </row>
     <row r="67" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M67">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="N67" s="12">
-        <v>45153</v>
+        <v>45212</v>
       </c>
     </row>
     <row r="68" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M68">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="N68" s="12">
-        <v>45187</v>
+        <v>45153</v>
       </c>
     </row>
     <row r="69" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M69">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="N69" s="12">
-        <v>45168</v>
+        <v>45187</v>
       </c>
     </row>
     <row r="70" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M70">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="N70" s="12">
-        <v>45147</v>
+        <v>45168</v>
       </c>
     </row>
     <row r="71" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M71">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="N71" s="12">
-        <v>45183</v>
+        <v>45147</v>
       </c>
     </row>
     <row r="72" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M72">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="N72" s="12">
-        <v>45164</v>
+        <v>45183</v>
       </c>
     </row>
     <row r="73" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M73">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="N73" s="12">
-        <v>45140</v>
+        <v>45164</v>
       </c>
     </row>
     <row r="74" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M74">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="N74" s="12">
-        <v>45138</v>
+        <v>45140</v>
       </c>
     </row>
     <row r="75" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M75">
-        <v>-2210</v>
+        <v>0</v>
       </c>
       <c r="N75">
-        <v>45218</v>
+        <v>45138</v>
       </c>
     </row>
     <row r="76" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M76">
-        <v>0</v>
+        <v>-2210</v>
+      </c>
+      <c r="N76">
+        <v>45218</v>
       </c>
     </row>
     <row r="77" spans="13:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Biggest writing day EVER! Just shy of 6 pages!!
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D9D373-0038-FD42-8F87-E1EE118484CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24C742D1-F4A5-5C4B-A5D4-EBE88B50990A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="15080" windowHeight="16940" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
@@ -844,6 +844,9 @@
                 <c:pt idx="47">
                   <c:v>45225</c:v>
                 </c:pt>
+                <c:pt idx="48">
+                  <c:v>45227</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -974,28 +977,31 @@
                   <c:v>14566</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>12356</c:v>
+                  <c:v>11918</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>12931</c:v>
+                  <c:v>12493</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>13953</c:v>
+                  <c:v>13515</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>14978</c:v>
+                  <c:v>14540</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>16363</c:v>
+                  <c:v>15925</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>17398</c:v>
+                  <c:v>16960</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>18051</c:v>
+                  <c:v>17613</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>18776</c:v>
+                  <c:v>18338</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>20356</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1344,64 +1350,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1385</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>1279</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>1035</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>1025</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>1022</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>859</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>814</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>729</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>725</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>661</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>657</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>653</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>611</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>603</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>580</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>575</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>548</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>515</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>486</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>473</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1500,7 +1506,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2018</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1955,7 +1961,7 @@
                   <c:v>143</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>-2210</c:v>
+                  <c:v>-2648</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>575</c:v>
@@ -1977,6 +1983,9 @@
                 </c:pt>
                 <c:pt idx="46">
                   <c:v>725</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2018</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4331,8 +4340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4213BD91-B5D1-3B47-8D3F-04331482504C}">
   <dimension ref="A1:Q86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4585,7 +4594,7 @@
       <c r="I12" s="30"/>
       <c r="J12" s="10">
         <f>J8-MAX(D6:D63)</f>
-        <v>-1776</v>
+        <v>-3356</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
@@ -4641,7 +4650,7 @@
       <c r="I14" s="34"/>
       <c r="J14" s="11">
         <f>J12/J13</f>
-        <v>-2.5703979693321655</v>
+        <v>-4.8571258924992948</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
@@ -4980,23 +4989,23 @@
       </c>
       <c r="M29" cm="1">
         <f t="array" ref="M29:M86">_xlfn.SORTBY(C6:C63, C6:C63, -1)</f>
-        <v>1385</v>
+        <v>2018</v>
       </c>
       <c r="N29" s="12" cm="1">
-        <f t="array" ref="N29:N76">_xlfn.SORTBY(B6:B53,C6:C53, -1)</f>
-        <v>45222</v>
+        <f t="array" ref="N29:N77">_xlfn.SORTBY(B6:B54,C6:C54, -1)</f>
+        <v>45227</v>
       </c>
       <c r="O29" t="str">
         <f ca="1">IF(N29=TODAY(), "Green", "Blue")</f>
-        <v>Blue</v>
-      </c>
-      <c r="P29">
+        <v>Green</v>
+      </c>
+      <c r="P29" t="str">
         <f ca="1">IF(NOT(N29=TODAY()), M29, "")</f>
-        <v>1385</v>
-      </c>
-      <c r="Q29" t="str">
+        <v/>
+      </c>
+      <c r="Q29">
         <f ca="1">IF(N29=TODAY(), M29, "")</f>
-        <v/>
+        <v>2018</v>
       </c>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.2">
@@ -5025,10 +5034,10 @@
         <v>17</v>
       </c>
       <c r="M30">
-        <v>1279</v>
+        <v>1385</v>
       </c>
       <c r="N30" s="12">
-        <v>45148</v>
+        <v>45222</v>
       </c>
       <c r="O30" t="str">
         <f t="shared" ref="O30:O48" ca="1" si="3">IF(N30=TODAY(), "Green", "Blue")</f>
@@ -5036,7 +5045,7 @@
       </c>
       <c r="P30">
         <f t="shared" ref="P30:P48" ca="1" si="4">IF(NOT(N30=TODAY()), M30, "")</f>
-        <v>1279</v>
+        <v>1385</v>
       </c>
       <c r="Q30" t="str">
         <f t="shared" ref="Q30:Q48" ca="1" si="5">IF(N30=TODAY(), M30, "")</f>
@@ -5069,10 +5078,10 @@
         <v>18</v>
       </c>
       <c r="M31">
-        <v>1035</v>
+        <v>1279</v>
       </c>
       <c r="N31" s="12">
-        <v>45223</v>
+        <v>45148</v>
       </c>
       <c r="O31" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5080,7 +5089,7 @@
       </c>
       <c r="P31">
         <f t="shared" ca="1" si="4"/>
-        <v>1035</v>
+        <v>1279</v>
       </c>
       <c r="Q31" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5113,10 +5122,10 @@
         <v>19</v>
       </c>
       <c r="M32">
-        <v>1025</v>
+        <v>1035</v>
       </c>
       <c r="N32" s="12">
-        <v>45221</v>
+        <v>45223</v>
       </c>
       <c r="O32" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5124,7 +5133,7 @@
       </c>
       <c r="P32">
         <f t="shared" ca="1" si="4"/>
-        <v>1025</v>
+        <v>1035</v>
       </c>
       <c r="Q32" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5157,10 +5166,10 @@
         <v>20</v>
       </c>
       <c r="M33">
-        <v>1022</v>
+        <v>1025</v>
       </c>
       <c r="N33" s="12">
-        <v>45220</v>
+        <v>45221</v>
       </c>
       <c r="O33" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5168,7 +5177,7 @@
       </c>
       <c r="P33">
         <f t="shared" ca="1" si="4"/>
-        <v>1022</v>
+        <v>1025</v>
       </c>
       <c r="Q33" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5201,10 +5210,10 @@
         <v>25</v>
       </c>
       <c r="M34">
-        <v>859</v>
+        <v>1022</v>
       </c>
       <c r="N34" s="12">
-        <v>45146</v>
+        <v>45220</v>
       </c>
       <c r="O34" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5212,7 +5221,7 @@
       </c>
       <c r="P34">
         <f t="shared" ca="1" si="4"/>
-        <v>859</v>
+        <v>1022</v>
       </c>
       <c r="Q34" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5245,10 +5254,10 @@
         <v>26</v>
       </c>
       <c r="M35">
-        <v>814</v>
+        <v>859</v>
       </c>
       <c r="N35" s="12">
-        <v>45211</v>
+        <v>45146</v>
       </c>
       <c r="O35" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5256,7 +5265,7 @@
       </c>
       <c r="P35">
         <f t="shared" ca="1" si="4"/>
-        <v>814</v>
+        <v>859</v>
       </c>
       <c r="Q35" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5289,10 +5298,10 @@
         <v>27</v>
       </c>
       <c r="M36">
-        <v>729</v>
+        <v>814</v>
       </c>
       <c r="N36" s="12">
-        <v>45145</v>
+        <v>45211</v>
       </c>
       <c r="O36" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5300,7 +5309,7 @@
       </c>
       <c r="P36">
         <f t="shared" ca="1" si="4"/>
-        <v>729</v>
+        <v>814</v>
       </c>
       <c r="Q36" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5333,10 +5342,10 @@
         <v>28</v>
       </c>
       <c r="M37">
-        <v>725</v>
+        <v>729</v>
       </c>
       <c r="N37" s="12">
-        <v>45225</v>
+        <v>45145</v>
       </c>
       <c r="O37" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5344,7 +5353,7 @@
       </c>
       <c r="P37">
         <f t="shared" ca="1" si="4"/>
-        <v>725</v>
+        <v>729</v>
       </c>
       <c r="Q37" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5374,10 +5383,10 @@
         <v>29</v>
       </c>
       <c r="M38">
-        <v>661</v>
+        <v>725</v>
       </c>
       <c r="N38" s="12">
-        <v>45159</v>
+        <v>45225</v>
       </c>
       <c r="O38" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5385,7 +5394,7 @@
       </c>
       <c r="P38">
         <f t="shared" ca="1" si="4"/>
-        <v>661</v>
+        <v>725</v>
       </c>
       <c r="Q38" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5415,10 +5424,10 @@
         <v>30</v>
       </c>
       <c r="M39">
-        <v>657</v>
+        <v>661</v>
       </c>
       <c r="N39" s="12">
-        <v>45149</v>
+        <v>45159</v>
       </c>
       <c r="O39" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5426,7 +5435,7 @@
       </c>
       <c r="P39">
         <f t="shared" ca="1" si="4"/>
-        <v>657</v>
+        <v>661</v>
       </c>
       <c r="Q39" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5456,10 +5465,10 @@
         <v>31</v>
       </c>
       <c r="M40">
-        <v>653</v>
+        <v>657</v>
       </c>
       <c r="N40" s="12">
-        <v>45224</v>
+        <v>45149</v>
       </c>
       <c r="O40" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5467,7 +5476,7 @@
       </c>
       <c r="P40">
         <f t="shared" ca="1" si="4"/>
-        <v>653</v>
+        <v>657</v>
       </c>
       <c r="Q40" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5479,7 +5488,7 @@
         <v>45208</v>
       </c>
       <c r="C41" s="21">
-        <f t="shared" ref="C41:C53" si="8">D41-D40</f>
+        <f t="shared" ref="C41:C54" si="8">D41-D40</f>
         <v>548</v>
       </c>
       <c r="D41" s="23">
@@ -5497,10 +5506,10 @@
         <v>32</v>
       </c>
       <c r="M41">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="N41" s="12">
-        <v>45163</v>
+        <v>45224</v>
       </c>
       <c r="O41" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5508,7 +5517,7 @@
       </c>
       <c r="P41">
         <f t="shared" ca="1" si="4"/>
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="Q41" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5538,10 +5547,10 @@
         <v>33</v>
       </c>
       <c r="M42">
-        <v>603</v>
+        <v>611</v>
       </c>
       <c r="N42" s="12">
-        <v>45193</v>
+        <v>45163</v>
       </c>
       <c r="O42" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5549,7 +5558,7 @@
       </c>
       <c r="P42">
         <f t="shared" ca="1" si="4"/>
-        <v>603</v>
+        <v>611</v>
       </c>
       <c r="Q42" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5579,10 +5588,10 @@
         <v>34</v>
       </c>
       <c r="M43">
-        <v>580</v>
+        <v>603</v>
       </c>
       <c r="N43" s="12">
-        <v>45160</v>
+        <v>45193</v>
       </c>
       <c r="O43" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5590,7 +5599,7 @@
       </c>
       <c r="P43">
         <f t="shared" ca="1" si="4"/>
-        <v>580</v>
+        <v>603</v>
       </c>
       <c r="Q43" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5620,10 +5629,10 @@
         <v>36</v>
       </c>
       <c r="M44">
-        <v>575</v>
+        <v>580</v>
       </c>
       <c r="N44" s="12">
-        <v>45219</v>
+        <v>45160</v>
       </c>
       <c r="O44" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5631,7 +5640,7 @@
       </c>
       <c r="P44">
         <f t="shared" ca="1" si="4"/>
-        <v>575</v>
+        <v>580</v>
       </c>
       <c r="Q44" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5661,10 +5670,10 @@
         <v>37</v>
       </c>
       <c r="M45">
-        <v>548</v>
+        <v>575</v>
       </c>
       <c r="N45" s="12">
-        <v>45208</v>
+        <v>45219</v>
       </c>
       <c r="O45" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5672,7 +5681,7 @@
       </c>
       <c r="P45">
         <f t="shared" ca="1" si="4"/>
-        <v>548</v>
+        <v>575</v>
       </c>
       <c r="Q45" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5685,28 +5694,28 @@
       </c>
       <c r="C46" s="21">
         <f t="shared" si="8"/>
-        <v>-2210</v>
+        <v>-2648</v>
       </c>
       <c r="D46" s="23">
-        <f>13793-105-84-134-144-170-800</f>
-        <v>12356</v>
+        <f>13793-105-84-134-144-170-800-438</f>
+        <v>11918</v>
       </c>
       <c r="E46" s="24">
         <f t="shared" si="6"/>
-        <v>36.341176470588238</v>
+        <v>35.05294117647059</v>
       </c>
       <c r="F46" s="4">
         <f t="shared" si="7"/>
-        <v>0.72682352941176476</v>
+        <v>0.70105882352941173</v>
       </c>
       <c r="L46" t="s">
         <v>38</v>
       </c>
       <c r="M46">
-        <v>515</v>
+        <v>548</v>
       </c>
       <c r="N46" s="12">
-        <v>45191</v>
+        <v>45208</v>
       </c>
       <c r="O46" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5714,7 +5723,7 @@
       </c>
       <c r="P46">
         <f t="shared" ca="1" si="4"/>
-        <v>515</v>
+        <v>548</v>
       </c>
       <c r="Q46" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5730,25 +5739,25 @@
         <v>575</v>
       </c>
       <c r="D47" s="23">
-        <f>14368-105-84-134-144-170-800</f>
-        <v>12931</v>
+        <f>14368-105-84-134-144-170-800-438</f>
+        <v>12493</v>
       </c>
       <c r="E47" s="24">
         <f t="shared" si="6"/>
-        <v>38.03235294117647</v>
+        <v>36.744117647058822</v>
       </c>
       <c r="F47" s="4">
         <f t="shared" si="7"/>
-        <v>0.76064705882352945</v>
+        <v>0.73488235294117643</v>
       </c>
       <c r="L47" t="s">
         <v>39</v>
       </c>
       <c r="M47">
-        <v>486</v>
+        <v>515</v>
       </c>
       <c r="N47" s="12">
-        <v>45141</v>
+        <v>45191</v>
       </c>
       <c r="O47" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5756,7 +5765,7 @@
       </c>
       <c r="P47">
         <f t="shared" ca="1" si="4"/>
-        <v>486</v>
+        <v>515</v>
       </c>
       <c r="Q47" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5772,25 +5781,25 @@
         <v>1022</v>
       </c>
       <c r="D48" s="23">
-        <f>15201-134-144-170-800</f>
-        <v>13953</v>
+        <f>15201-134-144-170-800-438</f>
+        <v>13515</v>
       </c>
       <c r="E48" s="24">
         <f t="shared" si="6"/>
-        <v>41.038235294117648</v>
+        <v>39.75</v>
       </c>
       <c r="F48" s="4">
         <f t="shared" si="7"/>
-        <v>0.82076470588235295</v>
+        <v>0.79500000000000004</v>
       </c>
       <c r="L48" t="s">
         <v>35</v>
       </c>
       <c r="M48">
-        <v>473</v>
+        <v>486</v>
       </c>
       <c r="N48" s="12">
-        <v>45174</v>
+        <v>45141</v>
       </c>
       <c r="O48" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5798,7 +5807,7 @@
       </c>
       <c r="P48">
         <f t="shared" ca="1" si="4"/>
-        <v>473</v>
+        <v>486</v>
       </c>
       <c r="Q48" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5814,22 +5823,22 @@
         <v>1025</v>
       </c>
       <c r="D49" s="23">
-        <f>16092-144-170-800</f>
-        <v>14978</v>
+        <f>16092-144-170-800-438</f>
+        <v>14540</v>
       </c>
       <c r="E49" s="24">
         <f t="shared" si="6"/>
-        <v>44.05294117647059</v>
+        <v>42.764705882352942</v>
       </c>
       <c r="F49" s="4">
         <f t="shared" si="7"/>
-        <v>0.88105882352941178</v>
+        <v>0.85529411764705887</v>
       </c>
       <c r="M49">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="N49" s="12">
-        <v>45154</v>
+        <v>45174</v>
       </c>
     </row>
     <row r="50" spans="2:14" x14ac:dyDescent="0.2">
@@ -5841,22 +5850,22 @@
         <v>1385</v>
       </c>
       <c r="D50" s="23">
-        <f>17163-800</f>
-        <v>16363</v>
+        <f>17163-800-438</f>
+        <v>15925</v>
       </c>
       <c r="E50" s="24">
         <f t="shared" si="6"/>
-        <v>48.126470588235293</v>
+        <v>46.838235294117645</v>
       </c>
       <c r="F50" s="4">
         <f t="shared" si="7"/>
-        <v>0.96252941176470586</v>
+        <v>0.93676470588235294</v>
       </c>
       <c r="M50">
-        <v>448</v>
+        <v>467</v>
       </c>
       <c r="N50" s="12">
-        <v>45155</v>
+        <v>45154</v>
       </c>
     </row>
     <row r="51" spans="2:14" x14ac:dyDescent="0.2">
@@ -5868,22 +5877,22 @@
         <v>1035</v>
       </c>
       <c r="D51" s="23">
-        <f>18198-800</f>
-        <v>17398</v>
+        <f>18198-800-438</f>
+        <v>16960</v>
       </c>
       <c r="E51" s="24">
         <f t="shared" si="6"/>
-        <v>51.170588235294119</v>
+        <v>49.882352941176471</v>
       </c>
       <c r="F51" s="4">
         <f t="shared" si="7"/>
-        <v>1.0234117647058822</v>
+        <v>0.99764705882352944</v>
       </c>
       <c r="M51">
-        <v>419</v>
+        <v>448</v>
       </c>
       <c r="N51" s="12">
-        <v>45156</v>
+        <v>45155</v>
       </c>
     </row>
     <row r="52" spans="2:14" x14ac:dyDescent="0.2">
@@ -5895,21 +5904,22 @@
         <v>653</v>
       </c>
       <c r="D52" s="23">
-        <v>18051</v>
+        <f>18051-438</f>
+        <v>17613</v>
       </c>
       <c r="E52" s="24">
         <f t="shared" si="6"/>
-        <v>53.091176470588238</v>
+        <v>51.80294117647059</v>
       </c>
       <c r="F52" s="4">
         <f t="shared" si="7"/>
-        <v>1.0618235294117646</v>
+        <v>1.0360588235294117</v>
       </c>
       <c r="M52">
-        <v>410</v>
+        <v>419</v>
       </c>
       <c r="N52" s="12">
-        <v>45209</v>
+        <v>45156</v>
       </c>
     </row>
     <row r="53" spans="2:14" x14ac:dyDescent="0.2">
@@ -5921,40 +5931,48 @@
         <v>725</v>
       </c>
       <c r="D53" s="23">
-        <v>18776</v>
+        <f>18776-438</f>
+        <v>18338</v>
       </c>
       <c r="E53" s="24">
         <f t="shared" si="6"/>
-        <v>55.223529411764709</v>
+        <v>53.935294117647061</v>
       </c>
       <c r="F53" s="4">
         <f t="shared" si="7"/>
-        <v>1.1044705882352941</v>
+        <v>1.0787058823529412</v>
       </c>
       <c r="M53">
-        <v>375</v>
+        <v>410</v>
       </c>
       <c r="N53" s="12">
-        <v>45194</v>
+        <v>45209</v>
       </c>
     </row>
     <row r="54" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B54" s="28"/>
-      <c r="C54" s="21"/>
-      <c r="D54" s="23"/>
+      <c r="B54" s="2">
+        <v>45227</v>
+      </c>
+      <c r="C54" s="21">
+        <f t="shared" si="8"/>
+        <v>2018</v>
+      </c>
+      <c r="D54" s="23">
+        <v>20356</v>
+      </c>
       <c r="E54" s="24">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>59.870588235294115</v>
       </c>
       <c r="F54" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1.1974117647058824</v>
       </c>
       <c r="M54">
-        <v>349</v>
+        <v>375</v>
       </c>
       <c r="N54" s="12">
-        <v>45161</v>
+        <v>45194</v>
       </c>
     </row>
     <row r="55" spans="2:14" x14ac:dyDescent="0.2">
@@ -5970,10 +5988,10 @@
         <v>0</v>
       </c>
       <c r="M55">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="N55" s="12">
-        <v>45142</v>
+        <v>45161</v>
       </c>
     </row>
     <row r="56" spans="2:14" x14ac:dyDescent="0.2">
@@ -5989,10 +6007,10 @@
         <v>0</v>
       </c>
       <c r="M56">
-        <v>300</v>
+        <v>346</v>
       </c>
       <c r="N56" s="12">
-        <v>45181</v>
+        <v>45142</v>
       </c>
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.2">
@@ -6008,10 +6026,10 @@
         <v>0</v>
       </c>
       <c r="M57">
-        <v>272</v>
+        <v>300</v>
       </c>
       <c r="N57" s="12">
-        <v>45188</v>
+        <v>45181</v>
       </c>
     </row>
     <row r="58" spans="2:14" x14ac:dyDescent="0.2">
@@ -6027,10 +6045,10 @@
         <v>0</v>
       </c>
       <c r="M58">
-        <v>220</v>
+        <v>272</v>
       </c>
       <c r="N58" s="12">
-        <v>45175</v>
+        <v>45188</v>
       </c>
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.2">
@@ -6046,10 +6064,10 @@
         <v>0</v>
       </c>
       <c r="M59">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="N59" s="12">
-        <v>45173</v>
+        <v>45175</v>
       </c>
     </row>
     <row r="60" spans="2:14" x14ac:dyDescent="0.2">
@@ -6065,10 +6083,10 @@
         <v>0</v>
       </c>
       <c r="M60">
-        <v>159</v>
+        <v>217</v>
       </c>
       <c r="N60" s="12">
-        <v>45182</v>
+        <v>45173</v>
       </c>
     </row>
     <row r="61" spans="2:14" x14ac:dyDescent="0.2">
@@ -6084,10 +6102,10 @@
         <v>0</v>
       </c>
       <c r="M61">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="N61" s="12">
-        <v>45139</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="62" spans="2:14" x14ac:dyDescent="0.2">
@@ -6103,10 +6121,10 @@
         <v>0</v>
       </c>
       <c r="M62">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="N62" s="12">
-        <v>45210</v>
+        <v>45139</v>
       </c>
     </row>
     <row r="63" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -6122,34 +6140,34 @@
         <v>0</v>
       </c>
       <c r="M63">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="N63" s="12">
-        <v>45162</v>
+        <v>45210</v>
       </c>
     </row>
     <row r="64" spans="2:14" x14ac:dyDescent="0.2">
       <c r="M64">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="N64" s="12">
-        <v>45196</v>
+        <v>45162</v>
       </c>
     </row>
     <row r="65" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M65">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="N65" s="12">
-        <v>45152</v>
+        <v>45196</v>
       </c>
     </row>
     <row r="66" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M66">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="N66" s="12">
-        <v>45195</v>
+        <v>45152</v>
       </c>
     </row>
     <row r="67" spans="13:14" x14ac:dyDescent="0.2">
@@ -6157,84 +6175,87 @@
         <v>143</v>
       </c>
       <c r="N67" s="12">
-        <v>45212</v>
+        <v>45195</v>
       </c>
     </row>
     <row r="68" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M68">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="N68" s="12">
-        <v>45153</v>
+        <v>45212</v>
       </c>
     </row>
     <row r="69" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M69">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="N69" s="12">
-        <v>45187</v>
+        <v>45153</v>
       </c>
     </row>
     <row r="70" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M70">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="N70" s="12">
-        <v>45168</v>
+        <v>45187</v>
       </c>
     </row>
     <row r="71" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M71">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="N71" s="12">
-        <v>45147</v>
+        <v>45168</v>
       </c>
     </row>
     <row r="72" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M72">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="N72" s="12">
-        <v>45183</v>
+        <v>45147</v>
       </c>
     </row>
     <row r="73" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M73">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="N73" s="12">
-        <v>45164</v>
+        <v>45183</v>
       </c>
     </row>
     <row r="74" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M74">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="N74" s="12">
-        <v>45140</v>
+        <v>45164</v>
       </c>
     </row>
     <row r="75" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M75">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="N75">
-        <v>45138</v>
+        <v>45140</v>
       </c>
     </row>
     <row r="76" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M76">
-        <v>-2210</v>
+        <v>0</v>
       </c>
       <c r="N76">
-        <v>45218</v>
+        <v>45138</v>
       </c>
     </row>
     <row r="77" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M77">
-        <v>0</v>
+        <v>-2648</v>
+      </c>
+      <c r="N77">
+        <v>45218</v>
       </c>
     </row>
     <row r="78" spans="13:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Another insane writing day
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24C742D1-F4A5-5C4B-A5D4-EBE88B50990A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A114A095-9D38-E14D-9B4E-A7B9BDD7D9E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="15080" windowHeight="16940" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Keeping up with the thesis</t>
   </si>
@@ -178,6 +178,24 @@
   </si>
   <si>
     <t>Nineteenth best</t>
+  </si>
+  <si>
+    <t>Twentyfifth best</t>
+  </si>
+  <si>
+    <t>Twentysixth best</t>
+  </si>
+  <si>
+    <t>Twentyseventh best</t>
+  </si>
+  <si>
+    <t>Twentyeight best</t>
+  </si>
+  <si>
+    <t>Twentyninth best</t>
+  </si>
+  <si>
+    <t>Thirtieth best</t>
   </si>
 </sst>
 </file>
@@ -845,7 +863,10 @@
                   <c:v>45225</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>45227</c:v>
+                  <c:v>45226</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>45228</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -977,31 +998,34 @@
                   <c:v>14566</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>11918</c:v>
+                  <c:v>11486</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>12493</c:v>
+                  <c:v>12061</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>13515</c:v>
+                  <c:v>13083</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>14540</c:v>
+                  <c:v>14108</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>15925</c:v>
+                  <c:v>15493</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>16960</c:v>
+                  <c:v>16528</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>17613</c:v>
+                  <c:v>17181</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>18338</c:v>
+                  <c:v>17906</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>20356</c:v>
+                  <c:v>19924</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>21380</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1277,9 +1301,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$L$29:$L$48</c:f>
+              <c:f>Sheet1!$L$29:$L$54</c:f>
               <c:strCache>
-                <c:ptCount val="20"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>Best day</c:v>
                 </c:pt>
@@ -1339,75 +1363,111 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>Twentieth best</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Twentyfifth best</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Twentysixth best</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Twentyseventh best</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Twentyeight best</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Twentyninth best</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Thirtieth best</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$29:$P$48</c:f>
+              <c:f>Sheet1!$P$29:$P$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>1385</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>1279</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>1035</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>1025</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>1022</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>859</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>814</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>729</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>725</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>661</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>657</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>653</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>611</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>603</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>580</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>575</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>548</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>515</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>486</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>473</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>467</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>448</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>419</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>410</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1433,9 +1493,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$L$29:$L$48</c:f>
+              <c:f>Sheet1!$L$29:$L$54</c:f>
               <c:strCache>
-                <c:ptCount val="20"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
                   <c:v>Best day</c:v>
                 </c:pt>
@@ -1495,21 +1555,39 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>Twentieth best</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Twentyfifth best</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Twentysixth best</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Twentyseventh best</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Twentyeight best</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Twentyninth best</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Thirtieth best</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$29:$Q$48</c:f>
+              <c:f>Sheet1!$Q$29:$Q$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>2018</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1456</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1563,6 +1641,24 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1839,10 +1935,10 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$7:$C$54</c:f>
+              <c:f>Sheet1!$C$7:$C$55</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="48"/>
+                <c:ptCount val="49"/>
                 <c:pt idx="0">
                   <c:v>156</c:v>
                 </c:pt>
@@ -1961,7 +2057,7 @@
                   <c:v>143</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>-2648</c:v>
+                  <c:v>-3080</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>575</c:v>
@@ -1986,6 +2082,9 @@
                 </c:pt>
                 <c:pt idx="47">
                   <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1456</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2109,6 +2208,7 @@
         <c:axId val="173252928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3945,15 +4045,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>730904</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>160215</xdr:rowOff>
+      <xdr:colOff>42987</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>33216</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>410523</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>548106</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>82426</xdr:rowOff>
+      <xdr:rowOff>156510</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3968,7 +4068,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11134321" y="5483632"/>
+          <a:off x="10446404" y="5557716"/>
           <a:ext cx="5458119" cy="8187794"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4340,8 +4440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4213BD91-B5D1-3B47-8D3F-04331482504C}">
   <dimension ref="A1:Q86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4463,14 +4563,14 @@
       </c>
       <c r="F7" s="4">
         <f t="shared" ref="F7:F37" si="1">D7/$J$8</f>
-        <v>9.1764705882352946E-3</v>
+        <v>7.6470588235294122E-3</v>
       </c>
       <c r="H7" s="49" t="s">
         <v>5</v>
       </c>
       <c r="I7" s="50"/>
       <c r="J7" s="8">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4490,7 +4590,7 @@
       </c>
       <c r="F8" s="4">
         <f t="shared" si="1"/>
-        <v>1.1411764705882352E-2</v>
+        <v>9.5098039215686277E-3</v>
       </c>
       <c r="H8" s="51" t="s">
         <v>6</v>
@@ -4498,7 +4598,7 @@
       <c r="I8" s="52"/>
       <c r="J8" s="9">
         <f>J6*J7</f>
-        <v>17000</v>
+        <v>20400</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4518,7 +4618,7 @@
       </c>
       <c r="F9" s="4">
         <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>3.3333333333333333E-2</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
@@ -4538,7 +4638,7 @@
       </c>
       <c r="F10" s="4">
         <f t="shared" si="1"/>
-        <v>6.0352941176470588E-2</v>
+        <v>5.0294117647058822E-2</v>
       </c>
       <c r="H10" s="53" t="s">
         <v>10</v>
@@ -4563,7 +4663,7 @@
       </c>
       <c r="F11" s="4">
         <f t="shared" si="1"/>
-        <v>0.10323529411764706</v>
+        <v>8.6029411764705882E-2</v>
       </c>
       <c r="H11" s="56"/>
       <c r="I11" s="57"/>
@@ -4586,7 +4686,7 @@
       </c>
       <c r="F12" s="4">
         <f t="shared" si="1"/>
-        <v>0.15376470588235294</v>
+        <v>0.12813725490196079</v>
       </c>
       <c r="H12" s="29" t="s">
         <v>11</v>
@@ -4594,7 +4694,7 @@
       <c r="I12" s="30"/>
       <c r="J12" s="10">
         <f>J8-MAX(D6:D63)</f>
-        <v>-3356</v>
+        <v>-980</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
@@ -4614,15 +4714,15 @@
       </c>
       <c r="F13" s="4">
         <f t="shared" si="1"/>
-        <v>0.16005882352941175</v>
+        <v>0.13338235294117648</v>
       </c>
       <c r="H13" s="31" t="s">
         <v>12</v>
       </c>
       <c r="I13" s="32"/>
       <c r="J13" s="10">
-        <f>(AVERAGE(C7:C45)+AVERAGE(C47:C51))/2</f>
-        <v>690.94358974358977</v>
+        <f>(AVERAGE(C7:C45)+AVERAGE(C47:C55))/2</f>
+        <v>736.41025641025635</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4642,7 +4742,7 @@
       </c>
       <c r="F14" s="4">
         <f t="shared" si="1"/>
-        <v>0.23529411764705882</v>
+        <v>0.19607843137254902</v>
       </c>
       <c r="H14" s="33" t="s">
         <v>13</v>
@@ -4650,7 +4750,7 @@
       <c r="I14" s="34"/>
       <c r="J14" s="11">
         <f>J12/J13</f>
-        <v>-4.8571258924992948</v>
+        <v>-1.3307799442896937</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
@@ -4670,7 +4770,7 @@
       </c>
       <c r="F15" s="4">
         <f t="shared" si="1"/>
-        <v>0.27394117647058824</v>
+        <v>0.22828431372549018</v>
       </c>
       <c r="O15" s="7" t="s">
         <v>24</v>
@@ -4699,7 +4799,7 @@
       </c>
       <c r="F16" s="4">
         <f t="shared" si="1"/>
-        <v>0.28252941176470586</v>
+        <v>0.23544117647058824</v>
       </c>
       <c r="J16" s="16"/>
     </row>
@@ -4720,7 +4820,7 @@
       </c>
       <c r="F17" s="4">
         <f t="shared" si="1"/>
-        <v>0.29076470588235293</v>
+        <v>0.24230392156862746</v>
       </c>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.2">
@@ -4740,7 +4840,7 @@
       </c>
       <c r="F18" s="4">
         <f t="shared" si="1"/>
-        <v>0.31823529411764706</v>
+        <v>0.26519607843137255</v>
       </c>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.2">
@@ -4760,7 +4860,7 @@
       </c>
       <c r="F19" s="4">
         <f t="shared" si="1"/>
-        <v>0.34458823529411764</v>
+        <v>0.28715686274509805</v>
       </c>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.2">
@@ -4780,7 +4880,7 @@
       </c>
       <c r="F20" s="4">
         <f t="shared" si="1"/>
-        <v>0.36923529411764705</v>
+        <v>0.30769607843137253</v>
       </c>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.2">
@@ -4800,7 +4900,7 @@
       </c>
       <c r="F21" s="4">
         <f t="shared" si="1"/>
-        <v>0.40811764705882353</v>
+        <v>0.34009803921568627</v>
       </c>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.2">
@@ -4820,7 +4920,7 @@
       </c>
       <c r="F22" s="4">
         <f t="shared" si="1"/>
-        <v>0.44223529411764706</v>
+        <v>0.36852941176470588</v>
       </c>
       <c r="M22">
         <f>(AVERAGE(C7:C45)+AVERAGE(C47:C50))/2</f>
@@ -4844,7 +4944,7 @@
       </c>
       <c r="F23" s="4">
         <f t="shared" si="1"/>
-        <v>0.46276470588235297</v>
+        <v>0.38563725490196077</v>
       </c>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.2">
@@ -4864,7 +4964,7 @@
       </c>
       <c r="F24" s="4">
         <f t="shared" si="1"/>
-        <v>0.4718235294117647</v>
+        <v>0.39318627450980392</v>
       </c>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.2">
@@ -4884,7 +4984,7 @@
       </c>
       <c r="F25" s="4">
         <f t="shared" si="1"/>
-        <v>0.5077647058823529</v>
+        <v>0.4231372549019608</v>
       </c>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.2">
@@ -4904,7 +5004,7 @@
       </c>
       <c r="F26" s="4">
         <f t="shared" si="1"/>
-        <v>0.51335294117647057</v>
+        <v>0.42779411764705882</v>
       </c>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.2">
@@ -4924,7 +5024,7 @@
       </c>
       <c r="F27" s="4">
         <f t="shared" si="1"/>
-        <v>0.52035294117647057</v>
+        <v>0.43362745098039218</v>
       </c>
     </row>
     <row r="28" spans="2:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -4944,7 +5044,7 @@
       </c>
       <c r="F28" s="4">
         <f t="shared" si="1"/>
-        <v>0.53311764705882347</v>
+        <v>0.44426470588235295</v>
       </c>
       <c r="M28" t="s">
         <v>14</v>
@@ -4979,7 +5079,7 @@
       </c>
       <c r="F29" s="4">
         <f t="shared" si="1"/>
-        <v>0.56094117647058828</v>
+        <v>0.46745098039215688</v>
       </c>
       <c r="H29" s="13"/>
       <c r="I29" s="13"/>
@@ -4992,20 +5092,20 @@
         <v>2018</v>
       </c>
       <c r="N29" s="12" cm="1">
-        <f t="array" ref="N29:N77">_xlfn.SORTBY(B6:B54,C6:C54, -1)</f>
-        <v>45227</v>
+        <f t="array" ref="N29:N78">_xlfn.SORTBY(B6:B55,C6:C55, -1)</f>
+        <v>45226</v>
       </c>
       <c r="O29" t="str">
         <f ca="1">IF(N29=TODAY(), "Green", "Blue")</f>
-        <v>Green</v>
-      </c>
-      <c r="P29" t="str">
+        <v>Blue</v>
+      </c>
+      <c r="P29">
         <f ca="1">IF(NOT(N29=TODAY()), M29, "")</f>
+        <v>2018</v>
+      </c>
+      <c r="Q29" t="str">
+        <f ca="1">IF(N29=TODAY(), M29, "")</f>
         <v/>
-      </c>
-      <c r="Q29">
-        <f ca="1">IF(N29=TODAY(), M29, "")</f>
-        <v>2018</v>
       </c>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.2">
@@ -5025,7 +5125,7 @@
       </c>
       <c r="F30" s="4">
         <f t="shared" si="1"/>
-        <v>0.57388235294117651</v>
+        <v>0.47823529411764704</v>
       </c>
       <c r="H30" s="13"/>
       <c r="I30" s="13"/>
@@ -5034,22 +5134,22 @@
         <v>17</v>
       </c>
       <c r="M30">
-        <v>1385</v>
+        <v>1456</v>
       </c>
       <c r="N30" s="12">
-        <v>45222</v>
+        <v>45228</v>
       </c>
       <c r="O30" t="str">
-        <f t="shared" ref="O30:O48" ca="1" si="3">IF(N30=TODAY(), "Green", "Blue")</f>
-        <v>Blue</v>
-      </c>
-      <c r="P30">
-        <f t="shared" ref="P30:P48" ca="1" si="4">IF(NOT(N30=TODAY()), M30, "")</f>
-        <v>1385</v>
-      </c>
-      <c r="Q30" t="str">
-        <f t="shared" ref="Q30:Q48" ca="1" si="5">IF(N30=TODAY(), M30, "")</f>
+        <f t="shared" ref="O30:O54" ca="1" si="3">IF(N30=TODAY(), "Green", "Blue")</f>
+        <v>Green</v>
+      </c>
+      <c r="P30" t="str">
+        <f t="shared" ref="P30:P54" ca="1" si="4">IF(NOT(N30=TODAY()), M30, "")</f>
         <v/>
+      </c>
+      <c r="Q30">
+        <f t="shared" ref="Q30:Q54" ca="1" si="5">IF(N30=TODAY(), M30, "")</f>
+        <v>1456</v>
       </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.2">
@@ -5069,7 +5169,7 @@
       </c>
       <c r="F31" s="4">
         <f t="shared" si="1"/>
-        <v>0.59152941176470586</v>
+        <v>0.49294117647058822</v>
       </c>
       <c r="H31" s="13"/>
       <c r="I31" s="13"/>
@@ -5078,10 +5178,10 @@
         <v>18</v>
       </c>
       <c r="M31">
-        <v>1279</v>
+        <v>1385</v>
       </c>
       <c r="N31" s="12">
-        <v>45148</v>
+        <v>45222</v>
       </c>
       <c r="O31" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5089,7 +5189,7 @@
       </c>
       <c r="P31">
         <f t="shared" ca="1" si="4"/>
-        <v>1279</v>
+        <v>1385</v>
       </c>
       <c r="Q31" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5113,7 +5213,7 @@
       </c>
       <c r="F32" s="4">
         <f t="shared" si="1"/>
-        <v>0.60088235294117642</v>
+        <v>0.50073529411764706</v>
       </c>
       <c r="H32" s="13"/>
       <c r="I32" s="13"/>
@@ -5122,10 +5222,10 @@
         <v>19</v>
       </c>
       <c r="M32">
-        <v>1035</v>
+        <v>1279</v>
       </c>
       <c r="N32" s="12">
-        <v>45223</v>
+        <v>45148</v>
       </c>
       <c r="O32" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5133,7 +5233,7 @@
       </c>
       <c r="P32">
         <f t="shared" ca="1" si="4"/>
-        <v>1035</v>
+        <v>1279</v>
       </c>
       <c r="Q32" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5157,7 +5257,7 @@
       </c>
       <c r="F33" s="4">
         <f t="shared" si="1"/>
-        <v>0.60658823529411765</v>
+        <v>0.50549019607843138</v>
       </c>
       <c r="H33" s="13"/>
       <c r="I33" s="13"/>
@@ -5166,10 +5266,10 @@
         <v>20</v>
       </c>
       <c r="M33">
-        <v>1025</v>
+        <v>1035</v>
       </c>
       <c r="N33" s="12">
-        <v>45221</v>
+        <v>45223</v>
       </c>
       <c r="O33" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5177,7 +5277,7 @@
       </c>
       <c r="P33">
         <f t="shared" ca="1" si="4"/>
-        <v>1025</v>
+        <v>1035</v>
       </c>
       <c r="Q33" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5201,7 +5301,7 @@
       </c>
       <c r="F34" s="4">
         <f t="shared" si="1"/>
-        <v>0.61394117647058821</v>
+        <v>0.51161764705882351</v>
       </c>
       <c r="H34" s="13"/>
       <c r="I34" s="13"/>
@@ -5210,10 +5310,10 @@
         <v>25</v>
       </c>
       <c r="M34">
-        <v>1022</v>
+        <v>1025</v>
       </c>
       <c r="N34" s="12">
-        <v>45220</v>
+        <v>45221</v>
       </c>
       <c r="O34" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5221,7 +5321,7 @@
       </c>
       <c r="P34">
         <f t="shared" ca="1" si="4"/>
-        <v>1022</v>
+        <v>1025</v>
       </c>
       <c r="Q34" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5245,7 +5345,7 @@
       </c>
       <c r="F35" s="4">
         <f t="shared" si="1"/>
-        <v>0.62994117647058823</v>
+        <v>0.52495098039215682</v>
       </c>
       <c r="H35" s="13"/>
       <c r="I35" s="13"/>
@@ -5254,10 +5354,10 @@
         <v>26</v>
       </c>
       <c r="M35">
-        <v>859</v>
+        <v>1022</v>
       </c>
       <c r="N35" s="12">
-        <v>45146</v>
+        <v>45220</v>
       </c>
       <c r="O35" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5265,7 +5365,7 @@
       </c>
       <c r="P35">
         <f t="shared" ca="1" si="4"/>
-        <v>859</v>
+        <v>1022</v>
       </c>
       <c r="Q35" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5289,7 +5389,7 @@
       </c>
       <c r="F36" s="4">
         <f t="shared" si="1"/>
-        <v>0.66023529411764703</v>
+        <v>0.55019607843137253</v>
       </c>
       <c r="H36" s="13"/>
       <c r="I36" s="13"/>
@@ -5298,10 +5398,10 @@
         <v>27</v>
       </c>
       <c r="M36">
-        <v>814</v>
+        <v>859</v>
       </c>
       <c r="N36" s="12">
-        <v>45211</v>
+        <v>45146</v>
       </c>
       <c r="O36" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5309,7 +5409,7 @@
       </c>
       <c r="P36">
         <f t="shared" ca="1" si="4"/>
-        <v>814</v>
+        <v>859</v>
       </c>
       <c r="Q36" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5333,7 +5433,7 @@
       </c>
       <c r="F37" s="4">
         <f t="shared" si="1"/>
-        <v>0.69570588235294117</v>
+        <v>0.57975490196078427</v>
       </c>
       <c r="H37" s="13"/>
       <c r="I37" s="13"/>
@@ -5342,10 +5442,10 @@
         <v>28</v>
       </c>
       <c r="M37">
-        <v>729</v>
+        <v>814</v>
       </c>
       <c r="N37" s="12">
-        <v>45145</v>
+        <v>45211</v>
       </c>
       <c r="O37" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5353,7 +5453,7 @@
       </c>
       <c r="P37">
         <f t="shared" ca="1" si="4"/>
-        <v>729</v>
+        <v>814</v>
       </c>
       <c r="Q37" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5377,16 +5477,16 @@
       </c>
       <c r="F38" s="4">
         <f t="shared" ref="F38:F63" si="7">D38/$J$8</f>
-        <v>0.71776470588235297</v>
+        <v>0.59813725490196079</v>
       </c>
       <c r="L38" t="s">
         <v>29</v>
       </c>
       <c r="M38">
-        <v>725</v>
+        <v>729</v>
       </c>
       <c r="N38" s="12">
-        <v>45225</v>
+        <v>45145</v>
       </c>
       <c r="O38" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5394,7 +5494,7 @@
       </c>
       <c r="P38">
         <f t="shared" ca="1" si="4"/>
-        <v>725</v>
+        <v>729</v>
       </c>
       <c r="Q38" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5418,16 +5518,16 @@
       </c>
       <c r="F39" s="4">
         <f t="shared" si="7"/>
-        <v>0.72617647058823531</v>
+        <v>0.60514705882352937</v>
       </c>
       <c r="L39" t="s">
         <v>30</v>
       </c>
       <c r="M39">
-        <v>661</v>
+        <v>725</v>
       </c>
       <c r="N39" s="12">
-        <v>45159</v>
+        <v>45225</v>
       </c>
       <c r="O39" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5435,7 +5535,7 @@
       </c>
       <c r="P39">
         <f t="shared" ca="1" si="4"/>
-        <v>661</v>
+        <v>725</v>
       </c>
       <c r="Q39" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5459,16 +5559,16 @@
       </c>
       <c r="F40" s="4">
         <f t="shared" si="7"/>
-        <v>0.73505882352941176</v>
+        <v>0.61254901960784314</v>
       </c>
       <c r="L40" t="s">
         <v>31</v>
       </c>
       <c r="M40">
-        <v>657</v>
+        <v>661</v>
       </c>
       <c r="N40" s="12">
-        <v>45149</v>
+        <v>45159</v>
       </c>
       <c r="O40" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5476,7 +5576,7 @@
       </c>
       <c r="P40">
         <f t="shared" ca="1" si="4"/>
-        <v>657</v>
+        <v>661</v>
       </c>
       <c r="Q40" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5488,7 +5588,7 @@
         <v>45208</v>
       </c>
       <c r="C41" s="21">
-        <f t="shared" ref="C41:C54" si="8">D41-D40</f>
+        <f t="shared" ref="C41:C55" si="8">D41-D40</f>
         <v>548</v>
       </c>
       <c r="D41" s="23">
@@ -5500,16 +5600,16 @@
       </c>
       <c r="F41" s="4">
         <f>D41/$J$8</f>
-        <v>0.76729411764705879</v>
+        <v>0.63941176470588235</v>
       </c>
       <c r="L41" t="s">
         <v>32</v>
       </c>
       <c r="M41">
-        <v>653</v>
+        <v>657</v>
       </c>
       <c r="N41" s="12">
-        <v>45224</v>
+        <v>45149</v>
       </c>
       <c r="O41" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5517,7 +5617,7 @@
       </c>
       <c r="P41">
         <f t="shared" ca="1" si="4"/>
-        <v>653</v>
+        <v>657</v>
       </c>
       <c r="Q41" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5541,16 +5641,16 @@
       </c>
       <c r="F42" s="4">
         <f>D42/$J$8</f>
-        <v>0.79141176470588237</v>
+        <v>0.65950980392156866</v>
       </c>
       <c r="L42" t="s">
         <v>33</v>
       </c>
       <c r="M42">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="N42" s="12">
-        <v>45163</v>
+        <v>45224</v>
       </c>
       <c r="O42" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5558,7 +5658,7 @@
       </c>
       <c r="P42">
         <f t="shared" ca="1" si="4"/>
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="Q42" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5582,16 +5682,16 @@
       </c>
       <c r="F43" s="4">
         <f t="shared" si="7"/>
-        <v>0.80052941176470593</v>
+        <v>0.66710784313725491</v>
       </c>
       <c r="L43" t="s">
         <v>34</v>
       </c>
       <c r="M43">
-        <v>603</v>
+        <v>611</v>
       </c>
       <c r="N43" s="12">
-        <v>45193</v>
+        <v>45163</v>
       </c>
       <c r="O43" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5599,7 +5699,7 @@
       </c>
       <c r="P43">
         <f t="shared" ca="1" si="4"/>
-        <v>603</v>
+        <v>611</v>
       </c>
       <c r="Q43" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5623,16 +5723,16 @@
       </c>
       <c r="F44" s="4">
         <f t="shared" si="7"/>
-        <v>0.84841176470588231</v>
+        <v>0.70700980392156865</v>
       </c>
       <c r="L44" t="s">
         <v>36</v>
       </c>
       <c r="M44">
-        <v>580</v>
+        <v>603</v>
       </c>
       <c r="N44" s="12">
-        <v>45160</v>
+        <v>45193</v>
       </c>
       <c r="O44" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5640,7 +5740,7 @@
       </c>
       <c r="P44">
         <f t="shared" ca="1" si="4"/>
-        <v>580</v>
+        <v>603</v>
       </c>
       <c r="Q44" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5664,16 +5764,16 @@
       </c>
       <c r="F45" s="4">
         <f t="shared" si="7"/>
-        <v>0.85682352941176465</v>
+        <v>0.71401960784313723</v>
       </c>
       <c r="L45" t="s">
         <v>37</v>
       </c>
       <c r="M45">
-        <v>575</v>
+        <v>580</v>
       </c>
       <c r="N45" s="12">
-        <v>45219</v>
+        <v>45160</v>
       </c>
       <c r="O45" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5681,7 +5781,7 @@
       </c>
       <c r="P45">
         <f t="shared" ca="1" si="4"/>
-        <v>575</v>
+        <v>580</v>
       </c>
       <c r="Q45" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5694,28 +5794,28 @@
       </c>
       <c r="C46" s="21">
         <f t="shared" si="8"/>
-        <v>-2648</v>
+        <v>-3080</v>
       </c>
       <c r="D46" s="23">
-        <f>13793-105-84-134-144-170-800-438</f>
-        <v>11918</v>
+        <f>13793-105-84-134-144-170-800-438-432</f>
+        <v>11486</v>
       </c>
       <c r="E46" s="24">
         <f t="shared" si="6"/>
-        <v>35.05294117647059</v>
+        <v>33.78235294117647</v>
       </c>
       <c r="F46" s="4">
         <f t="shared" si="7"/>
-        <v>0.70105882352941173</v>
+        <v>0.56303921568627446</v>
       </c>
       <c r="L46" t="s">
         <v>38</v>
       </c>
       <c r="M46">
-        <v>548</v>
+        <v>575</v>
       </c>
       <c r="N46" s="12">
-        <v>45208</v>
+        <v>45219</v>
       </c>
       <c r="O46" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5723,7 +5823,7 @@
       </c>
       <c r="P46">
         <f t="shared" ca="1" si="4"/>
-        <v>548</v>
+        <v>575</v>
       </c>
       <c r="Q46" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5739,25 +5839,25 @@
         <v>575</v>
       </c>
       <c r="D47" s="23">
-        <f>14368-105-84-134-144-170-800-438</f>
-        <v>12493</v>
+        <f>14368-105-84-134-144-170-800-438-432</f>
+        <v>12061</v>
       </c>
       <c r="E47" s="24">
         <f t="shared" si="6"/>
-        <v>36.744117647058822</v>
+        <v>35.473529411764709</v>
       </c>
       <c r="F47" s="4">
         <f t="shared" si="7"/>
-        <v>0.73488235294117643</v>
+        <v>0.5912254901960784</v>
       </c>
       <c r="L47" t="s">
         <v>39</v>
       </c>
       <c r="M47">
-        <v>515</v>
+        <v>548</v>
       </c>
       <c r="N47" s="12">
-        <v>45191</v>
+        <v>45208</v>
       </c>
       <c r="O47" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5765,7 +5865,7 @@
       </c>
       <c r="P47">
         <f t="shared" ca="1" si="4"/>
-        <v>515</v>
+        <v>548</v>
       </c>
       <c r="Q47" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5781,25 +5881,25 @@
         <v>1022</v>
       </c>
       <c r="D48" s="23">
-        <f>15201-134-144-170-800-438</f>
-        <v>13515</v>
+        <f>15201-134-144-170-800-438-432</f>
+        <v>13083</v>
       </c>
       <c r="E48" s="24">
         <f t="shared" si="6"/>
-        <v>39.75</v>
+        <v>38.47941176470588</v>
       </c>
       <c r="F48" s="4">
         <f t="shared" si="7"/>
-        <v>0.79500000000000004</v>
+        <v>0.64132352941176474</v>
       </c>
       <c r="L48" t="s">
         <v>35</v>
       </c>
       <c r="M48">
-        <v>486</v>
+        <v>515</v>
       </c>
       <c r="N48" s="12">
-        <v>45141</v>
+        <v>45191</v>
       </c>
       <c r="O48" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5807,14 +5907,14 @@
       </c>
       <c r="P48">
         <f t="shared" ca="1" si="4"/>
-        <v>486</v>
+        <v>515</v>
       </c>
       <c r="Q48" t="str">
         <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="49" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B49" s="2">
         <v>45221</v>
       </c>
@@ -5823,25 +5923,40 @@
         <v>1025</v>
       </c>
       <c r="D49" s="23">
-        <f>16092-144-170-800-438</f>
-        <v>14540</v>
+        <f>16092-144-170-800-438-432</f>
+        <v>14108</v>
       </c>
       <c r="E49" s="24">
         <f t="shared" si="6"/>
-        <v>42.764705882352942</v>
+        <v>41.494117647058822</v>
       </c>
       <c r="F49" s="4">
         <f t="shared" si="7"/>
-        <v>0.85529411764705887</v>
+        <v>0.69156862745098036</v>
+      </c>
+      <c r="L49" t="s">
+        <v>40</v>
       </c>
       <c r="M49">
-        <v>473</v>
+        <v>486</v>
       </c>
       <c r="N49" s="12">
-        <v>45174</v>
-      </c>
-    </row>
-    <row r="50" spans="2:14" x14ac:dyDescent="0.2">
+        <v>45141</v>
+      </c>
+      <c r="O49" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>Blue</v>
+      </c>
+      <c r="P49">
+        <f t="shared" ca="1" si="4"/>
+        <v>486</v>
+      </c>
+      <c r="Q49" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B50" s="2">
         <v>45222</v>
       </c>
@@ -5850,25 +5965,40 @@
         <v>1385</v>
       </c>
       <c r="D50" s="23">
-        <f>17163-800-438</f>
-        <v>15925</v>
+        <f>17163-800-438-432</f>
+        <v>15493</v>
       </c>
       <c r="E50" s="24">
         <f t="shared" si="6"/>
-        <v>46.838235294117645</v>
+        <v>45.567647058823532</v>
       </c>
       <c r="F50" s="4">
         <f t="shared" si="7"/>
-        <v>0.93676470588235294</v>
+        <v>0.75946078431372555</v>
+      </c>
+      <c r="L50" t="s">
+        <v>41</v>
       </c>
       <c r="M50">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="N50" s="12">
-        <v>45154</v>
-      </c>
-    </row>
-    <row r="51" spans="2:14" x14ac:dyDescent="0.2">
+        <v>45174</v>
+      </c>
+      <c r="O50" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>Blue</v>
+      </c>
+      <c r="P50">
+        <f t="shared" ca="1" si="4"/>
+        <v>473</v>
+      </c>
+      <c r="Q50" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B51" s="2">
         <v>45223</v>
       </c>
@@ -5877,25 +6007,40 @@
         <v>1035</v>
       </c>
       <c r="D51" s="23">
-        <f>18198-800-438</f>
-        <v>16960</v>
+        <f>18198-800-438-432</f>
+        <v>16528</v>
       </c>
       <c r="E51" s="24">
         <f t="shared" si="6"/>
-        <v>49.882352941176471</v>
+        <v>48.611764705882351</v>
       </c>
       <c r="F51" s="4">
         <f t="shared" si="7"/>
-        <v>0.99764705882352944</v>
+        <v>0.81019607843137254</v>
+      </c>
+      <c r="L51" t="s">
+        <v>42</v>
       </c>
       <c r="M51">
-        <v>448</v>
+        <v>467</v>
       </c>
       <c r="N51" s="12">
-        <v>45155</v>
-      </c>
-    </row>
-    <row r="52" spans="2:14" x14ac:dyDescent="0.2">
+        <v>45154</v>
+      </c>
+      <c r="O51" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>Blue</v>
+      </c>
+      <c r="P51">
+        <f t="shared" ca="1" si="4"/>
+        <v>467</v>
+      </c>
+      <c r="Q51" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B52" s="2">
         <v>45224</v>
       </c>
@@ -5904,25 +6049,40 @@
         <v>653</v>
       </c>
       <c r="D52" s="23">
-        <f>18051-438</f>
-        <v>17613</v>
+        <f>18051-438-432</f>
+        <v>17181</v>
       </c>
       <c r="E52" s="24">
         <f t="shared" si="6"/>
-        <v>51.80294117647059</v>
+        <v>50.53235294117647</v>
       </c>
       <c r="F52" s="4">
         <f t="shared" si="7"/>
-        <v>1.0360588235294117</v>
+        <v>0.84220588235294114</v>
+      </c>
+      <c r="L52" t="s">
+        <v>43</v>
       </c>
       <c r="M52">
-        <v>419</v>
+        <v>448</v>
       </c>
       <c r="N52" s="12">
-        <v>45156</v>
-      </c>
-    </row>
-    <row r="53" spans="2:14" x14ac:dyDescent="0.2">
+        <v>45155</v>
+      </c>
+      <c r="O52" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>Blue</v>
+      </c>
+      <c r="P52">
+        <f t="shared" ca="1" si="4"/>
+        <v>448</v>
+      </c>
+      <c r="Q52" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B53" s="2">
         <v>45225</v>
       </c>
@@ -5931,70 +6091,108 @@
         <v>725</v>
       </c>
       <c r="D53" s="23">
-        <f>18776-438</f>
-        <v>18338</v>
+        <f>18776-438-432</f>
+        <v>17906</v>
       </c>
       <c r="E53" s="24">
         <f t="shared" si="6"/>
-        <v>53.935294117647061</v>
+        <v>52.664705882352941</v>
       </c>
       <c r="F53" s="4">
         <f t="shared" si="7"/>
-        <v>1.0787058823529412</v>
+        <v>0.87774509803921563</v>
+      </c>
+      <c r="L53" t="s">
+        <v>44</v>
       </c>
       <c r="M53">
-        <v>410</v>
+        <v>419</v>
       </c>
       <c r="N53" s="12">
-        <v>45209</v>
-      </c>
-    </row>
-    <row r="54" spans="2:14" x14ac:dyDescent="0.2">
+        <v>45156</v>
+      </c>
+      <c r="O53" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>Blue</v>
+      </c>
+      <c r="P53">
+        <f t="shared" ca="1" si="4"/>
+        <v>419</v>
+      </c>
+      <c r="Q53" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B54" s="2">
-        <v>45227</v>
+        <v>45226</v>
       </c>
       <c r="C54" s="21">
         <f t="shared" si="8"/>
         <v>2018</v>
       </c>
       <c r="D54" s="23">
-        <v>20356</v>
+        <f>20356-432</f>
+        <v>19924</v>
       </c>
       <c r="E54" s="24">
         <f t="shared" si="6"/>
-        <v>59.870588235294115</v>
+        <v>58.6</v>
       </c>
       <c r="F54" s="4">
         <f t="shared" si="7"/>
-        <v>1.1974117647058824</v>
+        <v>0.97666666666666668</v>
+      </c>
+      <c r="L54" t="s">
+        <v>45</v>
       </c>
       <c r="M54">
-        <v>375</v>
+        <v>410</v>
       </c>
       <c r="N54" s="12">
-        <v>45194</v>
-      </c>
-    </row>
-    <row r="55" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B55" s="28"/>
-      <c r="C55" s="21"/>
-      <c r="D55" s="23"/>
+        <v>45209</v>
+      </c>
+      <c r="O54" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>Blue</v>
+      </c>
+      <c r="P54">
+        <f t="shared" ca="1" si="4"/>
+        <v>410</v>
+      </c>
+      <c r="Q54" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B55" s="2">
+        <v>45228</v>
+      </c>
+      <c r="C55" s="21">
+        <f t="shared" si="8"/>
+        <v>1456</v>
+      </c>
+      <c r="D55" s="23">
+        <v>21380</v>
+      </c>
       <c r="E55" s="24">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>62.882352941176471</v>
       </c>
       <c r="F55" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1.0480392156862746</v>
       </c>
       <c r="M55">
-        <v>349</v>
+        <v>375</v>
       </c>
       <c r="N55" s="12">
-        <v>45161</v>
-      </c>
-    </row>
-    <row r="56" spans="2:14" x14ac:dyDescent="0.2">
+        <v>45194</v>
+      </c>
+    </row>
+    <row r="56" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B56" s="28"/>
       <c r="C56" s="21"/>
       <c r="D56" s="23"/>
@@ -6007,13 +6205,13 @@
         <v>0</v>
       </c>
       <c r="M56">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="N56" s="12">
-        <v>45142</v>
-      </c>
-    </row>
-    <row r="57" spans="2:14" x14ac:dyDescent="0.2">
+        <v>45161</v>
+      </c>
+    </row>
+    <row r="57" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B57" s="28"/>
       <c r="C57" s="21"/>
       <c r="D57" s="23"/>
@@ -6026,15 +6224,18 @@
         <v>0</v>
       </c>
       <c r="M57">
-        <v>300</v>
+        <v>346</v>
       </c>
       <c r="N57" s="12">
-        <v>45181</v>
-      </c>
-    </row>
-    <row r="58" spans="2:14" x14ac:dyDescent="0.2">
+        <v>45142</v>
+      </c>
+    </row>
+    <row r="58" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B58" s="28"/>
-      <c r="C58" s="21"/>
+      <c r="C58" s="21">
+        <f>SUM(C47:C55)/340</f>
+        <v>29.1</v>
+      </c>
       <c r="D58" s="23"/>
       <c r="E58" s="24">
         <f t="shared" si="6"/>
@@ -6045,13 +6246,13 @@
         <v>0</v>
       </c>
       <c r="M58">
-        <v>272</v>
+        <v>300</v>
       </c>
       <c r="N58" s="12">
-        <v>45188</v>
-      </c>
-    </row>
-    <row r="59" spans="2:14" x14ac:dyDescent="0.2">
+        <v>45181</v>
+      </c>
+    </row>
+    <row r="59" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B59" s="28"/>
       <c r="C59" s="21"/>
       <c r="D59" s="23"/>
@@ -6064,13 +6265,13 @@
         <v>0</v>
       </c>
       <c r="M59">
-        <v>220</v>
+        <v>272</v>
       </c>
       <c r="N59" s="12">
-        <v>45175</v>
-      </c>
-    </row>
-    <row r="60" spans="2:14" x14ac:dyDescent="0.2">
+        <v>45188</v>
+      </c>
+    </row>
+    <row r="60" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B60" s="28"/>
       <c r="C60" s="21"/>
       <c r="D60" s="23"/>
@@ -6083,13 +6284,13 @@
         <v>0</v>
       </c>
       <c r="M60">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="N60" s="12">
-        <v>45173</v>
-      </c>
-    </row>
-    <row r="61" spans="2:14" x14ac:dyDescent="0.2">
+        <v>45175</v>
+      </c>
+    </row>
+    <row r="61" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B61" s="28"/>
       <c r="C61" s="21"/>
       <c r="D61" s="23"/>
@@ -6102,13 +6303,13 @@
         <v>0</v>
       </c>
       <c r="M61">
-        <v>159</v>
+        <v>217</v>
       </c>
       <c r="N61" s="12">
-        <v>45182</v>
-      </c>
-    </row>
-    <row r="62" spans="2:14" x14ac:dyDescent="0.2">
+        <v>45173</v>
+      </c>
+    </row>
+    <row r="62" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B62" s="28"/>
       <c r="C62" s="21"/>
       <c r="D62" s="23"/>
@@ -6121,13 +6322,13 @@
         <v>0</v>
       </c>
       <c r="M62">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="N62" s="12">
-        <v>45139</v>
-      </c>
-    </row>
-    <row r="63" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>45182</v>
+      </c>
+    </row>
+    <row r="63" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B63" s="3"/>
       <c r="C63" s="22"/>
       <c r="D63" s="1"/>
@@ -6140,42 +6341,42 @@
         <v>0</v>
       </c>
       <c r="M63">
+        <v>156</v>
+      </c>
+      <c r="N63" s="12">
+        <v>45139</v>
+      </c>
+    </row>
+    <row r="64" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="M64">
         <v>155</v>
       </c>
-      <c r="N63" s="12">
+      <c r="N64" s="12">
         <v>45210</v>
-      </c>
-    </row>
-    <row r="64" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="M64">
-        <v>154</v>
-      </c>
-      <c r="N64" s="12">
-        <v>45162</v>
       </c>
     </row>
     <row r="65" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M65">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="N65" s="12">
-        <v>45196</v>
+        <v>45162</v>
       </c>
     </row>
     <row r="66" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M66">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="N66" s="12">
-        <v>45152</v>
+        <v>45196</v>
       </c>
     </row>
     <row r="67" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M67">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="N67" s="12">
-        <v>45195</v>
+        <v>45152</v>
       </c>
     </row>
     <row r="68" spans="13:14" x14ac:dyDescent="0.2">
@@ -6183,89 +6384,92 @@
         <v>143</v>
       </c>
       <c r="N68" s="12">
-        <v>45212</v>
+        <v>45195</v>
       </c>
     </row>
     <row r="69" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M69">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="N69" s="12">
-        <v>45153</v>
+        <v>45212</v>
       </c>
     </row>
     <row r="70" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M70">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="N70" s="12">
-        <v>45187</v>
+        <v>45153</v>
       </c>
     </row>
     <row r="71" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M71">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="N71" s="12">
-        <v>45168</v>
+        <v>45187</v>
       </c>
     </row>
     <row r="72" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M72">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="N72" s="12">
-        <v>45147</v>
+        <v>45168</v>
       </c>
     </row>
     <row r="73" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M73">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="N73" s="12">
-        <v>45183</v>
+        <v>45147</v>
       </c>
     </row>
     <row r="74" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M74">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="N74" s="12">
-        <v>45164</v>
+        <v>45183</v>
       </c>
     </row>
     <row r="75" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M75">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="N75">
-        <v>45140</v>
+        <v>45164</v>
       </c>
     </row>
     <row r="76" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M76">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="N76">
-        <v>45138</v>
+        <v>45140</v>
       </c>
     </row>
     <row r="77" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M77">
-        <v>-2648</v>
+        <v>29.1</v>
       </c>
       <c r="N77">
-        <v>45218</v>
+        <v>45138</v>
       </c>
     </row>
     <row r="78" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M78">
         <v>0</v>
       </c>
+      <c r="N78">
+        <v>45218</v>
+      </c>
     </row>
     <row r="79" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M79">
-        <v>0</v>
+        <v>-3080</v>
       </c>
     </row>
     <row r="80" spans="13:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Final plots fixed, conclusion kinda done, all references done
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A114A095-9D38-E14D-9B4E-A7B9BDD7D9E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C8E49E5-DC7B-094B-9294-9A1B12582BFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="15080" windowHeight="16940" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
@@ -866,7 +866,10 @@
                   <c:v>45226</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>45228</c:v>
+                  <c:v>45227</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>45229</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1026,6 +1029,9 @@
                 </c:pt>
                 <c:pt idx="49">
                   <c:v>21380</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>22819</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1395,79 +1401,79 @@
                   <c:v>2018</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>1456</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>1385</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>1279</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>1035</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>1025</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>1022</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>859</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>814</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>729</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>725</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>661</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>657</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>653</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>611</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>603</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>580</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>575</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>548</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>515</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="21">
                   <c:v>486</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>473</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="23">
                   <c:v>467</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="24">
                   <c:v>448</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="25">
                   <c:v>419</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>410</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1587,10 +1593,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1456</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1439</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -4440,8 +4446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4213BD91-B5D1-3B47-8D3F-04331482504C}">
   <dimension ref="A1:Q86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4694,7 +4700,7 @@
       <c r="I12" s="30"/>
       <c r="J12" s="10">
         <f>J8-MAX(D6:D63)</f>
-        <v>-980</v>
+        <v>-2419</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
@@ -4750,7 +4756,7 @@
       <c r="I14" s="34"/>
       <c r="J14" s="11">
         <f>J12/J13</f>
-        <v>-1.3307799442896937</v>
+        <v>-3.2848537604456829</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
@@ -5092,7 +5098,7 @@
         <v>2018</v>
       </c>
       <c r="N29" s="12" cm="1">
-        <f t="array" ref="N29:N78">_xlfn.SORTBY(B6:B55,C6:C55, -1)</f>
+        <f t="array" ref="N29:N79">_xlfn.SORTBY(B6:B56,C6:C56, -1)</f>
         <v>45226</v>
       </c>
       <c r="O29" t="str">
@@ -5137,19 +5143,19 @@
         <v>1456</v>
       </c>
       <c r="N30" s="12">
-        <v>45228</v>
+        <v>45227</v>
       </c>
       <c r="O30" t="str">
         <f t="shared" ref="O30:O54" ca="1" si="3">IF(N30=TODAY(), "Green", "Blue")</f>
-        <v>Green</v>
-      </c>
-      <c r="P30" t="str">
+        <v>Blue</v>
+      </c>
+      <c r="P30">
         <f t="shared" ref="P30:P54" ca="1" si="4">IF(NOT(N30=TODAY()), M30, "")</f>
+        <v>1456</v>
+      </c>
+      <c r="Q30" t="str">
+        <f t="shared" ref="Q30:Q54" ca="1" si="5">IF(N30=TODAY(), M30, "")</f>
         <v/>
-      </c>
-      <c r="Q30">
-        <f t="shared" ref="Q30:Q54" ca="1" si="5">IF(N30=TODAY(), M30, "")</f>
-        <v>1456</v>
       </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.2">
@@ -5178,22 +5184,22 @@
         <v>18</v>
       </c>
       <c r="M31">
-        <v>1385</v>
+        <v>1439</v>
       </c>
       <c r="N31" s="12">
-        <v>45222</v>
+        <v>45229</v>
       </c>
       <c r="O31" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Blue</v>
-      </c>
-      <c r="P31">
+        <v>Green</v>
+      </c>
+      <c r="P31" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>1385</v>
-      </c>
-      <c r="Q31" t="str">
+        <v/>
+      </c>
+      <c r="Q31">
         <f t="shared" ca="1" si="5"/>
-        <v/>
+        <v>1439</v>
       </c>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.2">
@@ -5222,10 +5228,10 @@
         <v>19</v>
       </c>
       <c r="M32">
-        <v>1279</v>
+        <v>1385</v>
       </c>
       <c r="N32" s="12">
-        <v>45148</v>
+        <v>45222</v>
       </c>
       <c r="O32" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5233,7 +5239,7 @@
       </c>
       <c r="P32">
         <f t="shared" ca="1" si="4"/>
-        <v>1279</v>
+        <v>1385</v>
       </c>
       <c r="Q32" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5266,10 +5272,10 @@
         <v>20</v>
       </c>
       <c r="M33">
-        <v>1035</v>
+        <v>1279</v>
       </c>
       <c r="N33" s="12">
-        <v>45223</v>
+        <v>45148</v>
       </c>
       <c r="O33" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5277,7 +5283,7 @@
       </c>
       <c r="P33">
         <f t="shared" ca="1" si="4"/>
-        <v>1035</v>
+        <v>1279</v>
       </c>
       <c r="Q33" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5310,10 +5316,10 @@
         <v>25</v>
       </c>
       <c r="M34">
-        <v>1025</v>
+        <v>1035</v>
       </c>
       <c r="N34" s="12">
-        <v>45221</v>
+        <v>45223</v>
       </c>
       <c r="O34" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5321,7 +5327,7 @@
       </c>
       <c r="P34">
         <f t="shared" ca="1" si="4"/>
-        <v>1025</v>
+        <v>1035</v>
       </c>
       <c r="Q34" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5354,10 +5360,10 @@
         <v>26</v>
       </c>
       <c r="M35">
-        <v>1022</v>
+        <v>1025</v>
       </c>
       <c r="N35" s="12">
-        <v>45220</v>
+        <v>45221</v>
       </c>
       <c r="O35" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5365,7 +5371,7 @@
       </c>
       <c r="P35">
         <f t="shared" ca="1" si="4"/>
-        <v>1022</v>
+        <v>1025</v>
       </c>
       <c r="Q35" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5398,10 +5404,10 @@
         <v>27</v>
       </c>
       <c r="M36">
-        <v>859</v>
+        <v>1022</v>
       </c>
       <c r="N36" s="12">
-        <v>45146</v>
+        <v>45220</v>
       </c>
       <c r="O36" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5409,7 +5415,7 @@
       </c>
       <c r="P36">
         <f t="shared" ca="1" si="4"/>
-        <v>859</v>
+        <v>1022</v>
       </c>
       <c r="Q36" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5442,10 +5448,10 @@
         <v>28</v>
       </c>
       <c r="M37">
-        <v>814</v>
+        <v>859</v>
       </c>
       <c r="N37" s="12">
-        <v>45211</v>
+        <v>45146</v>
       </c>
       <c r="O37" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5453,7 +5459,7 @@
       </c>
       <c r="P37">
         <f t="shared" ca="1" si="4"/>
-        <v>814</v>
+        <v>859</v>
       </c>
       <c r="Q37" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5483,10 +5489,10 @@
         <v>29</v>
       </c>
       <c r="M38">
-        <v>729</v>
+        <v>814</v>
       </c>
       <c r="N38" s="12">
-        <v>45145</v>
+        <v>45211</v>
       </c>
       <c r="O38" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5494,7 +5500,7 @@
       </c>
       <c r="P38">
         <f t="shared" ca="1" si="4"/>
-        <v>729</v>
+        <v>814</v>
       </c>
       <c r="Q38" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5524,10 +5530,10 @@
         <v>30</v>
       </c>
       <c r="M39">
-        <v>725</v>
+        <v>729</v>
       </c>
       <c r="N39" s="12">
-        <v>45225</v>
+        <v>45145</v>
       </c>
       <c r="O39" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5535,7 +5541,7 @@
       </c>
       <c r="P39">
         <f t="shared" ca="1" si="4"/>
-        <v>725</v>
+        <v>729</v>
       </c>
       <c r="Q39" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5565,10 +5571,10 @@
         <v>31</v>
       </c>
       <c r="M40">
-        <v>661</v>
+        <v>725</v>
       </c>
       <c r="N40" s="12">
-        <v>45159</v>
+        <v>45225</v>
       </c>
       <c r="O40" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5576,7 +5582,7 @@
       </c>
       <c r="P40">
         <f t="shared" ca="1" si="4"/>
-        <v>661</v>
+        <v>725</v>
       </c>
       <c r="Q40" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5588,7 +5594,7 @@
         <v>45208</v>
       </c>
       <c r="C41" s="21">
-        <f t="shared" ref="C41:C55" si="8">D41-D40</f>
+        <f t="shared" ref="C41:C56" si="8">D41-D40</f>
         <v>548</v>
       </c>
       <c r="D41" s="23">
@@ -5606,10 +5612,10 @@
         <v>32</v>
       </c>
       <c r="M41">
-        <v>657</v>
+        <v>661</v>
       </c>
       <c r="N41" s="12">
-        <v>45149</v>
+        <v>45159</v>
       </c>
       <c r="O41" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5617,7 +5623,7 @@
       </c>
       <c r="P41">
         <f t="shared" ca="1" si="4"/>
-        <v>657</v>
+        <v>661</v>
       </c>
       <c r="Q41" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5647,10 +5653,10 @@
         <v>33</v>
       </c>
       <c r="M42">
-        <v>653</v>
+        <v>657</v>
       </c>
       <c r="N42" s="12">
-        <v>45224</v>
+        <v>45149</v>
       </c>
       <c r="O42" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5658,7 +5664,7 @@
       </c>
       <c r="P42">
         <f t="shared" ca="1" si="4"/>
-        <v>653</v>
+        <v>657</v>
       </c>
       <c r="Q42" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5688,10 +5694,10 @@
         <v>34</v>
       </c>
       <c r="M43">
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="N43" s="12">
-        <v>45163</v>
+        <v>45224</v>
       </c>
       <c r="O43" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5699,7 +5705,7 @@
       </c>
       <c r="P43">
         <f t="shared" ca="1" si="4"/>
-        <v>611</v>
+        <v>653</v>
       </c>
       <c r="Q43" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5729,10 +5735,10 @@
         <v>36</v>
       </c>
       <c r="M44">
-        <v>603</v>
+        <v>611</v>
       </c>
       <c r="N44" s="12">
-        <v>45193</v>
+        <v>45163</v>
       </c>
       <c r="O44" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5740,7 +5746,7 @@
       </c>
       <c r="P44">
         <f t="shared" ca="1" si="4"/>
-        <v>603</v>
+        <v>611</v>
       </c>
       <c r="Q44" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5770,10 +5776,10 @@
         <v>37</v>
       </c>
       <c r="M45">
-        <v>580</v>
+        <v>603</v>
       </c>
       <c r="N45" s="12">
-        <v>45160</v>
+        <v>45193</v>
       </c>
       <c r="O45" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5781,7 +5787,7 @@
       </c>
       <c r="P45">
         <f t="shared" ca="1" si="4"/>
-        <v>580</v>
+        <v>603</v>
       </c>
       <c r="Q45" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5812,10 +5818,10 @@
         <v>38</v>
       </c>
       <c r="M46">
-        <v>575</v>
+        <v>580</v>
       </c>
       <c r="N46" s="12">
-        <v>45219</v>
+        <v>45160</v>
       </c>
       <c r="O46" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5823,7 +5829,7 @@
       </c>
       <c r="P46">
         <f t="shared" ca="1" si="4"/>
-        <v>575</v>
+        <v>580</v>
       </c>
       <c r="Q46" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5854,10 +5860,10 @@
         <v>39</v>
       </c>
       <c r="M47">
-        <v>548</v>
+        <v>575</v>
       </c>
       <c r="N47" s="12">
-        <v>45208</v>
+        <v>45219</v>
       </c>
       <c r="O47" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5865,7 +5871,7 @@
       </c>
       <c r="P47">
         <f t="shared" ca="1" si="4"/>
-        <v>548</v>
+        <v>575</v>
       </c>
       <c r="Q47" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5896,10 +5902,10 @@
         <v>35</v>
       </c>
       <c r="M48">
-        <v>515</v>
+        <v>548</v>
       </c>
       <c r="N48" s="12">
-        <v>45191</v>
+        <v>45208</v>
       </c>
       <c r="O48" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5907,7 +5913,7 @@
       </c>
       <c r="P48">
         <f t="shared" ca="1" si="4"/>
-        <v>515</v>
+        <v>548</v>
       </c>
       <c r="Q48" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5938,10 +5944,10 @@
         <v>40</v>
       </c>
       <c r="M49">
-        <v>486</v>
+        <v>515</v>
       </c>
       <c r="N49" s="12">
-        <v>45141</v>
+        <v>45191</v>
       </c>
       <c r="O49" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5949,7 +5955,7 @@
       </c>
       <c r="P49">
         <f t="shared" ca="1" si="4"/>
-        <v>486</v>
+        <v>515</v>
       </c>
       <c r="Q49" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -5980,10 +5986,10 @@
         <v>41</v>
       </c>
       <c r="M50">
-        <v>473</v>
+        <v>486</v>
       </c>
       <c r="N50" s="12">
-        <v>45174</v>
+        <v>45141</v>
       </c>
       <c r="O50" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -5991,7 +5997,7 @@
       </c>
       <c r="P50">
         <f t="shared" ca="1" si="4"/>
-        <v>473</v>
+        <v>486</v>
       </c>
       <c r="Q50" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -6022,10 +6028,10 @@
         <v>42</v>
       </c>
       <c r="M51">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="N51" s="12">
-        <v>45154</v>
+        <v>45174</v>
       </c>
       <c r="O51" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -6033,7 +6039,7 @@
       </c>
       <c r="P51">
         <f t="shared" ca="1" si="4"/>
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="Q51" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -6064,10 +6070,10 @@
         <v>43</v>
       </c>
       <c r="M52">
-        <v>448</v>
+        <v>467</v>
       </c>
       <c r="N52" s="12">
-        <v>45155</v>
+        <v>45154</v>
       </c>
       <c r="O52" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -6075,7 +6081,7 @@
       </c>
       <c r="P52">
         <f t="shared" ca="1" si="4"/>
-        <v>448</v>
+        <v>467</v>
       </c>
       <c r="Q52" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -6106,10 +6112,10 @@
         <v>44</v>
       </c>
       <c r="M53">
-        <v>419</v>
+        <v>448</v>
       </c>
       <c r="N53" s="12">
-        <v>45156</v>
+        <v>45155</v>
       </c>
       <c r="O53" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -6117,7 +6123,7 @@
       </c>
       <c r="P53">
         <f t="shared" ca="1" si="4"/>
-        <v>419</v>
+        <v>448</v>
       </c>
       <c r="Q53" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -6148,10 +6154,10 @@
         <v>45</v>
       </c>
       <c r="M54">
-        <v>410</v>
+        <v>419</v>
       </c>
       <c r="N54" s="12">
-        <v>45209</v>
+        <v>45156</v>
       </c>
       <c r="O54" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -6159,7 +6165,7 @@
       </c>
       <c r="P54">
         <f t="shared" ca="1" si="4"/>
-        <v>410</v>
+        <v>419</v>
       </c>
       <c r="Q54" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -6168,7 +6174,7 @@
     </row>
     <row r="55" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B55" s="2">
-        <v>45228</v>
+        <v>45227</v>
       </c>
       <c r="C55" s="21">
         <f t="shared" si="8"/>
@@ -6186,29 +6192,36 @@
         <v>1.0480392156862746</v>
       </c>
       <c r="M55">
-        <v>375</v>
+        <v>410</v>
       </c>
       <c r="N55" s="12">
-        <v>45194</v>
+        <v>45209</v>
       </c>
     </row>
     <row r="56" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B56" s="28"/>
-      <c r="C56" s="21"/>
-      <c r="D56" s="23"/>
+      <c r="B56" s="2">
+        <v>45229</v>
+      </c>
+      <c r="C56" s="21">
+        <f t="shared" si="8"/>
+        <v>1439</v>
+      </c>
+      <c r="D56" s="23">
+        <v>22819</v>
+      </c>
       <c r="E56" s="24">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>67.114705882352936</v>
       </c>
       <c r="F56" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1.1185784313725491</v>
       </c>
       <c r="M56">
-        <v>349</v>
+        <v>375</v>
       </c>
       <c r="N56" s="12">
-        <v>45161</v>
+        <v>45194</v>
       </c>
     </row>
     <row r="57" spans="2:17" x14ac:dyDescent="0.2">
@@ -6224,10 +6237,10 @@
         <v>0</v>
       </c>
       <c r="M57">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="N57" s="12">
-        <v>45142</v>
+        <v>45161</v>
       </c>
     </row>
     <row r="58" spans="2:17" x14ac:dyDescent="0.2">
@@ -6246,10 +6259,10 @@
         <v>0</v>
       </c>
       <c r="M58">
-        <v>300</v>
+        <v>346</v>
       </c>
       <c r="N58" s="12">
-        <v>45181</v>
+        <v>45142</v>
       </c>
     </row>
     <row r="59" spans="2:17" x14ac:dyDescent="0.2">
@@ -6265,10 +6278,10 @@
         <v>0</v>
       </c>
       <c r="M59">
-        <v>272</v>
+        <v>300</v>
       </c>
       <c r="N59" s="12">
-        <v>45188</v>
+        <v>45181</v>
       </c>
     </row>
     <row r="60" spans="2:17" x14ac:dyDescent="0.2">
@@ -6284,10 +6297,10 @@
         <v>0</v>
       </c>
       <c r="M60">
-        <v>220</v>
+        <v>272</v>
       </c>
       <c r="N60" s="12">
-        <v>45175</v>
+        <v>45188</v>
       </c>
     </row>
     <row r="61" spans="2:17" x14ac:dyDescent="0.2">
@@ -6303,10 +6316,10 @@
         <v>0</v>
       </c>
       <c r="M61">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="N61" s="12">
-        <v>45173</v>
+        <v>45175</v>
       </c>
     </row>
     <row r="62" spans="2:17" x14ac:dyDescent="0.2">
@@ -6322,10 +6335,10 @@
         <v>0</v>
       </c>
       <c r="M62">
-        <v>159</v>
+        <v>217</v>
       </c>
       <c r="N62" s="12">
-        <v>45182</v>
+        <v>45173</v>
       </c>
     </row>
     <row r="63" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -6341,50 +6354,50 @@
         <v>0</v>
       </c>
       <c r="M63">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="N63" s="12">
-        <v>45139</v>
+        <v>45182</v>
       </c>
     </row>
     <row r="64" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M64">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="N64" s="12">
-        <v>45210</v>
+        <v>45139</v>
       </c>
     </row>
     <row r="65" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M65">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="N65" s="12">
-        <v>45162</v>
+        <v>45210</v>
       </c>
     </row>
     <row r="66" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M66">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="N66" s="12">
-        <v>45196</v>
+        <v>45162</v>
       </c>
     </row>
     <row r="67" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M67">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="N67" s="12">
-        <v>45152</v>
+        <v>45196</v>
       </c>
     </row>
     <row r="68" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M68">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="N68" s="12">
-        <v>45195</v>
+        <v>45152</v>
       </c>
     </row>
     <row r="69" spans="13:14" x14ac:dyDescent="0.2">
@@ -6392,89 +6405,92 @@
         <v>143</v>
       </c>
       <c r="N69" s="12">
-        <v>45212</v>
+        <v>45195</v>
       </c>
     </row>
     <row r="70" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M70">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="N70" s="12">
-        <v>45153</v>
+        <v>45212</v>
       </c>
     </row>
     <row r="71" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M71">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="N71" s="12">
-        <v>45187</v>
+        <v>45153</v>
       </c>
     </row>
     <row r="72" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M72">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="N72" s="12">
-        <v>45168</v>
+        <v>45187</v>
       </c>
     </row>
     <row r="73" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M73">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="N73" s="12">
-        <v>45147</v>
+        <v>45168</v>
       </c>
     </row>
     <row r="74" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M74">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="N74" s="12">
-        <v>45183</v>
+        <v>45147</v>
       </c>
     </row>
     <row r="75" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M75">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="N75">
-        <v>45164</v>
+        <v>45183</v>
       </c>
     </row>
     <row r="76" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M76">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="N76">
-        <v>45140</v>
+        <v>45164</v>
       </c>
     </row>
     <row r="77" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M77">
-        <v>29.1</v>
+        <v>38</v>
       </c>
       <c r="N77">
-        <v>45138</v>
+        <v>45140</v>
       </c>
     </row>
     <row r="78" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M78">
-        <v>0</v>
+        <v>29.1</v>
       </c>
       <c r="N78">
-        <v>45218</v>
+        <v>45138</v>
       </c>
     </row>
     <row r="79" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M79">
-        <v>-3080</v>
+        <v>0</v>
+      </c>
+      <c r="N79">
+        <v>45218</v>
       </c>
     </row>
     <row r="80" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M80">
-        <v>0</v>
+        <v>-3080</v>
       </c>
     </row>
     <row r="81" spans="13:13" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Abstract finished, discussion and conclusion almost
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C8E49E5-DC7B-094B-9294-9A1B12582BFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982DCB72-DAF2-D540-8D5B-083A91621B2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="15080" windowHeight="16940" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
@@ -1031,7 +1031,7 @@
                   <c:v>21380</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>22819</c:v>
+                  <c:v>23413</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1398,13 +1398,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2018</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>1456</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1385</c:v>
@@ -1590,13 +1590,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2033</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1439</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1941,10 +1941,10 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$7:$C$55</c:f>
+              <c:f>Sheet1!$C$7:$C$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="49"/>
+                <c:ptCount val="50"/>
                 <c:pt idx="0">
                   <c:v>156</c:v>
                 </c:pt>
@@ -2091,6 +2091,9 @@
                 </c:pt>
                 <c:pt idx="48">
                   <c:v>1456</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2033</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4446,8 +4449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4213BD91-B5D1-3B47-8D3F-04331482504C}">
   <dimension ref="A1:Q86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="B33" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4700,7 +4703,7 @@
       <c r="I12" s="30"/>
       <c r="J12" s="10">
         <f>J8-MAX(D6:D63)</f>
-        <v>-2419</v>
+        <v>-3013</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
@@ -4756,7 +4759,7 @@
       <c r="I14" s="34"/>
       <c r="J14" s="11">
         <f>J12/J13</f>
-        <v>-3.2848537604456829</v>
+        <v>-4.0914693593314766</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
@@ -5095,23 +5098,23 @@
       </c>
       <c r="M29" cm="1">
         <f t="array" ref="M29:M86">_xlfn.SORTBY(C6:C63, C6:C63, -1)</f>
-        <v>2018</v>
+        <v>2033</v>
       </c>
       <c r="N29" s="12" cm="1">
         <f t="array" ref="N29:N79">_xlfn.SORTBY(B6:B56,C6:C56, -1)</f>
-        <v>45226</v>
+        <v>45229</v>
       </c>
       <c r="O29" t="str">
         <f ca="1">IF(N29=TODAY(), "Green", "Blue")</f>
-        <v>Blue</v>
-      </c>
-      <c r="P29">
+        <v>Green</v>
+      </c>
+      <c r="P29" t="str">
         <f ca="1">IF(NOT(N29=TODAY()), M29, "")</f>
-        <v>2018</v>
-      </c>
-      <c r="Q29" t="str">
+        <v/>
+      </c>
+      <c r="Q29">
         <f ca="1">IF(N29=TODAY(), M29, "")</f>
-        <v/>
+        <v>2033</v>
       </c>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.2">
@@ -5140,10 +5143,10 @@
         <v>17</v>
       </c>
       <c r="M30">
-        <v>1456</v>
+        <v>2018</v>
       </c>
       <c r="N30" s="12">
-        <v>45227</v>
+        <v>45226</v>
       </c>
       <c r="O30" t="str">
         <f t="shared" ref="O30:O54" ca="1" si="3">IF(N30=TODAY(), "Green", "Blue")</f>
@@ -5151,7 +5154,7 @@
       </c>
       <c r="P30">
         <f t="shared" ref="P30:P54" ca="1" si="4">IF(NOT(N30=TODAY()), M30, "")</f>
-        <v>1456</v>
+        <v>2018</v>
       </c>
       <c r="Q30" t="str">
         <f t="shared" ref="Q30:Q54" ca="1" si="5">IF(N30=TODAY(), M30, "")</f>
@@ -5184,22 +5187,22 @@
         <v>18</v>
       </c>
       <c r="M31">
-        <v>1439</v>
+        <v>1456</v>
       </c>
       <c r="N31" s="12">
-        <v>45229</v>
+        <v>45227</v>
       </c>
       <c r="O31" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>Green</v>
-      </c>
-      <c r="P31" t="str">
+        <v>Blue</v>
+      </c>
+      <c r="P31">
         <f t="shared" ca="1" si="4"/>
+        <v>1456</v>
+      </c>
+      <c r="Q31" t="str">
+        <f t="shared" ca="1" si="5"/>
         <v/>
-      </c>
-      <c r="Q31">
-        <f t="shared" ca="1" si="5"/>
-        <v>1439</v>
       </c>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.2">
@@ -6204,18 +6207,18 @@
       </c>
       <c r="C56" s="21">
         <f t="shared" si="8"/>
-        <v>1439</v>
+        <v>2033</v>
       </c>
       <c r="D56" s="23">
-        <v>22819</v>
+        <v>23413</v>
       </c>
       <c r="E56" s="24">
         <f t="shared" si="6"/>
-        <v>67.114705882352936</v>
+        <v>68.861764705882351</v>
       </c>
       <c r="F56" s="4">
         <f t="shared" si="7"/>
-        <v>1.1185784313725491</v>
+        <v>1.1476960784313726</v>
       </c>
       <c r="M56">
         <v>375</v>
@@ -6246,8 +6249,8 @@
     <row r="58" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B58" s="28"/>
       <c r="C58" s="21">
-        <f>SUM(C47:C55)/340</f>
-        <v>29.1</v>
+        <f>SUM(C47:C56)/340</f>
+        <v>35.079411764705881</v>
       </c>
       <c r="D58" s="23"/>
       <c r="E58" s="24">
@@ -6474,7 +6477,7 @@
     </row>
     <row r="78" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M78">
-        <v>29.1</v>
+        <v>35.079411764705881</v>
       </c>
       <c r="N78">
         <v>45138</v>

</xml_diff>

<commit_message>
All text written, now move stuff to SI and proofread
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F4CDD9-0716-EA49-8AF7-06C7F1200F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B50518DA-F147-D240-9D29-B7BE417533B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="15420" windowHeight="16940" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
@@ -1037,7 +1037,7 @@
                   <c:v>23413</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>23545</c:v>
+                  <c:v>23734</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4455,8 +4455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4213BD91-B5D1-3B47-8D3F-04331482504C}">
   <dimension ref="A1:Q86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B14" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4709,7 +4709,7 @@
       <c r="I12" s="30"/>
       <c r="J12" s="10">
         <f>J8-MAX(D6:D63)</f>
-        <v>-3145</v>
+        <v>-3334</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
@@ -4765,7 +4765,7 @@
       <c r="I14" s="34"/>
       <c r="J14" s="11">
         <f>J12/J13</f>
-        <v>-4.2707172701949867</v>
+        <v>-4.5273676880222844</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
@@ -6239,18 +6239,18 @@
       </c>
       <c r="C57" s="21">
         <f t="shared" si="8"/>
-        <v>132</v>
+        <v>321</v>
       </c>
       <c r="D57" s="23">
-        <v>23545</v>
+        <v>23734</v>
       </c>
       <c r="E57" s="24">
         <f t="shared" si="6"/>
-        <v>69.25</v>
+        <v>69.805882352941182</v>
       </c>
       <c r="F57" s="4">
         <f t="shared" si="7"/>
-        <v>1.1541666666666666</v>
+        <v>1.1634313725490195</v>
       </c>
       <c r="M57">
         <v>349</v>
@@ -6294,7 +6294,7 @@
         <v>0</v>
       </c>
       <c r="M59">
-        <v>300</v>
+        <v>321</v>
       </c>
       <c r="N59" s="12">
         <v>45181</v>
@@ -6313,7 +6313,7 @@
         <v>0</v>
       </c>
       <c r="M60">
-        <v>272</v>
+        <v>300</v>
       </c>
       <c r="N60" s="12">
         <v>45188</v>
@@ -6332,7 +6332,7 @@
         <v>0</v>
       </c>
       <c r="M61">
-        <v>220</v>
+        <v>272</v>
       </c>
       <c r="N61" s="12">
         <v>45175</v>
@@ -6351,7 +6351,7 @@
         <v>0</v>
       </c>
       <c r="M62">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="N62" s="12">
         <v>45173</v>
@@ -6370,7 +6370,7 @@
         <v>0</v>
       </c>
       <c r="M63">
-        <v>159</v>
+        <v>217</v>
       </c>
       <c r="N63" s="12">
         <v>45182</v>
@@ -6378,7 +6378,7 @@
     </row>
     <row r="64" spans="2:17" x14ac:dyDescent="0.2">
       <c r="M64">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="N64" s="12">
         <v>45139</v>
@@ -6386,7 +6386,7 @@
     </row>
     <row r="65" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M65">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="N65" s="12">
         <v>45210</v>
@@ -6394,7 +6394,7 @@
     </row>
     <row r="66" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M66">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="N66" s="12">
         <v>45162</v>
@@ -6402,7 +6402,7 @@
     </row>
     <row r="67" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M67">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="N67" s="12">
         <v>45196</v>
@@ -6410,7 +6410,7 @@
     </row>
     <row r="68" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M68">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="N68" s="12">
         <v>45152</v>
@@ -6418,7 +6418,7 @@
     </row>
     <row r="69" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M69">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="N69" s="12">
         <v>45195</v>
@@ -6434,7 +6434,7 @@
     </row>
     <row r="71" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M71">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="N71" s="12">
         <v>45153</v>
@@ -6442,7 +6442,7 @@
     </row>
     <row r="72" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M72">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="N72" s="12">
         <v>45187</v>

</xml_diff>

<commit_message>
Finished with cover figure
</commit_message>
<xml_diff>
--- a/Writing/Keeping up with the Thesis.xlsx
+++ b/Writing/Keeping up with the Thesis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcusnorgaardweng/Documents/Kurser/Speciale/CatalysisThesis/Writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59EE4F09-644C-3E46-A9BC-603273F9A4C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0136A2-8163-BB4A-9D13-F0E031DE2E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="15420" windowHeight="16940" xr2:uid="{D9A0D74E-C532-634B-A410-F0487A6735A9}"/>
   </bookViews>
@@ -1043,7 +1043,7 @@
                   <c:v>23734</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>23515</c:v>
+                  <c:v>20735</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6271,18 +6271,18 @@
       </c>
       <c r="C58" s="21">
         <f t="shared" si="8"/>
-        <v>-219</v>
+        <v>-2999</v>
       </c>
       <c r="D58" s="23">
-        <v>23515</v>
+        <v>20735</v>
       </c>
       <c r="E58" s="24">
         <f t="shared" si="6"/>
-        <v>69.161764705882348</v>
+        <v>60.985294117647058</v>
       </c>
       <c r="F58" s="4">
         <f t="shared" si="7"/>
-        <v>1.1526960784313725</v>
+        <v>1.0164215686274509</v>
       </c>
       <c r="M58">
         <v>346</v>
@@ -6520,7 +6520,7 @@
     </row>
     <row r="80" spans="3:14" x14ac:dyDescent="0.2">
       <c r="M80">
-        <v>-219</v>
+        <v>-2999</v>
       </c>
     </row>
     <row r="81" spans="13:13" x14ac:dyDescent="0.2">

</xml_diff>